<commit_message>
Add in fixed macGenConverter.js script
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="0" windowWidth="25294" windowHeight="12549" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="4020" yWindow="0" windowWidth="24300" windowHeight="17100" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="settings" sheetId="4" r:id="rId3"/>
     <sheet name="choices" sheetId="6" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="140001"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
   <si>
     <t>comments</t>
   </si>
@@ -117,9 +117,6 @@
     <t>exampleForm</t>
   </si>
   <si>
-    <t>household_new</t>
-  </si>
-  <si>
     <t>imnci_test</t>
   </si>
   <si>
@@ -246,9 +243,6 @@
     <t>'?' + opendatakit.getHashString('../config/tables/exampleForm/forms/exampleForm/',null)</t>
   </si>
   <si>
-    <t>'?' + opendatakit.getHashString('../config/tables/household/forms/household_new/',null)</t>
-  </si>
-  <si>
     <t>'?' + opendatakit.getHashString('../config/tables/imnci/forms/imnci_test/',null)</t>
   </si>
   <si>
@@ -292,6 +286,15 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../config/tables/eonasdan/forms/eonasdan/',null)</t>
+  </si>
+  <si>
+    <t>table_id</t>
+  </si>
+  <si>
+    <t>household</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/household/forms/household/',null)</t>
   </si>
 </sst>
 </file>
@@ -819,13 +822,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.84375" customWidth="1"/>
-    <col min="2" max="2" width="20.84375" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -833,7 +836,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1">
       <c r="B2" t="s">
         <v>17</v>
       </c>
@@ -852,27 +855,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.15234375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="101.15234375" customWidth="1"/>
-    <col min="3" max="3" width="22.23046875" customWidth="1"/>
-    <col min="4" max="4" width="46.15234375" customWidth="1"/>
+    <col min="2" max="2" width="101.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.84375" customWidth="1"/>
-    <col min="8" max="8" width="31.4609375" customWidth="1"/>
-    <col min="9" max="9" width="22.15234375" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
+    <col min="8" max="8" width="31.5" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
         <v>16</v>
@@ -884,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>
@@ -894,7 +897,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -903,7 +906,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -911,16 +914,16 @@
         <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1">
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -931,547 +934,547 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1">
       <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1">
       <c r="C7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17.25" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.5" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.5" customHeight="1">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="66" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="17.5" customHeight="1">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="66" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17.25" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="17.5" customHeight="1">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="66" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="17.25" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="17.5" customHeight="1">
       <c r="A29" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="66" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G30" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="17.25" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="17.5" customHeight="1">
       <c r="A32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="66" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G33" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17.25" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17.5" customHeight="1">
       <c r="A35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G36" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="17.25" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="17.5" customHeight="1">
       <c r="A38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G39" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="17.25" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="17.5" customHeight="1">
       <c r="A41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G42" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="17.25" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="17.5" customHeight="1">
       <c r="A44" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="17.25" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="17.5" customHeight="1">
       <c r="A47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G48" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="17.25" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.5" customHeight="1">
       <c r="A50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="66" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G51" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="17.25" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="17.5" customHeight="1">
       <c r="A53" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="66" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="17.25" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="17.5" customHeight="1">
       <c r="A56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="66" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G57" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="17.25" customHeight="1">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="17.5" customHeight="1">
       <c r="A59" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="66" customHeight="1">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G60" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="17.25" customHeight="1">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="17.5" customHeight="1">
       <c r="A62" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="66" customHeight="1">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G63" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="17.25" customHeight="1">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="17.5" customHeight="1">
       <c r="A65" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="66" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G66" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="17.25" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="17.5" customHeight="1">
       <c r="A68" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="66" customHeight="1">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="17.25" customHeight="1">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="17.5" customHeight="1">
       <c r="A71" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="66" customHeight="1">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G72" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="17.25" customHeight="1">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1487,19 +1490,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.15234375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="24.69140625" customWidth="1"/>
-    <col min="4" max="4" width="41.23046875" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1513,101 +1516,110 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>20130828</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" ht="28" customHeight="1">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1">
       <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="16" spans="1:5" ht="12.75" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1">
       <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="12.75" customHeight="1">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="22" spans="1:3" ht="12.75" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1">
       <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="12.75" customHeight="1">
       <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+      <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,18 +1635,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.4609375" customWidth="1"/>
-    <col min="2" max="2" width="22.23046875" customWidth="1"/>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1645,18 +1657,18 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1667,18 +1679,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1689,7 +1701,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1700,191 +1712,191 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
         <v>35</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
         <v>47</v>
       </c>
-      <c r="C14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>52</v>
       </c>
-      <c r="C17" t="s">
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
         <v>54</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
         <v>61</v>
       </c>
-      <c r="C20" t="s">
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="C22" t="s">
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I think what I'm doing is committing all the changes I have made in my first week to the development branch of my own individual fork
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="0" windowWidth="24300" windowHeight="17100" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="4220" yWindow="1340" windowWidth="24300" windowHeight="17100" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="106">
   <si>
     <t>comments</t>
   </si>
@@ -295,6 +295,51 @@
   </si>
   <si>
     <t>'?' + opendatakit.getHashString('../config/tables/household/forms/household/',null)</t>
+  </si>
+  <si>
+    <t>screenClient</t>
+  </si>
+  <si>
+    <t>Screen Female Client</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/femaleClients/forms/screenClient/',null)</t>
+  </si>
+  <si>
+    <t>client6Week</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/femaleClients/forms/client6Week/',null)</t>
+  </si>
+  <si>
+    <t>Client 6 Week</t>
+  </si>
+  <si>
+    <t>client6Month</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/femaleClients/forms/client6Month/',null)</t>
+  </si>
+  <si>
+    <t>Client 6 Month</t>
+  </si>
+  <si>
+    <t>screenPartner</t>
+  </si>
+  <si>
+    <t>Screen Partner</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/maleClients/forms/screenPartner/',null)</t>
+  </si>
+  <si>
+    <t>partner6Month</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/maleClients/forms/partner6Month/',null)</t>
+  </si>
+  <si>
+    <t>Partner 6 Month</t>
   </si>
 </sst>
 </file>
@@ -342,8 +387,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -438,7 +495,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="91">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -478,6 +535,12 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -517,6 +580,12 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -853,10 +922,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1470,10 +1539,130 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.25" customHeight="1">
+    <row r="73" spans="1:7" ht="17" customHeight="1">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="62" customHeight="1">
+      <c r="A75" s="3"/>
+      <c r="B75" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E75" t="s">
+        <v>39</v>
+      </c>
+      <c r="G75" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A77" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="62" customHeight="1">
+      <c r="A78" s="3"/>
+      <c r="B78" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3"/>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="12" customHeight="1">
+      <c r="A80" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="58" customHeight="1">
+      <c r="A81" s="3"/>
+      <c r="B81" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E81" t="s">
+        <v>39</v>
+      </c>
+      <c r="G81" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A82" s="3"/>
+      <c r="B82" s="3"/>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="12" customHeight="1">
+      <c r="A83" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="58" customHeight="1">
+      <c r="A84" s="3"/>
+      <c r="B84" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E84" t="s">
+        <v>39</v>
+      </c>
+      <c r="G84" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A85" s="3"/>
+      <c r="B85" s="3"/>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="12" customHeight="1">
+      <c r="A86" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="58" customHeight="1">
+      <c r="A87" s="3"/>
+      <c r="B87" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E87" t="s">
+        <v>39</v>
+      </c>
+      <c r="G87" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="12.75" customHeight="1">
+      <c r="A88" s="3"/>
+      <c r="B88" s="3"/>
+      <c r="C88" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1633,10 +1822,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1899,6 +2088,61 @@
         <v>65</v>
       </c>
     </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
All sorts of red cross commits
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="49160" windowHeight="24680" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="49160" windowHeight="24680" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="65">
   <si>
     <t>comments</t>
   </si>
@@ -199,6 +199,24 @@
   </si>
   <si>
     <t>table_id</t>
+  </si>
+  <si>
+    <t>distribution_summary</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/distribution/forms/distribution/',null)</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/deployment/forms/deployment/',null)</t>
+  </si>
+  <si>
+    <t>deployment</t>
+  </si>
+  <si>
+    <t>Red Cross Distribution Summary</t>
+  </si>
+  <si>
+    <t>Red Cross Deployment</t>
   </si>
 </sst>
 </file>
@@ -251,8 +269,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,7 +408,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -436,6 +462,10 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -489,6 +519,10 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -827,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A34" sqref="A33:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1093,62 +1127,94 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1"/>
-    <row r="30" spans="1:7" ht="66" customHeight="1">
+    <row r="29" spans="1:7" ht="50" customHeight="1">
+      <c r="A29" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:7" ht="148" customHeight="1">
       <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
+      <c r="B30" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="17" customHeight="1">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1"/>
-    <row r="33" spans="1:2" ht="66" customHeight="1">
+      <c r="C31" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="50" customHeight="1">
+      <c r="A32" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" ht="148" customHeight="1">
       <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" ht="17" customHeight="1">
+      <c r="B33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="17" customHeight="1">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:2" ht="17.5" customHeight="1"/>
-    <row r="36" spans="1:2" ht="66" customHeight="1">
+      <c r="C34" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="36" spans="1:7" ht="66" customHeight="1">
       <c r="A36" s="5"/>
       <c r="B36" s="6"/>
     </row>
-    <row r="37" spans="1:2" ht="17" customHeight="1">
+    <row r="37" spans="1:7" ht="17" customHeight="1">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
     </row>
-    <row r="38" spans="1:2" ht="17.5" customHeight="1"/>
-    <row r="39" spans="1:2" ht="66" customHeight="1">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="39" spans="1:7" ht="66" customHeight="1">
       <c r="A39" s="5"/>
       <c r="B39" s="6"/>
     </row>
-    <row r="40" spans="1:2" ht="17" customHeight="1">
+    <row r="40" spans="1:7" ht="17" customHeight="1">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
     </row>
-    <row r="41" spans="1:2" ht="17.5" customHeight="1"/>
-    <row r="42" spans="1:2" ht="66" customHeight="1">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="42" spans="1:7" ht="66" customHeight="1">
       <c r="A42" s="5"/>
       <c r="B42" s="6"/>
     </row>
-    <row r="43" spans="1:2" ht="17" customHeight="1">
+    <row r="43" spans="1:7" ht="17" customHeight="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
     </row>
-    <row r="44" spans="1:2" ht="17.5" customHeight="1"/>
-    <row r="45" spans="1:2" ht="66" customHeight="1">
+    <row r="44" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="45" spans="1:7" ht="66" customHeight="1">
       <c r="A45" s="5"/>
       <c r="B45" s="6"/>
     </row>
-    <row r="46" spans="1:2" ht="17" customHeight="1">
+    <row r="46" spans="1:7" ht="17" customHeight="1">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
     </row>
-    <row r="47" spans="1:2" ht="17.5" customHeight="1"/>
-    <row r="48" spans="1:2" ht="66" customHeight="1">
+    <row r="47" spans="1:7" ht="17.5" customHeight="1"/>
+    <row r="48" spans="1:7" ht="66" customHeight="1">
       <c r="A48" s="5"/>
       <c r="B48" s="6"/>
     </row>
@@ -1243,7 +1309,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1384,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" x14ac:dyDescent="0"/>
@@ -1486,6 +1552,28 @@
         <v>50</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="42">
+      <c r="A9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Health Facility Survey Changes
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegan/Documents/app-designer/app/config/assets/framework/forms/framework/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="1340" windowWidth="24300" windowHeight="17100" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26740" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="109">
   <si>
     <t>comments</t>
   </si>
@@ -340,6 +348,15 @@
   </si>
   <si>
     <t>Partner 6 Month</t>
+  </si>
+  <si>
+    <t>health_facility</t>
+  </si>
+  <si>
+    <t>'?' + opendatakit.getHashString('../config/tables/health_facility/forms/health_facility/',null)</t>
+  </si>
+  <si>
+    <t>Health Facility</t>
   </si>
 </sst>
 </file>
@@ -891,13 +908,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="26.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -905,30 +922,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="101.1640625" customWidth="1"/>
     <col min="3" max="3" width="22.1640625" customWidth="1"/>
@@ -939,7 +951,7 @@
     <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -966,7 +978,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>20</v>
       </c>
@@ -975,7 +987,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" t="s">
         <v>24</v>
       </c>
@@ -986,13 +998,13 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -1003,23 +1015,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>67</v>
@@ -1031,20 +1043,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>68</v>
@@ -1056,20 +1068,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>69</v>
@@ -1081,20 +1093,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.5" customHeight="1">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>70</v>
@@ -1106,20 +1118,20 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.5" customHeight="1">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1">
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>71</v>
@@ -1131,19 +1143,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.5" customHeight="1">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1">
+    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>72</v>
@@ -1155,19 +1167,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.5" customHeight="1">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>90</v>
@@ -1179,19 +1191,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.5" customHeight="1">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1">
+    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>73</v>
@@ -1203,19 +1215,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" customHeight="1">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.5" customHeight="1">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1">
+    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>74</v>
@@ -1227,19 +1239,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.5" customHeight="1">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1">
+    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>75</v>
@@ -1251,19 +1263,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.5" customHeight="1">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1">
+    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>76</v>
@@ -1275,19 +1287,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.25" customHeight="1">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.5" customHeight="1">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1">
+    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>77</v>
@@ -1299,19 +1311,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" customHeight="1">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.5" customHeight="1">
+    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1">
+    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
         <v>78</v>
@@ -1323,19 +1335,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.5" customHeight="1">
+    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1">
+    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
         <v>79</v>
@@ -1347,19 +1359,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.5" customHeight="1">
+    <row r="50" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1">
+    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>80</v>
@@ -1371,19 +1383,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" customHeight="1">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.5" customHeight="1">
+    <row r="53" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1">
+    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
         <v>81</v>
@@ -1395,19 +1407,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.25" customHeight="1">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.5" customHeight="1">
+    <row r="56" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1">
+    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
         <v>82</v>
@@ -1419,19 +1431,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.5" customHeight="1">
+    <row r="59" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1">
+    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
         <v>83</v>
@@ -1443,19 +1455,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.25" customHeight="1">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.5" customHeight="1">
+    <row r="62" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1">
+    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
         <v>84</v>
@@ -1467,19 +1479,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.25" customHeight="1">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.5" customHeight="1">
+    <row r="65" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1">
+    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
         <v>85</v>
@@ -1491,19 +1503,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.25" customHeight="1">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.5" customHeight="1">
+    <row r="68" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1">
+    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
         <v>86</v>
@@ -1515,19 +1527,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.25" customHeight="1">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.5" customHeight="1">
+    <row r="71" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1">
+    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
         <v>87</v>
@@ -1539,19 +1551,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17" customHeight="1">
+    <row r="73" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="12.75" customHeight="1">
+    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="62" customHeight="1">
+    <row r="75" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
         <v>93</v>
@@ -1563,19 +1575,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="12.75" customHeight="1">
+    <row r="76" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="12.75" customHeight="1">
+    <row r="77" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="62" customHeight="1">
+    <row r="78" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
         <v>95</v>
@@ -1587,19 +1599,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="12.75" customHeight="1">
+    <row r="79" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="12" customHeight="1">
+    <row r="80" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="58" customHeight="1">
+    <row r="81" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
         <v>98</v>
@@ -1611,19 +1623,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="12.75" customHeight="1">
+    <row r="82" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="12" customHeight="1">
+    <row r="83" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="58" customHeight="1">
+    <row r="84" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
       <c r="B84" s="4" t="s">
         <v>102</v>
@@ -1635,19 +1647,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="12.75" customHeight="1">
+    <row r="85" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="12" customHeight="1">
+    <row r="86" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="58" customHeight="1">
+    <row r="87" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="3"/>
       <c r="B87" s="4" t="s">
         <v>104</v>
@@ -1659,21 +1671,40 @@
         <v>40</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="12.75" customHeight="1">
+    <row r="88" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" t="s">
         <v>38</v>
       </c>
     </row>
+    <row r="89" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="3"/>
+      <c r="B90" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E90" t="s">
+        <v>39</v>
+      </c>
+      <c r="G90" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="3"/>
+      <c r="B91" s="3"/>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1685,13 +1716,13 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.75" customHeight="1">
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -1708,7 +1739,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="18.75" customHeight="1">
+    <row r="2" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>88</v>
       </c>
@@ -1717,7 +1748,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="18.75" customHeight="1">
+    <row r="3" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1729,7 +1760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.75" customHeight="1">
+    <row r="4" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1740,7 +1771,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28" customHeight="1">
+    <row r="5" spans="1:5" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1754,88 +1785,83 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.75" customHeight="1">
+    <row r="6" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="18.75" customHeight="1">
+    <row r="7" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="9" spans="1:5" ht="18.75" customHeight="1"/>
-    <row r="10" spans="1:5" ht="18.75" customHeight="1">
+    <row r="8" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="9" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="10" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="18.75" customHeight="1">
+    <row r="11" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1">
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="18.75" customHeight="1">
+    <row r="13" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="12.75" customHeight="1">
+    <row r="16" spans="1:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="12.75" customHeight="1">
+    <row r="17" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" ht="12.75" customHeight="1">
+    <row r="18" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="12.75" customHeight="1">
+    <row r="19" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="12.75" customHeight="1">
+    <row r="22" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="12.75" customHeight="1">
+    <row r="23" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="12.75" customHeight="1">
+    <row r="24" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" ht="12.75" customHeight="1">
+    <row r="25" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.5" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +1872,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>27</v>
       </c>
@@ -1857,7 +1883,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>27</v>
       </c>
@@ -1868,7 +1894,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
@@ -1879,7 +1905,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="3" t="s">
         <v>27</v>
       </c>
@@ -1901,7 +1927,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -1912,7 +1938,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>27</v>
       </c>
@@ -1923,7 +1949,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +1960,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -1945,7 +1971,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1956,7 +1982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="3" t="s">
         <v>27</v>
       </c>
@@ -1967,7 +1993,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="3" t="s">
         <v>27</v>
       </c>
@@ -1978,7 +2004,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1989,7 +2015,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
@@ -2000,7 +2026,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -2011,7 +2037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>27</v>
       </c>
@@ -2022,7 +2048,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="3" t="s">
         <v>27</v>
       </c>
@@ -2033,7 +2059,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
@@ -2044,7 +2070,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -2055,7 +2081,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
@@ -2066,7 +2092,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -2077,7 +2103,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -2088,7 +2114,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -2099,7 +2125,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -2110,7 +2136,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -2121,7 +2147,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -2132,7 +2158,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2141,15 +2167,21 @@
       </c>
       <c r="C28" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates to library versions and miscellaneous bug fixes. Update scan designer to emit display.prompt.text and display.title.text
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="4"/>
+    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -378,9 +378,6 @@
     <t>सामान्य जावास्क्रिप्ट फ़्रेमवर्क</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -438,13 +435,7 @@
     <t>display.hint.text</t>
   </si>
   <si>
-    <t>display.title.text</t>
-  </si>
-  <si>
     <t>display.title.text.hindi</t>
-  </si>
-  <si>
-    <t>display.locale.text</t>
   </si>
   <si>
     <t>display.locale.text.hindi</t>
@@ -727,6 +718,15 @@
   </si>
   <si>
     <t>जारी रहना</t>
+  </si>
+  <si>
+    <t>display.title.text.english</t>
+  </si>
+  <si>
+    <t>display.locale.text.english</t>
+  </si>
+  <si>
+    <t>english</t>
   </si>
 </sst>
 </file>
@@ -1359,10 +1359,10 @@
         <v>35</v>
       </c>
       <c r="G1" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" t="s">
         <v>134</v>
-      </c>
-      <c r="H1" t="s">
-        <v>135</v>
       </c>
       <c r="I1" s="2"/>
     </row>
@@ -2081,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2099,16 +2099,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>227</v>
+      </c>
+      <c r="F1" t="s">
         <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" t="s">
-        <v>139</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -2174,24 +2174,24 @@
     </row>
     <row r="7" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>228</v>
+      </c>
+      <c r="E7" t="s">
         <v>116</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>117</v>
-      </c>
-      <c r="F7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
         <v>119</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>120</v>
-      </c>
-      <c r="F8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
@@ -2608,7 +2608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2624,50 +2624,50 @@
         <v>104</v>
       </c>
       <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
         <v>132</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2683,40 +2683,40 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B8" t="s">
         <v>110</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B9" t="s">
         <v>111</v>
       </c>
       <c r="C9" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C10" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B11" t="s">
         <v>112</v>
@@ -2732,255 +2732,255 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B24" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B28" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>178</v>
+      </c>
+      <c r="B33" t="s">
         <v>181</v>
-      </c>
-      <c r="B33" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B34" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B35" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="161.69999999999999" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B36" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B40" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B41" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B42" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B43" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B45" t="s">
         <v>108</v>
@@ -2991,82 +2991,82 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B46" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B47" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B48" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B49" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B51" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B53" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B54" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B55" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: table specific translation failure. Example form changed to illustrate use of table specific translations.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="2"/>
+    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="233">
   <si>
     <t>comments</t>
   </si>
@@ -727,6 +727,18 @@
   </si>
   <si>
     <t>english</t>
+  </si>
+  <si>
+    <t>invalid_numeric_message</t>
+  </si>
+  <si>
+    <t>Numeric value expected</t>
+  </si>
+  <si>
+    <t>Integer value expected</t>
+  </si>
+  <si>
+    <t>invalid_integer_message</t>
   </si>
 </sst>
 </file>
@@ -1324,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2081,8 +2093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2606,10 +2618,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -3069,6 +3081,22 @@
         <v>222</v>
       </c>
     </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>229</v>
+      </c>
+      <c r="B56" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>232</v>
+      </c>
+      <c r="B57" t="s">
+        <v>231</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
small changes to translations support and dist_ben_detail
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\toolsuite\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/assets/framework/forms/framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="1"/>
+    <workbookView xWindow="4220" yWindow="1340" windowWidth="24300" windowHeight="17100" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
     <sheet name="survey" sheetId="1" r:id="rId2"/>
-    <sheet name="settings" sheetId="4" r:id="rId3"/>
-    <sheet name="choices" sheetId="6" r:id="rId4"/>
-    <sheet name="framework_translations" sheetId="7" r:id="rId5"/>
+    <sheet name="common_translations" sheetId="8" r:id="rId3"/>
+    <sheet name="settings" sheetId="4" r:id="rId4"/>
+    <sheet name="choices" sheetId="6" r:id="rId5"/>
+    <sheet name="framework_translations" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="243">
   <si>
     <t>comments</t>
   </si>
@@ -740,11 +744,41 @@
   <si>
     <t>invalid_integer_message</t>
   </si>
+  <si>
+    <t>select_user</t>
+  </si>
+  <si>
+    <t>Please Select User</t>
+  </si>
+  <si>
+    <t>text.spanish</t>
+  </si>
+  <si>
+    <t>por favor</t>
+  </si>
+  <si>
+    <t>display.locale.text.spanish</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>spanish</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>Espanol</t>
+  </si>
+  <si>
+    <t>display.title.text.spanish</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1303,13 +1337,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="26.875" customWidth="1"/>
-    <col min="2" max="2" width="20.875" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1317,18 +1351,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1336,22 +1365,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="101.125" customWidth="1"/>
-    <col min="3" max="3" width="22.125" customWidth="1"/>
-    <col min="4" max="4" width="46.125" customWidth="1"/>
+    <col min="2" max="2" width="101.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.875" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" customWidth="1"/>
     <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="22.125" customWidth="1"/>
+    <col min="9" max="9" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1378,7 +1407,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>18</v>
       </c>
@@ -1387,7 +1416,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" t="s">
         <v>22</v>
       </c>
@@ -1398,13 +1427,13 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>20</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>2</v>
       </c>
@@ -1415,23 +1444,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" s="4" t="s">
         <v>65</v>
@@ -1443,20 +1472,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="3"/>
       <c r="B12" s="4" t="s">
         <v>66</v>
@@ -1468,20 +1497,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="3"/>
       <c r="B15" s="4" t="s">
         <v>67</v>
@@ -1493,20 +1522,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="3"/>
       <c r="B18" s="4" t="s">
         <v>68</v>
@@ -1518,20 +1547,20 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="3"/>
       <c r="B21" s="4" t="s">
         <v>69</v>
@@ -1543,19 +1572,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
         <v>70</v>
@@ -1567,19 +1596,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
       <c r="B27" s="4" t="s">
         <v>88</v>
@@ -1591,19 +1620,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
         <v>71</v>
@@ -1615,19 +1644,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
       <c r="B33" s="4" t="s">
         <v>72</v>
@@ -1639,19 +1668,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
         <v>73</v>
@@ -1663,19 +1692,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="3"/>
       <c r="B39" s="4" t="s">
         <v>74</v>
@@ -1687,19 +1716,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="3"/>
       <c r="B42" s="4" t="s">
         <v>75</v>
@@ -1711,19 +1740,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="3"/>
       <c r="B45" s="4" t="s">
         <v>76</v>
@@ -1735,19 +1764,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="3"/>
       <c r="B48" s="4" t="s">
         <v>77</v>
@@ -1759,19 +1788,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="3"/>
       <c r="B51" s="4" t="s">
         <v>78</v>
@@ -1783,19 +1812,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="3"/>
       <c r="B54" s="4" t="s">
         <v>79</v>
@@ -1807,19 +1836,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="3"/>
       <c r="B57" s="4" t="s">
         <v>80</v>
@@ -1831,19 +1860,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="s">
         <v>81</v>
@@ -1855,19 +1884,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="3"/>
       <c r="B63" s="4" t="s">
         <v>82</v>
@@ -1879,19 +1908,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="3"/>
       <c r="B66" s="4" t="s">
         <v>83</v>
@@ -1903,19 +1932,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="3"/>
       <c r="B69" s="4" t="s">
         <v>84</v>
@@ -1927,19 +1956,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="65.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="3"/>
       <c r="B72" s="4" t="s">
         <v>85</v>
@@ -1951,19 +1980,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.05" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="62.05" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="3"/>
       <c r="B75" s="4" t="s">
         <v>91</v>
@@ -1975,19 +2004,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="62.05" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="3"/>
       <c r="B78" s="4" t="s">
         <v>93</v>
@@ -1999,19 +2028,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="3"/>
       <c r="B81" s="4" t="s">
         <v>96</v>
@@ -2023,19 +2052,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="3"/>
       <c r="B84" s="4" t="s">
         <v>100</v>
@@ -2047,19 +2076,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="11.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="58" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="3"/>
       <c r="B87" s="4" t="s">
         <v>102</v>
@@ -2071,7 +2100,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" t="s">
@@ -2081,29 +2110,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="6" width="24.625" customWidth="1"/>
-    <col min="7" max="7" width="41.125" customWidth="1"/>
+    <col min="1" max="1" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -2113,23 +2179,29 @@
       <c r="C1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>227</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>86</v>
       </c>
@@ -2140,8 +2212,10 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2152,22 +2226,24 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2175,448 +2251,467 @@
         <v>11</v>
       </c>
       <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
         <v>115</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="b">
+      <c r="J5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>228</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>116</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>238</v>
+      </c>
+      <c r="H7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>118</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>119</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="2" t="s">
+        <v>239</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-    </row>
-    <row r="22" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:6" ht="12.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.125" customWidth="1"/>
-    <col min="3" max="3" width="34" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" t="s">
-        <v>58</v>
-      </c>
-      <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>92</v>
-      </c>
-      <c r="C25" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18.5" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C57"/>
   <sheetViews>
@@ -2624,14 +2719,14 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="49.75" customWidth="1"/>
-    <col min="2" max="2" width="73.25" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="49.6640625" customWidth="1"/>
+    <col min="2" max="2" width="73.1640625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -2642,7 +2737,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>121</v>
       </c>
@@ -2650,7 +2745,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>122</v>
       </c>
@@ -2658,7 +2753,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>123</v>
       </c>
@@ -2666,7 +2761,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>128</v>
       </c>
@@ -2674,7 +2769,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>130</v>
       </c>
@@ -2682,7 +2777,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>105</v>
       </c>
@@ -2693,7 +2788,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -2704,7 +2799,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -2715,7 +2810,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -2726,7 +2821,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>204</v>
       </c>
@@ -2734,7 +2829,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2742,7 +2837,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -2750,7 +2845,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>143</v>
       </c>
@@ -2758,7 +2853,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>144</v>
       </c>
@@ -2766,7 +2861,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>145</v>
       </c>
@@ -2774,7 +2869,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>146</v>
       </c>
@@ -2782,7 +2877,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>147</v>
       </c>
@@ -2790,7 +2885,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -2798,7 +2893,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>151</v>
       </c>
@@ -2806,7 +2901,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>153</v>
       </c>
@@ -2814,7 +2909,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>155</v>
       </c>
@@ -2822,7 +2917,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>157</v>
       </c>
@@ -2830,7 +2925,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>159</v>
       </c>
@@ -2838,7 +2933,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>161</v>
       </c>
@@ -2846,7 +2941,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>163</v>
       </c>
@@ -2854,7 +2949,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>170</v>
       </c>
@@ -2862,7 +2957,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>184</v>
       </c>
@@ -2870,7 +2965,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>173</v>
       </c>
@@ -2878,7 +2973,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>174</v>
       </c>
@@ -2886,7 +2981,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>176</v>
       </c>
@@ -2894,7 +2989,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -2902,7 +2997,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>179</v>
       </c>
@@ -2910,7 +3005,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>182</v>
       </c>
@@ -2918,7 +3013,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="161.69999999999999" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="169" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>185</v>
       </c>
@@ -2926,7 +3021,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>187</v>
       </c>
@@ -2934,7 +3029,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>191</v>
       </c>
@@ -2942,7 +3037,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>190</v>
       </c>
@@ -2950,7 +3045,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
         <v>193</v>
       </c>
@@ -2958,7 +3053,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>195</v>
       </c>
@@ -2966,7 +3061,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
         <v>197</v>
       </c>
@@ -2974,7 +3069,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
         <v>199</v>
       </c>
@@ -2982,7 +3077,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
         <v>201</v>
       </c>
@@ -2990,7 +3085,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -3001,7 +3096,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
         <v>205</v>
       </c>
@@ -3009,7 +3104,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
         <v>206</v>
       </c>
@@ -3017,7 +3112,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
         <v>208</v>
       </c>
@@ -3025,7 +3120,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
         <v>210</v>
       </c>
@@ -3033,7 +3128,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="13.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
         <v>212</v>
       </c>
@@ -3041,7 +3136,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
         <v>216</v>
       </c>
@@ -3049,7 +3144,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
         <v>217</v>
       </c>
@@ -3057,7 +3152,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
         <v>218</v>
       </c>
@@ -3065,7 +3160,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
         <v>219</v>
       </c>
@@ -3073,7 +3168,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
         <v>220</v>
       </c>
@@ -3081,7 +3176,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
         <v>229</v>
       </c>
@@ -3089,7 +3184,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
         <v>232</v>
       </c>

</xml_diff>

<commit_message>
a little over half of translations implemented.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="1340" windowWidth="24300" windowHeight="17100" activeTab="4"/>
+    <workbookView xWindow="18600" yWindow="13580" windowWidth="24300" windowHeight="17100" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="296">
   <si>
     <t>comments</t>
   </si>
@@ -754,9 +754,6 @@
     <t>text.spanish</t>
   </si>
   <si>
-    <t>por favor</t>
-  </si>
-  <si>
     <t>display.locale.text.spanish</t>
   </si>
   <si>
@@ -773,13 +770,175 @@
   </si>
   <si>
     <t>display.title.text.spanish</t>
+  </si>
+  <si>
+    <t>Seleccione usuario</t>
+  </si>
+  <si>
+    <t>main_title</t>
+  </si>
+  <si>
+    <t>Disaster Relief</t>
+  </si>
+  <si>
+    <t>registration_path</t>
+  </si>
+  <si>
+    <t>delivery_path</t>
+  </si>
+  <si>
+    <t>data_path</t>
+  </si>
+  <si>
+    <t>override_path</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>View Data</t>
+  </si>
+  <si>
+    <t>Administrator Overrides</t>
+  </si>
+  <si>
+    <t>Registro</t>
+  </si>
+  <si>
+    <t>Entrega</t>
+  </si>
+  <si>
+    <t>Ver Datos</t>
+  </si>
+  <si>
+    <t>registration_title</t>
+  </si>
+  <si>
+    <t>Register Beneficiary Code</t>
+  </si>
+  <si>
+    <t>delivery_title</t>
+  </si>
+  <si>
+    <t>Verify Beneficiary Code</t>
+  </si>
+  <si>
+    <t>Alivio de Desastres</t>
+  </si>
+  <si>
+    <t>Anulación del Administrador</t>
+  </si>
+  <si>
+    <t>Registro del Código de Beneficiario</t>
+  </si>
+  <si>
+    <t>Verificar el Código del Beneficiario</t>
+  </si>
+  <si>
+    <t>disabled_beneficiary_notification</t>
+  </si>
+  <si>
+    <t>This beneficiary is disabled</t>
+  </si>
+  <si>
+    <t>missing_beneficiary_notification</t>
+  </si>
+  <si>
+    <t>Scanned code not found in system</t>
+  </si>
+  <si>
+    <t>Este beneficiario está deshabilitado</t>
+  </si>
+  <si>
+    <t>Código del beneficiario no encontrado en el sistema</t>
+  </si>
+  <si>
+    <t>barcode_available</t>
+  </si>
+  <si>
+    <t>Barcode Available</t>
+  </si>
+  <si>
+    <t>Código disponible</t>
+  </si>
+  <si>
+    <t>voucher_detected</t>
+  </si>
+  <si>
+    <t>Voucher Barcode Detected</t>
+  </si>
+  <si>
+    <t>Código del vale detectado</t>
+  </si>
+  <si>
+    <t>barcode_unavailable</t>
+  </si>
+  <si>
+    <t>Barcode Unavailable</t>
+  </si>
+  <si>
+    <t>Beneficiario no disponible</t>
+  </si>
+  <si>
+    <t>already_qualifies_override</t>
+  </si>
+  <si>
+    <t>Scanned beneficiary already qualifies for this authorization</t>
+  </si>
+  <si>
+    <t>El beneficiario escaneado ya califica para esta autorización</t>
+  </si>
+  <si>
+    <t>eligible_override</t>
+  </si>
+  <si>
+    <t>Beneficiary eligible for override</t>
+  </si>
+  <si>
+    <t>Beneficiario elegible para derecho</t>
+  </si>
+  <si>
+    <t>override_creation_success</t>
+  </si>
+  <si>
+    <t>Override Successfully Created</t>
+  </si>
+  <si>
+    <t>Derecho creada correctamente</t>
+  </si>
+  <si>
+    <t>view_authorization_details</t>
+  </si>
+  <si>
+    <t>View Authorization Details</t>
+  </si>
+  <si>
+    <t>scan_barcode</t>
+  </si>
+  <si>
+    <t>Ver Detalles de Autorización</t>
+  </si>
+  <si>
+    <t>Escanear Código</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>Enter</t>
+  </si>
+  <si>
+    <t>Entrar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -809,6 +968,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -920,7 +1089,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -935,6 +1104,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2115,10 +2290,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2146,8 +2321,206 @@
       <c r="B2" t="s">
         <v>234</v>
       </c>
-      <c r="C2" t="s">
-        <v>236</v>
+      <c r="C2" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>246</v>
+      </c>
+      <c r="B5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>247</v>
+      </c>
+      <c r="B6" t="s">
+        <v>251</v>
+      </c>
+      <c r="C6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B7" t="s">
+        <v>252</v>
+      </c>
+      <c r="C7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>258</v>
+      </c>
+      <c r="B9" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>264</v>
+      </c>
+      <c r="B10" t="s">
+        <v>265</v>
+      </c>
+      <c r="C10" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>266</v>
+      </c>
+      <c r="B11" t="s">
+        <v>267</v>
+      </c>
+      <c r="C11" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>270</v>
+      </c>
+      <c r="B12" t="s">
+        <v>271</v>
+      </c>
+      <c r="C12" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" t="s">
+        <v>274</v>
+      </c>
+      <c r="C13" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>276</v>
+      </c>
+      <c r="B14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>279</v>
+      </c>
+      <c r="B15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C15" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>282</v>
+      </c>
+      <c r="B16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="C17" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>288</v>
+      </c>
+      <c r="B18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C19" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>293</v>
+      </c>
+      <c r="B20" t="s">
+        <v>294</v>
+      </c>
+      <c r="C20" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -2160,7 +2533,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2180,7 +2553,7 @@
         <v>226</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E1" t="s">
         <v>135</v>
@@ -2189,7 +2562,7 @@
         <v>227</v>
       </c>
       <c r="G1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H1" t="s">
         <v>136</v>
@@ -2271,7 +2644,7 @@
         <v>116</v>
       </c>
       <c r="G7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H7" t="s">
         <v>117</v>
@@ -2293,20 +2666,20 @@
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>241</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2386,7 +2759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Intermediate check-in. Change all suffix-based subsets to infix-based subsets. Add framework_variant setting to framework settings and split framework forms into directories qualified by those variants (allows simultaneous edits of all framework files). Add proper doctype heading to all html files.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="1"/>
+    <workbookView xWindow="4215" yWindow="1335" windowWidth="24297" windowHeight="17097" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="235">
   <si>
     <t>comments</t>
   </si>
@@ -739,6 +739,12 @@
   </si>
   <si>
     <t>'?' +  odkSurvey.getHashString('maleClients','partner6Month')</t>
+  </si>
+  <si>
+    <t>framework_variant</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -886,7 +892,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -902,6 +908,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="91">
@@ -1336,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
@@ -2093,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.125" defaultRowHeight="12.8" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2207,8 +2216,12 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="18.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>234</v>
+      </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>

</xml_diff>

<commit_message>
translations changes before pull from upstream
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18600" yWindow="13580" windowWidth="24300" windowHeight="17100" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12020" windowHeight="16220" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="360">
   <si>
     <t>comments</t>
   </si>
@@ -932,6 +932,198 @@
   </si>
   <si>
     <t>Entrar</t>
+  </si>
+  <si>
+    <t>greek</t>
+  </si>
+  <si>
+    <t>Greek</t>
+  </si>
+  <si>
+    <t>Greek (as greek name)</t>
+  </si>
+  <si>
+    <t>no_active_beneficiary</t>
+  </si>
+  <si>
+    <t>No Active Beneficiary Detected</t>
+  </si>
+  <si>
+    <t>No Disabled Beneficiary Detected</t>
+  </si>
+  <si>
+    <t>no_disabled_beneficiary</t>
+  </si>
+  <si>
+    <t>enter_beneficiary_code</t>
+  </si>
+  <si>
+    <t>Please Enter Beneficiary Code</t>
+  </si>
+  <si>
+    <t>active_beneficiaries_title</t>
+  </si>
+  <si>
+    <t>Active Beneficiaries</t>
+  </si>
+  <si>
+    <t>Disabled Beneficiaries</t>
+  </si>
+  <si>
+    <t>beneficiary_data_title</t>
+  </si>
+  <si>
+    <t>Beneficiary Data</t>
+  </si>
+  <si>
+    <t>delivery_data_title</t>
+  </si>
+  <si>
+    <t>Delivery Data</t>
+  </si>
+  <si>
+    <t>beneficiary_lists</t>
+  </si>
+  <si>
+    <t>Beneficiary Lists</t>
+  </si>
+  <si>
+    <t>view_all_deliveries</t>
+  </si>
+  <si>
+    <t>View All Deliveries</t>
+  </si>
+  <si>
+    <t>advanced_search</t>
+  </si>
+  <si>
+    <t>Advanced Search</t>
+  </si>
+  <si>
+    <t>data_categories</t>
+  </si>
+  <si>
+    <t>view_beneficiary_data</t>
+  </si>
+  <si>
+    <t>view_delivery_data</t>
+  </si>
+  <si>
+    <t>Data Categories</t>
+  </si>
+  <si>
+    <t>View Delivery Data</t>
+  </si>
+  <si>
+    <t>View Beneficiary Data</t>
+  </si>
+  <si>
+    <t>enable_beneficiary</t>
+  </si>
+  <si>
+    <t>Enable Beneficiary</t>
+  </si>
+  <si>
+    <t>disable_beneficiary</t>
+  </si>
+  <si>
+    <t>Disable Beneficiary</t>
+  </si>
+  <si>
+    <t>choose_method</t>
+  </si>
+  <si>
+    <t>Choose Method</t>
+  </si>
+  <si>
+    <t>Override Options</t>
+  </si>
+  <si>
+    <t>override_options</t>
+  </si>
+  <si>
+    <t>override_registration</t>
+  </si>
+  <si>
+    <t>Override Registration</t>
+  </si>
+  <si>
+    <t>override_entitlement</t>
+  </si>
+  <si>
+    <t>Override Entitlement</t>
+  </si>
+  <si>
+    <t>serach_beneficiaries</t>
+  </si>
+  <si>
+    <t>Search for Beneficiaries</t>
+  </si>
+  <si>
+    <t>search_deliveries</t>
+  </si>
+  <si>
+    <t>Search for Deliveries</t>
+  </si>
+  <si>
+    <t>beneficiary</t>
+  </si>
+  <si>
+    <t>beneficiaries</t>
+  </si>
+  <si>
+    <t>delivery</t>
+  </si>
+  <si>
+    <t>deliveries</t>
+  </si>
+  <si>
+    <t>found</t>
+  </si>
+  <si>
+    <t>invalid_search</t>
+  </si>
+  <si>
+    <t>Invalid Search</t>
+  </si>
+  <si>
+    <t>authorization_name</t>
+  </si>
+  <si>
+    <t>Authorization Name</t>
+  </si>
+  <si>
+    <t>authorization_id</t>
+  </si>
+  <si>
+    <t>Authorization ID</t>
+  </si>
+  <si>
+    <t>item_pack_name</t>
+  </si>
+  <si>
+    <t>Item Pack Name</t>
+  </si>
+  <si>
+    <t>item_pack_description</t>
+  </si>
+  <si>
+    <t>Item Pack Description</t>
+  </si>
+  <si>
+    <t>item_pack_id</t>
+  </si>
+  <si>
+    <t>Item Pack ID</t>
+  </si>
+  <si>
+    <t>beneficiary_code</t>
+  </si>
+  <si>
+    <t>Beneficiary Code</t>
+  </si>
+  <si>
+    <t>disabled_beneficiaries_title</t>
   </si>
 </sst>
 </file>
@@ -2290,10 +2482,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2523,6 +2715,275 @@
         <v>295</v>
       </c>
     </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>299</v>
+      </c>
+      <c r="B21" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="26" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>302</v>
+      </c>
+      <c r="B22" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>303</v>
+      </c>
+      <c r="B23" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>305</v>
+      </c>
+      <c r="B24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>359</v>
+      </c>
+      <c r="B25" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
+        <v>308</v>
+      </c>
+      <c r="B26" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B27" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
+        <v>312</v>
+      </c>
+      <c r="B28" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
+        <v>314</v>
+      </c>
+      <c r="B29" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
+        <v>316</v>
+      </c>
+      <c r="B30" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
+        <v>318</v>
+      </c>
+      <c r="B31" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
+        <v>319</v>
+      </c>
+      <c r="B32" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>320</v>
+      </c>
+      <c r="B33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>324</v>
+      </c>
+      <c r="B34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>326</v>
+      </c>
+      <c r="B35" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>328</v>
+      </c>
+      <c r="B36" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>331</v>
+      </c>
+      <c r="B37" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
+        <v>332</v>
+      </c>
+      <c r="B38" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
+        <v>334</v>
+      </c>
+      <c r="B39" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
+        <v>336</v>
+      </c>
+      <c r="B40" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
+        <v>338</v>
+      </c>
+      <c r="B41" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
+        <v>340</v>
+      </c>
+      <c r="B42" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>341</v>
+      </c>
+      <c r="B43" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>342</v>
+      </c>
+      <c r="B44" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>343</v>
+      </c>
+      <c r="B45" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
+        <v>344</v>
+      </c>
+      <c r="B46" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
+        <v>345</v>
+      </c>
+      <c r="B47" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>358</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2533,7 +2994,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2683,14 +3144,22 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
+      <c r="A10" s="2" t="s">
+        <v>296</v>
+      </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>298</v>
+      </c>
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
refactor ranges out of entitlements
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -2332,8 +2332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
detail view fixes, other small ui improvements
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/app/config/assets/framework/forms/framework/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="2300" windowWidth="24660" windowHeight="17960" tabRatio="989" activeTab="4"/>
+    <workbookView xWindow="2080" yWindow="2260" windowWidth="24660" windowHeight="17960" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -14,13 +19,13 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -393,9 +398,6 @@
   </si>
   <si>
     <t>Override Entitlement</t>
-  </si>
-  <si>
-    <t>serach_beneficiaries</t>
   </si>
   <si>
     <t>Search for Beneficiaries</t>
@@ -939,6 +941,9 @@
   </si>
   <si>
     <t>Deliveries</t>
+  </si>
+  <si>
+    <t>search_beneficiaries</t>
   </si>
 </sst>
 </file>
@@ -1383,7 +1388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1397,9 +1402,9 @@
       <selection activeCell="B23" activeCellId="1" sqref="B87 B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -1415,11 +1420,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1431,7 +1431,7 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="38.33203125" customWidth="1"/>
@@ -1442,7 +1442,7 @@
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -1478,7 +1478,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1">
+    <row r="3" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -1489,13 +1489,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -1506,26 +1506,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -1534,23 +1534,23 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -1559,7 +1559,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" t="s">
@@ -1569,11 +1569,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1581,17 +1576,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -1602,7 +1597,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1613,7 +1608,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1624,7 +1619,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1635,7 +1630,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1646,7 +1641,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1657,7 +1652,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -1668,7 +1663,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -1679,7 +1674,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1690,7 +1685,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1701,7 +1696,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -1712,7 +1707,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1723,7 +1718,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1734,7 +1729,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -1745,7 +1740,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1756,7 +1751,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1767,7 +1762,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="48">
+    <row r="17" spans="1:3" ht="52" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>71</v>
       </c>
@@ -1778,7 +1773,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -1789,7 +1784,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -1800,7 +1795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -1811,7 +1806,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>83</v>
       </c>
@@ -1819,7 +1814,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>85</v>
       </c>
@@ -1827,7 +1822,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -1835,7 +1830,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>89</v>
       </c>
@@ -1843,7 +1838,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1851,7 +1846,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -1859,7 +1854,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -1867,7 +1862,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>97</v>
       </c>
@@ -1875,7 +1870,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -1883,7 +1878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>101</v>
       </c>
@@ -1891,7 +1886,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>103</v>
       </c>
@@ -1899,7 +1894,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>105</v>
       </c>
@@ -1907,7 +1902,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>107</v>
       </c>
@@ -1915,7 +1910,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>109</v>
       </c>
@@ -1923,7 +1918,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>111</v>
       </c>
@@ -1931,7 +1926,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>113</v>
       </c>
@@ -1939,7 +1934,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -1947,7 +1942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>117</v>
       </c>
@@ -1955,7 +1950,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
         <v>119</v>
       </c>
@@ -1963,139 +1958,134 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B40" t="s">
         <v>121</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>123</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
         <v>125</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
         <v>126</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B44" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
         <v>127</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
         <v>128</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
         <v>129</v>
       </c>
-      <c r="B46" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>130</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A49" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A50" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C49" s="2"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A51" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A52" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C52" s="2"/>
-    </row>
-    <row r="53" spans="1:3" s="2" customFormat="1">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>292</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>293</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2107,46 +2097,46 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" t="s">
         <v>147</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>148</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>149</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>150</v>
-      </c>
-      <c r="H1" t="s">
-        <v>151</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
       </c>
       <c r="J1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>154</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -2155,12 +2145,12 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2169,118 +2159,113 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="I4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="28" customHeight="1">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>159</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D5" t="s">
-        <v>160</v>
-      </c>
-      <c r="E5" s="6" t="s">
+      <c r="I5" t="s">
         <v>161</v>
-      </c>
-      <c r="I5" t="s">
-        <v>162</v>
       </c>
       <c r="J5" t="b">
         <f>FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1">
+    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>162</v>
+      </c>
+      <c r="F7" t="s">
         <v>163</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>164</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>165</v>
       </c>
-      <c r="H7" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
         <v>167</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H8" t="s">
         <v>168</v>
       </c>
-      <c r="G8" t="s">
-        <v>168</v>
-      </c>
-      <c r="H8" t="s">
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A10" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2288,58 +2273,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2351,13 +2331,13 @@
       <selection activeCellId="1" sqref="B87 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="3" max="3" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2365,471 +2345,466 @@
         <v>24</v>
       </c>
       <c r="C1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>180</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="13" customHeight="1">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>182</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="13" customHeight="1">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>184</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13" customHeight="1">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>186</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="13" customHeight="1">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>188</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="13">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>190</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="C7" s="6" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="13">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
         <v>193</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="7" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="13">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
         <v>196</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="C9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="13">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>199</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="C10" s="6" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
         <v>202</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
         <v>204</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
         <v>206</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
         <v>208</v>
       </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
         <v>210</v>
       </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
         <v>212</v>
       </c>
-      <c r="B16" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>214</v>
       </c>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>216</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>218</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>220</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>222</v>
       </c>
-      <c r="B21" t="s">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>224</v>
       </c>
-      <c r="B22" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>226</v>
       </c>
-      <c r="B23" t="s">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>228</v>
       </c>
-      <c r="B24" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>230</v>
       </c>
-      <c r="B25" t="s">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>232</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>234</v>
       </c>
-      <c r="B27" t="s">
+    </row>
+    <row r="28" spans="1:2" ht="28.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="28.25" customHeight="1">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>236</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>238</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>240</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>242</v>
       </c>
-      <c r="B31" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>244</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>246</v>
       </c>
-      <c r="B34" t="s">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>248</v>
       </c>
-      <c r="B35" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="409" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="409">
-      <c r="A36" t="s">
+      <c r="B36" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B36" s="3" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
+      <c r="B37" t="s">
         <v>252</v>
       </c>
-      <c r="B37" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A38" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+      <c r="B38" t="s">
         <v>254</v>
       </c>
-      <c r="B38" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A39" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
+      <c r="B39" t="s">
         <v>256</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A40" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
         <v>258</v>
       </c>
-      <c r="B40" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A41" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
+      <c r="B41" t="s">
         <v>260</v>
       </c>
-      <c r="B41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A42" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
+      <c r="B42" t="s">
         <v>262</v>
       </c>
-      <c r="B42" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
+      <c r="B43" t="s">
         <v>264</v>
       </c>
-      <c r="B43" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" t="s">
+      <c r="B44" t="s">
         <v>266</v>
       </c>
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="13">
-      <c r="A45" t="s">
+      <c r="B45" t="s">
         <v>268</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="C45" s="6" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
+      <c r="B46" t="s">
         <v>271</v>
       </c>
-      <c r="B46" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A47" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
+      <c r="B47" t="s">
         <v>273</v>
       </c>
-      <c r="B47" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
+      <c r="B48" t="s">
         <v>275</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A49" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+      <c r="B49" t="s">
         <v>277</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:2" ht="13" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="13" customHeight="1">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
         <v>279</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A51" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>281</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A52" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A53" t="s">
         <v>283</v>
       </c>
-      <c r="B52" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
         <v>284</v>
       </c>
-      <c r="B53" t="s">
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A55" t="s">
         <v>286</v>
-      </c>
-      <c r="B54" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>287</v>
       </c>
       <c r="B55" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
+        <v>287</v>
+      </c>
+      <c r="B56" t="s">
         <v>288</v>
       </c>
-      <c r="B56" t="s">
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A57" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+      <c r="B57" t="s">
         <v>290</v>
-      </c>
-      <c r="B57" t="s">
-        <v>291</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
many changes in app level files to migrate to new schema. Changes to allow for multiple overrides on an entitlement. Refactor a lot of functions and constants into util.js and queryUtil.js. Still need to work on all html/js files under tables directory. All changes completely untested.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/assets/framework/forms/framework/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/new_redcross_repos/redcross-app-designer/app/config/assets/framework/forms/framework/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3520" yWindow="1260" windowWidth="27160" windowHeight="26060" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="30220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="choices" sheetId="5" r:id="rId5"/>
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$77</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -35,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="713">
   <si>
     <t>comments</t>
   </si>
@@ -235,12 +238,6 @@
     <t>Enter</t>
   </si>
   <si>
-    <t>no_active_beneficiary</t>
-  </si>
-  <si>
-    <t>No Active Beneficiary Detected</t>
-  </si>
-  <si>
     <t>no_disabled_beneficiary</t>
   </si>
   <si>
@@ -251,12 +248,6 @@
   </si>
   <si>
     <t>Please Enter Beneficiary Code</t>
-  </si>
-  <si>
-    <t>active_beneficiaries_title</t>
-  </si>
-  <si>
-    <t>Active Beneficiaries</t>
   </si>
   <si>
     <t>disabled_beneficiaries_title</t>
@@ -2047,27 +2038,15 @@
     <t>View Household Data</t>
   </si>
   <si>
-    <t>active_households</t>
-  </si>
-  <si>
-    <t>Active Households</t>
-  </si>
-  <si>
     <t>disabled_households</t>
   </si>
   <si>
     <t>Disabled Households</t>
   </si>
   <si>
-    <t>search_members</t>
-  </si>
-  <si>
     <t>search_households</t>
   </si>
   <si>
-    <t>Beneficiary Advanced Search</t>
-  </si>
-  <si>
     <t>Household Advanced Search</t>
   </si>
   <si>
@@ -2171,6 +2150,45 @@
   </si>
   <si>
     <t>Please Select Group</t>
+  </si>
+  <si>
+    <t>disabled_beneficiaries</t>
+  </si>
+  <si>
+    <t>Enabled Beneficiaries</t>
+  </si>
+  <si>
+    <t>Enabled Households</t>
+  </si>
+  <si>
+    <t>enabled_households</t>
+  </si>
+  <si>
+    <t>enabled_beneficiaries</t>
+  </si>
+  <si>
+    <t>Individual Advanced Search</t>
+  </si>
+  <si>
+    <t>search_individuals</t>
+  </si>
+  <si>
+    <t>Beneficiaries Advanced Search</t>
+  </si>
+  <si>
+    <t>no_enabled_beneficiary</t>
+  </si>
+  <si>
+    <t>No Enabled Beneficiary Detected</t>
+  </si>
+  <si>
+    <t>enabled_beneficiaries_title</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>individuals</t>
   </si>
 </sst>
 </file>
@@ -2735,14 +2753,14 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2760,14 +2778,14 @@
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -2791,10 +2809,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2813,13 +2831,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>25</v>
@@ -2833,16 +2851,16 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -2853,16 +2871,16 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -2873,13 +2891,13 @@
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>32</v>
@@ -2893,13 +2911,13 @@
         <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>35</v>
@@ -2913,16 +2931,16 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -2933,16 +2951,16 @@
         <v>39</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2953,16 +2971,16 @@
         <v>41</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2973,16 +2991,16 @@
         <v>43</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2993,13 +3011,13 @@
         <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>46</v>
@@ -3013,16 +3031,16 @@
         <v>48</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -3033,16 +3051,16 @@
         <v>50</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -3053,16 +3071,16 @@
         <v>52</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -3073,16 +3091,16 @@
         <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.2">
@@ -3093,16 +3111,16 @@
         <v>56</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -3113,16 +3131,16 @@
         <v>58</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3133,16 +3151,16 @@
         <v>60</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3150,19 +3168,19 @@
         <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3173,16 +3191,16 @@
         <v>63</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3193,493 +3211,493 @@
         <v>65</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>708</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>709</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>710</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>701</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>35</v>
@@ -3687,350 +3705,391 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>666</v>
+        <v>703</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>667</v>
+        <v>702</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>700</v>
+        <v>704</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>701</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>698</v>
+        <v>692</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>702</v>
+        <v>693</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>670</v>
+        <v>711</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>672</v>
+        <v>711</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>671</v>
+        <v>712</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>673</v>
+        <v>712</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>684</v>
+        <v>690</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>687</v>
+        <v>691</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>685</v>
+        <v>694</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>686</v>
+        <v>706</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>689</v>
+        <v>705</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" t="s">
-        <v>690</v>
+      <c r="A67" s="2" t="s">
+        <v>664</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>693</v>
+        <v>665</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>691</v>
+      <c r="A68" s="2" t="s">
+        <v>255</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>694</v>
+        <v>707</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>692</v>
+      <c r="A69" s="2" t="s">
+        <v>676</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>695</v>
+        <v>679</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>696</v>
+      <c r="A70" s="2" t="s">
+        <v>677</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" t="s">
-        <v>704</v>
+      <c r="A71" s="2" t="s">
+        <v>678</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>705</v>
+        <v>681</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>706</v>
+        <v>682</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>707</v>
+        <v>685</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>683</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>684</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>688</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>696</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>698</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>699</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F77"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4048,54 +4107,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="H1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>663</v>
-      </c>
-      <c r="H1" t="s">
-        <v>128</v>
-      </c>
-      <c r="I1" t="s">
-        <v>129</v>
-      </c>
       <c r="J1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="K1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="L1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4110,10 +4169,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4126,41 +4185,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="G5" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="M5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4169,27 +4228,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="H7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="I7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="L7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4198,24 +4257,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4224,24 +4283,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4250,24 +4309,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4276,24 +4335,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4319,13 +4378,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4333,7 +4392,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -4344,10 +4403,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -4378,13 +4437,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="D1" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="E1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -4392,530 +4451,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B9" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B10" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B17" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B18" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B21" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B22" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B23" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B24" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B25" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B28" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4924,10 +4983,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4936,42 +4995,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B30" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B31" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -4982,70 +5041,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B33" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B35" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5054,367 +5113,367 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B37" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B38" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B39" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B40" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B41" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B42" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B43" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B46" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B47" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B48" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B49" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B50" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B51" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B52" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B53" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>674</v>
+        <v>666</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>63</v>
@@ -5424,37 +5483,37 @@
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
-        <v>679</v>
+        <v>671</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>675</v>
+        <v>667</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>676</v>
+        <v>668</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>682</v>
+        <v>674</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
-        <v>680</v>
+        <v>672</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>677</v>
+        <v>669</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>678</v>
+        <v>670</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>683</v>
+        <v>675</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>681</v>
+        <v>673</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to gruntfile, changes to framework translations. more refactoring of code into queryUtil.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="30220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="30220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="714">
   <si>
     <t>comments</t>
   </si>
@@ -2170,9 +2170,6 @@
     <t>Individual Advanced Search</t>
   </si>
   <si>
-    <t>search_individuals</t>
-  </si>
-  <si>
     <t>Beneficiaries Advanced Search</t>
   </si>
   <si>
@@ -2189,6 +2186,12 @@
   </si>
   <si>
     <t>individuals</t>
+  </si>
+  <si>
+    <t>search_beneficiaries_title</t>
+  </si>
+  <si>
+    <t>search_individuals_title</t>
   </si>
 </sst>
 </file>
@@ -2812,7 +2815,7 @@
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3225,10 +3228,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>707</v>
+      </c>
+      <c r="B21" t="s">
         <v>708</v>
-      </c>
-      <c r="B21" t="s">
-        <v>709</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>567</v>
@@ -3285,7 +3288,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B24" t="s">
         <v>701</v>
@@ -3962,18 +3965,18 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3986,7 +3989,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>694</v>
+        <v>664</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>695</v>
@@ -3994,7 +3997,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>705</v>
@@ -4002,7 +4005,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>664</v>
+        <v>694</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>665</v>
@@ -4010,10 +4013,10 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>255</v>
+        <v>712</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to list and detail views and util classes. not fully working
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="30220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="7460" windowWidth="41600" windowHeight="17540" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$78</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="716">
   <si>
     <t>comments</t>
   </si>
@@ -2170,6 +2170,9 @@
     <t>Individual Advanced Search</t>
   </si>
   <si>
+    <t>search_individuals</t>
+  </si>
+  <si>
     <t>Beneficiaries Advanced Search</t>
   </si>
   <si>
@@ -2186,6 +2189,9 @@
   </si>
   <si>
     <t>individuals</t>
+  </si>
+  <si>
+    <t>Search for Individuals</t>
   </si>
   <si>
     <t>search_beneficiaries_title</t>
@@ -2812,10 +2818,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3228,10 +3234,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B21" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>567</v>
@@ -3288,7 +3294,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B24" t="s">
         <v>701</v>
@@ -3965,18 +3971,18 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3997,102 +4003,110 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>713</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>694</v>
+        <v>715</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>665</v>
+        <v>705</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>706</v>
+        <v>665</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>676</v>
+        <v>714</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>679</v>
+        <v>707</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>681</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>682</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>696</v>
+        <v>688</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>697</v>
+        <v>689</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>696</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>698</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B78" s="2" t="s">
         <v>699</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F77"/>
+  <autoFilter ref="A1:F78"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
add feature that shows rows since last sync on registration and delivery root pages
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7460" windowWidth="41600" windowHeight="17540" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="4620" yWindow="4420" windowWidth="41600" windowHeight="17540" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -154,22 +154,10 @@
     <t>View Data</t>
   </si>
   <si>
-    <t>override_path</t>
-  </si>
-  <si>
-    <t>Administrator Overrides</t>
-  </si>
-  <si>
     <t>registration_title</t>
   </si>
   <si>
-    <t>Register Beneficiary Code</t>
-  </si>
-  <si>
     <t>delivery_title</t>
-  </si>
-  <si>
-    <t>Verify Beneficiary Code</t>
   </si>
   <si>
     <t>disabled_beneficiary_notification</t>
@@ -2199,12 +2187,24 @@
   <si>
     <t>search_individuals_title</t>
   </si>
+  <si>
+    <t>administrator_path</t>
+  </si>
+  <si>
+    <t>Administrator Options</t>
+  </si>
+  <si>
+    <t>Register Beneficiary Entity</t>
+  </si>
+  <si>
+    <t>Deliver to Beneficiary Entity</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2242,13 +2242,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2267,7 +2280,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2291,6 +2304,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2762,14 +2779,14 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2787,14 +2804,14 @@
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -2818,10 +2835,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2832,7 +2849,7 @@
     <col min="4" max="6" width="8.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -2840,19 +2857,19 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2860,19 +2877,19 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -2880,19 +2897,19 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2900,19 +2917,19 @@
         <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -2920,19 +2937,19 @@
         <v>34</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2940,773 +2957,775 @@
         <v>37</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>712</v>
+      </c>
+      <c r="B7" t="s">
+        <v>713</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>714</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>550</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>715</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>552</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="5" t="s">
+      <c r="D10" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>553</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D11" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>273</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="D12" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>555</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="5" t="s">
+      <c r="D13" s="5" t="s">
+        <v>282</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>556</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="D14" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>557</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="5" t="s">
+      <c r="D15" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>558</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>559</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>287</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>560</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="F14" s="5" t="s">
+      <c r="D16" s="5" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>561</v>
-      </c>
-      <c r="D15" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F16" s="8" t="s">
         <v>292</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>562</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="B21" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="B24" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B35" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B40" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B41" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F44" s="5" t="s">
         <v>35</v>
@@ -3714,395 +3733,395 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F54" s="8" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
     </row>
   </sheetData>
@@ -4124,54 +4143,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="H1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="H1" t="s">
-        <v>124</v>
-      </c>
-      <c r="I1" t="s">
-        <v>125</v>
-      </c>
       <c r="J1" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="K1" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="L1" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4186,10 +4205,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4202,41 +4221,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="M5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4245,27 +4264,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="I7" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="K7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="L7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4274,24 +4293,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4300,24 +4319,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4326,24 +4345,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4352,24 +4371,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -4395,13 +4414,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4409,7 +4428,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -4420,10 +4439,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4454,13 +4473,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="D1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="E1" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -4468,530 +4487,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B10" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B12" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="B14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B15" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B18" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B19" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B20" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B21" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B22" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B24" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B25" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B26" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5000,10 +5019,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B29" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -5012,42 +5031,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B30" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B31" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -5058,70 +5077,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B33" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="B34" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B35" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5130,407 +5149,407 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B37" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="B38" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B39" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B40" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B41" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B43" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B44" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B45" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B46" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B47" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B48" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B49" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B50" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B51" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B52" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B53" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B54" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
attempt to put entitlement enable/disable button in list view. difficult because the radio button css is not acting correctly in this context. need to fix
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -20,7 +20,7 @@
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$80</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="721">
   <si>
     <t>comments</t>
   </si>
@@ -308,12 +308,6 @@
   </si>
   <si>
     <t>Choose Method</t>
-  </si>
-  <si>
-    <t>override_options</t>
-  </si>
-  <si>
-    <t>Override Options</t>
   </si>
   <si>
     <t>override_registration</t>
@@ -2198,6 +2192,27 @@
   </si>
   <si>
     <t>Deliver to Beneficiary Entity</t>
+  </si>
+  <si>
+    <t>administrator_options</t>
+  </si>
+  <si>
+    <t>distribution</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>change_entitlement_status</t>
+  </si>
+  <si>
+    <t>Change Entitlement Status</t>
+  </si>
+  <si>
+    <t>create_new_entitlement</t>
+  </si>
+  <si>
+    <t>Create New Entitlement</t>
   </si>
 </sst>
 </file>
@@ -2779,14 +2794,14 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2804,14 +2819,14 @@
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -2835,10 +2850,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2857,13 +2872,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>25</v>
@@ -2871,1261 +2886,1296 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>544</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>253</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>254</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>715</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>545</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>257</v>
-      </c>
+        <v>716</v>
+      </c>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>32</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>35</v>
+        <v>255</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>264</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>712</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>713</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>549</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>266</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="G7" s="12"/>
+        <v>34</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>545</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>714</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>550</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="G8" s="14"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>710</v>
       </c>
       <c r="B9" t="s">
-        <v>715</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>551</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>273</v>
-      </c>
+        <v>711</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>547</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>264</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>274</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>42</v>
-      </c>
+        <v>712</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>548</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G10" s="14"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>713</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>281</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>553</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="36" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>287</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>289</v>
+        <v>281</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>296</v>
+        <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>299</v>
+        <v>289</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>561</v>
+        <v>55</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>557</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>302</v>
+        <v>292</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>294</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>704</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s">
-        <v>705</v>
+        <v>59</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>64</v>
+        <v>702</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>703</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>706</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>697</v>
+        <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>704</v>
       </c>
       <c r="B26" t="s">
-        <v>69</v>
+        <v>695</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>337</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>338</v>
+        <v>329</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>570</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>571</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>80</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C34" s="5" t="s">
+        <v>572</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+      <c r="B36" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>574</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>339</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>340</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>82</v>
-      </c>
-      <c r="B33" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="D36" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B37" t="s">
+        <v>87</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>575</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>342</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>343</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="D37" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="5" t="s">
         <v>576</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>345</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>346</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="D38" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>714</v>
+      </c>
+      <c r="B39" t="s">
+        <v>711</v>
+      </c>
+      <c r="C39" s="13" t="s">
         <v>577</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>348</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>349</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>88</v>
-      </c>
-      <c r="B36" t="s">
-        <v>89</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="D39" s="13" t="s">
+        <v>352</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="G39" s="14"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>578</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>351</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>352</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="D40" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>579</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>354</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>92</v>
-      </c>
-      <c r="B38" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="D41" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>249</v>
+      </c>
+      <c r="B42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>357</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>358</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>94</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="D42" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>95</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="B43" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>581</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>360</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>251</v>
-      </c>
-      <c r="B40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="D43" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" t="s">
+        <v>97</v>
+      </c>
+      <c r="C44" s="5" t="s">
         <v>582</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>363</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>364</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>97</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="D44" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>98</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>583</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>366</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>367</v>
-      </c>
-      <c r="F41" s="5" t="s">
+      <c r="D45" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="F45" s="5" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>99</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B46" t="s">
         <v>99</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C46" s="5" t="s">
         <v>584</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>369</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D46" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B47" t="s">
         <v>100</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>585</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>372</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="F43" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="E47" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>101</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B48" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C48" s="5" t="s">
         <v>586</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>374</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D48" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>102</v>
       </c>
-      <c r="B45" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="5" t="s">
+      <c r="B49" t="s">
+        <v>103</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>587</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>375</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>103</v>
-      </c>
-      <c r="B46" t="s">
-        <v>103</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>588</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>378</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="E49" s="5" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" t="s">
-        <v>105</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="D47" s="5" t="s">
+      <c r="F49" s="5" t="s">
         <v>380</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>381</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>387</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>388</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>381</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>385</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>395</v>
+        <v>386</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>387</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="E52" s="9" t="s">
-        <v>398</v>
+        <v>389</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>390</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>400</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>401</v>
+        <v>392</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>393</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B54" s="5" t="s">
-        <v>403</v>
+        <v>110</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>395</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>656</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>657</v>
-      </c>
-      <c r="F55" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>593</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="F55" s="5" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>699</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>698</v>
+        <v>243</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>594</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>404</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>658</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>659</v>
-      </c>
+        <v>654</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="F57" s="8"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>696</v>
+        <v>656</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>67</v>
+        <v>657</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>688</v>
+        <v>698</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>689</v>
+        <v>694</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>689</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>707</v>
+        <v>686</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>707</v>
+        <v>686</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>708</v>
+        <v>687</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>708</v>
+        <v>687</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>686</v>
+        <v>705</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>687</v>
+        <v>705</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>660</v>
+        <v>706</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>691</v>
+        <v>706</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>702</v>
+        <v>684</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>709</v>
+        <v>685</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>711</v>
+        <v>658</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>701</v>
+        <v>689</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>690</v>
+        <v>700</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>661</v>
+        <v>707</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>672</v>
+        <v>688</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>673</v>
+        <v>708</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>676</v>
+        <v>701</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
+        <v>670</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>674</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>678</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>681</v>
-      </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>679</v>
+      <c r="A74" s="2" t="s">
+        <v>672</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>693</v>
+        <v>681</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>694</v>
+        <v>682</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>695</v>
+        <v>683</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>690</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>692</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>717</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>719</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>720</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F78"/>
+  <autoFilter ref="A1:F80"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4143,54 +4193,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="H1" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="H1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I1" t="s">
-        <v>121</v>
-      </c>
       <c r="J1" t="s">
+        <v>644</v>
+      </c>
+      <c r="K1" t="s">
+        <v>645</v>
+      </c>
+      <c r="L1" t="s">
         <v>646</v>
-      </c>
-      <c r="K1" t="s">
-        <v>647</v>
-      </c>
-      <c r="L1" t="s">
-        <v>648</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4205,10 +4255,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4221,41 +4271,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" t="s">
         <v>129</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" t="s">
-        <v>130</v>
-      </c>
-      <c r="M5" t="s">
-        <v>131</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4264,27 +4314,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+      <c r="I7" t="s">
         <v>132</v>
       </c>
-      <c r="H7" t="s">
-        <v>133</v>
-      </c>
-      <c r="I7" t="s">
-        <v>134</v>
-      </c>
       <c r="J7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4293,24 +4343,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4319,24 +4369,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4345,24 +4395,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4371,24 +4421,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -4414,13 +4464,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4428,7 +4478,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -4439,10 +4489,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -4473,13 +4523,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="D1" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E1" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -4487,530 +4537,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>407</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>408</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>408</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>409</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>410</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>411</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="D5" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>416</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>417</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>417</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="F6" s="7" t="s">
         <v>419</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>420</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>421</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>422</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>423</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>423</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>425</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>426</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>428</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>431</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>432</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>434</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>412</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>437</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>438</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>530</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>531</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>532</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>536</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B16" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B17" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>440</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="F18" s="5" t="s">
         <v>442</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>443</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>443</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>445</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>446</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>446</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>447</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>448</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>449</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>449</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>450</v>
+      </c>
+      <c r="F21" s="5" t="s">
         <v>451</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B22" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>452</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>454</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>455</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B23" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>456</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>457</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>458</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>458</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>459</v>
+      </c>
+      <c r="F24" s="5" t="s">
         <v>460</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>461</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B25" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>463</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>465</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B27" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>467</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>468</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5019,10 +5069,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -5031,42 +5081,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B30" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D30" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>470</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>471</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="F31" s="5" t="s">
         <v>474</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -5077,70 +5127,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B33" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>477</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B34" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>479</v>
+      </c>
+      <c r="F34" s="5" t="s">
         <v>480</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>481</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="F35" s="8" t="s">
         <v>483</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>484</v>
-      </c>
-      <c r="F35" s="8" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5149,367 +5199,367 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B37" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F37" s="8" t="s">
         <v>486</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>487</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="F38" s="5" t="s">
         <v>489</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B39" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="F39" s="5" t="s">
         <v>492</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>493</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>494</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>495</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B41" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="D41" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>499</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B42" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>499</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="F42" s="5" t="s">
         <v>501</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>502</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B43" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B44" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="F44" s="5" t="s">
         <v>506</v>
-      </c>
-      <c r="E44" s="5" t="s">
-        <v>507</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="F45" s="5" t="s">
         <v>509</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>510</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B46" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D46" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="F46" s="5" t="s">
         <v>512</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B47" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F47" s="5" t="s">
         <v>515</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B48" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>516</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>517</v>
+      </c>
+      <c r="F48" s="5" t="s">
         <v>518</v>
-      </c>
-      <c r="E48" s="5" t="s">
-        <v>519</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B49" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D49" s="5" t="s">
+        <v>519</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>520</v>
+      </c>
+      <c r="F49" s="5" t="s">
         <v>521</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>522</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B50" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>522</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>523</v>
+      </c>
+      <c r="F50" s="5" t="s">
         <v>524</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>525</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B51" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B52" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>473</v>
+      </c>
+      <c r="F52" s="5" t="s">
         <v>474</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>475</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B53" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>527</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>528</v>
+      </c>
+      <c r="F53" s="5" t="s">
         <v>529</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>530</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B54" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>513</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="F54" s="5" t="s">
         <v>515</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>516</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>59</v>
@@ -5519,37 +5569,37 @@
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to how detail views are rendered, and thus changes to translations sheets
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="4420" windowWidth="41600" windowHeight="17540" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,9 @@
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$68</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="681">
   <si>
     <t>comments</t>
   </si>
@@ -350,36 +350,6 @@
   </si>
   <si>
     <t>Invalid Search</t>
-  </si>
-  <si>
-    <t>authorization_name</t>
-  </si>
-  <si>
-    <t>authorization_id</t>
-  </si>
-  <si>
-    <t>item_pack_name</t>
-  </si>
-  <si>
-    <t>Item Pack Name</t>
-  </si>
-  <si>
-    <t>item_pack_description</t>
-  </si>
-  <si>
-    <t>Item Pack Description</t>
-  </si>
-  <si>
-    <t>item_pack_id</t>
-  </si>
-  <si>
-    <t>Item Pack ID</t>
-  </si>
-  <si>
-    <t>beneficiary_code</t>
-  </si>
-  <si>
-    <t>Beneficiary Code</t>
   </si>
   <si>
     <t>setting_name</t>
@@ -1195,66 +1165,6 @@
     <t>Búsqueda inválida</t>
   </si>
   <si>
-    <t>Distribution Name</t>
-  </si>
-  <si>
-    <t>اسم التوزيع</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> توزیع نام</t>
-  </si>
-  <si>
-    <t>Nombre de la distribución</t>
-  </si>
-  <si>
-    <t>Distribution ID</t>
-  </si>
-  <si>
-    <t>رقم التوزيع</t>
-  </si>
-  <si>
-    <t>شماره توزیع</t>
-  </si>
-  <si>
-    <t>ID de la distribución</t>
-  </si>
-  <si>
-    <t>اسم الحزمة</t>
-  </si>
-  <si>
-    <t>نام بسته</t>
-  </si>
-  <si>
-    <t>Nombre del artículo</t>
-  </si>
-  <si>
-    <t>وصف الحزمة</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> شرح بسته</t>
-  </si>
-  <si>
-    <t>Descripción del artículo</t>
-  </si>
-  <si>
-    <t>رقم الحزمة</t>
-  </si>
-  <si>
-    <t>شماره بسته</t>
-  </si>
-  <si>
-    <t>ID del artículo</t>
-  </si>
-  <si>
-    <t>رمز المستفيد</t>
-  </si>
-  <si>
-    <t>کد ذینفع</t>
-  </si>
-  <si>
-    <t>Código de beneficiario</t>
-  </si>
-  <si>
     <t>No Distributions</t>
   </si>
   <si>
@@ -1816,24 +1726,6 @@
     <t>Μη έγκυρη αναζήτηση</t>
   </si>
   <si>
-    <t>Όνομα διανομής</t>
-  </si>
-  <si>
-    <t>Αναγνωριστικό διανομής</t>
-  </si>
-  <si>
-    <t>Όνομα πακέτου στοιχείου</t>
-  </si>
-  <si>
-    <t>Περιγραφή πακέτου στοιχείου</t>
-  </si>
-  <si>
-    <t>Αναγνωριστικό πακέτου στοιχείου</t>
-  </si>
-  <si>
-    <t>Κωδικός Δικαιούχου</t>
-  </si>
-  <si>
     <t>Καμία διανομή</t>
   </si>
   <si>
@@ -2062,42 +1954,6 @@
     <t>Αναμενόμενη τιμή ακέραιας</t>
   </si>
   <si>
-    <t>delivery_site</t>
-  </si>
-  <si>
-    <t>household_size</t>
-  </si>
-  <si>
-    <t>tent_caravan</t>
-  </si>
-  <si>
-    <t>Delivery Site</t>
-  </si>
-  <si>
-    <t>Household Size</t>
-  </si>
-  <si>
-    <t>Tent/Caravan Code</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>household_head</t>
-  </si>
-  <si>
-    <t>vulnerability</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Household Head</t>
-  </si>
-  <si>
-    <t>Vulnerability Critieria</t>
-  </si>
-  <si>
     <t>view_registration_data</t>
   </si>
   <si>
@@ -2213,6 +2069,30 @@
   </si>
   <si>
     <t>Create New Entitlement</t>
+  </si>
+  <si>
+    <t>No Entitlements to Deliver</t>
+  </si>
+  <si>
+    <t>no_entitlements</t>
+  </si>
+  <si>
+    <t>Choose an Entitlement</t>
+  </si>
+  <si>
+    <t>choose_entitlement</t>
+  </si>
+  <si>
+    <t>Successfully Disabled!</t>
+  </si>
+  <si>
+    <t>disable_success</t>
+  </si>
+  <si>
+    <t>Successfully Enabled!</t>
+  </si>
+  <si>
+    <t>enable_success</t>
   </si>
 </sst>
 </file>
@@ -2295,7 +2175,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2315,7 +2195,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2794,14 +2673,14 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2826,7 +2705,7 @@
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -2850,10 +2729,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2872,13 +2751,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>643</v>
+        <v>607</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>25</v>
@@ -2886,7 +2765,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
@@ -2895,10 +2774,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>715</v>
+        <v>667</v>
       </c>
       <c r="B3" t="s">
-        <v>716</v>
+        <v>668</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -2910,16 +2789,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>542</v>
+        <v>512</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2930,16 +2809,16 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>543</v>
+        <v>513</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2950,13 +2829,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>544</v>
+        <v>514</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>32</v>
@@ -2970,13 +2849,13 @@
         <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>545</v>
+        <v>515</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>35</v>
@@ -2990,78 +2869,78 @@
         <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>546</v>
+        <v>516</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>710</v>
+        <v>662</v>
       </c>
       <c r="B9" t="s">
-        <v>711</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>263</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>264</v>
-      </c>
-      <c r="F9" s="11" t="s">
-        <v>265</v>
-      </c>
-      <c r="G9" s="12"/>
+        <v>663</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>254</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>712</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>548</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>266</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>267</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>268</v>
-      </c>
-      <c r="G10" s="14"/>
+        <v>664</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>518</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="G10" s="13"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>713</v>
+        <v>665</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>549</v>
+        <v>519</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -3072,13 +2951,13 @@
         <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>550</v>
+        <v>520</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>42</v>
@@ -3092,16 +2971,16 @@
         <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>551</v>
+        <v>521</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3112,16 +2991,16 @@
         <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>552</v>
+        <v>522</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3132,16 +3011,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>553</v>
+        <v>523</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -3152,16 +3031,16 @@
         <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>554</v>
+        <v>524</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.2">
@@ -3172,16 +3051,16 @@
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>555</v>
+        <v>525</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3192,16 +3071,16 @@
         <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>556</v>
+        <v>526</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3212,16 +3091,16 @@
         <v>56</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>557</v>
+        <v>527</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3229,19 +3108,19 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>558</v>
+        <v>528</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3252,16 +3131,16 @@
         <v>59</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>559</v>
+        <v>529</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3272,36 +3151,36 @@
         <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>560</v>
+        <v>530</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>702</v>
+        <v>654</v>
       </c>
       <c r="B23" t="s">
-        <v>703</v>
+        <v>655</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>561</v>
+        <v>531</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3312,16 +3191,16 @@
         <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>562</v>
+        <v>532</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3332,36 +3211,36 @@
         <v>65</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>563</v>
+        <v>533</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>704</v>
+        <v>656</v>
       </c>
       <c r="B26" t="s">
-        <v>695</v>
+        <v>647</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>564</v>
+        <v>534</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3372,16 +3251,16 @@
         <v>67</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>565</v>
+        <v>535</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -3392,16 +3271,16 @@
         <v>69</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>566</v>
+        <v>536</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -3412,16 +3291,16 @@
         <v>71</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>567</v>
+        <v>537</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -3432,16 +3311,16 @@
         <v>73</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>568</v>
+        <v>538</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -3452,16 +3331,16 @@
         <v>75</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>569</v>
+        <v>539</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -3472,16 +3351,16 @@
         <v>77</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>570</v>
+        <v>540</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -3492,16 +3371,16 @@
         <v>79</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>571</v>
+        <v>541</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3512,16 +3391,16 @@
         <v>81</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>572</v>
+        <v>542</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -3532,16 +3411,16 @@
         <v>83</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>573</v>
+        <v>543</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -3552,16 +3431,16 @@
         <v>85</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>574</v>
+        <v>544</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -3572,16 +3451,16 @@
         <v>87</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>575</v>
+        <v>545</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -3592,38 +3471,38 @@
         <v>89</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>576</v>
+        <v>546</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>714</v>
+        <v>666</v>
       </c>
       <c r="B39" t="s">
-        <v>711</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>577</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>353</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="G39" s="14"/>
+        <v>663</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="D39" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>344</v>
+      </c>
+      <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
@@ -3633,16 +3512,16 @@
         <v>91</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>578</v>
+        <v>548</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>356</v>
+        <v>346</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3653,36 +3532,36 @@
         <v>93</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>579</v>
+        <v>549</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>358</v>
+        <v>348</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B42" t="s">
         <v>94</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>580</v>
+        <v>550</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -3693,16 +3572,16 @@
         <v>96</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>581</v>
+        <v>551</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>365</v>
+        <v>355</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3713,16 +3592,16 @@
         <v>97</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>582</v>
+        <v>552</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -3733,16 +3612,16 @@
         <v>98</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>583</v>
+        <v>553</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3753,13 +3632,13 @@
         <v>99</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>584</v>
+        <v>554</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>35</v>
@@ -3773,16 +3652,16 @@
         <v>100</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>585</v>
+        <v>555</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -3793,16 +3672,16 @@
         <v>101</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>586</v>
+        <v>556</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -3813,369 +3692,249 @@
         <v>103</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>587</v>
+        <v>557</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>104</v>
+        <v>233</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>588</v>
+        <v>558</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>384</v>
+        <v>373</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>105</v>
+        <v>618</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>385</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>589</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>386</v>
-      </c>
-      <c r="E51" s="9" t="s">
-        <v>387</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>388</v>
-      </c>
+        <v>619</v>
+      </c>
+      <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>106</v>
+        <v>649</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>590</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>389</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>390</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>108</v>
+        <v>620</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>591</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>392</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>393</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>394</v>
+        <v>621</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>110</v>
+        <v>650</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>592</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>395</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>112</v>
+        <v>646</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>593</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>398</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>399</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>400</v>
+        <v>67</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>401</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>594</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>402</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="F56" s="8" t="s">
-        <v>404</v>
+        <v>638</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="F57" s="8"/>
+        <v>639</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>639</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>697</v>
+        <v>657</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>696</v>
+        <v>657</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>656</v>
+        <v>658</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>698</v>
+        <v>636</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>695</v>
+        <v>637</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>694</v>
+        <v>622</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>67</v>
+        <v>641</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>686</v>
+        <v>652</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>686</v>
+        <v>659</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>687</v>
+        <v>661</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>687</v>
+        <v>651</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>705</v>
+        <v>640</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>706</v>
+        <v>660</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>684</v>
+        <v>653</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>634</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>658</v>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>642</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>689</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>700</v>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>644</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>709</v>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>669</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>688</v>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>671</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="B72" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>680</v>
+      </c>
+      <c r="B71" t="s">
+        <v>679</v>
+      </c>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+    </row>
+    <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>678</v>
+      </c>
+      <c r="B72" t="s">
+        <v>677</v>
+      </c>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+    </row>
+    <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>676</v>
+      </c>
+      <c r="B73" t="s">
+        <v>675</v>
+      </c>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+    </row>
+    <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>674</v>
+      </c>
+      <c r="B74" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>671</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>676</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>677</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>678</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>682</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>690</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>692</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>717</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>718</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>719</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>720</v>
-      </c>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F80"/>
+  <autoFilter ref="A1:F68"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -4193,54 +3952,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>651</v>
+        <v>615</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>652</v>
+        <v>616</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>653</v>
+        <v>617</v>
       </c>
       <c r="H1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="I1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="J1" t="s">
-        <v>644</v>
+        <v>608</v>
       </c>
       <c r="K1" t="s">
-        <v>645</v>
+        <v>609</v>
       </c>
       <c r="L1" t="s">
-        <v>646</v>
+        <v>610</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4255,10 +4014,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4271,41 +4030,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G5" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="M5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4314,27 +4073,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="H7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="I7" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="J7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="L7" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4343,24 +4102,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>649</v>
+        <v>613</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4369,24 +4128,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>647</v>
+        <v>611</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>650</v>
+        <v>614</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4395,24 +4154,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4421,24 +4180,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -4464,13 +4223,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4478,7 +4237,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -4492,7 +4251,7 @@
         <v>100</v>
       </c>
       <c r="C3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -4523,13 +4282,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>643</v>
+        <v>607</v>
       </c>
       <c r="D1" t="s">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="E1" t="s">
-        <v>541</v>
+        <v>511</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -4537,530 +4296,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>595</v>
+        <v>559</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>405</v>
+        <v>375</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>406</v>
+        <v>376</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>596</v>
+        <v>560</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>597</v>
+        <v>561</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B5" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>598</v>
+        <v>562</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>416</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>599</v>
+        <v>563</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>417</v>
+        <v>387</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>418</v>
+        <v>388</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>419</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>600</v>
+        <v>564</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>420</v>
+        <v>390</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>421</v>
+        <v>391</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>422</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>601</v>
+        <v>565</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>423</v>
+        <v>393</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>424</v>
+        <v>394</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>425</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>602</v>
+        <v>566</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>426</v>
+        <v>396</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>427</v>
+        <v>397</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>428</v>
+        <v>398</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>603</v>
+        <v>567</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>429</v>
+        <v>399</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>430</v>
+        <v>400</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>431</v>
+        <v>401</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>604</v>
+        <v>568</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>432</v>
+        <v>402</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>433</v>
+        <v>403</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>434</v>
+        <v>404</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B12" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>605</v>
+        <v>569</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>606</v>
+        <v>570</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>435</v>
+        <v>405</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>436</v>
+        <v>406</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>437</v>
+        <v>407</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>607</v>
+        <v>571</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>530</v>
+        <v>500</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>531</v>
+        <v>501</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>532</v>
+        <v>502</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B15" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>608</v>
+        <v>572</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>533</v>
+        <v>503</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>534</v>
+        <v>504</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>535</v>
+        <v>505</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B16" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>609</v>
+        <v>573</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>536</v>
+        <v>506</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>537</v>
+        <v>507</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>438</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>610</v>
+        <v>574</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>538</v>
+        <v>508</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>539</v>
+        <v>509</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>439</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>611</v>
+        <v>575</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>440</v>
+        <v>410</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>441</v>
+        <v>411</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>442</v>
+        <v>412</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B19" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>612</v>
+        <v>576</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>443</v>
+        <v>413</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>444</v>
+        <v>414</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>445</v>
+        <v>415</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>613</v>
+        <v>577</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>446</v>
+        <v>416</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>447</v>
+        <v>417</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>448</v>
+        <v>418</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B21" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>614</v>
+        <v>578</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>449</v>
+        <v>419</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>450</v>
+        <v>420</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>451</v>
+        <v>421</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B22" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>615</v>
+        <v>579</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>452</v>
+        <v>422</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>453</v>
+        <v>423</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>454</v>
+        <v>424</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B23" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>616</v>
+        <v>580</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>455</v>
+        <v>425</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>456</v>
+        <v>426</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>457</v>
+        <v>427</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B24" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>617</v>
+        <v>581</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>458</v>
+        <v>428</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>459</v>
+        <v>429</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>460</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B25" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>618</v>
+        <v>582</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>461</v>
+        <v>431</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>462</v>
+        <v>432</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B26" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>619</v>
+        <v>583</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>463</v>
+        <v>433</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>464</v>
+        <v>434</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>465</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B27" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>620</v>
+        <v>584</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>466</v>
+        <v>436</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>467</v>
+        <v>437</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>468</v>
+        <v>438</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -5069,10 +4828,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B29" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -5081,42 +4840,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B30" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>621</v>
+        <v>585</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>469</v>
+        <v>439</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>470</v>
+        <v>440</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>471</v>
+        <v>441</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B31" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>622</v>
+        <v>586</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>472</v>
+        <v>442</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>473</v>
+        <v>443</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>474</v>
+        <v>444</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -5127,70 +4886,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B33" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>623</v>
+        <v>587</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>475</v>
+        <v>445</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>476</v>
+        <v>446</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>477</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B34" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>624</v>
+        <v>588</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>478</v>
+        <v>448</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>479</v>
+        <v>449</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>480</v>
+        <v>450</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B35" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>625</v>
+        <v>589</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>481</v>
+        <v>451</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>482</v>
+        <v>452</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>483</v>
+        <v>453</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -5199,369 +4958,369 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B37" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>626</v>
+        <v>590</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>484</v>
+        <v>454</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>485</v>
+        <v>455</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>486</v>
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B38" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>627</v>
+        <v>591</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>487</v>
+        <v>457</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>488</v>
+        <v>458</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>489</v>
+        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B39" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>628</v>
+        <v>592</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>490</v>
+        <v>460</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>491</v>
+        <v>461</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>492</v>
+        <v>462</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>629</v>
+        <v>593</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>493</v>
+        <v>463</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>494</v>
+        <v>464</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>495</v>
+        <v>465</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B41" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>630</v>
+        <v>594</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>496</v>
+        <v>466</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>497</v>
+        <v>467</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>498</v>
+        <v>468</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B42" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>631</v>
+        <v>595</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>499</v>
+        <v>469</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>500</v>
+        <v>470</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>501</v>
+        <v>471</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B43" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>632</v>
+        <v>596</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>502</v>
+        <v>472</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>503</v>
+        <v>473</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B44" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>633</v>
+        <v>597</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>504</v>
+        <v>474</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>506</v>
+        <v>476</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B45" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>634</v>
+        <v>598</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>507</v>
+        <v>477</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B46" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>635</v>
+        <v>599</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>511</v>
+        <v>481</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>512</v>
+        <v>482</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B47" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>636</v>
+        <v>600</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>515</v>
+        <v>485</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B48" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>637</v>
+        <v>601</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>516</v>
+        <v>486</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>517</v>
+        <v>487</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>518</v>
+        <v>488</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B49" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>638</v>
+        <v>602</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>519</v>
+        <v>489</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>520</v>
+        <v>490</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>521</v>
+        <v>491</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>639</v>
+        <v>603</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>522</v>
+        <v>492</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>523</v>
+        <v>493</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>524</v>
+        <v>494</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B51" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>640</v>
+        <v>604</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>525</v>
+        <v>495</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>470</v>
+        <v>440</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>526</v>
+        <v>496</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B52" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>622</v>
+        <v>586</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>472</v>
+        <v>442</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>473</v>
+        <v>443</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>474</v>
+        <v>444</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B53" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>641</v>
+        <v>605</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>527</v>
+        <v>497</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>528</v>
+        <v>498</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>529</v>
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B54" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>642</v>
+        <v>606</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>513</v>
+        <v>483</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>514</v>
+        <v>484</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>515</v>
+        <v>485</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>660</v>
-      </c>
-      <c r="B55" s="10" t="s">
+      <c r="A55" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="B55" s="9" t="s">
         <v>59</v>
       </c>
       <c r="C55" s="5" t="s">
@@ -5569,37 +5328,37 @@
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
-        <v>665</v>
+        <v>629</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
-        <v>661</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>662</v>
+      <c r="A56" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>626</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>668</v>
+        <v>632</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
-        <v>666</v>
+        <v>630</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>663</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>664</v>
+      <c r="A57" s="9" t="s">
+        <v>627</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>628</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>669</v>
+        <v>633</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>667</v>
+        <v>631</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
make list views render correctly, which called for a overhaul of how the search function works. Also fix some wordings in adminstrator paths
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="677">
   <si>
     <t>comments</t>
   </si>
@@ -230,12 +230,6 @@
   </si>
   <si>
     <t>No Disabled Beneficiary Detected</t>
-  </si>
-  <si>
-    <t>enter_beneficiary_code</t>
-  </si>
-  <si>
-    <t>Please Enter Beneficiary Code</t>
   </si>
   <si>
     <t>disabled_beneficiaries_title</t>
@@ -904,18 +898,6 @@
     <t>Anulación creada satisfactoriamente</t>
   </si>
   <si>
-    <t>View Distribution Details</t>
-  </si>
-  <si>
-    <t>انظر تفاصيل التوزيع</t>
-  </si>
-  <si>
-    <t>جزئیات نمایش توزیع</t>
-  </si>
-  <si>
-    <t>Ver detalles de la distribución</t>
-  </si>
-  <si>
     <t>مسح الباركود</t>
   </si>
   <si>
@@ -952,15 +934,6 @@
     <t>Detectado beneficiario no desactivado</t>
   </si>
   <si>
-    <t>الرجاء إدخال رمز المستفيد</t>
-  </si>
-  <si>
-    <t xml:space="preserve">لطفا کد ذینفع را وارد کنید </t>
-  </si>
-  <si>
-    <t>Por favor introduce el código del beneficiario</t>
-  </si>
-  <si>
     <t>المستفيدين النشطين</t>
   </si>
   <si>
@@ -1636,9 +1609,6 @@
     <t>Η παράκαμψη δημιουργήθηκε με επιτυχία</t>
   </si>
   <si>
-    <t>Προβολή λεπτομερειών διανομής</t>
-  </si>
-  <si>
     <t>Σάρωση γραμμωτού κώδικα</t>
   </si>
   <si>
@@ -1651,9 +1621,6 @@
     <t>Δεν εντοπίστηκε δικαιούχος με αναπηρία</t>
   </si>
   <si>
-    <t>Εισαγάγετε τον Κωδικό Δικαιούχου</t>
-  </si>
-  <si>
     <t>Ενεργοί Δικαιούχοι</t>
   </si>
   <si>
@@ -2093,6 +2060,27 @@
   </si>
   <si>
     <t>enable_success</t>
+  </si>
+  <si>
+    <t>Authorization Details</t>
+  </si>
+  <si>
+    <t>authorization_details</t>
+  </si>
+  <si>
+    <t>choose_authorization</t>
+  </si>
+  <si>
+    <t>Choose Authorization</t>
+  </si>
+  <si>
+    <t>View Authorization Details</t>
+  </si>
+  <si>
+    <t>enter_beneficiary_entity_id</t>
+  </si>
+  <si>
+    <t>Enter Beneficiary Entity ID</t>
   </si>
 </sst>
 </file>
@@ -2673,14 +2661,14 @@
     </row>
     <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -2698,14 +2686,14 @@
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E12" t="s">
         <v>21</v>
@@ -2729,10 +2717,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2751,13 +2739,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>25</v>
@@ -2765,7 +2753,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
@@ -2774,10 +2762,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>667</v>
+        <v>656</v>
       </c>
       <c r="B3" t="s">
-        <v>668</v>
+        <v>657</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -2789,16 +2777,16 @@
         <v>27</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>240</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2809,16 +2797,16 @@
         <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="D5" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2829,13 +2817,13 @@
         <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>32</v>
@@ -2849,13 +2837,13 @@
         <v>34</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>35</v>
@@ -2869,36 +2857,36 @@
         <v>37</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="B9" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D9" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>255</v>
       </c>
       <c r="G9" s="11"/>
     </row>
@@ -2907,19 +2895,19 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="D10" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F10" s="12" t="s">
         <v>256</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>257</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>258</v>
       </c>
       <c r="G10" s="13"/>
     </row>
@@ -2928,19 +2916,19 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>665</v>
+        <v>654</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>259</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2951,13 +2939,13 @@
         <v>41</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>42</v>
@@ -2971,16 +2959,16 @@
         <v>44</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>264</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2991,16 +2979,16 @@
         <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>267</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3011,16 +2999,16 @@
         <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -3031,16 +3019,16 @@
         <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.2">
@@ -3051,16 +3039,16 @@
         <v>52</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="F17" s="8" t="s">
         <v>275</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3071,16 +3059,16 @@
         <v>54</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>278</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -3091,16 +3079,16 @@
         <v>56</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="F19" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
@@ -3108,19 +3096,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>284</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>528</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>286</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>287</v>
+        <v>674</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3131,16 +3107,16 @@
         <v>59</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -3151,36 +3127,36 @@
         <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>654</v>
+        <v>643</v>
       </c>
       <c r="B23" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -3191,454 +3167,442 @@
         <v>63</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>675</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>302</v>
+        <v>676</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>656</v>
+        <v>645</v>
       </c>
       <c r="B26" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>534</v>
+        <v>523</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>536</v>
+        <v>525</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>537</v>
+        <v>526</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>538</v>
+        <v>527</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B31" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>539</v>
+        <v>528</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>540</v>
+        <v>529</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>541</v>
+        <v>530</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>542</v>
+        <v>531</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>543</v>
+        <v>532</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>544</v>
+        <v>533</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>666</v>
+        <v>655</v>
       </c>
       <c r="B39" t="s">
-        <v>663</v>
+        <v>652</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>547</v>
+        <v>536</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="F39" s="12" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>549</v>
+        <v>538</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>550</v>
+        <v>539</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>551</v>
+        <v>540</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>553</v>
+        <v>542</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>554</v>
+        <v>543</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F46" s="5" t="s">
         <v>35</v>
@@ -3646,251 +3610,251 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>555</v>
+        <v>544</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>556</v>
+        <v>545</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>558</v>
+        <v>547</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>618</v>
+        <v>607</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>619</v>
+        <v>608</v>
       </c>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>649</v>
+        <v>638</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>648</v>
+        <v>637</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>620</v>
+        <v>609</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>621</v>
+        <v>610</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>650</v>
+        <v>639</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>647</v>
+        <v>636</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>646</v>
+        <v>635</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>638</v>
+        <v>627</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>639</v>
+        <v>628</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>657</v>
+        <v>646</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>658</v>
+        <v>647</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>636</v>
+        <v>625</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>637</v>
+        <v>626</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>622</v>
+        <v>611</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>641</v>
+        <v>630</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>652</v>
+        <v>641</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>659</v>
+        <v>648</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>661</v>
+        <v>650</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>651</v>
+        <v>640</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>640</v>
+        <v>629</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>623</v>
+        <v>612</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>653</v>
+        <v>642</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>634</v>
+        <v>623</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>635</v>
+        <v>624</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>642</v>
+        <v>631</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>645</v>
+        <v>634</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>669</v>
+        <v>658</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>670</v>
+        <v>659</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>671</v>
+        <v>660</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>672</v>
+        <v>661</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>680</v>
+        <v>669</v>
       </c>
       <c r="B71" t="s">
-        <v>679</v>
+        <v>668</v>
       </c>
       <c r="C71"/>
       <c r="D71"/>
@@ -3899,10 +3863,10 @@
     </row>
     <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>678</v>
+        <v>667</v>
       </c>
       <c r="B72" t="s">
-        <v>677</v>
+        <v>666</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
@@ -3911,10 +3875,10 @@
     </row>
     <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>676</v>
+        <v>665</v>
       </c>
       <c r="B73" t="s">
-        <v>675</v>
+        <v>664</v>
       </c>
       <c r="C73"/>
       <c r="D73"/>
@@ -3923,15 +3887,31 @@
     </row>
     <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>674</v>
+        <v>663</v>
       </c>
       <c r="B74" t="s">
-        <v>673</v>
+        <v>662</v>
       </c>
       <c r="C74"/>
       <c r="D74"/>
       <c r="E74"/>
       <c r="F74"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>671</v>
+      </c>
+      <c r="B75" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>672</v>
+      </c>
+      <c r="B76" t="s">
+        <v>673</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F68"/>
@@ -3952,54 +3932,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="H1" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="I1" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="H1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I1" t="s">
-        <v>109</v>
-      </c>
       <c r="J1" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
       <c r="K1" t="s">
-        <v>609</v>
+        <v>598</v>
       </c>
       <c r="L1" t="s">
-        <v>610</v>
+        <v>599</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4014,10 +3994,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4030,41 +4010,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G5" t="s">
+        <v>116</v>
+      </c>
+      <c r="M5" t="s">
         <v>117</v>
-      </c>
-      <c r="C5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-      <c r="F5" t="s">
-        <v>118</v>
-      </c>
-      <c r="G5" t="s">
-        <v>118</v>
-      </c>
-      <c r="M5" t="s">
-        <v>119</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4073,27 +4053,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H7" t="s">
+        <v>119</v>
+      </c>
+      <c r="I7" t="s">
         <v>120</v>
       </c>
-      <c r="H7" t="s">
-        <v>121</v>
-      </c>
-      <c r="I7" t="s">
-        <v>122</v>
-      </c>
       <c r="J7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="L7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4102,24 +4082,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4128,24 +4108,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -4154,24 +4134,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -4180,24 +4160,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -4223,13 +4203,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -4237,7 +4217,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -4248,10 +4228,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -4282,13 +4262,13 @@
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>607</v>
+        <v>596</v>
       </c>
       <c r="D1" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="E1" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="F1" t="s">
         <v>25</v>
@@ -4296,530 +4276,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>559</v>
+        <v>548</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>560</v>
+        <v>549</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>561</v>
+        <v>550</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>562</v>
+        <v>551</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>563</v>
+        <v>552</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>564</v>
+        <v>553</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>565</v>
+        <v>554</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>566</v>
+        <v>555</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>567</v>
+        <v>556</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>568</v>
+        <v>557</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>569</v>
+        <v>558</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>570</v>
+        <v>559</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>571</v>
+        <v>560</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>572</v>
+        <v>561</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>577</v>
+        <v>566</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>578</v>
+        <v>567</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B25" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B26" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -4828,10 +4808,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4840,42 +4820,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B30" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -4886,70 +4866,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>587</v>
+        <v>576</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B35" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -4958,367 +4938,367 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B37" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="F37" s="8" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>592</v>
+        <v>581</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B40" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>593</v>
+        <v>582</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B41" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B42" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B43" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>596</v>
+        <v>585</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>597</v>
+        <v>586</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B45" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>598</v>
+        <v>587</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B46" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>599</v>
+        <v>588</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B47" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B48" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>601</v>
+        <v>590</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B49" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>602</v>
+        <v>591</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B50" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>603</v>
+        <v>592</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B51" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>604</v>
+        <v>593</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B52" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>586</v>
+        <v>575</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>605</v>
+        <v>594</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B54" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>606</v>
+        <v>595</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>624</v>
+        <v>613</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>59</v>
@@ -5328,37 +5308,37 @@
       </c>
       <c r="D55" s="5"/>
       <c r="F55" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
-        <v>625</v>
+        <v>614</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>626</v>
+        <v>615</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>632</v>
+        <v>621</v>
       </c>
       <c r="D56" s="5"/>
       <c r="F56" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>627</v>
+        <v>616</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>628</v>
+        <v>617</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>633</v>
+        <v>622</v>
       </c>
       <c r="D57" s="5"/>
       <c r="F57" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
authorization creation in token mode working as intended
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="685">
   <si>
     <t>comments</t>
   </si>
@@ -2081,6 +2081,30 @@
   </si>
   <si>
     <t>Enter Beneficiary Entity ID</t>
+  </si>
+  <si>
+    <t>choose_authorization_name</t>
+  </si>
+  <si>
+    <t>Choose Authorization Name</t>
+  </si>
+  <si>
+    <t>administrator_reset_succeeded</t>
+  </si>
+  <si>
+    <t>Administrator Reset Succeeded</t>
+  </si>
+  <si>
+    <t>administrator_reset_failed</t>
+  </si>
+  <si>
+    <t>Administrator Reset Failed</t>
+  </si>
+  <si>
+    <t>trigger_reset</t>
+  </si>
+  <si>
+    <t>Trigger Reset</t>
   </si>
 </sst>
 </file>
@@ -2717,10 +2741,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G76"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3911,6 +3935,38 @@
       </c>
       <c r="B76" t="s">
         <v>673</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>677</v>
+      </c>
+      <c r="B77" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>679</v>
+      </c>
+      <c r="B78" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>681</v>
+      </c>
+      <c r="B79" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>683</v>
+      </c>
+      <c r="B80" t="s">
+        <v>684</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
authorization_reports -> distribution reports. translations individual -> member. More table column name changes.
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="7300" yWindow="2560" windowWidth="38400" windowHeight="22220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -1972,12 +1972,6 @@
     <t>enabled_beneficiaries</t>
   </si>
   <si>
-    <t>Individual Advanced Search</t>
-  </si>
-  <si>
-    <t>search_individuals</t>
-  </si>
-  <si>
     <t>Beneficiaries Advanced Search</t>
   </si>
   <si>
@@ -1990,21 +1984,9 @@
     <t>enabled_beneficiaries_title</t>
   </si>
   <si>
-    <t>individual</t>
-  </si>
-  <si>
-    <t>individuals</t>
-  </si>
-  <si>
-    <t>Search for Individuals</t>
-  </si>
-  <si>
     <t>search_beneficiaries_title</t>
   </si>
   <si>
-    <t>search_individuals_title</t>
-  </si>
-  <si>
     <t>administrator_path</t>
   </si>
   <si>
@@ -2105,6 +2087,24 @@
   </si>
   <si>
     <t>Trigger Reset</t>
+  </si>
+  <si>
+    <t>member</t>
+  </si>
+  <si>
+    <t>members</t>
+  </si>
+  <si>
+    <t>search_members</t>
+  </si>
+  <si>
+    <t>Search for Members</t>
+  </si>
+  <si>
+    <t>search_members_title</t>
+  </si>
+  <si>
+    <t>Member Advanced Search</t>
   </si>
 </sst>
 </file>
@@ -2743,8 +2743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2786,10 +2786,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="B3" t="s">
-        <v>657</v>
+        <v>651</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -2895,10 +2895,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="B9" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>508</v>
@@ -2919,7 +2919,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>509</v>
@@ -2940,7 +2940,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>510</v>
@@ -3120,7 +3120,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>674</v>
+        <v>668</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3165,10 +3165,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="B23" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>521</v>
@@ -3205,15 +3205,15 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>675</v>
+        <v>669</v>
       </c>
       <c r="B25" t="s">
-        <v>676</v>
+        <v>670</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="B26" t="s">
         <v>636</v>
@@ -3473,10 +3473,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="B39" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>536</v>
@@ -3771,18 +3771,18 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>646</v>
+        <v>679</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>646</v>
+        <v>679</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>647</v>
+        <v>680</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>647</v>
+        <v>680</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3803,18 +3803,18 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>641</v>
+        <v>681</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>648</v>
+        <v>682</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>650</v>
+        <v>683</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>640</v>
+        <v>684</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3827,10 +3827,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3859,26 +3859,26 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>658</v>
+        <v>652</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>659</v>
+        <v>653</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>660</v>
+        <v>654</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>661</v>
+        <v>655</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>669</v>
+        <v>663</v>
       </c>
       <c r="B71" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
       <c r="C71"/>
       <c r="D71"/>
@@ -3887,10 +3887,10 @@
     </row>
     <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="B72" t="s">
-        <v>666</v>
+        <v>660</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
@@ -3899,10 +3899,10 @@
     </row>
     <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>665</v>
+        <v>659</v>
       </c>
       <c r="B73" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C73"/>
       <c r="D73"/>
@@ -3911,10 +3911,10 @@
     </row>
     <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>663</v>
+        <v>657</v>
       </c>
       <c r="B74" t="s">
-        <v>662</v>
+        <v>656</v>
       </c>
       <c r="C74"/>
       <c r="D74"/>
@@ -3923,50 +3923,50 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
       <c r="B75" t="s">
-        <v>670</v>
+        <v>664</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
       <c r="B76" t="s">
-        <v>673</v>
+        <v>667</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>677</v>
+        <v>671</v>
       </c>
       <c r="B77" t="s">
-        <v>678</v>
+        <v>672</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
       <c r="B78" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>681</v>
+        <v>675</v>
       </c>
       <c r="B79" t="s">
-        <v>682</v>
+        <v>676</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>683</v>
+        <v>677</v>
       </c>
       <c r="B80" t="s">
-        <v>684</v>
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add authorization progress summary view
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7300" yWindow="2560" windowWidth="38400" windowHeight="22220" tabRatio="989" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="989" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="689">
   <si>
     <t>comments</t>
   </si>
@@ -2105,6 +2105,18 @@
   </si>
   <si>
     <t>Member Advanced Search</t>
+  </si>
+  <si>
+    <t>view_authorization_progress</t>
+  </si>
+  <si>
+    <t>view_deliveries</t>
+  </si>
+  <si>
+    <t>View Deliveries</t>
+  </si>
+  <si>
+    <t>Progress By Authorization</t>
   </si>
 </sst>
 </file>
@@ -2741,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G80"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3967,6 +3979,22 @@
       </c>
       <c r="B80" t="s">
         <v>678</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>685</v>
+      </c>
+      <c r="B81" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>686</v>
+      </c>
+      <c r="B82" t="s">
+        <v>687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit before mergining in development
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="793">
   <si>
     <t>comments</t>
   </si>
@@ -1942,9 +1942,6 @@
     <t>search_households_title</t>
   </si>
   <si>
-    <t>Search for Households</t>
-  </si>
-  <si>
     <t>view</t>
   </si>
   <si>
@@ -2098,9 +2095,6 @@
     <t>search_members</t>
   </si>
   <si>
-    <t>Search for Members</t>
-  </si>
-  <si>
     <t>search_members_title</t>
   </si>
   <si>
@@ -2117,6 +2111,324 @@
   </si>
   <si>
     <t>Progress By Authorization</t>
+  </si>
+  <si>
+    <t>Search by Household</t>
+  </si>
+  <si>
+    <t>Search by Member</t>
+  </si>
+  <si>
+    <t>is_override</t>
+  </si>
+  <si>
+    <t>Is Override</t>
+  </si>
+  <si>
+    <t>beneficiary_entity_id</t>
+  </si>
+  <si>
+    <t>Beneficiary Entity ID</t>
+  </si>
+  <si>
+    <t>date_created</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>custom_beneficiary_entity_form_id</t>
+  </si>
+  <si>
+    <t>Custom Beneficiary Entity Form ID</t>
+  </si>
+  <si>
+    <t>custom_beneficiary_entity_row_id</t>
+  </si>
+  <si>
+    <t>Custom Beneficiary Entity Row ID</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>status_reason</t>
+  </si>
+  <si>
+    <t>Status Reason</t>
+  </si>
+  <si>
+    <t>id_number</t>
+  </si>
+  <si>
+    <t>ID Number</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>telephone</t>
+  </si>
+  <si>
+    <t>Telephone</t>
+  </si>
+  <si>
+    <t>mobile_provider</t>
+  </si>
+  <si>
+    <t>Mobile Provider</t>
+  </si>
+  <si>
+    <t>delivery_site</t>
+  </si>
+  <si>
+    <t>Delivery Site</t>
+  </si>
+  <si>
+    <t>hh_size</t>
+  </si>
+  <si>
+    <t>Household Size</t>
+  </si>
+  <si>
+    <t>disabled_reason</t>
+  </si>
+  <si>
+    <t>Disabled Reason</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>tent_caravan</t>
+  </si>
+  <si>
+    <t>Tent/Caravan Code</t>
+  </si>
+  <si>
+    <t>authorization_id</t>
+  </si>
+  <si>
+    <t>Authorization ID</t>
+  </si>
+  <si>
+    <t>authorization_type</t>
+  </si>
+  <si>
+    <t>Authorization Type</t>
+  </si>
+  <si>
+    <t>authorization_name</t>
+  </si>
+  <si>
+    <t>Authorization Name</t>
+  </si>
+  <si>
+    <t>authorization_description</t>
+  </si>
+  <si>
+    <t>Authorization Description</t>
+  </si>
+  <si>
+    <t>member_id</t>
+  </si>
+  <si>
+    <t>Member ID</t>
+  </si>
+  <si>
+    <t>entitlement_id</t>
+  </si>
+  <si>
+    <t>Entitlement ID</t>
+  </si>
+  <si>
+    <t>item_pack_id</t>
+  </si>
+  <si>
+    <t>Item Pack ID</t>
+  </si>
+  <si>
+    <t>Αναγνωριστικό πακέτου στοιχείου</t>
+  </si>
+  <si>
+    <t>رقم الحزمة</t>
+  </si>
+  <si>
+    <t>شماره بسته</t>
+  </si>
+  <si>
+    <t>ID del artículo</t>
+  </si>
+  <si>
+    <t>item_pack_name</t>
+  </si>
+  <si>
+    <t>Item Pack Name</t>
+  </si>
+  <si>
+    <t>Όνομα πακέτου στοιχείου</t>
+  </si>
+  <si>
+    <t>اسم الحزمة</t>
+  </si>
+  <si>
+    <t>نام بسته</t>
+  </si>
+  <si>
+    <t>Nombre del artículo</t>
+  </si>
+  <si>
+    <t>item_pack_description</t>
+  </si>
+  <si>
+    <t>Item Pack Description</t>
+  </si>
+  <si>
+    <t>Περιγραφή πακέτου στοιχείου</t>
+  </si>
+  <si>
+    <t>وصف الحزمة</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> شرح بسته</t>
+  </si>
+  <si>
+    <t>Descripción del artículo</t>
+  </si>
+  <si>
+    <t>custom_delivery_form_id</t>
+  </si>
+  <si>
+    <t>Custom Delivery Form ID</t>
+  </si>
+  <si>
+    <t>custom_delivery_row_id</t>
+  </si>
+  <si>
+    <t>Custom Delivery Row ID</t>
+  </si>
+  <si>
+    <t>assigned_item_pack_code</t>
+  </si>
+  <si>
+    <t>Assigned Item Pack Barcode</t>
+  </si>
+  <si>
+    <t>beneficiary_entity_row_id</t>
+  </si>
+  <si>
+    <t>Beneficiary Entity Row ID</t>
+  </si>
+  <si>
+    <t>custom_member_form_id</t>
+  </si>
+  <si>
+    <t>Custom Member Form ID</t>
+  </si>
+  <si>
+    <t>custom_member_row_id</t>
+  </si>
+  <si>
+    <t>Custom Member Row ID</t>
+  </si>
+  <si>
+    <t>date_screened</t>
+  </si>
+  <si>
+    <t>Date Screened</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>first_last_name</t>
+  </si>
+  <si>
+    <t>First and Last Name</t>
+  </si>
+  <si>
+    <t>birth_date</t>
+  </si>
+  <si>
+    <t>Birth Date</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>ID Type</t>
+  </si>
+  <si>
+    <t>beneficiary_code</t>
+  </si>
+  <si>
+    <t>Beneficiary Code</t>
+  </si>
+  <si>
+    <t>verify_user</t>
+  </si>
+  <si>
+    <t>Verify User</t>
+  </si>
+  <si>
+    <t>is_head_of_household</t>
+  </si>
+  <si>
+    <t>Is Head of Household</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>Picture</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>vulnerability</t>
+  </si>
+  <si>
+    <t>Vulnerability</t>
   </si>
 </sst>
 </file>
@@ -2169,7 +2481,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2182,11 +2494,43 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -2199,7 +2543,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2226,6 +2570,9 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2753,10 +3100,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G82"/>
+  <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2798,10 +3145,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>649</v>
+      </c>
+      <c r="B3" t="s">
         <v>650</v>
-      </c>
-      <c r="B3" t="s">
-        <v>651</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -2907,10 +3254,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>644</v>
+      </c>
+      <c r="B9" t="s">
         <v>645</v>
-      </c>
-      <c r="B9" t="s">
-        <v>646</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>508</v>
@@ -2931,7 +3278,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>509</v>
@@ -2952,7 +3299,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>510</v>
@@ -3132,7 +3479,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -3177,10 +3524,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>640</v>
+      </c>
+      <c r="B23" t="s">
         <v>641</v>
-      </c>
-      <c r="B23" t="s">
-        <v>642</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>521</v>
@@ -3217,18 +3564,18 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>668</v>
+      </c>
+      <c r="B25" t="s">
         <v>669</v>
-      </c>
-      <c r="B25" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B26" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>523</v>
@@ -3485,10 +3832,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B39" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>536</v>
@@ -3735,10 +4082,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
@@ -3751,15 +4098,15 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>65</v>
@@ -3783,18 +4130,18 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -3810,23 +4157,23 @@
         <v>611</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>630</v>
+        <v>687</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>682</v>
+        <v>688</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
@@ -3839,10 +4186,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -3855,42 +4202,42 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>630</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>632</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>633</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>651</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>652</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>653</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A71" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B71" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C71"/>
       <c r="D71"/>
@@ -3899,10 +4246,10 @@
     </row>
     <row r="72" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A72" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B72" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C72"/>
       <c r="D72"/>
@@ -3911,10 +4258,10 @@
     </row>
     <row r="73" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A73" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B73" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C73"/>
       <c r="D73"/>
@@ -3923,10 +4270,10 @@
     </row>
     <row r="74" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A74" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B74" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C74"/>
       <c r="D74"/>
@@ -3935,66 +4282,656 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B75" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>665</v>
+      </c>
+      <c r="B76" t="s">
         <v>666</v>
-      </c>
-      <c r="B76" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>670</v>
+      </c>
+      <c r="B77" t="s">
         <v>671</v>
-      </c>
-      <c r="B77" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>672</v>
+      </c>
+      <c r="B78" t="s">
         <v>673</v>
-      </c>
-      <c r="B78" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>674</v>
+      </c>
+      <c r="B79" t="s">
         <v>675</v>
-      </c>
-      <c r="B79" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>676</v>
+      </c>
+      <c r="B80" t="s">
         <v>677</v>
       </c>
-      <c r="B80" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>683</v>
+      </c>
+      <c r="B81" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>684</v>
+      </c>
+      <c r="B82" t="s">
         <v>685</v>
       </c>
-      <c r="B81" t="s">
-        <v>688</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>686</v>
-      </c>
-      <c r="B82" t="s">
-        <v>687</v>
+    </row>
+    <row r="84" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A84" t="s">
+        <v>691</v>
+      </c>
+      <c r="B84" t="s">
+        <v>692</v>
+      </c>
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A85" t="s">
+        <v>693</v>
+      </c>
+      <c r="B85" t="s">
+        <v>694</v>
+      </c>
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A86" t="s">
+        <v>695</v>
+      </c>
+      <c r="B86" t="s">
+        <v>696</v>
+      </c>
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A87" t="s">
+        <v>697</v>
+      </c>
+      <c r="B87" t="s">
+        <v>698</v>
+      </c>
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A88" t="s">
+        <v>699</v>
+      </c>
+      <c r="B88" t="s">
+        <v>700</v>
+      </c>
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A89" t="s">
+        <v>701</v>
+      </c>
+      <c r="B89" t="s">
+        <v>702</v>
+      </c>
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A91" t="s">
+        <v>705</v>
+      </c>
+      <c r="B91" t="s">
+        <v>706</v>
+      </c>
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A92" t="s">
+        <v>707</v>
+      </c>
+      <c r="B92" t="s">
+        <v>708</v>
+      </c>
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A93" t="s">
+        <v>709</v>
+      </c>
+      <c r="B93" t="s">
+        <v>710</v>
+      </c>
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A94" t="s">
+        <v>711</v>
+      </c>
+      <c r="B94" t="s">
+        <v>712</v>
+      </c>
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A95" t="s">
+        <v>713</v>
+      </c>
+      <c r="B95" t="s">
+        <v>714</v>
+      </c>
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A96" t="s">
+        <v>717</v>
+      </c>
+      <c r="B96" t="s">
+        <v>718</v>
+      </c>
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A97" t="s">
+        <v>719</v>
+      </c>
+      <c r="B97" t="s">
+        <v>720</v>
+      </c>
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A99" t="s">
+        <v>721</v>
+      </c>
+      <c r="B99" t="s">
+        <v>722</v>
+      </c>
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A100" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="B100" t="s">
+        <v>724</v>
+      </c>
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A101" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="B101" t="s">
+        <v>726</v>
+      </c>
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A102" s="14" t="s">
+        <v>727</v>
+      </c>
+      <c r="B102" t="s">
+        <v>728</v>
+      </c>
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A103" s="14" t="s">
+        <v>729</v>
+      </c>
+      <c r="B103" t="s">
+        <v>730</v>
+      </c>
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A104" s="14" t="s">
+        <v>731</v>
+      </c>
+      <c r="B104" t="s">
+        <v>732</v>
+      </c>
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A105" s="14" t="s">
+        <v>733</v>
+      </c>
+      <c r="B105" t="s">
+        <v>734</v>
+      </c>
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A106" s="14" t="s">
+        <v>689</v>
+      </c>
+      <c r="B106" t="s">
+        <v>690</v>
+      </c>
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106"/>
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="14" t="s">
+        <v>735</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C107" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="E107" s="15" t="s">
+        <v>739</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="14" t="s">
+        <v>741</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="D108" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A109" s="14" t="s">
+        <v>747</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A110" s="14" t="s">
+        <v>753</v>
+      </c>
+      <c r="B110" t="s">
+        <v>754</v>
+      </c>
+      <c r="C110"/>
+      <c r="D110"/>
+      <c r="E110"/>
+      <c r="F110"/>
+    </row>
+    <row r="111" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A111" s="14" t="s">
+        <v>755</v>
+      </c>
+      <c r="B111" t="s">
+        <v>756</v>
+      </c>
+      <c r="C111"/>
+      <c r="D111"/>
+      <c r="E111"/>
+      <c r="F111"/>
+    </row>
+    <row r="112" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A112" t="s">
+        <v>757</v>
+      </c>
+      <c r="B112" t="s">
+        <v>758</v>
+      </c>
+      <c r="C112"/>
+      <c r="D112"/>
+      <c r="E112"/>
+      <c r="F112"/>
+    </row>
+    <row r="113" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="C113"/>
+      <c r="D113"/>
+      <c r="E113"/>
+      <c r="F113"/>
+    </row>
+    <row r="114" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A114" s="14" t="s">
+        <v>759</v>
+      </c>
+      <c r="B114" t="s">
+        <v>760</v>
+      </c>
+      <c r="C114"/>
+      <c r="D114"/>
+      <c r="E114"/>
+      <c r="F114"/>
+    </row>
+    <row r="115" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A115" s="14" t="s">
+        <v>761</v>
+      </c>
+      <c r="B115" t="s">
+        <v>762</v>
+      </c>
+      <c r="C115"/>
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="F115"/>
+    </row>
+    <row r="116" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A116" s="14" t="s">
+        <v>763</v>
+      </c>
+      <c r="B116" t="s">
+        <v>764</v>
+      </c>
+      <c r="C116"/>
+      <c r="D116"/>
+      <c r="E116"/>
+      <c r="F116"/>
+    </row>
+    <row r="117" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A117" s="14" t="s">
+        <v>765</v>
+      </c>
+      <c r="B117" t="s">
+        <v>766</v>
+      </c>
+      <c r="C117"/>
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="F117"/>
+    </row>
+    <row r="118" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A118" s="14" t="s">
+        <v>767</v>
+      </c>
+      <c r="B118" t="s">
+        <v>768</v>
+      </c>
+      <c r="C118"/>
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="F118"/>
+    </row>
+    <row r="119" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A119" s="14" t="s">
+        <v>769</v>
+      </c>
+      <c r="B119" t="s">
+        <v>770</v>
+      </c>
+      <c r="C119"/>
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119"/>
+    </row>
+    <row r="120" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A120" s="14" t="s">
+        <v>771</v>
+      </c>
+      <c r="B120" t="s">
+        <v>772</v>
+      </c>
+      <c r="C120"/>
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120"/>
+    </row>
+    <row r="121" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A121" s="14" t="s">
+        <v>773</v>
+      </c>
+      <c r="B121" t="s">
+        <v>774</v>
+      </c>
+      <c r="C121"/>
+      <c r="D121"/>
+      <c r="E121"/>
+      <c r="F121"/>
+    </row>
+    <row r="122" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A122" s="14" t="s">
+        <v>775</v>
+      </c>
+      <c r="B122" t="s">
+        <v>776</v>
+      </c>
+      <c r="C122"/>
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122"/>
+    </row>
+    <row r="123" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A123" s="14" t="s">
+        <v>777</v>
+      </c>
+      <c r="B123" t="s">
+        <v>778</v>
+      </c>
+      <c r="C123"/>
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+    </row>
+    <row r="124" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A124" s="14" t="s">
+        <v>779</v>
+      </c>
+      <c r="B124" t="s">
+        <v>780</v>
+      </c>
+      <c r="C124"/>
+      <c r="D124"/>
+      <c r="E124"/>
+      <c r="F124"/>
+    </row>
+    <row r="125" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A125" s="14" t="s">
+        <v>703</v>
+      </c>
+      <c r="B125" t="s">
+        <v>704</v>
+      </c>
+      <c r="C125"/>
+      <c r="D125"/>
+      <c r="E125"/>
+      <c r="F125"/>
+    </row>
+    <row r="126" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A126" s="14" t="s">
+        <v>781</v>
+      </c>
+      <c r="B126" t="s">
+        <v>782</v>
+      </c>
+      <c r="C126"/>
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126"/>
+    </row>
+    <row r="127" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A127" s="14" t="s">
+        <v>783</v>
+      </c>
+      <c r="B127" t="s">
+        <v>784</v>
+      </c>
+      <c r="C127"/>
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+    </row>
+    <row r="128" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A128" s="14" t="s">
+        <v>785</v>
+      </c>
+      <c r="B128" t="s">
+        <v>786</v>
+      </c>
+      <c r="C128"/>
+      <c r="D128"/>
+      <c r="E128"/>
+      <c r="F128"/>
+    </row>
+    <row r="129" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A129" s="14" t="s">
+        <v>787</v>
+      </c>
+      <c r="B129" t="s">
+        <v>788</v>
+      </c>
+      <c r="C129"/>
+      <c r="D129"/>
+      <c r="E129"/>
+      <c r="F129"/>
+    </row>
+    <row r="130" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A130" s="14" t="s">
+        <v>789</v>
+      </c>
+      <c r="B130" t="s">
+        <v>790</v>
+      </c>
+      <c r="C130"/>
+      <c r="D130"/>
+      <c r="E130"/>
+      <c r="F130"/>
+    </row>
+    <row r="131" spans="1:6" ht="13" x14ac:dyDescent="0.15">
+      <c r="A131" s="14" t="s">
+        <v>791</v>
+      </c>
+      <c r="B131" t="s">
+        <v>792</v>
+      </c>
+      <c r="C131"/>
+      <c r="D131"/>
+      <c r="E131"/>
+      <c r="F131"/>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="16" t="s">
+        <v>715</v>
+      </c>
+      <c r="B132" t="s">
+        <v>716</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
various ui fixes for red cross march binaries, including alphabetizing fields and css
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="460" windowWidth="25140" windowHeight="16220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -916,9 +916,6 @@
     <t>no_authorizations</t>
   </si>
   <si>
-    <t>No Distributions</t>
-  </si>
-  <si>
     <t>Καμία διανομή</t>
   </si>
   <si>
@@ -2486,6 +2483,9 @@
   </si>
   <si>
     <t>View By Authorization</t>
+  </si>
+  <si>
+    <t>No Authorizations</t>
   </si>
 </sst>
 </file>
@@ -3097,8 +3097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -4052,49 +4052,49 @@
         <v>291</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>811</v>
+      </c>
+      <c r="C50" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="11" t="s">
         <v>295</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>297</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>299</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>301</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>159</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>165</v>
@@ -4110,630 +4110,630 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>311</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>313</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="B64" s="3" t="s">
         <v>317</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="B65" s="3" t="s">
         <v>319</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>320</v>
+      </c>
+      <c r="B66" s="3" t="s">
         <v>321</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
+        <v>322</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>323</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
+        <v>324</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>325</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>326</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>327</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
+        <v>328</v>
+      </c>
+      <c r="B70" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>330</v>
+      </c>
+      <c r="B71" t="s">
         <v>331</v>
-      </c>
-      <c r="B71" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
+        <v>332</v>
+      </c>
+      <c r="B72" t="s">
         <v>333</v>
-      </c>
-      <c r="B72" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
+        <v>334</v>
+      </c>
+      <c r="B73" t="s">
         <v>335</v>
-      </c>
-      <c r="B73" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>336</v>
+      </c>
+      <c r="B74" t="s">
         <v>337</v>
-      </c>
-      <c r="B74" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
+        <v>338</v>
+      </c>
+      <c r="B75" t="s">
         <v>339</v>
-      </c>
-      <c r="B75" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>340</v>
+      </c>
+      <c r="B76" t="s">
         <v>341</v>
-      </c>
-      <c r="B76" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>342</v>
+      </c>
+      <c r="B77" t="s">
         <v>343</v>
-      </c>
-      <c r="B77" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>344</v>
+      </c>
+      <c r="B78" t="s">
         <v>345</v>
-      </c>
-      <c r="B78" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
+        <v>346</v>
+      </c>
+      <c r="B79" t="s">
         <v>347</v>
-      </c>
-      <c r="B79" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>348</v>
+      </c>
+      <c r="B80" t="s">
         <v>349</v>
-      </c>
-      <c r="B80" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
+        <v>809</v>
+      </c>
+      <c r="B81" t="s">
         <v>810</v>
-      </c>
-      <c r="B81" t="s">
-        <v>811</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
+        <v>350</v>
+      </c>
+      <c r="B82" t="s">
         <v>351</v>
-      </c>
-      <c r="B82" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>352</v>
+      </c>
+      <c r="B84" t="s">
         <v>353</v>
-      </c>
-      <c r="B84" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
+        <v>354</v>
+      </c>
+      <c r="B85" t="s">
         <v>355</v>
-      </c>
-      <c r="B85" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>356</v>
+      </c>
+      <c r="B86" t="s">
         <v>357</v>
-      </c>
-      <c r="B86" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
+        <v>358</v>
+      </c>
+      <c r="B87" t="s">
         <v>359</v>
-      </c>
-      <c r="B87" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>360</v>
+      </c>
+      <c r="B88" t="s">
         <v>361</v>
-      </c>
-      <c r="B88" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
+        <v>362</v>
+      </c>
+      <c r="B89" t="s">
         <v>363</v>
-      </c>
-      <c r="B89" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
+        <v>364</v>
+      </c>
+      <c r="B91" t="s">
         <v>365</v>
-      </c>
-      <c r="B91" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>366</v>
+      </c>
+      <c r="B92" t="s">
         <v>367</v>
-      </c>
-      <c r="B92" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
+        <v>368</v>
+      </c>
+      <c r="B93" t="s">
         <v>369</v>
-      </c>
-      <c r="B93" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
+        <v>370</v>
+      </c>
+      <c r="B94" t="s">
         <v>371</v>
-      </c>
-      <c r="B94" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
+        <v>372</v>
+      </c>
+      <c r="B95" t="s">
         <v>373</v>
-      </c>
-      <c r="B95" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
+        <v>374</v>
+      </c>
+      <c r="B96" t="s">
         <v>375</v>
-      </c>
-      <c r="B96" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>376</v>
+      </c>
+      <c r="B97" t="s">
         <v>377</v>
-      </c>
-      <c r="B97" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
+        <v>378</v>
+      </c>
+      <c r="B99" t="s">
         <v>379</v>
-      </c>
-      <c r="B99" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="12" t="s">
+        <v>380</v>
+      </c>
+      <c r="B100" t="s">
         <v>381</v>
-      </c>
-      <c r="B100" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="12" t="s">
+        <v>382</v>
+      </c>
+      <c r="B101" t="s">
         <v>383</v>
-      </c>
-      <c r="B101" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="12" t="s">
+        <v>384</v>
+      </c>
+      <c r="B102" t="s">
         <v>385</v>
-      </c>
-      <c r="B102" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B103" t="s">
         <v>387</v>
-      </c>
-      <c r="B103" t="s">
-        <v>388</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="12" t="s">
+        <v>388</v>
+      </c>
+      <c r="B104" t="s">
         <v>389</v>
-      </c>
-      <c r="B104" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="12" t="s">
+        <v>390</v>
+      </c>
+      <c r="B105" t="s">
         <v>391</v>
-      </c>
-      <c r="B105" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="12" t="s">
+        <v>392</v>
+      </c>
+      <c r="B106" t="s">
         <v>393</v>
-      </c>
-      <c r="B106" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="12" t="s">
+        <v>394</v>
+      </c>
+      <c r="B107" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="B107" s="3" t="s">
+      <c r="C107" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="D107" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="D107" s="4" t="s">
+      <c r="E107" s="13" t="s">
         <v>398</v>
       </c>
-      <c r="E107" s="13" t="s">
+      <c r="F107" s="4" t="s">
         <v>399</v>
-      </c>
-      <c r="F107" s="4" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="C108" s="4" t="s">
         <v>402</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="D108" s="4" t="s">
         <v>403</v>
       </c>
-      <c r="D108" s="4" t="s">
+      <c r="E108" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="E108" s="4" t="s">
+      <c r="F108" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="F108" s="4" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="109" spans="1:6" ht="36" x14ac:dyDescent="0.2">
       <c r="A109" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="B109" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="C109" s="4" t="s">
         <v>408</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="D109" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="E109" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="E109" s="10" t="s">
+      <c r="F109" s="4" t="s">
         <v>411</v>
-      </c>
-      <c r="F109" s="4" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="B110" t="s">
         <v>413</v>
-      </c>
-      <c r="B110" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="B111" t="s">
         <v>415</v>
-      </c>
-      <c r="B111" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
+        <v>416</v>
+      </c>
+      <c r="B112" t="s">
         <v>417</v>
-      </c>
-      <c r="B112" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="12" t="s">
+        <v>418</v>
+      </c>
+      <c r="B114" t="s">
         <v>419</v>
-      </c>
-      <c r="B114" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="B115" t="s">
         <v>421</v>
-      </c>
-      <c r="B115" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="12" t="s">
+        <v>422</v>
+      </c>
+      <c r="B116" t="s">
         <v>423</v>
-      </c>
-      <c r="B116" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="B117" t="s">
         <v>425</v>
-      </c>
-      <c r="B117" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="12" t="s">
+        <v>426</v>
+      </c>
+      <c r="B118" t="s">
         <v>427</v>
-      </c>
-      <c r="B118" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="12" t="s">
+        <v>428</v>
+      </c>
+      <c r="B119" t="s">
         <v>429</v>
-      </c>
-      <c r="B119" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="B120" t="s">
         <v>431</v>
-      </c>
-      <c r="B120" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="12" t="s">
+        <v>432</v>
+      </c>
+      <c r="B121" t="s">
         <v>433</v>
-      </c>
-      <c r="B121" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="12" t="s">
+        <v>434</v>
+      </c>
+      <c r="B122" t="s">
         <v>435</v>
-      </c>
-      <c r="B122" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="12" t="s">
+        <v>436</v>
+      </c>
+      <c r="B123" t="s">
         <v>437</v>
-      </c>
-      <c r="B123" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="12" t="s">
+        <v>438</v>
+      </c>
+      <c r="B124" t="s">
         <v>439</v>
-      </c>
-      <c r="B124" t="s">
-        <v>440</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="B125" t="s">
         <v>441</v>
-      </c>
-      <c r="B125" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B126" t="s">
         <v>443</v>
-      </c>
-      <c r="B126" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="12" t="s">
+        <v>444</v>
+      </c>
+      <c r="B127" t="s">
         <v>445</v>
-      </c>
-      <c r="B127" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="12" t="s">
+        <v>446</v>
+      </c>
+      <c r="B128" t="s">
         <v>447</v>
-      </c>
-      <c r="B128" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="12" t="s">
+        <v>448</v>
+      </c>
+      <c r="B129" t="s">
         <v>449</v>
-      </c>
-      <c r="B129" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="12" t="s">
+        <v>450</v>
+      </c>
+      <c r="B130" t="s">
         <v>451</v>
-      </c>
-      <c r="B130" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="12" t="s">
+        <v>452</v>
+      </c>
+      <c r="B131" t="s">
         <v>453</v>
-      </c>
-      <c r="B131" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
+        <v>454</v>
+      </c>
+      <c r="B132" t="s">
         <v>455</v>
-      </c>
-      <c r="B132" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="12" t="s">
+        <v>796</v>
+      </c>
+      <c r="B134" s="13" t="s">
         <v>797</v>
-      </c>
-      <c r="B134" s="13" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
@@ -4741,47 +4741,47 @@
         <v>6</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="15" t="s">
+        <v>799</v>
+      </c>
+      <c r="B136" t="s">
         <v>800</v>
-      </c>
-      <c r="B136" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="15" t="s">
+        <v>801</v>
+      </c>
+      <c r="B137" t="s">
         <v>802</v>
-      </c>
-      <c r="B137" t="s">
-        <v>803</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="15" t="s">
+        <v>803</v>
+      </c>
+      <c r="B138" t="s">
         <v>804</v>
-      </c>
-      <c r="B138" t="s">
-        <v>805</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="16" t="s">
+        <v>805</v>
+      </c>
+      <c r="B139" t="s">
         <v>806</v>
-      </c>
-      <c r="B139" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
+        <v>807</v>
+      </c>
+      <c r="B140" t="s">
         <v>808</v>
-      </c>
-      <c r="B140" t="s">
-        <v>809</v>
       </c>
     </row>
   </sheetData>
@@ -4806,54 +4806,54 @@
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>458</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>460</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>461</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" t="s">
         <v>463</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>464</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>465</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>466</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>467</v>
-      </c>
-      <c r="L1" t="s">
-        <v>468</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>470</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>471</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -4868,10 +4868,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -4884,41 +4884,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>475</v>
+      </c>
+      <c r="C5" t="s">
         <v>476</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>476</v>
+      </c>
+      <c r="E5" t="s">
+        <v>476</v>
+      </c>
+      <c r="F5" t="s">
+        <v>476</v>
+      </c>
+      <c r="G5" t="s">
+        <v>476</v>
+      </c>
+      <c r="M5" t="s">
         <v>477</v>
-      </c>
-      <c r="D5" t="s">
-        <v>477</v>
-      </c>
-      <c r="E5" t="s">
-        <v>477</v>
-      </c>
-      <c r="F5" t="s">
-        <v>477</v>
-      </c>
-      <c r="G5" t="s">
-        <v>477</v>
-      </c>
-      <c r="M5" t="s">
-        <v>478</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -4927,27 +4927,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>478</v>
+      </c>
+      <c r="H7" t="s">
         <v>479</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>480</v>
       </c>
-      <c r="I7" t="s">
-        <v>481</v>
-      </c>
       <c r="J7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="K7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="L7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -4956,24 +4956,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>483</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>484</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -4982,24 +4982,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -5008,24 +5008,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5034,24 +5034,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
   </sheetData>
@@ -5078,13 +5078,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>493</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -5106,7 +5106,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -5152,530 +5152,530 @@
     </row>
     <row r="2" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>495</v>
+      </c>
+      <c r="B2" t="s">
         <v>496</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="4" t="s">
         <v>497</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>498</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>499</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="11" t="s">
         <v>500</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>501</v>
+      </c>
+      <c r="B3" t="s">
         <v>502</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>504</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>505</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>506</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B4" t="s">
         <v>508</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>510</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>512</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>513</v>
+      </c>
+      <c r="B5" t="s">
         <v>514</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="E5" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>518</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>519</v>
+      </c>
+      <c r="B6" t="s">
         <v>520</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="10" t="s">
         <v>522</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="E6" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>524</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>525</v>
+      </c>
+      <c r="B7" t="s">
         <v>526</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>530</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>531</v>
+      </c>
+      <c r="B8" t="s">
         <v>532</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>536</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>537</v>
+      </c>
+      <c r="B9" t="s">
         <v>538</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="E9" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>542</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>543</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>543</v>
+      </c>
+      <c r="B10" t="s">
         <v>544</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>546</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>547</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>548</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>549</v>
+      </c>
+      <c r="B11" t="s">
         <v>550</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="4" t="s">
         <v>551</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>555</v>
+      </c>
+      <c r="B12" t="s">
         <v>556</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>558</v>
-      </c>
       <c r="D12" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>511</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="F12" s="4" t="s">
         <v>512</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>558</v>
+      </c>
+      <c r="B13" t="s">
         <v>559</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>561</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>564</v>
+      </c>
+      <c r="B14" t="s">
         <v>565</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" s="4" t="s">
         <v>566</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>569</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>570</v>
+      </c>
+      <c r="B15" t="s">
         <v>571</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>575</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>576</v>
+      </c>
+      <c r="B16" t="s">
         <v>577</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>582</v>
+      </c>
+      <c r="B17" t="s">
         <v>583</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="4" t="s">
         <v>584</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>588</v>
+      </c>
+      <c r="B18" t="s">
         <v>589</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>593</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>594</v>
+      </c>
+      <c r="B19" t="s">
         <v>595</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="4" t="s">
         <v>596</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>600</v>
+      </c>
+      <c r="B20" t="s">
         <v>601</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="4" t="s">
         <v>602</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>606</v>
+      </c>
+      <c r="B21" t="s">
         <v>607</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="4" t="s">
         <v>608</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>609</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="E21" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>611</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>612</v>
+      </c>
+      <c r="B22" t="s">
         <v>613</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>618</v>
+      </c>
+      <c r="B23" t="s">
         <v>619</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>621</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>624</v>
+      </c>
+      <c r="B24" t="s">
         <v>625</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>627</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>628</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>630</v>
+      </c>
+      <c r="B25" t="s">
         <v>631</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>634</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>635</v>
-      </c>
       <c r="F25" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>635</v>
+      </c>
+      <c r="B26" t="s">
         <v>636</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>638</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
         <v>639</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>640</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>641</v>
+      </c>
+      <c r="B27" t="s">
         <v>642</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>646</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>647</v>
+      </c>
+      <c r="B28" t="s">
         <v>648</v>
-      </c>
-      <c r="B28" t="s">
-        <v>649</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -5684,10 +5684,10 @@
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>649</v>
+      </c>
+      <c r="B29" t="s">
         <v>650</v>
-      </c>
-      <c r="B29" t="s">
-        <v>651</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
@@ -5696,42 +5696,42 @@
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>651</v>
+      </c>
+      <c r="B30" t="s">
         <v>652</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="4" t="s">
         <v>653</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>654</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>655</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>656</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>657</v>
+      </c>
+      <c r="B31" t="s">
         <v>658</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="E31" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="F31" s="4" t="s">
         <v>662</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.2">
@@ -5742,70 +5742,70 @@
     </row>
     <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>663</v>
+      </c>
+      <c r="B33" t="s">
         <v>664</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>668</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>669</v>
+      </c>
+      <c r="B34" t="s">
         <v>670</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" s="4" t="s">
         <v>671</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>672</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>673</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>674</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>675</v>
+      </c>
+      <c r="B35" t="s">
         <v>676</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>679</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="F35" s="11" t="s">
         <v>680</v>
-      </c>
-      <c r="F35" s="11" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="170" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>681</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>682</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>683</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
@@ -5814,367 +5814,367 @@
     </row>
     <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>683</v>
+      </c>
+      <c r="B37" t="s">
         <v>684</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>686</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="E37" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="11" t="s">
         <v>688</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>689</v>
+      </c>
+      <c r="B38" t="s">
         <v>690</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>692</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="E38" s="4" t="s">
         <v>693</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>694</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>695</v>
+      </c>
+      <c r="B39" t="s">
         <v>696</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="D39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="E39" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>700</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>701</v>
+      </c>
+      <c r="B40" t="s">
         <v>702</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" s="4" t="s">
         <v>703</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>704</v>
       </c>
-      <c r="D40" s="4" t="s">
+      <c r="E40" s="4" t="s">
         <v>705</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>706</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
+        <v>707</v>
+      </c>
+      <c r="B41" t="s">
         <v>708</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" s="4" t="s">
         <v>709</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="E41" s="4" t="s">
+      <c r="F41" s="4" t="s">
         <v>712</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>713</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>713</v>
+      </c>
+      <c r="B42" t="s">
         <v>714</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" s="4" t="s">
         <v>715</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>716</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>718</v>
-      </c>
-      <c r="F42" s="4" t="s">
-        <v>719</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>719</v>
+      </c>
+      <c r="B43" t="s">
         <v>720</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" s="4" t="s">
         <v>721</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>722</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>723</v>
       </c>
-      <c r="E43" s="4" t="s">
-        <v>724</v>
-      </c>
       <c r="F43" s="4" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>724</v>
+      </c>
+      <c r="B44" t="s">
         <v>725</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" s="4" t="s">
         <v>726</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>727</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>728</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="4" t="s">
         <v>729</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
+        <v>730</v>
+      </c>
+      <c r="B45" t="s">
         <v>731</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" s="4" t="s">
         <v>732</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>733</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="E45" s="4" t="s">
         <v>734</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="F45" s="4" t="s">
         <v>735</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>736</v>
+      </c>
+      <c r="B46" t="s">
         <v>737</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" s="4" t="s">
         <v>738</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>739</v>
       </c>
-      <c r="D46" s="4" t="s">
+      <c r="E46" s="4" t="s">
         <v>740</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="F46" s="4" t="s">
         <v>741</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>742</v>
+      </c>
+      <c r="B47" t="s">
         <v>743</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" s="4" t="s">
         <v>744</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>745</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E47" s="4" t="s">
+      <c r="F47" s="4" t="s">
         <v>747</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
+        <v>748</v>
+      </c>
+      <c r="B48" t="s">
         <v>749</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" s="4" t="s">
         <v>750</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>751</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="E48" s="4" t="s">
         <v>752</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="F48" s="4" t="s">
         <v>753</v>
-      </c>
-      <c r="F48" s="4" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
+        <v>754</v>
+      </c>
+      <c r="B49" t="s">
         <v>755</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" s="4" t="s">
         <v>756</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>757</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="E49" s="4" t="s">
         <v>758</v>
       </c>
-      <c r="E49" s="4" t="s">
+      <c r="F49" s="4" t="s">
         <v>759</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>760</v>
+      </c>
+      <c r="B50" t="s">
         <v>761</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" s="4" t="s">
         <v>762</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>763</v>
       </c>
-      <c r="D50" s="4" t="s">
+      <c r="E50" s="4" t="s">
         <v>764</v>
       </c>
-      <c r="E50" s="4" t="s">
+      <c r="F50" s="4" t="s">
         <v>765</v>
-      </c>
-      <c r="F50" s="4" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
+        <v>766</v>
+      </c>
+      <c r="B51" t="s">
         <v>767</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="4" t="s">
         <v>768</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>769</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="F51" s="4" t="s">
         <v>770</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>656</v>
-      </c>
-      <c r="F51" s="4" t="s">
-        <v>771</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B52" t="s">
+        <v>658</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>660</v>
       </c>
-      <c r="D52" s="4" t="s">
+      <c r="E52" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="E52" s="4" t="s">
+      <c r="F52" s="4" t="s">
         <v>662</v>
-      </c>
-      <c r="F52" s="4" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>772</v>
+      </c>
+      <c r="B53" t="s">
         <v>773</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="4" t="s">
         <v>774</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>775</v>
       </c>
-      <c r="D53" s="4" t="s">
+      <c r="E53" s="4" t="s">
         <v>776</v>
       </c>
-      <c r="E53" s="4" t="s">
+      <c r="F53" s="4" t="s">
         <v>777</v>
-      </c>
-      <c r="F53" s="4" t="s">
-        <v>778</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
+        <v>778</v>
+      </c>
+      <c r="B54" t="s">
+        <v>743</v>
+      </c>
+      <c r="C54" s="4" t="s">
         <v>779</v>
       </c>
-      <c r="B54" t="s">
-        <v>744</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>780</v>
-      </c>
       <c r="D54" s="4" t="s">
+        <v>745</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>746</v>
       </c>
-      <c r="E54" s="4" t="s">
+      <c r="F54" s="4" t="s">
         <v>747</v>
-      </c>
-      <c r="F54" s="4" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>133</v>
@@ -6184,65 +6184,65 @@
       </c>
       <c r="D55" s="4"/>
       <c r="F55" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>783</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="4" t="s">
         <v>784</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>785</v>
       </c>
       <c r="D56" s="4"/>
       <c r="F56" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>787</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="4" t="s">
         <v>788</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>789</v>
       </c>
       <c r="D57" s="4"/>
       <c r="F57" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
+        <v>790</v>
+      </c>
+      <c r="B58" t="s">
         <v>791</v>
-      </c>
-      <c r="B58" t="s">
-        <v>792</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
+        <v>792</v>
+      </c>
+      <c r="B59" t="s">
         <v>793</v>
-      </c>
-      <c r="B59" t="s">
-        <v>794</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
+        <v>794</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>795</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>796</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>

</xml_diff>

<commit_message>
add translations for authorization columns
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="49180" windowHeight="27020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="890" uniqueCount="812">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="816">
   <si>
     <t>comments</t>
   </si>
@@ -2486,6 +2486,18 @@
   </si>
   <si>
     <t>No Authorizations</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>extra_field_entitlements</t>
+  </si>
+  <si>
+    <t>Extra Field Entitlements</t>
   </si>
 </sst>
 </file>
@@ -2608,7 +2620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2635,6 +2647,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3095,10 +3108,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G140"/>
+  <dimension ref="A1:G142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="B142" sqref="B142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -4782,6 +4795,22 @@
       </c>
       <c r="B140" t="s">
         <v>808</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A141" s="18" t="s">
+        <v>812</v>
+      </c>
+      <c r="B141" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A142" s="18" t="s">
+        <v>814</v>
+      </c>
+      <c r="B142" t="s">
+        <v>815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update translations. still need to remove duplicate translations tokens
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="816">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="860">
   <si>
     <t>comments</t>
   </si>
@@ -2499,12 +2499,144 @@
   <si>
     <t>Extra Field Entitlements</t>
   </si>
+  <si>
+    <t>Beneficiary Entity custom form not defined</t>
+  </si>
+  <si>
+    <t>be_custom_form_undefined</t>
+  </si>
+  <si>
+    <t>fill_field_report</t>
+  </si>
+  <si>
+    <t>Fill Field Report</t>
+  </si>
+  <si>
+    <t>terminate_authorization</t>
+  </si>
+  <si>
+    <t>Terminate Authorization</t>
+  </si>
+  <si>
+    <t>terminate_authorization_success</t>
+  </si>
+  <si>
+    <t>Authorization Successfully Terminated</t>
+  </si>
+  <si>
+    <t>terminate_authorization_failed</t>
+  </si>
+  <si>
+    <t>Authorization Termination Failed</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>delivered</t>
+  </si>
+  <si>
+    <t>Delivered</t>
+  </si>
+  <si>
+    <t>delivered_since_sync</t>
+  </si>
+  <si>
+    <t>Delivered since sync</t>
+  </si>
+  <si>
+    <t>deliver</t>
+  </si>
+  <si>
+    <t>Deliver</t>
+  </si>
+  <si>
+    <t>new_since_sync</t>
+  </si>
+  <si>
+    <t>New since last sync</t>
+  </si>
+  <si>
+    <t>edited_since_sync</t>
+  </si>
+  <si>
+    <t>Edited since last sync</t>
+  </si>
+  <si>
+    <t>new_hh_mem_since_sync</t>
+  </si>
+  <si>
+    <t>edited_hh_mem_since_sync</t>
+  </si>
+  <si>
+    <t>New households [members] since last sync</t>
+  </si>
+  <si>
+    <t>Edited households [members] since last sync</t>
+  </si>
+  <si>
+    <t>There currently are no active authorizations</t>
+  </si>
+  <si>
+    <t>no_active_authorizations</t>
+  </si>
+  <si>
+    <t>internal_error</t>
+  </si>
+  <si>
+    <t>Internal Error: please contact administrator</t>
+  </si>
+  <si>
+    <t>beneficiary_already_received</t>
+  </si>
+  <si>
+    <t>This beneficiary entity id has already received the current authorization</t>
+  </si>
+  <si>
+    <t>delivery_confirmed</t>
+  </si>
+  <si>
+    <t>Delivery Confirmed!</t>
+  </si>
+  <si>
+    <t>distribution_options</t>
+  </si>
+  <si>
+    <t>Distribution Options</t>
+  </si>
+  <si>
+    <t>create_authorization</t>
+  </si>
+  <si>
+    <t>create_authorization_success</t>
+  </si>
+  <si>
+    <t>create_authorization_failed</t>
+  </si>
+  <si>
+    <t>Create Authorization</t>
+  </si>
+  <si>
+    <t>Authorization Successfully Created</t>
+  </si>
+  <si>
+    <t>Authorization Creation Failed</t>
+  </si>
+  <si>
+    <t>start_new_authorization</t>
+  </si>
+  <si>
+    <t>Start New Authorization</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2529,6 +2661,22 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -2617,8 +2765,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2649,7 +2823,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="27">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3108,10 +3308,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:G164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="B142" sqref="B142"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -4811,6 +5011,214 @@
       </c>
       <c r="B142" t="s">
         <v>815</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A143" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="B143" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A144" s="18" t="s">
+        <v>818</v>
+      </c>
+      <c r="B144" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="18" t="s">
+        <v>820</v>
+      </c>
+      <c r="B145" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="18" t="s">
+        <v>822</v>
+      </c>
+      <c r="B146" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="18" t="s">
+        <v>824</v>
+      </c>
+      <c r="B147" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="18" t="s">
+        <v>852</v>
+      </c>
+      <c r="B148" t="s">
+        <v>855</v>
+      </c>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="13"/>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="18" t="s">
+        <v>853</v>
+      </c>
+      <c r="B149" t="s">
+        <v>856</v>
+      </c>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="13"/>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="18" t="s">
+        <v>854</v>
+      </c>
+      <c r="B150" t="s">
+        <v>857</v>
+      </c>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="13"/>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="18" t="s">
+        <v>858</v>
+      </c>
+      <c r="B151" t="s">
+        <v>859</v>
+      </c>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="13"/>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="18" t="s">
+        <v>826</v>
+      </c>
+      <c r="B152" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="18" t="s">
+        <v>828</v>
+      </c>
+      <c r="B153" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="18" t="s">
+        <v>830</v>
+      </c>
+      <c r="B154" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B155" t="s">
+        <v>835</v>
+      </c>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="13"/>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B156" t="s">
+        <v>837</v>
+      </c>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="13"/>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="18" t="s">
+        <v>838</v>
+      </c>
+      <c r="B157" t="s">
+        <v>840</v>
+      </c>
+      <c r="C157" s="13"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="13"/>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="18" t="s">
+        <v>839</v>
+      </c>
+      <c r="B158" t="s">
+        <v>841</v>
+      </c>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="13"/>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="18" t="s">
+        <v>832</v>
+      </c>
+      <c r="B159" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="18" t="s">
+        <v>843</v>
+      </c>
+      <c r="B160" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A161" s="18" t="s">
+        <v>844</v>
+      </c>
+      <c r="B161" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A162" s="18" t="s">
+        <v>846</v>
+      </c>
+      <c r="B162" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A163" s="18" t="s">
+        <v>848</v>
+      </c>
+      <c r="B163" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A164" s="18" t="s">
+        <v>850</v>
+      </c>
+      <c r="B164" t="s">
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
migrate alerts to bootstrap/bootbox. fix missing locale parameters in two places
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="30240" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="framework_translations" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$103</definedName>
   </definedNames>
   <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="736">
   <si>
     <t>comments</t>
   </si>
@@ -2255,6 +2255,9 @@
   </si>
   <si>
     <t>Confirm Delivery</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -2939,10 +2942,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G159"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -3624,42 +3627,42 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>735</v>
+      </c>
+      <c r="B46" t="s">
+        <v>576</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>112</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>113</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C47" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D47" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="E46" s="12" t="s">
+      <c r="E47" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="F46" s="12" t="s">
+      <c r="F47" s="12" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>674</v>
-      </c>
-      <c r="B47" t="s">
-        <v>675</v>
-      </c>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="B48" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
@@ -3667,11 +3670,11 @@
       <c r="F48" s="12"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>202</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>203</v>
+      <c r="A49" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="B49" t="s">
+        <v>689</v>
       </c>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
@@ -3680,10 +3683,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
@@ -3692,10 +3695,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
@@ -3704,10 +3707,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>212</v>
-      </c>
-      <c r="B52" t="s">
-        <v>213</v>
+        <v>208</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>209</v>
       </c>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -3716,10 +3719,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>665</v>
+        <v>212</v>
       </c>
       <c r="B53" t="s">
-        <v>666</v>
+        <v>213</v>
       </c>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -3728,10 +3731,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>665</v>
       </c>
       <c r="B54" t="s">
-        <v>217</v>
+        <v>666</v>
       </c>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -3740,10 +3743,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>204</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>205</v>
+        <v>216</v>
+      </c>
+      <c r="B55" t="s">
+        <v>217</v>
       </c>
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
@@ -3752,10 +3755,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>730</v>
+        <v>204</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>729</v>
+        <v>205</v>
       </c>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
@@ -3764,10 +3767,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="12"/>
@@ -3776,10 +3779,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="12"/>
@@ -3787,14 +3790,18 @@
       <c r="F58" s="12"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B59" s="3"/>
+      <c r="A59" t="s">
+        <v>733</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>734</v>
+      </c>
       <c r="C59" s="12"/>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="12"/>
       <c r="D60" s="12"/>
@@ -3802,31 +3809,32 @@
       <c r="F60" s="12"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>716</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>717</v>
-      </c>
-      <c r="C61" s="9"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="12"/>
-      <c r="F61" s="10"/>
+      <c r="F61" s="12"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>704</v>
-      </c>
-      <c r="B62" t="s">
-        <v>705</v>
-      </c>
-      <c r="C62" s="12"/>
+      <c r="A62" t="s">
+        <v>716</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="C62" s="9"/>
       <c r="D62" s="12"/>
       <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
+      <c r="F62" s="10"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
+      <c r="A63" s="17" t="s">
+        <v>704</v>
+      </c>
+      <c r="B63" t="s">
+        <v>705</v>
+      </c>
       <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -3840,12 +3848,7 @@
       <c r="F64" s="12"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>719</v>
-      </c>
-      <c r="B65" t="s">
-        <v>720</v>
-      </c>
+      <c r="A65" s="17"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
@@ -3853,10 +3856,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>74</v>
+        <v>719</v>
       </c>
       <c r="B66" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="12"/>
@@ -3865,10 +3868,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>722</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
@@ -3876,89 +3879,89 @@
       <c r="F67" s="12"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>722</v>
+      </c>
+      <c r="B68" t="s">
+        <v>723</v>
+      </c>
       <c r="C68" s="12"/>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
       <c r="F68" s="12"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
       <c r="C69" s="12"/>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
       <c r="F69" s="12"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" t="s">
-        <v>173</v>
-      </c>
-      <c r="B70" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="F70" s="12" t="s">
-        <v>178</v>
-      </c>
+      <c r="A70" s="3"/>
+      <c r="B70" s="3"/>
+      <c r="C70" s="12"/>
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="D71" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>73</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>724</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-    </row>
-    <row r="72" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+    </row>
+    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>75</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>76</v>
       </c>
-      <c r="C72" s="9" t="s">
+      <c r="C73" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D72" s="12" t="s">
+      <c r="D73" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E72" s="12" t="s">
+      <c r="E73" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F72" s="10" t="s">
+      <c r="F73" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>673</v>
-      </c>
-      <c r="B73" t="s">
-        <v>672</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="17" t="s">
-        <v>702</v>
+        <v>673</v>
       </c>
       <c r="B74" t="s">
-        <v>703</v>
+        <v>672</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
@@ -3967,10 +3970,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="17" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="B75" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="12"/>
@@ -3978,58 +3981,58 @@
       <c r="F75" s="12"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
+      <c r="A76" s="17" t="s">
+        <v>700</v>
+      </c>
+      <c r="B76" t="s">
+        <v>701</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>67</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="12" t="s">
+      <c r="C77" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D76" s="12" t="s">
+      <c r="D77" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E76" s="12" t="s">
+      <c r="E77" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="F76" s="12" t="s">
+      <c r="F77" s="12" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>667</v>
       </c>
-      <c r="C77" s="12" t="s">
+      <c r="C78" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="12" t="s">
+      <c r="D78" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="E77" s="12" t="s">
+      <c r="E78" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="F77" s="10" t="s">
+      <c r="F78" s="10" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C78" s="12"/>
-      <c r="D78" s="12"/>
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-    </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
@@ -4037,10 +4040,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C80" s="12"/>
       <c r="D80" s="12"/>
@@ -4049,49 +4052,55 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="B81" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="D81" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="E81" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="F81" s="12" t="s">
-        <v>101</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C81" s="12"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="12"/>
+      <c r="F81" s="12"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B82" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="D82" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E82" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>102</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C83" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D82" s="12" t="s">
+      <c r="D83" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E82" s="12" t="s">
+      <c r="E83" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F82" s="12" t="s">
+      <c r="F83" s="12" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C84" s="12"/>
@@ -4100,12 +4109,6 @@
       <c r="F84" s="12"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
-        <v>686</v>
-      </c>
-      <c r="B85" t="s">
-        <v>687</v>
-      </c>
       <c r="C85" s="12"/>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
@@ -4113,10 +4116,10 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="B86" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="12"/>
@@ -4125,10 +4128,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="17" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B87" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="12"/>
@@ -4137,10 +4140,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="17" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B88" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="12"/>
@@ -4149,10 +4152,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="17" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B89" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C89" s="12"/>
       <c r="D89" s="12"/>
@@ -4160,6 +4163,12 @@
       <c r="F89" s="12"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
+        <v>695</v>
+      </c>
+      <c r="B90" t="s">
+        <v>697</v>
+      </c>
       <c r="C90" s="12"/>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
@@ -4172,12 +4181,6 @@
       <c r="F91" s="12"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
-        <v>714</v>
-      </c>
-      <c r="B92" t="s">
-        <v>715</v>
-      </c>
       <c r="C92" s="12"/>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
@@ -4185,10 +4188,10 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="17" t="s">
-        <v>708</v>
+        <v>714</v>
       </c>
       <c r="B93" t="s">
-        <v>711</v>
+        <v>715</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="12"/>
@@ -4196,11 +4199,11 @@
       <c r="F93" s="12"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>214</v>
+      <c r="A94" s="17" t="s">
+        <v>708</v>
       </c>
       <c r="B94" t="s">
-        <v>215</v>
+        <v>711</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="12"/>
@@ -4208,11 +4211,11 @@
       <c r="F94" s="12"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
-        <v>709</v>
+      <c r="A95" t="s">
+        <v>214</v>
       </c>
       <c r="B95" t="s">
-        <v>712</v>
+        <v>215</v>
       </c>
       <c r="C95" s="12"/>
       <c r="D95" s="12"/>
@@ -4221,10 +4224,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="17" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B96" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="C96" s="12"/>
       <c r="D96" s="12"/>
@@ -4233,10 +4236,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>676</v>
+        <v>710</v>
       </c>
       <c r="B97" t="s">
-        <v>677</v>
+        <v>713</v>
       </c>
       <c r="C97" s="12"/>
       <c r="D97" s="12"/>
@@ -4245,10 +4248,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="17" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B98" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="C98" s="12"/>
       <c r="D98" s="12"/>
@@ -4257,10 +4260,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="17" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="B99" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C99" s="12"/>
       <c r="D99" s="12"/>
@@ -4269,10 +4272,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="17" t="s">
-        <v>699</v>
+        <v>680</v>
       </c>
       <c r="B100" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
       <c r="C100" s="12"/>
       <c r="D100" s="12"/>
@@ -4280,79 +4283,79 @@
       <c r="F100" s="12"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="17"/>
+      <c r="A101" s="17" t="s">
+        <v>699</v>
+      </c>
+      <c r="B101" t="s">
+        <v>698</v>
+      </c>
       <c r="C101" s="12"/>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
       <c r="F101" s="12"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="17"/>
       <c r="C102" s="12"/>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
       <c r="F102" s="12"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>218</v>
-      </c>
-      <c r="B103" t="s">
-        <v>219</v>
-      </c>
+      <c r="C103" s="12"/>
+      <c r="D103" s="12"/>
+      <c r="E103" s="12"/>
+      <c r="F103" s="12"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B104" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B105" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B106" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B107" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>228</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B109" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C109" s="12"/>
-      <c r="D109" s="12"/>
-      <c r="E109" s="12"/>
-      <c r="F109" s="12"/>
-    </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="11" t="s">
-        <v>280</v>
-      </c>
-      <c r="B110" t="s">
-        <v>281</v>
-      </c>
       <c r="C110" s="12"/>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -4360,10 +4363,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B111" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C111" s="12"/>
       <c r="D111" s="12"/>
@@ -4372,10 +4375,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B112" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C112" s="12"/>
       <c r="D112" s="12"/>
@@ -4384,226 +4387,231 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>250</v>
+        <v>284</v>
       </c>
       <c r="B113" t="s">
-        <v>251</v>
+        <v>285</v>
       </c>
       <c r="C113" s="12"/>
       <c r="D113" s="12"/>
       <c r="E113" s="12"/>
       <c r="F113" s="12"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B115" t="s">
-        <v>243</v>
-      </c>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="B114" t="s">
+        <v>251</v>
+      </c>
+      <c r="C114" s="12"/>
+      <c r="D114" s="12"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B116" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B117" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B119" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B120" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>256</v>
-      </c>
-      <c r="B121" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="C121" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="D121" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="E121" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="F121" s="4" t="s">
-        <v>261</v>
+        <v>254</v>
+      </c>
+      <c r="B121" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
+        <v>256</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="E122" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B123" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C123" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="D122" s="4" t="s">
+      <c r="D123" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E122" s="4" t="s">
+      <c r="E123" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="F122" s="4" t="s">
+      <c r="F123" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="36" x14ac:dyDescent="0.2">
-      <c r="A123" s="11" t="s">
+    <row r="124" spans="1:6" ht="36" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
         <v>268</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B124" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="D123" s="4" t="s">
+      <c r="D124" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="E123" s="9" t="s">
+      <c r="E124" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="F123" s="4" t="s">
+      <c r="F124" s="4" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="11" t="s">
-        <v>274</v>
-      </c>
-      <c r="B124" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
+        <v>274</v>
+      </c>
+      <c r="B125" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>278</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="11" t="s">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
         <v>652</v>
       </c>
-      <c r="B128" s="12" t="s">
+      <c r="B129" s="12" t="s">
         <v>653</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B129" s="12" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
-        <v>655</v>
-      </c>
-      <c r="B130" t="s">
-        <v>656</v>
+        <v>6</v>
+      </c>
+      <c r="B130" s="12" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="14" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B131" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="14" t="s">
+        <v>657</v>
+      </c>
+      <c r="B132" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="14" t="s">
         <v>659</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B133" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="15" t="s">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="15" t="s">
         <v>661</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B134" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134" s="16" t="s">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="16" t="s">
         <v>663</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>664</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="17" t="s">
-        <v>668</v>
-      </c>
-      <c r="B135" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136" s="17" t="s">
+        <v>668</v>
+      </c>
+      <c r="B136" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="17" t="s">
         <v>670</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B137" t="s">
         <v>671</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" s="17"/>
-      <c r="C137" s="12"/>
-      <c r="D137" s="12"/>
-      <c r="E137" s="12"/>
-      <c r="F137" s="12"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="17"/>
@@ -4613,12 +4621,7 @@
       <c r="F138" s="12"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>230</v>
-      </c>
-      <c r="B139" t="s">
-        <v>231</v>
-      </c>
+      <c r="A139" s="17"/>
       <c r="C139" s="12"/>
       <c r="D139" s="12"/>
       <c r="E139" s="12"/>
@@ -4626,10 +4629,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B140" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C140" s="12"/>
       <c r="D140" s="12"/>
@@ -4638,10 +4641,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B141" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C141" s="12"/>
       <c r="D141" s="12"/>
@@ -4650,10 +4653,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B142" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C142" s="12"/>
       <c r="D142" s="12"/>
@@ -4662,10 +4665,10 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B143" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C143" s="12"/>
       <c r="D143" s="12"/>
@@ -4674,10 +4677,10 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B144" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C144" s="12"/>
       <c r="D144" s="12"/>
@@ -4685,11 +4688,11 @@
       <c r="F144" s="12"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="13" t="s">
-        <v>310</v>
+      <c r="A145" t="s">
+        <v>240</v>
       </c>
       <c r="B145" t="s">
-        <v>311</v>
+        <v>241</v>
       </c>
       <c r="C145" s="12"/>
       <c r="D145" s="12"/>
@@ -4697,19 +4700,19 @@
       <c r="F145" s="12"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="13"/>
+      <c r="A146" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="B146" t="s">
+        <v>311</v>
+      </c>
       <c r="C146" s="12"/>
       <c r="D146" s="12"/>
       <c r="E146" s="12"/>
       <c r="F146" s="12"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="11" t="s">
-        <v>286</v>
-      </c>
-      <c r="B147" t="s">
-        <v>287</v>
-      </c>
+      <c r="A147" s="13"/>
       <c r="C147" s="12"/>
       <c r="D147" s="12"/>
       <c r="E147" s="12"/>
@@ -4717,10 +4720,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B148" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C148" s="12"/>
       <c r="D148" s="12"/>
@@ -4729,10 +4732,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B149" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C149" s="12"/>
       <c r="D149" s="12"/>
@@ -4741,10 +4744,10 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B150" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C150" s="12"/>
       <c r="D150" s="12"/>
@@ -4753,10 +4756,10 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B151" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C151" s="12"/>
       <c r="D151" s="12"/>
@@ -4765,10 +4768,10 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B152" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C152" s="12"/>
       <c r="D152" s="12"/>
@@ -4777,10 +4780,10 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B153" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C153" s="12"/>
       <c r="D153" s="12"/>
@@ -4789,10 +4792,10 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B154" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C154" s="12"/>
       <c r="D154" s="12"/>
@@ -4801,10 +4804,10 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="11" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C155" s="12"/>
       <c r="D155" s="12"/>
@@ -4813,10 +4816,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C156" s="12"/>
       <c r="D156" s="12"/>
@@ -4825,10 +4828,10 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="11" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B157" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C157" s="12"/>
       <c r="D157" s="12"/>
@@ -4837,18 +4840,30 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B158" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C158" s="12"/>
       <c r="D158" s="12"/>
       <c r="E158" s="12"/>
       <c r="F158" s="12"/>
     </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="B159" t="s">
+        <v>309</v>
+      </c>
+      <c r="C159" s="12"/>
+      <c r="D159" s="12"/>
+      <c r="E159" s="12"/>
+      <c r="F159" s="12"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F102"/>
+  <autoFilter ref="A1:F103"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>

<commit_message>
Add in missing translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\app-designer\app\config\assets\framework\forms\framework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16300" yWindow="5020" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="16305" yWindow="5025" windowWidth="25605" windowHeight="16065" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
     <sheet name="framework_translations" sheetId="5" r:id="rId5"/>
     <sheet name="common_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="972" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="631">
   <si>
     <t>comments</t>
   </si>
@@ -1953,12 +1958,49 @@
     <t xml:space="preserve">
 ¿Seguro que quieres borrar la fila</t>
   </si>
+  <si>
+    <t>confirm_exit_label</t>
+  </si>
+  <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>confirm_cancel_label</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>confirm_message</t>
+  </si>
+  <si>
+    <t>Are you sure you want to exit and lose all changes?</t>
+  </si>
+  <si>
+    <t>Editar</t>
+  </si>
+  <si>
+    <t>Suprimir</t>
+  </si>
+  <si>
+    <t>Cancelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+¿Estás seguro de que quieres salir y perder todos los cambios?</t>
+  </si>
+  <si>
+    <t>¿Estás seguro de que quieres eliminar la fila?</t>
+  </si>
+  <si>
+    <t>Salida</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1991,6 +2033,18 @@
       <color theme="11"/>
       <name val="Arial"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2039,7 +2093,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2054,6 +2108,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2086,6 +2157,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2417,14 +2496,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.83203125" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2432,7 +2511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2456,20 +2535,20 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="101.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.83203125" customWidth="1"/>
-    <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="22.1640625" customWidth="1"/>
-    <col min="10" max="1025" width="17.1640625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="1025" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1">
+    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2496,7 +2575,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>10</v>
       </c>
@@ -2505,85 +2584,85 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.5" customHeight="1"/>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1"/>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1"/>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1"/>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1"/>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1"/>
-    <row r="17" ht="17.5" customHeight="1"/>
-    <row r="18" ht="59.25" customHeight="1"/>
-    <row r="19" ht="17.25" customHeight="1"/>
-    <row r="20" ht="17.5" customHeight="1"/>
-    <row r="21" ht="66" customHeight="1"/>
-    <row r="22" ht="17.25" customHeight="1"/>
-    <row r="23" ht="17.5" customHeight="1"/>
-    <row r="24" ht="66" customHeight="1"/>
-    <row r="25" ht="17.25" customHeight="1"/>
-    <row r="26" ht="17.5" customHeight="1"/>
-    <row r="27" ht="66" customHeight="1"/>
-    <row r="28" ht="17.25" customHeight="1"/>
-    <row r="29" ht="17.5" customHeight="1"/>
-    <row r="30" ht="66" customHeight="1"/>
-    <row r="31" ht="17.25" customHeight="1"/>
-    <row r="32" ht="17.5" customHeight="1"/>
-    <row r="33" ht="66" customHeight="1"/>
-    <row r="34" ht="17.25" customHeight="1"/>
-    <row r="35" ht="17.5" customHeight="1"/>
-    <row r="36" ht="66" customHeight="1"/>
-    <row r="37" ht="17.25" customHeight="1"/>
-    <row r="38" ht="17.5" customHeight="1"/>
-    <row r="39" ht="66" customHeight="1"/>
-    <row r="40" ht="17.25" customHeight="1"/>
-    <row r="41" ht="17.5" customHeight="1"/>
-    <row r="42" ht="66" customHeight="1"/>
-    <row r="43" ht="17.25" customHeight="1"/>
-    <row r="44" ht="17.5" customHeight="1"/>
-    <row r="45" ht="66" customHeight="1"/>
-    <row r="46" ht="17.25" customHeight="1"/>
-    <row r="47" ht="17.5" customHeight="1"/>
-    <row r="48" ht="66" customHeight="1"/>
-    <row r="49" ht="17.25" customHeight="1"/>
-    <row r="50" ht="17.5" customHeight="1"/>
-    <row r="51" ht="66" customHeight="1"/>
-    <row r="52" ht="17.25" customHeight="1"/>
-    <row r="53" ht="17.5" customHeight="1"/>
-    <row r="54" ht="66" customHeight="1"/>
-    <row r="55" ht="17.25" customHeight="1"/>
-    <row r="56" ht="17.5" customHeight="1"/>
-    <row r="57" ht="66" customHeight="1"/>
-    <row r="58" ht="17.25" customHeight="1"/>
-    <row r="59" ht="17.5" customHeight="1"/>
-    <row r="60" ht="66" customHeight="1"/>
-    <row r="61" ht="17.25" customHeight="1"/>
-    <row r="62" ht="17.5" customHeight="1"/>
-    <row r="63" ht="66" customHeight="1"/>
-    <row r="64" ht="17.25" customHeight="1"/>
-    <row r="65" ht="17.5" customHeight="1"/>
-    <row r="66" ht="66" customHeight="1"/>
-    <row r="67" ht="17.25" customHeight="1"/>
-    <row r="68" ht="17.5" customHeight="1"/>
-    <row r="69" ht="66" customHeight="1"/>
-    <row r="70" ht="17.25" customHeight="1"/>
-    <row r="71" ht="17.5" customHeight="1"/>
-    <row r="72" ht="66" customHeight="1"/>
-    <row r="73" ht="17" customHeight="1"/>
-    <row r="75" ht="62" customHeight="1"/>
-    <row r="78" ht="62" customHeight="1"/>
-    <row r="80" ht="12" customHeight="1"/>
-    <row r="81" ht="58" customHeight="1"/>
-    <row r="83" ht="12" customHeight="1"/>
-    <row r="84" ht="58" customHeight="1"/>
-    <row r="86" ht="12" customHeight="1"/>
-    <row r="87" ht="58" customHeight="1"/>
+    <row r="3" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2603,15 +2682,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="6" width="24.6640625" customWidth="1"/>
-    <col min="7" max="7" width="41.1640625" customWidth="1"/>
-    <col min="8" max="1025" width="17.1640625" customWidth="1"/>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="6" width="24.7109375" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="8" max="1025" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2637,7 +2716,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2649,7 +2728,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2664,7 +2743,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2675,7 +2754,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" customHeight="1">
+    <row r="5" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2693,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2704,7 +2783,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2715,7 +2794,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2725,9 +2804,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1"/>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1"/>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1"/>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2747,15 +2826,15 @@
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.83203125" customWidth="1"/>
+    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2779,21 +2858,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C173"/>
+  <dimension ref="A1:C179"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD173"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.6640625" customWidth="1"/>
-    <col min="2" max="2" width="52.1640625" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="1025" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="49.7109375" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="1025" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1">
+    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2804,7 +2883,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1">
+    <row r="2" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2815,7 +2894,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" customHeight="1">
+    <row r="3" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2826,7 +2905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" customHeight="1">
+    <row r="4" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2837,7 +2916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13" customHeight="1">
+    <row r="5" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2848,7 +2927,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13" customHeight="1">
+    <row r="6" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2859,7 +2938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2870,7 +2949,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2881,7 +2960,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -2892,7 +2971,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -2903,7 +2982,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1">
+    <row r="11" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -2914,7 +2993,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1">
+    <row r="12" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -2925,7 +3004,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -2936,7 +3015,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -2947,7 +3026,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -2958,7 +3037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -2969,7 +3048,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -2980,7 +3059,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -2991,7 +3070,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -3002,7 +3081,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -3013,7 +3092,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -3024,7 +3103,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -3035,7 +3114,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3046,7 +3125,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -3057,7 +3136,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3068,7 +3147,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3079,7 +3158,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -3090,7 +3169,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.25" customHeight="1">
+    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3101,7 +3180,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3112,7 +3191,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -3123,7 +3202,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3134,7 +3213,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -3145,7 +3224,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -3156,7 +3235,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3167,7 +3246,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="216">
+    <row r="36" spans="1:3" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3178,7 +3257,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -3189,7 +3268,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -3200,7 +3279,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -3211,7 +3290,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -3222,7 +3301,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3233,7 +3312,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>156</v>
       </c>
@@ -3244,7 +3323,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -3255,7 +3334,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -3266,7 +3345,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -3277,7 +3356,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3288,7 +3367,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -3299,7 +3378,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -3310,7 +3389,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -3321,7 +3400,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13" customHeight="1">
+    <row r="50" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3332,7 +3411,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -3343,7 +3422,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -3354,7 +3433,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -3365,7 +3444,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>189</v>
       </c>
@@ -3376,7 +3455,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -3387,7 +3466,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -3398,7 +3477,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -3409,1285 +3488,1351 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="36">
-      <c r="A58" t="s">
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>620</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>622</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>617</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="8" t="s">
+        <v>556</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>559</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>199</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B64" t="s">
         <v>200</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C64" s="11" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
-      <c r="A59" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>201</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B65" t="s">
         <v>202</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C65" s="12" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
-      <c r="A60" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>204</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B66" t="s">
         <v>205</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C66" s="12" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>207</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B67" t="s">
         <v>208</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C67" s="5" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>212</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B68" t="s">
         <v>211</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C68" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>213</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B69" t="s">
         <v>214</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C69" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>216</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B70" t="s">
         <v>217</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C70" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
-      <c r="A65" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>219</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B71" t="s">
         <v>220</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C71" s="5" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="36">
-      <c r="A66" t="s">
+    <row r="72" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>223</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B72" t="s">
         <v>221</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C72" s="4" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>224</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B73" t="s">
         <v>225</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C73" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
-      <c r="A68" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>227</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B74" t="s">
         <v>228</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C74" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="36">
-      <c r="A69" t="s">
+    <row r="75" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>230</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B75" t="s">
         <v>231</v>
       </c>
-      <c r="C69" s="4" t="s">
+      <c r="C75" s="4" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>233</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B76" t="s">
         <v>234</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C76" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
-      <c r="A71" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>236</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B77" t="s">
         <v>237</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C77" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="24">
-      <c r="A72" t="s">
+    <row r="78" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>239</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B78" t="s">
         <v>240</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>242</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B79" t="s">
         <v>244</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C79" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>245</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B80" t="s">
         <v>246</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C80" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>248</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B81" t="s">
         <v>249</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C81" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>251</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B82" t="s">
         <v>252</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C82" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="36">
-      <c r="A77" t="s">
+    <row r="83" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>254</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B83" t="s">
         <v>255</v>
       </c>
-      <c r="C77" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>257</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B84" t="s">
         <v>258</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C84" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
-      <c r="A79" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
         <v>260</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B85" t="s">
         <v>261</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C85" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
-      <c r="A80" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
         <v>263</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B86" t="s">
         <v>264</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C86" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
         <v>265</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B87" t="s">
         <v>266</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C87" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="36">
-      <c r="A82" t="s">
+    <row r="88" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
         <v>267</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B88" t="s">
         <v>268</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C88" s="4" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="24">
-      <c r="A83" t="s">
+    <row r="89" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
         <v>271</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B89" t="s">
         <v>272</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C89" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="24">
-      <c r="A84" t="s">
+    <row r="90" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
         <v>274</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B90" t="s">
         <v>275</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="48">
-      <c r="A85" t="s">
+    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
         <v>277</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B91" t="s">
         <v>278</v>
       </c>
-      <c r="C85" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="86" spans="1:3" ht="36">
-      <c r="A86" t="s">
+    <row r="92" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
         <v>280</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B92" t="s">
         <v>281</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C92" s="4" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="36">
-      <c r="A87" t="s">
+    <row r="93" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
         <v>283</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B93" t="s">
         <v>284</v>
       </c>
-      <c r="C87" s="4" t="s">
+      <c r="C93" s="4" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
         <v>286</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B94" t="s">
         <v>287</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C94" s="4" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
-      <c r="A89" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
         <v>289</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B95" t="s">
         <v>290</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C95" s="4" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
-      <c r="A90" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
         <v>291</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B96" t="s">
         <v>292</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C96" s="4" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
-      <c r="A91" t="s">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
         <v>294</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B97" t="s">
         <v>295</v>
       </c>
-      <c r="C91" s="4" t="s">
+      <c r="C97" s="4" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
         <v>296</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B98" t="s">
         <v>297</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C98" s="4" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="36">
-      <c r="A93" t="s">
+    <row r="99" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
         <v>299</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B99" t="s">
         <v>300</v>
       </c>
-      <c r="C93" s="4" t="s">
+      <c r="C99" s="4" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="24">
-      <c r="A94" t="s">
+    <row r="100" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>304</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B100" t="s">
         <v>305</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C100" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="36">
-      <c r="A95" t="s">
+    <row r="101" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
         <v>307</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B101" t="s">
         <v>308</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C101" s="4" t="s">
         <v>309</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
-      <c r="A96" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
         <v>310</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B102" t="s">
         <v>311</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C102" s="4" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24">
-      <c r="A97" t="s">
+    <row r="103" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
         <v>313</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B103" t="s">
         <v>314</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C103" s="4" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="36">
-      <c r="A98" t="s">
+    <row r="104" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
         <v>316</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B104" t="s">
         <v>317</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C104" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="48">
-      <c r="A99" t="s">
+    <row r="105" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
         <v>319</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B105" t="s">
         <v>320</v>
       </c>
-      <c r="C99" s="4" t="s">
+      <c r="C105" s="4" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="24">
-      <c r="A100" t="s">
+    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
         <v>322</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B106" t="s">
         <v>324</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C106" s="4" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="36">
-      <c r="A101" t="s">
+    <row r="107" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
         <v>325</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B107" t="s">
         <v>326</v>
       </c>
-      <c r="C101" s="4" t="s">
+      <c r="C107" s="4" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="24">
-      <c r="A102" t="s">
+    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>328</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B108" t="s">
         <v>329</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C108" s="4" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="36">
-      <c r="A103" t="s">
+    <row r="109" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>331</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B109" t="s">
         <v>332</v>
       </c>
-      <c r="C103" s="4" t="s">
+      <c r="C109" s="4" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="36">
-      <c r="A104" t="s">
+    <row r="110" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>334</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B110" t="s">
         <v>335</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C110" s="4" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="36">
-      <c r="A105" t="s">
+    <row r="111" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>337</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B111" t="s">
         <v>338</v>
       </c>
-      <c r="C105" s="4" t="s">
+      <c r="C111" s="4" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="36">
-      <c r="A106" t="s">
+    <row r="112" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>340</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B112" t="s">
         <v>341</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C112" s="4" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>343</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B113" t="s">
         <v>344</v>
       </c>
-      <c r="C107" s="4" t="s">
+      <c r="C113" s="4" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>346</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B114" t="s">
         <v>347</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C114" s="4" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>349</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B115" t="s">
         <v>350</v>
       </c>
-      <c r="C109" s="4" t="s">
+      <c r="C115" s="4" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>352</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B116" t="s">
         <v>353</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C116" s="4" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="24">
-      <c r="A111" t="s">
+    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>355</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B117" t="s">
         <v>356</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="C117" s="4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="24">
-      <c r="A112" t="s">
+    <row r="118" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>358</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B118" t="s">
         <v>359</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="C118" s="4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="36">
-      <c r="A113" t="s">
+    <row r="119" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>361</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B119" t="s">
         <v>362</v>
       </c>
-      <c r="C113" s="4" t="s">
+      <c r="C119" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>364</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B120" t="s">
         <v>368</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C120" s="4" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>366</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B121" t="s">
         <v>367</v>
       </c>
-      <c r="C115" s="4" t="s">
+      <c r="C121" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="24">
-      <c r="A116" t="s">
+    <row r="122" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>370</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B122" t="s">
         <v>371</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C122" s="4" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="36">
-      <c r="A117" t="s">
+    <row r="123" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>373</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B123" t="s">
         <v>374</v>
       </c>
-      <c r="C117" s="4" t="s">
+      <c r="C123" s="4" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="24">
-      <c r="A118" t="s">
+    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>375</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B124" t="s">
         <v>376</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C124" s="4" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="24">
-      <c r="A119" t="s">
+    <row r="125" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>379</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B125" t="s">
         <v>380</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="C125" s="4" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
         <v>382</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B126" t="s">
         <v>383</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C126" s="4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
         <v>385</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B127" t="s">
         <v>386</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C127" s="4" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
         <v>388</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B128" t="s">
         <v>389</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C128" s="4" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="24">
-      <c r="A123" t="s">
+    <row r="129" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
         <v>391</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B129" t="s">
         <v>392</v>
       </c>
-      <c r="C123" s="4" t="s">
+      <c r="C129" s="4" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="36">
-      <c r="A124" t="s">
+    <row r="130" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
         <v>394</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B130" t="s">
         <v>395</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C130" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="48">
-      <c r="A125" t="s">
+    <row r="131" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>397</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B131" t="s">
         <v>398</v>
       </c>
-      <c r="C125" s="4" t="s">
+      <c r="C131" s="4" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="36">
-      <c r="A126" t="s">
+    <row r="132" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
         <v>400</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B132" t="s">
         <v>401</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C132" s="4" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24">
-      <c r="A127" t="s">
+    <row r="133" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
         <v>403</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B133" t="s">
         <v>404</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="C133" s="4" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="36">
-      <c r="A128" t="s">
+    <row r="134" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
         <v>406</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B134" t="s">
         <v>407</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C134" s="4" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
-      <c r="A129" t="s">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
         <v>409</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B135" t="s">
         <v>410</v>
       </c>
-      <c r="C129" s="4" t="s">
+      <c r="C135" s="4" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
-      <c r="A130" t="s">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
         <v>412</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B136" t="s">
         <v>413</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C136" s="4" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
         <v>415</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B137" t="s">
         <v>416</v>
       </c>
-      <c r="C131" s="4" t="s">
+      <c r="C137" s="4" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
-      <c r="A132" t="s">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
         <v>418</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B138" t="s">
         <v>419</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C138" s="4" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
-      <c r="A133" t="s">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
         <v>421</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B139" t="s">
         <v>422</v>
       </c>
-      <c r="C133" s="4" t="s">
+      <c r="C139" s="4" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
-      <c r="A134" t="s">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
         <v>424</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B140" t="s">
         <v>63</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C140" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
-      <c r="A135" t="s">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
         <v>425</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B141" t="s">
         <v>426</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C141" s="4" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
-      <c r="A136" t="s">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
         <v>428</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B142" t="s">
         <v>429</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C142" s="4" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
-      <c r="A137" t="s">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
         <v>431</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B143" t="s">
         <v>432</v>
       </c>
-      <c r="C137" s="4" t="s">
+      <c r="C143" s="4" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="48">
-      <c r="A138" t="s">
+    <row r="144" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
         <v>434</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B144" t="s">
         <v>435</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C144" s="4" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="139" spans="1:3">
-      <c r="A139" t="s">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
         <v>437</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B145" t="s">
         <v>438</v>
       </c>
-      <c r="C139" s="4" t="s">
+      <c r="C145" s="4" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
         <v>440</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B146" t="s">
         <v>441</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C146" s="4" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="24">
-      <c r="A141" t="s">
+    <row r="147" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
         <v>443</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B147" t="s">
         <v>444</v>
       </c>
-      <c r="C141" s="4" t="s">
+      <c r="C147" s="4" t="s">
         <v>445</v>
       </c>
     </row>
-    <row r="142" spans="1:3">
-      <c r="A142" t="s">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
         <v>446</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B148" t="s">
         <v>447</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C148" s="4" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="24">
-      <c r="A143" t="s">
+    <row r="149" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
         <v>449</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B149" t="s">
         <v>450</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="C149" s="4" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="144" spans="1:3">
-      <c r="A144" t="s">
+    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
         <v>452</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B150" t="s">
         <v>453</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C150" s="4" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="24">
-      <c r="A145" t="s">
+    <row r="151" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
         <v>455</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B151" t="s">
         <v>456</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C151" s="4" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="146" spans="1:3">
-      <c r="A146" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
         <v>458</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B152" t="s">
         <v>459</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C152" s="4" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="147" spans="1:3">
-      <c r="A147" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>461</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B153" t="s">
         <v>462</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="C153" s="4" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="24">
-      <c r="A148" t="s">
+    <row r="154" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
         <v>464</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B154" t="s">
         <v>465</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C154" s="4" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="36">
-      <c r="A149" t="s">
+    <row r="155" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
         <v>467</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B155" t="s">
         <v>468</v>
       </c>
-      <c r="C149" s="4" t="s">
+      <c r="C155" s="4" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="24">
-      <c r="A150" t="s">
+    <row r="156" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
         <v>470</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B156" t="s">
         <v>471</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C156" s="4" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="151" spans="1:3">
-      <c r="A151" t="s">
+    <row r="157" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
         <v>473</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B157" t="s">
         <v>474</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="C157" s="4" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="24">
-      <c r="A152" t="s">
+    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
         <v>476</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B158" t="s">
         <v>477</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C158" s="4" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="24">
-      <c r="A153" t="s">
+    <row r="159" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
         <v>479</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B159" t="s">
         <v>480</v>
       </c>
-      <c r="C153" s="4" t="s">
+      <c r="C159" s="4" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="154" spans="1:3">
-      <c r="A154" t="s">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
         <v>482</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B160" t="s">
         <v>483</v>
       </c>
-      <c r="C154" s="4" t="s">
+      <c r="C160" s="4" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="24">
-      <c r="A155" t="s">
+    <row r="161" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
         <v>485</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B161" t="s">
         <v>486</v>
       </c>
-      <c r="C155" s="4" t="s">
+      <c r="C161" s="4" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="24">
-      <c r="A156" t="s">
+    <row r="162" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
         <v>488</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B162" t="s">
         <v>489</v>
       </c>
-      <c r="C156" s="4" t="s">
+      <c r="C162" s="4" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="24">
-      <c r="A157" t="s">
+    <row r="163" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
         <v>492</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B163" t="s">
         <v>491</v>
       </c>
-      <c r="C157" s="4" t="s">
+      <c r="C163" s="4" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="158" spans="1:3">
-      <c r="A158" t="s">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
         <v>494</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B164" t="s">
         <v>495</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C164" s="4" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="159" spans="1:3">
-      <c r="A159" t="s">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
         <v>497</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B165" t="s">
         <v>498</v>
       </c>
-      <c r="C159" s="4" t="s">
+      <c r="C165" s="4" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="36">
-      <c r="A160" t="s">
+    <row r="166" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
         <v>500</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B166" t="s">
         <v>501</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C166" s="4" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="161" spans="1:3">
-      <c r="A161" t="s">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
         <v>503</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B167" t="s">
         <v>504</v>
       </c>
-      <c r="C161" s="4" t="s">
+      <c r="C167" s="4" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="24">
-      <c r="A162" t="s">
+    <row r="168" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
         <v>506</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B168" t="s">
         <v>507</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C168" s="4" t="s">
         <v>508</v>
       </c>
     </row>
-    <row r="163" spans="1:3">
-      <c r="A163" t="s">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
         <v>509</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B169" t="s">
         <v>510</v>
       </c>
-      <c r="C163" s="4" t="s">
+      <c r="C169" s="4" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="36">
-      <c r="A164" t="s">
+    <row r="170" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
         <v>512</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B170" t="s">
         <v>513</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C170" s="4" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="24">
-      <c r="A165" t="s">
+    <row r="171" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
         <v>515</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B171" t="s">
         <v>516</v>
       </c>
-      <c r="C165" s="4" t="s">
+      <c r="C171" s="4" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="36">
-      <c r="A166" t="s">
+    <row r="172" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
         <v>518</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B172" t="s">
         <v>519</v>
       </c>
-      <c r="C166" s="4" t="s">
+      <c r="C172" s="4" t="s">
         <v>520</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="36">
-      <c r="A167" t="s">
+    <row r="173" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
         <v>521</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B173" t="s">
         <v>522</v>
       </c>
-      <c r="C167" s="4" t="s">
+      <c r="C173" s="4" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="36">
-      <c r="A168" t="s">
+    <row r="174" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
         <v>524</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B174" t="s">
         <v>525</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="C174" s="4" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="36">
-      <c r="A169" t="s">
+    <row r="175" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
         <v>528</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B175" t="s">
         <v>527</v>
       </c>
-      <c r="C169" s="4" t="s">
+      <c r="C175" s="4" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="48">
-      <c r="A170" t="s">
+    <row r="176" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
         <v>531</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B176" t="s">
         <v>530</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C176" s="4" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="36">
-      <c r="A171" t="s">
+    <row r="177" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
         <v>534</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B177" t="s">
         <v>533</v>
       </c>
-      <c r="C171" s="4" t="s">
+      <c r="C177" s="4" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="172" spans="1:3">
-      <c r="A172" t="s">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
         <v>537</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B178" t="s">
         <v>536</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="C178" s="4" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="173" spans="1:3">
-      <c r="A173" t="s">
+    <row r="179" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
         <v>539</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B179" t="s">
         <v>540</v>
       </c>
-      <c r="C173" s="4" t="s">
+      <c r="C179" s="4" t="s">
         <v>541</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4700,18 +4845,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -4722,7 +4867,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24">
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -4733,7 +4878,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -4744,7 +4889,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -4755,7 +4900,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>603</v>
       </c>
@@ -4766,7 +4911,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -4777,7 +4922,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -4788,7 +4933,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>606</v>
       </c>
@@ -4799,7 +4944,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -4810,7 +4955,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -4821,7 +4966,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -4832,7 +4977,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="24">
+    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -4843,7 +4988,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -4854,7 +4999,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -4865,7 +5010,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24">
+    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -4876,7 +5021,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -4887,7 +5032,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -4898,7 +5043,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="24">
+    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -4909,7 +5054,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -4920,7 +5065,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>245</v>
       </c>
@@ -4931,7 +5076,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -4942,7 +5087,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -4953,7 +5098,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24">
+    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -4964,7 +5109,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -4975,7 +5120,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -4986,7 +5131,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -4997,7 +5142,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>265</v>
       </c>
@@ -5008,7 +5153,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="24">
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5019,7 +5164,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="24">
+    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5030,7 +5175,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="24">
+    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5041,7 +5186,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24">
+    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5052,7 +5197,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="24">
+    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5063,7 +5208,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24">
+    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5074,7 +5219,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>286</v>
       </c>
@@ -5085,7 +5230,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -5096,7 +5241,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>291</v>
       </c>
@@ -5107,7 +5252,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -5118,7 +5263,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -5129,7 +5274,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="24">
+    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5140,7 +5285,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24">
+    <row r="40" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5151,7 +5296,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="24">
+    <row r="41" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5162,7 +5307,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -5173,7 +5318,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>313</v>
       </c>
@@ -5184,7 +5329,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -5195,7 +5340,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24">
+    <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5206,7 +5351,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>322</v>
       </c>
@@ -5217,7 +5362,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>325</v>
       </c>
@@ -5228,7 +5373,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>328</v>
       </c>
@@ -5239,7 +5384,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="24">
+    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5250,7 +5395,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>334</v>
       </c>
@@ -5261,7 +5406,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="24">
+    <row r="51" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5272,7 +5417,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="24">
+    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5283,7 +5428,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>343</v>
       </c>
@@ -5294,7 +5439,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -5305,7 +5450,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>349</v>
       </c>
@@ -5316,7 +5461,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>352</v>
       </c>
@@ -5327,7 +5472,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="24">
+    <row r="57" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5338,7 +5483,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -5349,7 +5494,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="24">
+    <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5360,7 +5505,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>364</v>
       </c>
@@ -5371,7 +5516,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -5382,7 +5527,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -5393,7 +5538,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="24">
+    <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5404,7 +5549,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>375</v>
       </c>
@@ -5415,7 +5560,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>379</v>
       </c>
@@ -5426,7 +5571,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>382</v>
       </c>
@@ -5437,7 +5582,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>555</v>
       </c>
@@ -5448,7 +5593,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>388</v>
       </c>
@@ -5459,7 +5604,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5470,7 +5615,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="24">
+    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5481,7 +5626,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="24">
+    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5492,7 +5637,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="24">
+    <row r="72" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5503,7 +5648,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>403</v>
       </c>
@@ -5514,7 +5659,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="24">
+    <row r="74" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5525,7 +5670,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -5536,7 +5681,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>412</v>
       </c>
@@ -5547,7 +5692,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>415</v>
       </c>
@@ -5558,7 +5703,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>418</v>
       </c>
@@ -5569,7 +5714,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>421</v>
       </c>
@@ -5580,7 +5725,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="24">
+    <row r="80" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -5591,7 +5736,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>425</v>
       </c>
@@ -5602,7 +5747,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>428</v>
       </c>
@@ -5613,7 +5758,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>431</v>
       </c>
@@ -5624,7 +5769,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="24">
+    <row r="84" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -5635,7 +5780,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>437</v>
       </c>
@@ -5646,7 +5791,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>440</v>
       </c>
@@ -5657,7 +5802,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>443</v>
       </c>
@@ -5668,7 +5813,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>446</v>
       </c>
@@ -5679,7 +5824,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>449</v>
       </c>
@@ -5690,7 +5835,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>452</v>
       </c>
@@ -5701,7 +5846,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>455</v>
       </c>
@@ -5712,7 +5857,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>458</v>
       </c>
@@ -5723,7 +5868,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>461</v>
       </c>
@@ -5734,7 +5879,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="24">
+    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>464</v>
       </c>
@@ -5745,7 +5890,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="24">
+    <row r="95" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>467</v>
       </c>
@@ -5756,7 +5901,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="24">
+    <row r="96" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>470</v>
       </c>
@@ -5767,7 +5912,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>473</v>
       </c>
@@ -5778,7 +5923,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>476</v>
       </c>
@@ -5789,7 +5934,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>479</v>
       </c>
@@ -5800,7 +5945,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>482</v>
       </c>
@@ -5811,7 +5956,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="24">
+    <row r="101" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>485</v>
       </c>
@@ -5822,7 +5967,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>488</v>
       </c>
@@ -5833,7 +5978,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>492</v>
       </c>
@@ -5844,7 +5989,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>494</v>
       </c>
@@ -5855,7 +6000,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>497</v>
       </c>
@@ -5866,7 +6011,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="24">
+    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>500</v>
       </c>
@@ -5877,7 +6022,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>503</v>
       </c>
@@ -5888,7 +6033,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="24">
+    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>506</v>
       </c>
@@ -5899,7 +6044,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>509</v>
       </c>
@@ -5910,7 +6055,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="24">
+    <row r="110" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>512</v>
       </c>
@@ -5921,7 +6066,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="24">
+    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>515</v>
       </c>
@@ -5932,7 +6077,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="24">
+    <row r="112" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>518</v>
       </c>
@@ -5943,7 +6088,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24">
+    <row r="113" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>521</v>
       </c>
@@ -5954,7 +6099,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>524</v>
       </c>
@@ -5965,7 +6110,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="24">
+    <row r="115" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>528</v>
       </c>
@@ -5976,7 +6121,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="24">
+    <row r="116" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>531</v>
       </c>
@@ -5987,7 +6132,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="24">
+    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>534</v>
       </c>
@@ -5998,7 +6143,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>537</v>
       </c>
@@ -6009,7 +6154,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>539</v>
       </c>
@@ -6020,7 +6165,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>550</v>
       </c>
@@ -6031,7 +6176,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>553</v>
       </c>
@@ -6042,7 +6187,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>556</v>
       </c>
@@ -6053,7 +6198,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>558</v>
       </c>
@@ -6064,7 +6209,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="24">
+    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>560</v>
       </c>
@@ -6075,7 +6220,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>563</v>
       </c>
@@ -6086,7 +6231,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>566</v>
       </c>
@@ -6097,7 +6242,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>569</v>
       </c>
@@ -6108,7 +6253,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>571</v>
       </c>
@@ -6119,7 +6264,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>574</v>
       </c>
@@ -6130,7 +6275,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>577</v>
       </c>
@@ -6141,7 +6286,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="24">
+    <row r="131" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>580</v>
       </c>
@@ -6152,7 +6297,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="24">
+    <row r="132" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>585</v>
       </c>
@@ -6163,7 +6308,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>586</v>
       </c>
@@ -6174,7 +6319,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>589</v>
       </c>
@@ -6185,7 +6330,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="135" spans="1:3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>600</v>
       </c>
@@ -6196,7 +6341,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="136" spans="1:3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>609</v>
       </c>
@@ -6207,7 +6352,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="137" spans="1:3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>612</v>
       </c>
@@ -6218,7 +6363,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="24">
+    <row r="138" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>616</v>
       </c>

</xml_diff>

<commit_message>
switch to 2 digit language code
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="842">
   <si>
     <t>comments</t>
   </si>
@@ -121,18 +121,6 @@
     <t>text.default</t>
   </si>
   <si>
-    <t>text.greek</t>
-  </si>
-  <si>
-    <t>text.arabic</t>
-  </si>
-  <si>
-    <t>text.farsi</t>
-  </si>
-  <si>
-    <t>text.spanish</t>
-  </si>
-  <si>
     <t>main_title</t>
   </si>
   <si>
@@ -1546,21 +1534,6 @@
     <t>display.title.text.farsi</t>
   </si>
   <si>
-    <t>display.locale.text.english</t>
-  </si>
-  <si>
-    <t>display.locale.text.spanish</t>
-  </si>
-  <si>
-    <t>display.locale.text.greek</t>
-  </si>
-  <si>
-    <t>display.locale.text.arabic</t>
-  </si>
-  <si>
-    <t>display.locale.text.farsi</t>
-  </si>
-  <si>
     <t>showContents</t>
   </si>
   <si>
@@ -1591,37 +1564,22 @@
     <t>The title of the 'survey' section (a.k.a. form title)</t>
   </si>
   <si>
-    <t>english</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
     <t>Ingles</t>
   </si>
   <si>
-    <t>spanish</t>
-  </si>
-  <si>
     <t>Spanish</t>
   </si>
   <si>
     <t>Espanol</t>
   </si>
   <si>
-    <t>arabic</t>
-  </si>
-  <si>
     <t>Arabic</t>
   </si>
   <si>
-    <t>farsi</t>
-  </si>
-  <si>
     <t>Farsi</t>
-  </si>
-  <si>
-    <t>greek</t>
   </si>
   <si>
     <t>Greek</t>
@@ -2586,6 +2544,45 @@
   </si>
   <si>
     <t>&lt;p&gt;Instancias creadas previamente:&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>es</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>ar</t>
+  </si>
+  <si>
+    <t>fa</t>
+  </si>
+  <si>
+    <t>el</t>
+  </si>
+  <si>
+    <t>display.locale.text.en</t>
+  </si>
+  <si>
+    <t>display.locale.text.es</t>
+  </si>
+  <si>
+    <t>display.locale.text.fa</t>
+  </si>
+  <si>
+    <t>display.locale.text.ar</t>
+  </si>
+  <si>
+    <t>display.locale.text.el</t>
+  </si>
+  <si>
+    <t>text.ar</t>
+  </si>
+  <si>
+    <t>text.el</t>
+  </si>
+  <si>
+    <t>text.fa</t>
   </si>
 </sst>
 </file>
@@ -3229,7 +3226,7 @@
   <dimension ref="A1:G159"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
@@ -3237,7 +3234,8 @@
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="49.44140625" customWidth="1"/>
     <col min="3" max="3" width="62.109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="8.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" style="4" customWidth="1"/>
     <col min="6" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3249,36 +3247,36 @@
         <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>840</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>839</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>31</v>
+        <v>841</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>32</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3286,74 +3284,74 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>39</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="G5" s="11"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3368,62 +3366,62 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3434,102 +3432,102 @@
         <v>25</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B20" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -3544,104 +3542,104 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>91</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B23" t="s">
+      <c r="F23" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B24" t="s">
+      <c r="F24" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B27" t="s">
+      <c r="F27" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>114</v>
+      </c>
+      <c r="B28" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="B28" t="s">
+      <c r="F28" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -3654,95 +3652,95 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31" t="s">
+        <v>121</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B31" t="s">
+      <c r="F31" s="6" t="s">
         <v>125</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B32" t="s">
+      <c r="F32" s="6" t="s">
         <v>131</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" s="6" t="s">
         <v>137</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
@@ -3757,279 +3755,279 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>147</v>
+      </c>
+      <c r="B39" t="s">
+        <v>148</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B39" t="s">
+      <c r="F39" s="10" t="s">
         <v>152</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>155</v>
-      </c>
-      <c r="F39" s="10" t="s">
-        <v>156</v>
       </c>
       <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="B40" t="s">
+      <c r="F40" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B41" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
+        <v>165</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="B43" t="s">
+      <c r="F43" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>171</v>
+      </c>
+      <c r="B44" t="s">
+        <v>172</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B44" t="s">
+      <c r="F44" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B46" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B47" t="s">
+      <c r="F47" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B48" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B49" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B53" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B54" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B55" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -4043,25 +4041,25 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C62" s="15"/>
       <c r="F62" s="13" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B63" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
@@ -4074,35 +4072,35 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B66" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B67" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B68" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
@@ -4115,126 +4113,126 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
+        <v>239</v>
+      </c>
+      <c r="B71" t="s">
+        <v>240</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E71" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B71" t="s">
+      <c r="F71" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="D71" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>248</v>
+      </c>
+      <c r="B73" t="s">
+        <v>249</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E73" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="B73" t="s">
+      <c r="F73" s="13" t="s">
         <v>253</v>
-      </c>
-      <c r="C73" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F73" s="13" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B74" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B75" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="F75" s="7" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B76" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F76" s="7" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>263</v>
+      </c>
+      <c r="B77" t="s">
+        <v>264</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E77" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="B77" t="s">
+      <c r="F77" s="6" t="s">
         <v>268</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E78" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="F78" s="13" t="s">
         <v>274</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="D78" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
@@ -4242,64 +4240,64 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F80" s="7" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F81" s="7" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B82" t="s">
+        <v>282</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E82" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="B82" t="s">
+      <c r="F82" s="6" t="s">
         <v>286</v>
-      </c>
-      <c r="C82" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="E82" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B83" t="s">
+        <v>288</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="B83" t="s">
+      <c r="F83" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="D83" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
@@ -4310,57 +4308,57 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B86" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B87" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B88" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B89" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F89" s="7" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B90" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
@@ -4371,101 +4369,101 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B93" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="F93" s="7" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B94" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B95" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="F95" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B96" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B97" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="F97" s="7" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B98" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B99" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F99" s="7" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B100" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B101" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="F101" s="7" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
@@ -4477,68 +4475,68 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B104" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B105" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F105" s="7" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B106" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B107" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F107" s="7" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B108" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B109" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F109" s="7" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
@@ -4546,46 +4544,46 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="16" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B111" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F111" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B112" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="16" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B113" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="16" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B114" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.3">
@@ -4593,161 +4591,161 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="16" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B116" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F116" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B117" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F117" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="16" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B118" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="16" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B119" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="16" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B120" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="16" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B121" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D122" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E122" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="F122" s="6" t="s">
         <v>388</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="D122" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="E122" s="4" t="s">
-        <v>391</v>
-      </c>
-      <c r="F122" s="6" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="16" t="s">
+        <v>389</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="E123" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="F123" s="6" t="s">
         <v>394</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="D123" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="E123" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="124" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A124" s="16" t="s">
+        <v>395</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="E124" s="15" t="s">
         <v>399</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="F124" s="6" t="s">
         <v>400</v>
-      </c>
-      <c r="C124" s="4" t="s">
-        <v>401</v>
-      </c>
-      <c r="D124" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="E124" s="15" t="s">
-        <v>403</v>
-      </c>
-      <c r="F124" s="6" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="16" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B125" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F125" s="7" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="16" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="B126" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B127" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F127" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.3">
@@ -4755,13 +4753,13 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="16" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F129" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.3">
@@ -4769,87 +4767,87 @@
         <v>6</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F130" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B131" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F131" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="17" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B132" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="17" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B133" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F133" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="18" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B134" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="19" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B135" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F135" s="7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B136" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B137" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="F137" s="7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.3">
@@ -4862,79 +4860,79 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B140" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B141" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="F141" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B142" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="F142" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B143" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="F143" s="7" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B144" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F144" s="7" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B145" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F145" s="7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="20" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B146" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F146" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.3">
@@ -4943,134 +4941,134 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B148" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="F148" s="7" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B149" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="F149" s="7" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B150" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F150" s="7" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B151" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F151" s="7" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B152" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="F152" s="7" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B153" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="16" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B154" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="16" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B155" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F155" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="16" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B156" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="F156" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="16" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B157" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="F157" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="16" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B158" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="F158" s="7" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="16" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B159" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F159" s="7" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -5085,64 +5083,69 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="7" width="8.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" customWidth="1"/>
+    <col min="10" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" customWidth="1"/>
+    <col min="13" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>497</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>503</v>
-      </c>
       <c r="H1" t="s">
-        <v>504</v>
+        <v>834</v>
       </c>
       <c r="I1" t="s">
-        <v>505</v>
+        <v>835</v>
       </c>
       <c r="J1" t="s">
-        <v>506</v>
+        <v>838</v>
       </c>
       <c r="K1" t="s">
-        <v>507</v>
+        <v>837</v>
       </c>
       <c r="L1" t="s">
-        <v>508</v>
+        <v>836</v>
       </c>
       <c r="M1" t="s">
         <v>0</v>
       </c>
       <c r="N1" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -5157,10 +5160,10 @@
     </row>
     <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -5173,41 +5176,41 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="B4">
         <v>20130828</v>
       </c>
       <c r="M4" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="C5" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D5" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="E5" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="F5" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="G5" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="M5" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="N5" t="b">
         <f>FALSE()</f>
@@ -5216,27 +5219,27 @@
     </row>
     <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>519</v>
+        <v>830</v>
       </c>
       <c r="H7" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="I7" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="J7" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="K7" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="L7" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>522</v>
+        <v>829</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -5245,24 +5248,24 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>524</v>
+        <v>513</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>523</v>
+        <v>512</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>525</v>
+        <v>831</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -5271,24 +5274,24 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>527</v>
+        <v>832</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -5297,24 +5300,24 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>529</v>
+        <v>833</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5323,24 +5326,24 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>531</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -5367,13 +5370,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -5384,7 +5387,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -5395,7 +5398,7 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -5408,15 +5411,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.44140625" customWidth="1"/>
     <col min="2" max="2" width="41.77734375" customWidth="1"/>
-    <col min="3" max="5" width="8.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
     <col min="6" max="6" width="56.109375" style="21" customWidth="1"/>
     <col min="7" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
@@ -5429,604 +5434,604 @@
         <v>28</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>29</v>
+        <v>840</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>839</v>
       </c>
       <c r="E1" t="s">
-        <v>31</v>
+        <v>841</v>
       </c>
       <c r="F1" s="21" t="s">
-        <v>838</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="B2" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="B3" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>545</v>
+        <v>531</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="B4" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="B5" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="B6" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="B7" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="B8" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="B9" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="B10" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="B11" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="B12" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="B13" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="B14" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="B15" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="B16" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="B17" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="B18" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="B19" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="B20" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
       <c r="F20" s="21" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
       <c r="B21" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>651</v>
+        <v>637</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>652</v>
+        <v>638</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
       <c r="B22" t="s">
-        <v>654</v>
+        <v>640</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>655</v>
+        <v>641</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>656</v>
+        <v>642</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>657</v>
+        <v>643</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>658</v>
+        <v>644</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="B23" t="s">
-        <v>660</v>
+        <v>646</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="B24" t="s">
-        <v>666</v>
+        <v>652</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>669</v>
+        <v>655</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>670</v>
+        <v>656</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="B25" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="B26" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>681</v>
+        <v>667</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="B27" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>685</v>
+        <v>671</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="B28" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="22" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="B29" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="22" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>694</v>
+        <v>680</v>
       </c>
       <c r="B30" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
       <c r="B31" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
@@ -6036,520 +6041,520 @@
     </row>
     <row r="33" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="B33" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="B34" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="B35" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>722</v>
+        <v>708</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>723</v>
+        <v>709</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>724</v>
+        <v>710</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>725</v>
+        <v>711</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="22" t="s">
-        <v>839</v>
+        <v>825</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>726</v>
+        <v>712</v>
       </c>
       <c r="B37" t="s">
-        <v>727</v>
+        <v>713</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>728</v>
+        <v>714</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>729</v>
+        <v>715</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>730</v>
+        <v>716</v>
       </c>
       <c r="F37" s="21" t="s">
-        <v>731</v>
+        <v>717</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>732</v>
+        <v>718</v>
       </c>
       <c r="B38" t="s">
-        <v>733</v>
+        <v>719</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>734</v>
+        <v>720</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>735</v>
+        <v>721</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>736</v>
+        <v>722</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>737</v>
+        <v>723</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>738</v>
+        <v>724</v>
       </c>
       <c r="B39" t="s">
-        <v>739</v>
+        <v>725</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>740</v>
+        <v>726</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>741</v>
+        <v>727</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>742</v>
+        <v>728</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>743</v>
+        <v>729</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>744</v>
+        <v>730</v>
       </c>
       <c r="B40" t="s">
-        <v>745</v>
+        <v>731</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>746</v>
+        <v>732</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>747</v>
+        <v>733</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>748</v>
+        <v>734</v>
       </c>
       <c r="F40" s="22" t="s">
-        <v>749</v>
+        <v>735</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>750</v>
+        <v>736</v>
       </c>
       <c r="B41" t="s">
-        <v>751</v>
+        <v>737</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>752</v>
+        <v>738</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>753</v>
+        <v>739</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>754</v>
+        <v>740</v>
       </c>
       <c r="F41" s="21" t="s">
-        <v>755</v>
+        <v>741</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>756</v>
+        <v>742</v>
       </c>
       <c r="B42" t="s">
-        <v>757</v>
+        <v>743</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>758</v>
+        <v>744</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>759</v>
+        <v>745</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>760</v>
+        <v>746</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>761</v>
+        <v>747</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>762</v>
+        <v>748</v>
       </c>
       <c r="B43" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>763</v>
+        <v>749</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>764</v>
+        <v>750</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>765</v>
+        <v>751</v>
       </c>
       <c r="F43" s="21" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>766</v>
+        <v>752</v>
       </c>
       <c r="B44" t="s">
-        <v>767</v>
+        <v>753</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>768</v>
+        <v>754</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>769</v>
+        <v>755</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>770</v>
+        <v>756</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>840</v>
+        <v>826</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>771</v>
+        <v>757</v>
       </c>
       <c r="B45" t="s">
-        <v>772</v>
+        <v>758</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>773</v>
+        <v>759</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>774</v>
+        <v>760</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="F45" s="21" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>777</v>
+        <v>763</v>
       </c>
       <c r="B46" t="s">
-        <v>778</v>
+        <v>764</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
       <c r="F46" s="21" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
       <c r="B47" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
       <c r="B48" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>791</v>
+        <v>777</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>792</v>
+        <v>778</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>793</v>
+        <v>779</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>794</v>
+        <v>780</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>795</v>
+        <v>781</v>
       </c>
       <c r="B49" t="s">
-        <v>796</v>
+        <v>782</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>797</v>
+        <v>783</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>799</v>
+        <v>785</v>
       </c>
       <c r="F49" s="22" t="s">
-        <v>841</v>
+        <v>827</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>800</v>
+        <v>786</v>
       </c>
       <c r="B50" t="s">
-        <v>801</v>
+        <v>787</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>802</v>
+        <v>788</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>803</v>
+        <v>789</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>804</v>
+        <v>790</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>842</v>
+        <v>828</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>805</v>
+        <v>791</v>
       </c>
       <c r="B51" t="s">
-        <v>806</v>
+        <v>792</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>807</v>
+        <v>793</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>808</v>
+        <v>794</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>809</v>
+        <v>795</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>810</v>
+        <v>796</v>
       </c>
       <c r="B52" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="F52" s="21" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>811</v>
+        <v>797</v>
       </c>
       <c r="B53" t="s">
-        <v>812</v>
+        <v>798</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>813</v>
+        <v>799</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>814</v>
+        <v>800</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>815</v>
+        <v>801</v>
       </c>
       <c r="F53" s="21" t="s">
-        <v>816</v>
+        <v>802</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>817</v>
+        <v>803</v>
       </c>
       <c r="B54" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>818</v>
+        <v>804</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
       <c r="F54" s="21" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>819</v>
+        <v>805</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D55" s="4"/>
       <c r="F55" s="21" t="s">
-        <v>820</v>
+        <v>806</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>821</v>
+        <v>807</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>822</v>
+        <v>808</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>823</v>
+        <v>809</v>
       </c>
       <c r="D56" s="4"/>
       <c r="F56" s="21" t="s">
-        <v>824</v>
+        <v>810</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>825</v>
+        <v>811</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>826</v>
+        <v>812</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>827</v>
+        <v>813</v>
       </c>
       <c r="D57" s="4"/>
       <c r="F57" s="21" t="s">
-        <v>828</v>
+        <v>814</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>829</v>
+        <v>815</v>
       </c>
       <c r="B58" t="s">
-        <v>830</v>
+        <v>816</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="F58" s="21" t="s">
-        <v>831</v>
+        <v>817</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>832</v>
+        <v>818</v>
       </c>
       <c r="B59" t="s">
-        <v>833</v>
+        <v>819</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="F59" s="21" t="s">
-        <v>834</v>
+        <v>820</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>835</v>
+        <v>821</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>836</v>
+        <v>822</v>
       </c>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="F60" s="21" t="s">
-        <v>837</v>
+        <v>823</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
convert to 2 digit language code
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\odk-reference\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ODKWorkspace\app-designer\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16065" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25608" windowHeight="16068" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="5" r:id="rId1"/>
@@ -742,9 +742,6 @@
     <t>English (as hindi name)</t>
   </si>
   <si>
-    <t>text.hindi</t>
-  </si>
-  <si>
     <t>स्वीकार करना</t>
   </si>
   <si>
@@ -758,9 +755,6 @@
   </si>
   <si>
     <t>अचयनित</t>
-  </si>
-  <si>
-    <t>text.english</t>
   </si>
   <si>
     <t>text.es</t>
@@ -964,6 +958,12 @@
         {{/if}}
         &lt;hr&gt;
 </t>
+  </si>
+  <si>
+    <t>text.en</t>
+  </si>
+  <si>
+    <t>text.hi</t>
   </si>
 </sst>
 </file>
@@ -1620,13 +1620,13 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1657,20 +1657,20 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="4"/>
-    <col min="2" max="2" width="101.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="4"/>
+    <col min="2" max="2" width="101.109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.109375" style="4" customWidth="1"/>
     <col min="5" max="6" width="20" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="17.140625" style="4"/>
+    <col min="7" max="7" width="21.88671875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.109375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="17.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>25</v>
       </c>
@@ -1697,7 +1697,7 @@
       </c>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1717,13 +1717,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1734,23 +1734,23 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>160</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6" t="s">
         <v>161</v>
@@ -1762,20 +1762,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B11" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="6" t="s">
         <v>163</v>
@@ -1787,20 +1787,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="5"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6" t="s">
         <v>165</v>
@@ -1812,20 +1812,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>167</v>
@@ -1837,20 +1837,20 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6" t="s">
         <v>169</v>
@@ -1862,19 +1862,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6" t="s">
         <v>170</v>
@@ -1886,19 +1886,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="6" t="s">
         <v>172</v>
@@ -1910,19 +1910,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="6" t="s">
         <v>174</v>
@@ -1934,19 +1934,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="6" t="s">
         <v>176</v>
@@ -1958,19 +1958,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="6" t="s">
         <v>178</v>
@@ -1982,19 +1982,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="6" t="s">
         <v>180</v>
@@ -2006,19 +2006,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="6" t="s">
         <v>182</v>
@@ -2030,19 +2030,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="6" t="s">
         <v>184</v>
@@ -2054,19 +2054,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="6" t="s">
         <v>185</v>
@@ -2078,19 +2078,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="5"/>
       <c r="C49" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="6" t="s">
         <v>187</v>
@@ -2102,19 +2102,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5"/>
       <c r="C52" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="6" t="s">
         <v>189</v>
@@ -2126,19 +2126,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5"/>
       <c r="C55" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="6" t="s">
         <v>191</v>
@@ -2150,19 +2150,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="6" t="s">
         <v>193</v>
@@ -2174,19 +2174,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5"/>
       <c r="C61" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="6" t="s">
         <v>195</v>
@@ -2198,19 +2198,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="5"/>
       <c r="B64" s="5"/>
       <c r="C64" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="6" t="s">
         <v>197</v>
@@ -2222,19 +2222,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5"/>
       <c r="C67" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="6" t="s">
         <v>199</v>
@@ -2246,19 +2246,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5"/>
       <c r="C70" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="6" t="s">
         <v>201</v>
@@ -2270,19 +2270,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
       <c r="C73" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="6" t="s">
         <v>203</v>
@@ -2294,19 +2294,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="5"/>
       <c r="C76" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" ht="62.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="6" t="s">
         <v>205</v>
@@ -2318,19 +2318,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="5"/>
       <c r="C79" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="6" t="s">
         <v>207</v>
@@ -2342,19 +2342,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="6" t="s">
         <v>209</v>
@@ -2366,19 +2366,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5"/>
       <c r="C85" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:7" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="57.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:7" ht="57.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="6" t="s">
         <v>211</v>
@@ -2390,7 +2390,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="5"/>
       <c r="B88" s="5"/>
       <c r="C88" s="4" t="s">
@@ -2416,13 +2416,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="8" width="24.7109375" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
+    <col min="3" max="8" width="24.6640625" customWidth="1"/>
+    <col min="9" max="9" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>229</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F1" t="s">
         <v>155</v>
@@ -2445,7 +2445,7 @@
         <v>230</v>
       </c>
       <c r="H1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -2454,7 +2454,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
@@ -2468,7 +2468,7 @@
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2496,7 +2496,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="27.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>231</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
@@ -2516,8 +2516,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>157</v>
       </c>
@@ -2528,10 +2528,10 @@
         <v>232</v>
       </c>
       <c r="H7" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>212</v>
       </c>
@@ -2545,21 +2545,21 @@
         <v>213</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" t="s">
+        <v>242</v>
+      </c>
+      <c r="G9" t="s">
         <v>243</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>244</v>
       </c>
-      <c r="G9" t="s">
-        <v>245</v>
-      </c>
-      <c r="H9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2569,13 +2569,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2585,7 +2585,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2595,13 +2595,13 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2611,7 +2611,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2621,10 +2621,10 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
     </row>
   </sheetData>
@@ -2646,14 +2646,14 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>22</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>24</v>
       </c>
@@ -2675,7 +2675,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -2686,7 +2686,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>24</v>
       </c>
@@ -2719,7 +2719,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>24</v>
       </c>
@@ -2730,7 +2730,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -2752,7 +2752,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2763,7 +2763,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -2774,7 +2774,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>24</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>24</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>24</v>
       </c>
@@ -2862,7 +2862,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>24</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>24</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -2917,7 +2917,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -2950,7 +2950,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -2976,20 +2976,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="56.140625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="26.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="57.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="8.109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.109375" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>35</v>
       </c>
@@ -2997,13 +2997,13 @@
         <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>44</v>
       </c>
@@ -3011,10 +3011,10 @@
         <v>47</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>45</v>
       </c>
@@ -3022,10 +3022,10 @@
         <v>48</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>46</v>
       </c>
@@ -3033,10 +3033,10 @@
         <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>51</v>
       </c>
@@ -3044,10 +3044,10 @@
         <v>50</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
@@ -3055,10 +3055,10 @@
         <v>52</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -3066,13 +3066,13 @@
         <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
@@ -3080,13 +3080,13 @@
         <v>39</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>86</v>
       </c>
@@ -3094,13 +3094,13 @@
         <v>40</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
@@ -3108,13 +3108,13 @@
         <v>88</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>124</v>
       </c>
@@ -3122,10 +3122,10 @@
         <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -3133,10 +3133,10 @@
         <v>43</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
@@ -3144,10 +3144,10 @@
         <v>57</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
@@ -3155,10 +3155,10 @@
         <v>59</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>64</v>
       </c>
@@ -3166,10 +3166,10 @@
         <v>60</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>65</v>
       </c>
@@ -3177,10 +3177,10 @@
         <v>61</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>66</v>
       </c>
@@ -3188,10 +3188,10 @@
         <v>62</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>67</v>
       </c>
@@ -3199,10 +3199,10 @@
         <v>68</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>69</v>
       </c>
@@ -3210,10 +3210,10 @@
         <v>70</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>71</v>
       </c>
@@ -3221,10 +3221,10 @@
         <v>72</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>73</v>
       </c>
@@ -3232,10 +3232,10 @@
         <v>74</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>75</v>
       </c>
@@ -3243,10 +3243,10 @@
         <v>76</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>77</v>
       </c>
@@ -3254,10 +3254,10 @@
         <v>78</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>79</v>
       </c>
@@ -3265,10 +3265,10 @@
         <v>80</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>81</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>83</v>
       </c>
@@ -3287,10 +3287,10 @@
         <v>84</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>90</v>
       </c>
@@ -3298,10 +3298,10 @@
         <v>89</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>104</v>
       </c>
@@ -3309,10 +3309,10 @@
         <v>92</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>93</v>
       </c>
@@ -3320,10 +3320,10 @@
         <v>91</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>94</v>
       </c>
@@ -3331,10 +3331,10 @@
         <v>95</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>96</v>
       </c>
@@ -3342,10 +3342,10 @@
         <v>97</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>98</v>
       </c>
@@ -3353,10 +3353,10 @@
         <v>101</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>99</v>
       </c>
@@ -3364,10 +3364,10 @@
         <v>100</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>102</v>
       </c>
@@ -3375,10 +3375,10 @@
         <v>103</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="178.5" x14ac:dyDescent="0.2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="184.8" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>105</v>
       </c>
@@ -3386,10 +3386,10 @@
         <v>106</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>107</v>
       </c>
@@ -3397,10 +3397,10 @@
         <v>108</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>111</v>
       </c>
@@ -3408,10 +3408,10 @@
         <v>109</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>110</v>
       </c>
@@ -3419,10 +3419,10 @@
         <v>112</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>113</v>
       </c>
@@ -3430,10 +3430,10 @@
         <v>114</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>115</v>
       </c>
@@ -3441,10 +3441,10 @@
         <v>116</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>117</v>
       </c>
@@ -3452,10 +3452,10 @@
         <v>118</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>119</v>
       </c>
@@ -3463,10 +3463,10 @@
         <v>120</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>121</v>
       </c>
@@ -3474,10 +3474,10 @@
         <v>122</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>123</v>
       </c>
@@ -3485,13 +3485,13 @@
         <v>38</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>125</v>
       </c>
@@ -3499,10 +3499,10 @@
         <v>141</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>126</v>
       </c>
@@ -3510,10 +3510,10 @@
         <v>127</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>128</v>
       </c>
@@ -3521,10 +3521,10 @@
         <v>129</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>130</v>
       </c>
@@ -3532,10 +3532,10 @@
         <v>131</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="12.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>132</v>
       </c>
@@ -3543,10 +3543,10 @@
         <v>133</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>136</v>
       </c>
@@ -3554,10 +3554,10 @@
         <v>134</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>137</v>
       </c>
@@ -3565,10 +3565,10 @@
         <v>97</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>138</v>
       </c>
@@ -3576,10 +3576,10 @@
         <v>135</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>139</v>
       </c>
@@ -3587,10 +3587,10 @@
         <v>127</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>140</v>
       </c>
@@ -3598,10 +3598,10 @@
         <v>142</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>143</v>
       </c>
@@ -3609,10 +3609,10 @@
         <v>144</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>146</v>
       </c>
@@ -3620,10 +3620,10 @@
         <v>145</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>150</v>
       </c>
@@ -3631,10 +3631,10 @@
         <v>148</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>151</v>
       </c>
@@ -3642,10 +3642,10 @@
         <v>149</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>152</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>153</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3672,30 +3672,30 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>239</v>
+        <v>301</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>302</v>
       </c>
       <c r="D1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E1" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Add in new translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RC2\modules\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\red-cross\redcross-app-designer\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="847">
   <si>
     <t>comments</t>
   </si>
@@ -2586,6 +2586,18 @@
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('ex_beneficiary_units_form')</t>
+  </si>
+  <si>
+    <t>no_distributions</t>
+  </si>
+  <si>
+    <t>No Distributions</t>
+  </si>
+  <si>
+    <t>choose_distribution</t>
+  </si>
+  <si>
+    <t>Choose Distribution</t>
   </si>
 </sst>
 </file>
@@ -3082,7 +3094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -3230,10 +3242,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G159"/>
+  <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5076,6 +5088,22 @@
       </c>
       <c r="F159" s="7" t="s">
         <v>491</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" s="20" t="s">
+        <v>843</v>
+      </c>
+      <c r="B160" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="20" t="s">
+        <v>845</v>
+      </c>
+      <c r="B161" t="s">
+        <v>846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes to colombia delivery form
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$103</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="850">
   <si>
     <t>comments</t>
   </si>
@@ -2598,6 +2598,15 @@
   </si>
   <si>
     <t>Choose Distribution</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('colombia_delivery')</t>
+  </si>
+  <si>
+    <t>colombia</t>
+  </si>
+  <si>
+    <t>Colombia Delivery</t>
   </si>
 </sst>
 </file>
@@ -2623,13 +2632,13 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2642,7 +2651,7 @@
       <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -3064,14 +3073,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" customWidth="1"/>
+    <col min="3" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3079,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3092,25 +3101,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.26953125" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="8" width="30.7265625" customWidth="1"/>
+    <col min="9" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3137,7 +3146,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -3146,7 +3155,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -3157,13 +3166,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -3174,23 +3183,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>841</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="23" t="s">
         <v>842</v>
@@ -3202,20 +3211,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="23" t="s">
         <v>25</v>
@@ -3227,10 +3236,35 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+      <c r="B15" s="23" t="s">
+        <v>847</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3244,21 +3278,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A146" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
-    <col min="6" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.26953125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="3" max="3" width="62.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" style="4" customWidth="1"/>
+    <col min="6" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -3278,7 +3312,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3298,7 +3332,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3318,7 +3352,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3330,7 +3364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3351,7 +3385,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3362,7 +3396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -3373,17 +3407,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3403,7 +3437,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3423,7 +3457,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3443,7 +3477,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3463,7 +3497,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3474,7 +3508,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -3485,7 +3519,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3496,7 +3530,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -3507,7 +3541,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -3527,7 +3561,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -3538,7 +3572,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>86</v>
       </c>
@@ -3549,17 +3583,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3579,7 +3613,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -3599,7 +3633,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -3610,7 +3644,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -3621,7 +3655,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -3641,7 +3675,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -3661,15 +3695,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3689,7 +3723,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3709,7 +3743,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3729,7 +3763,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -3740,7 +3774,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3751,7 +3785,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3762,17 +3796,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3793,7 +3827,7 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3813,7 +3847,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3824,7 +3858,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -3835,7 +3869,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -3855,7 +3889,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -3875,7 +3909,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -3886,7 +3920,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -3897,7 +3931,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -3917,7 +3951,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -3928,7 +3962,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -3939,7 +3973,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -3950,7 +3984,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -3961,7 +3995,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -3972,7 +4006,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -3983,7 +4017,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -3994,7 +4028,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -4005,7 +4039,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -4016,7 +4050,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4027,7 +4061,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4038,7 +4072,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4049,16 +4083,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -4070,7 +4104,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>226</v>
       </c>
@@ -4081,15 +4115,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="12"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4100,7 +4134,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -4111,7 +4145,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -4122,15 +4156,15 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -4150,7 +4184,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>244</v>
       </c>
@@ -4161,7 +4195,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -4181,7 +4215,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>253</v>
       </c>
@@ -4192,7 +4226,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
         <v>256</v>
       </c>
@@ -4203,7 +4237,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>259</v>
       </c>
@@ -4214,7 +4248,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -4234,7 +4268,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>268</v>
       </c>
@@ -4254,10 +4288,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>274</v>
       </c>
@@ -4268,7 +4302,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>277</v>
       </c>
@@ -4279,7 +4313,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>280</v>
       </c>
@@ -4299,7 +4333,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>286</v>
       </c>
@@ -4319,13 +4353,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>292</v>
       </c>
@@ -4336,7 +4370,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
         <v>295</v>
       </c>
@@ -4347,7 +4381,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>298</v>
       </c>
@@ -4358,7 +4392,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>301</v>
       </c>
@@ -4369,7 +4403,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
         <v>304</v>
       </c>
@@ -4380,13 +4414,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
         <v>307</v>
       </c>
@@ -4397,7 +4431,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
         <v>310</v>
       </c>
@@ -4408,7 +4442,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -4419,7 +4453,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
         <v>316</v>
       </c>
@@ -4430,7 +4464,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
         <v>319</v>
       </c>
@@ -4441,7 +4475,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
         <v>322</v>
       </c>
@@ -4452,7 +4486,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
         <v>325</v>
       </c>
@@ -4463,7 +4497,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
         <v>328</v>
       </c>
@@ -4474,7 +4508,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
         <v>331</v>
       </c>
@@ -4485,14 +4519,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="12"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4503,7 +4537,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4514,7 +4548,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>340</v>
       </c>
@@ -4525,7 +4559,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>343</v>
       </c>
@@ -4536,7 +4570,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -4547,7 +4581,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -4558,10 +4592,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="16" t="s">
         <v>352</v>
       </c>
@@ -4572,7 +4606,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="16" t="s">
         <v>355</v>
       </c>
@@ -4583,7 +4617,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="16" t="s">
         <v>358</v>
       </c>
@@ -4594,7 +4628,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="16" t="s">
         <v>361</v>
       </c>
@@ -4605,10 +4639,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="16" t="s">
         <v>364</v>
       </c>
@@ -4619,7 +4653,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="16" t="s">
         <v>367</v>
       </c>
@@ -4630,7 +4664,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="16" t="s">
         <v>370</v>
       </c>
@@ -4641,7 +4675,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="16" t="s">
         <v>373</v>
       </c>
@@ -4652,7 +4686,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="16" t="s">
         <v>376</v>
       </c>
@@ -4663,7 +4697,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="16" t="s">
         <v>379</v>
       </c>
@@ -4674,7 +4708,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="16" t="s">
         <v>382</v>
       </c>
@@ -4694,7 +4728,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="16" t="s">
         <v>388</v>
       </c>
@@ -4714,7 +4748,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>394</v>
       </c>
@@ -4734,7 +4768,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>400</v>
       </c>
@@ -4745,7 +4779,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>403</v>
       </c>
@@ -4756,7 +4790,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>406</v>
       </c>
@@ -4767,10 +4801,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="16" t="s">
         <v>409</v>
       </c>
@@ -4781,7 +4815,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="17" t="s">
         <v>6</v>
       </c>
@@ -4792,7 +4826,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="17" t="s">
         <v>414</v>
       </c>
@@ -4803,7 +4837,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="17" t="s">
         <v>417</v>
       </c>
@@ -4814,7 +4848,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="17" t="s">
         <v>420</v>
       </c>
@@ -4825,7 +4859,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="18" t="s">
         <v>423</v>
       </c>
@@ -4836,7 +4870,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="19" t="s">
         <v>426</v>
       </c>
@@ -4847,7 +4881,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
         <v>429</v>
       </c>
@@ -4858,7 +4892,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
         <v>432</v>
       </c>
@@ -4869,15 +4903,15 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="12"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="12"/>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>435</v>
       </c>
@@ -4888,7 +4922,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>438</v>
       </c>
@@ -4899,7 +4933,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -4910,7 +4944,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>444</v>
       </c>
@@ -4921,7 +4955,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>447</v>
       </c>
@@ -4932,7 +4966,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>450</v>
       </c>
@@ -4943,7 +4977,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
         <v>453</v>
       </c>
@@ -4954,11 +4988,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="20"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="16" t="s">
         <v>456</v>
       </c>
@@ -4969,7 +5003,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="16" t="s">
         <v>459</v>
       </c>
@@ -4980,7 +5014,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="16" t="s">
         <v>462</v>
       </c>
@@ -4991,7 +5025,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="16" t="s">
         <v>465</v>
       </c>
@@ -5002,7 +5036,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="16" t="s">
         <v>468</v>
       </c>
@@ -5013,7 +5047,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="s">
         <v>471</v>
       </c>
@@ -5024,7 +5058,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="16" t="s">
         <v>474</v>
       </c>
@@ -5035,7 +5069,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="16" t="s">
         <v>477</v>
       </c>
@@ -5046,7 +5080,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="s">
         <v>480</v>
       </c>
@@ -5057,7 +5091,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="16" t="s">
         <v>483</v>
       </c>
@@ -5068,7 +5102,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="16" t="s">
         <v>486</v>
       </c>
@@ -5079,7 +5113,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="16" t="s">
         <v>489</v>
       </c>
@@ -5090,7 +5124,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
         <v>843</v>
       </c>
@@ -5098,7 +5132,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" s="20" t="s">
         <v>845</v>
       </c>
@@ -5121,18 +5155,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="41.7265625" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" customWidth="1"/>
+    <col min="6" max="6" width="56.1796875" style="21" customWidth="1"/>
+    <col min="7" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5152,7 +5186,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -5172,7 +5206,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5192,7 +5226,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>533</v>
       </c>
@@ -5212,7 +5246,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>539</v>
       </c>
@@ -5232,7 +5266,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5252,7 +5286,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5272,7 +5306,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>557</v>
       </c>
@@ -5292,7 +5326,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>563</v>
       </c>
@@ -5312,7 +5346,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>569</v>
       </c>
@@ -5332,7 +5366,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>575</v>
       </c>
@@ -5352,7 +5386,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -5372,7 +5406,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>584</v>
       </c>
@@ -5392,7 +5426,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -5412,7 +5446,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>596</v>
       </c>
@@ -5432,7 +5466,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>602</v>
       </c>
@@ -5452,7 +5486,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>608</v>
       </c>
@@ -5472,7 +5506,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>614</v>
       </c>
@@ -5492,7 +5526,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>620</v>
       </c>
@@ -5512,7 +5546,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>626</v>
       </c>
@@ -5532,7 +5566,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>632</v>
       </c>
@@ -5552,7 +5586,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -5572,7 +5606,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>644</v>
       </c>
@@ -5592,7 +5626,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>650</v>
       </c>
@@ -5612,7 +5646,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>656</v>
       </c>
@@ -5632,7 +5666,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>661</v>
       </c>
@@ -5652,7 +5686,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>667</v>
       </c>
@@ -5672,7 +5706,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>673</v>
       </c>
@@ -5686,7 +5720,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>676</v>
       </c>
@@ -5700,7 +5734,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -5720,7 +5754,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>685</v>
       </c>
@@ -5740,12 +5774,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>691</v>
       </c>
@@ -5765,7 +5799,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>697</v>
       </c>
@@ -5785,7 +5819,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>703</v>
       </c>
@@ -5805,7 +5839,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="179.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="176" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>709</v>
       </c>
@@ -5819,7 +5853,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>711</v>
       </c>
@@ -5839,7 +5873,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>717</v>
       </c>
@@ -5859,7 +5893,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -5879,7 +5913,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>729</v>
       </c>
@@ -5899,7 +5933,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>735</v>
       </c>
@@ -5919,7 +5953,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -5939,7 +5973,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -5959,7 +5993,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>751</v>
       </c>
@@ -5979,7 +6013,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>756</v>
       </c>
@@ -5999,7 +6033,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>762</v>
       </c>
@@ -6019,7 +6053,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>768</v>
       </c>
@@ -6039,7 +6073,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>774</v>
       </c>
@@ -6059,7 +6093,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>780</v>
       </c>
@@ -6079,7 +6113,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>785</v>
       </c>
@@ -6099,7 +6133,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>790</v>
       </c>
@@ -6119,7 +6153,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>795</v>
       </c>
@@ -6139,7 +6173,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>796</v>
       </c>
@@ -6159,7 +6193,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>802</v>
       </c>
@@ -6179,7 +6213,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>804</v>
       </c>
@@ -6194,7 +6228,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>806</v>
       </c>
@@ -6209,7 +6243,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>810</v>
       </c>
@@ -6224,7 +6258,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>814</v>
       </c>
@@ -6237,7 +6271,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>817</v>
       </c>
@@ -6250,7 +6284,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>820</v>
       </c>
@@ -6277,19 +6311,19 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="7" width="8.7109375" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" customWidth="1"/>
-    <col min="10" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" customWidth="1"/>
-    <col min="13" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="7" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="26.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="10" max="11" width="21.7265625" customWidth="1"/>
+    <col min="12" max="12" width="21.81640625" customWidth="1"/>
+    <col min="13" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6333,7 +6367,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>500</v>
       </c>
@@ -6351,7 +6385,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>502</v>
       </c>
@@ -6372,7 +6406,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>504</v>
       </c>
@@ -6383,7 +6417,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -6410,7 +6444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>829</v>
       </c>
@@ -6430,7 +6464,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>828</v>
       </c>
@@ -6456,7 +6490,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>830</v>
       </c>
@@ -6482,7 +6516,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>831</v>
       </c>
@@ -6508,7 +6542,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>832</v>
       </c>
@@ -6534,7 +6568,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>516</v>
       </c>
@@ -6547,21 +6581,21 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="2" max="2" width="27.7265625" customWidth="1"/>
+    <col min="3" max="3" width="26.7265625" customWidth="1"/>
+    <col min="4" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>517</v>
       </c>
@@ -6572,7 +6606,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -6583,7 +6617,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -6592,6 +6626,17 @@
       </c>
       <c r="C3" t="s">
         <v>520</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>848</v>
+      </c>
+      <c r="C4" t="s">
+        <v>849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrate optional registeration and authorization delivery
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="850">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="853">
   <si>
     <t>comments</t>
   </si>
@@ -2607,6 +2607,15 @@
   </si>
   <si>
     <t>Colombia Delivery</t>
+  </si>
+  <si>
+    <t>register</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Registrar</t>
   </si>
 </sst>
 </file>
@@ -3073,11 +3082,11 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12.7265625" customWidth="1"/>
-    <col min="3" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" customWidth="1"/>
+    <col min="3" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3107,19 +3116,19 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.26953125" customWidth="1"/>
-    <col min="3" max="3" width="8.7265625" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="8" width="30.7265625" customWidth="1"/>
-    <col min="9" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="23.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.21875" customWidth="1"/>
+    <col min="3" max="3" width="8.77734375" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="7" max="8" width="30.77734375" customWidth="1"/>
+    <col min="9" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3155,7 +3164,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -3276,23 +3285,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G161"/>
+  <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B161" sqref="B161"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" customWidth="1"/>
-    <col min="3" max="3" width="62.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="4" customWidth="1"/>
-    <col min="6" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="3" max="3" width="62.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" style="4" customWidth="1"/>
+    <col min="6" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3332,7 +3341,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3352,7 +3361,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3364,7 +3373,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3385,7 +3394,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3396,7 +3405,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -3407,17 +3416,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3437,7 +3446,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3457,7 +3466,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3477,7 +3486,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3497,7 +3506,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3508,7 +3517,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -3519,7 +3528,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3530,7 +3539,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -3541,7 +3550,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -3561,7 +3570,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -3572,7 +3581,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>86</v>
       </c>
@@ -3583,17 +3592,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3613,7 +3622,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -3633,7 +3642,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -3644,7 +3653,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -3655,7 +3664,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -3675,7 +3684,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -3695,15 +3704,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3723,7 +3732,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3743,7 +3752,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3763,7 +3772,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -3774,7 +3783,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3785,7 +3794,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3796,17 +3805,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3827,7 +3836,7 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3847,7 +3856,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -3869,7 +3878,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -3889,7 +3898,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -3909,7 +3918,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -3920,7 +3929,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -3931,7 +3940,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -3951,7 +3960,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -3962,7 +3971,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -3973,7 +3982,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -3984,7 +3993,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -3995,7 +4004,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -4006,7 +4015,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -4017,7 +4026,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -4028,7 +4037,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -4039,7 +4048,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -4050,7 +4059,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4061,7 +4070,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4072,7 +4081,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4083,16 +4092,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B60" s="3"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -4104,7 +4113,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="12" t="s">
         <v>226</v>
       </c>
@@ -4115,15 +4124,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="12"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="12"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4134,7 +4143,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -4145,7 +4154,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -4156,15 +4165,15 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -4184,7 +4193,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>244</v>
       </c>
@@ -4195,7 +4204,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -4215,7 +4224,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>253</v>
       </c>
@@ -4226,7 +4235,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="12" t="s">
         <v>256</v>
       </c>
@@ -4237,7 +4246,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>259</v>
       </c>
@@ -4248,7 +4257,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -4268,7 +4277,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>268</v>
       </c>
@@ -4288,10 +4297,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>274</v>
       </c>
@@ -4302,7 +4311,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>277</v>
       </c>
@@ -4313,7 +4322,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>280</v>
       </c>
@@ -4333,7 +4342,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>286</v>
       </c>
@@ -4353,13 +4362,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="12" t="s">
         <v>292</v>
       </c>
@@ -4370,7 +4379,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="12" t="s">
         <v>295</v>
       </c>
@@ -4381,7 +4390,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="12" t="s">
         <v>298</v>
       </c>
@@ -4392,7 +4401,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="12" t="s">
         <v>301</v>
       </c>
@@ -4403,7 +4412,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="12" t="s">
         <v>304</v>
       </c>
@@ -4414,13 +4423,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="12" t="s">
         <v>307</v>
       </c>
@@ -4431,7 +4440,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="12" t="s">
         <v>310</v>
       </c>
@@ -4442,7 +4451,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="12" t="s">
         <v>316</v>
       </c>
@@ -4464,7 +4473,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="12" t="s">
         <v>319</v>
       </c>
@@ -4475,7 +4484,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="12" t="s">
         <v>322</v>
       </c>
@@ -4486,7 +4495,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="12" t="s">
         <v>325</v>
       </c>
@@ -4497,7 +4506,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="12" t="s">
         <v>328</v>
       </c>
@@ -4508,7 +4517,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="12" t="s">
         <v>331</v>
       </c>
@@ -4519,14 +4528,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="12"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4548,7 +4557,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>340</v>
       </c>
@@ -4559,7 +4568,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>343</v>
       </c>
@@ -4570,7 +4579,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -4581,7 +4590,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -4592,10 +4601,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="16" t="s">
         <v>352</v>
       </c>
@@ -4606,7 +4615,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="16" t="s">
         <v>355</v>
       </c>
@@ -4617,7 +4626,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="16" t="s">
         <v>358</v>
       </c>
@@ -4628,7 +4637,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="16" t="s">
         <v>361</v>
       </c>
@@ -4639,10 +4648,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="16" t="s">
         <v>364</v>
       </c>
@@ -4653,7 +4662,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
         <v>367</v>
       </c>
@@ -4664,7 +4673,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="16" t="s">
         <v>370</v>
       </c>
@@ -4675,7 +4684,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="16" t="s">
         <v>373</v>
       </c>
@@ -4686,7 +4695,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="16" t="s">
         <v>376</v>
       </c>
@@ -4697,7 +4706,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="16" t="s">
         <v>379</v>
       </c>
@@ -4708,7 +4717,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="16" t="s">
         <v>382</v>
       </c>
@@ -4728,7 +4737,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="16" t="s">
         <v>388</v>
       </c>
@@ -4748,7 +4757,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="16" t="s">
         <v>394</v>
       </c>
@@ -4768,7 +4777,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="16" t="s">
         <v>400</v>
       </c>
@@ -4779,7 +4788,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="16" t="s">
         <v>403</v>
       </c>
@@ -4790,7 +4799,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>406</v>
       </c>
@@ -4801,10 +4810,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="16" t="s">
         <v>409</v>
       </c>
@@ -4815,7 +4824,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="17" t="s">
         <v>6</v>
       </c>
@@ -4826,7 +4835,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="17" t="s">
         <v>414</v>
       </c>
@@ -4837,7 +4846,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="17" t="s">
         <v>417</v>
       </c>
@@ -4848,7 +4857,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="17" t="s">
         <v>420</v>
       </c>
@@ -4859,7 +4868,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="18" t="s">
         <v>423</v>
       </c>
@@ -4870,7 +4879,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="19" t="s">
         <v>426</v>
       </c>
@@ -4881,7 +4890,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="12" t="s">
         <v>429</v>
       </c>
@@ -4892,7 +4901,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="12" t="s">
         <v>432</v>
       </c>
@@ -4903,15 +4912,15 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="12"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A139" s="12"/>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>435</v>
       </c>
@@ -4922,7 +4931,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>438</v>
       </c>
@@ -4933,7 +4942,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -4944,7 +4953,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>444</v>
       </c>
@@ -4955,7 +4964,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>447</v>
       </c>
@@ -4966,7 +4975,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>450</v>
       </c>
@@ -4977,7 +4986,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="20" t="s">
         <v>453</v>
       </c>
@@ -4988,11 +4997,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="20"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="16" t="s">
         <v>456</v>
       </c>
@@ -5003,7 +5012,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="16" t="s">
         <v>459</v>
       </c>
@@ -5014,7 +5023,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="16" t="s">
         <v>462</v>
       </c>
@@ -5025,7 +5034,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="16" t="s">
         <v>465</v>
       </c>
@@ -5036,7 +5045,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="16" t="s">
         <v>468</v>
       </c>
@@ -5047,7 +5056,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="16" t="s">
         <v>471</v>
       </c>
@@ -5058,7 +5067,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="16" t="s">
         <v>474</v>
       </c>
@@ -5069,7 +5078,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="16" t="s">
         <v>477</v>
       </c>
@@ -5080,7 +5089,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="16" t="s">
         <v>480</v>
       </c>
@@ -5091,7 +5100,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="16" t="s">
         <v>483</v>
       </c>
@@ -5102,7 +5111,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="16" t="s">
         <v>486</v>
       </c>
@@ -5113,7 +5122,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="16" t="s">
         <v>489</v>
       </c>
@@ -5124,7 +5133,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="20" t="s">
         <v>843</v>
       </c>
@@ -5132,12 +5141,23 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="20" t="s">
         <v>845</v>
       </c>
       <c r="B161" t="s">
         <v>846</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="20" t="s">
+        <v>850</v>
+      </c>
+      <c r="B162" t="s">
+        <v>851</v>
+      </c>
+      <c r="F162" t="s">
+        <v>852</v>
       </c>
     </row>
   </sheetData>
@@ -5155,18 +5175,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.453125" customWidth="1"/>
-    <col min="2" max="2" width="41.7265625" customWidth="1"/>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" customWidth="1"/>
-    <col min="6" max="6" width="56.1796875" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="38.44140625" customWidth="1"/>
+    <col min="2" max="2" width="41.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" customWidth="1"/>
+    <col min="6" max="6" width="56.21875" style="21" customWidth="1"/>
+    <col min="7" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5186,7 +5206,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -5206,7 +5226,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5226,7 +5246,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>533</v>
       </c>
@@ -5246,7 +5266,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>539</v>
       </c>
@@ -5266,7 +5286,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5286,7 +5306,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5306,7 +5326,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>557</v>
       </c>
@@ -5326,7 +5346,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>563</v>
       </c>
@@ -5346,7 +5366,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>569</v>
       </c>
@@ -5366,7 +5386,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>575</v>
       </c>
@@ -5386,7 +5406,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -5406,7 +5426,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>584</v>
       </c>
@@ -5426,7 +5446,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -5446,7 +5466,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>596</v>
       </c>
@@ -5466,7 +5486,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>602</v>
       </c>
@@ -5486,7 +5506,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>608</v>
       </c>
@@ -5506,7 +5526,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>614</v>
       </c>
@@ -5526,7 +5546,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>620</v>
       </c>
@@ -5546,7 +5566,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>626</v>
       </c>
@@ -5566,7 +5586,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>632</v>
       </c>
@@ -5586,7 +5606,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -5606,7 +5626,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>644</v>
       </c>
@@ -5626,7 +5646,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>650</v>
       </c>
@@ -5646,7 +5666,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>656</v>
       </c>
@@ -5666,7 +5686,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>661</v>
       </c>
@@ -5686,7 +5706,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>667</v>
       </c>
@@ -5706,7 +5726,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>673</v>
       </c>
@@ -5720,7 +5740,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>676</v>
       </c>
@@ -5734,7 +5754,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -5754,7 +5774,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>685</v>
       </c>
@@ -5774,12 +5794,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>691</v>
       </c>
@@ -5799,7 +5819,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>697</v>
       </c>
@@ -5819,7 +5839,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>703</v>
       </c>
@@ -5839,7 +5859,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="176" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="185.4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>709</v>
       </c>
@@ -5853,7 +5873,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>711</v>
       </c>
@@ -5873,7 +5893,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>717</v>
       </c>
@@ -5893,7 +5913,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -5913,7 +5933,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>729</v>
       </c>
@@ -5933,7 +5953,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>735</v>
       </c>
@@ -5953,7 +5973,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -5973,7 +5993,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -5993,7 +6013,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>751</v>
       </c>
@@ -6013,7 +6033,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>756</v>
       </c>
@@ -6033,7 +6053,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>762</v>
       </c>
@@ -6053,7 +6073,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>768</v>
       </c>
@@ -6073,7 +6093,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>774</v>
       </c>
@@ -6093,7 +6113,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>780</v>
       </c>
@@ -6113,7 +6133,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>785</v>
       </c>
@@ -6133,7 +6153,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>790</v>
       </c>
@@ -6153,7 +6173,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>795</v>
       </c>
@@ -6173,7 +6193,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>796</v>
       </c>
@@ -6193,7 +6213,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>802</v>
       </c>
@@ -6213,7 +6233,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>804</v>
       </c>
@@ -6228,7 +6248,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>806</v>
       </c>
@@ -6243,7 +6263,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>810</v>
       </c>
@@ -6258,7 +6278,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>814</v>
       </c>
@@ -6271,7 +6291,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>817</v>
       </c>
@@ -6284,7 +6304,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>820</v>
       </c>
@@ -6311,16 +6331,15 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="7" width="8.7265625" customWidth="1"/>
-    <col min="8" max="8" width="26.54296875" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
-    <col min="10" max="11" width="21.7265625" customWidth="1"/>
-    <col min="12" max="12" width="21.81640625" customWidth="1"/>
-    <col min="13" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="7" width="8.77734375" customWidth="1"/>
+    <col min="8" max="8" width="26.5546875" customWidth="1"/>
+    <col min="9" max="9" width="26.21875" customWidth="1"/>
+    <col min="10" max="12" width="21.77734375" customWidth="1"/>
+    <col min="13" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6417,7 +6436,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -6583,16 +6602,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="3" width="26.7265625" customWidth="1"/>
-    <col min="4" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" customWidth="1"/>
+    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
First pass at modifying forms as requested from 6/7
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">common_translations!$A$1:$F$103</definedName>
   </definedNames>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="859">
   <si>
     <t>comments</t>
   </si>
@@ -2603,9 +2603,6 @@
     <t>'?' + odkSurvey.getHashString('colombia_delivery')</t>
   </si>
   <si>
-    <t>colombia</t>
-  </si>
-  <si>
     <t>Colombia Delivery</t>
   </si>
   <si>
@@ -2616,6 +2613,27 @@
   </si>
   <si>
     <t>Registrar</t>
+  </si>
+  <si>
+    <t>colombia_delivery</t>
+  </si>
+  <si>
+    <t>colombia_registration</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('colombia_registration')</t>
+  </si>
+  <si>
+    <t>Colombia Registration</t>
+  </si>
+  <si>
+    <t>colombia_delivery_demo</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('colombia_delivery_demo')</t>
+  </si>
+  <si>
+    <t>Simple Colombia Delivery</t>
   </si>
 </sst>
 </file>
@@ -3082,11 +3100,11 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.77734375" customWidth="1"/>
-    <col min="3" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3110,25 +3128,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.77734375" customWidth="1"/>
-    <col min="4" max="4" width="30.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
-    <col min="7" max="8" width="30.77734375" customWidth="1"/>
-    <col min="9" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="8" width="30.81640625" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3164,7 +3182,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -3254,7 +3272,7 @@
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>848</v>
+        <v>852</v>
       </c>
       <c r="B14" s="3"/>
     </row>
@@ -3274,6 +3292,56 @@
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>853</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="23" t="s">
+        <v>854</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>856</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="23" t="s">
+        <v>857</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3287,21 +3355,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G162"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G160" sqref="G160"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.21875" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" customWidth="1"/>
-    <col min="3" max="3" width="62.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.21875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" style="4" customWidth="1"/>
-    <col min="6" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="3" max="3" width="62.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" style="4" customWidth="1"/>
+    <col min="6" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -3321,7 +3389,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3341,7 +3409,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3361,7 +3429,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3373,7 +3441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3394,7 +3462,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3405,7 +3473,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -3416,17 +3484,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3446,7 +3514,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3466,7 +3534,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3486,7 +3554,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3506,7 +3574,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3517,7 +3585,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -3528,7 +3596,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3539,7 +3607,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -3550,7 +3618,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -3570,7 +3638,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -3581,7 +3649,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>86</v>
       </c>
@@ -3592,17 +3660,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3622,7 +3690,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -3642,7 +3710,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -3653,7 +3721,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -3664,7 +3732,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -3684,7 +3752,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -3704,15 +3772,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3732,7 +3800,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3752,7 +3820,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3772,7 +3840,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -3783,7 +3851,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3794,7 +3862,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3805,17 +3873,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3836,7 +3904,7 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3856,7 +3924,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3867,7 +3935,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -3878,7 +3946,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -3898,7 +3966,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -3918,7 +3986,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -3929,7 +3997,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -3940,7 +4008,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -3960,7 +4028,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -3971,7 +4039,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -3982,7 +4050,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -3993,7 +4061,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -4004,7 +4072,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -4015,7 +4083,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -4026,7 +4094,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -4037,7 +4105,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -4048,7 +4116,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -4059,7 +4127,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4070,7 +4138,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4081,7 +4149,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4092,16 +4160,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -4113,7 +4181,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>226</v>
       </c>
@@ -4124,15 +4192,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="12"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4143,7 +4211,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -4154,7 +4222,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -4165,15 +4233,15 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -4193,7 +4261,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>244</v>
       </c>
@@ -4204,7 +4272,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -4224,7 +4292,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>253</v>
       </c>
@@ -4235,7 +4303,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
         <v>256</v>
       </c>
@@ -4246,7 +4314,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>259</v>
       </c>
@@ -4257,7 +4325,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -4277,7 +4345,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>268</v>
       </c>
@@ -4297,10 +4365,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>274</v>
       </c>
@@ -4311,7 +4379,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>277</v>
       </c>
@@ -4322,7 +4390,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>280</v>
       </c>
@@ -4342,7 +4410,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>286</v>
       </c>
@@ -4362,13 +4430,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>292</v>
       </c>
@@ -4379,7 +4447,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
         <v>295</v>
       </c>
@@ -4390,7 +4458,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>298</v>
       </c>
@@ -4401,7 +4469,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>301</v>
       </c>
@@ -4412,7 +4480,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
         <v>304</v>
       </c>
@@ -4423,13 +4491,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
         <v>307</v>
       </c>
@@ -4440,7 +4508,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
         <v>310</v>
       </c>
@@ -4451,7 +4519,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -4462,7 +4530,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
         <v>316</v>
       </c>
@@ -4473,7 +4541,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
         <v>319</v>
       </c>
@@ -4484,7 +4552,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
         <v>322</v>
       </c>
@@ -4495,7 +4563,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
         <v>325</v>
       </c>
@@ -4506,7 +4574,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
         <v>328</v>
       </c>
@@ -4517,7 +4585,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
         <v>331</v>
       </c>
@@ -4528,14 +4596,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="12"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4546,7 +4614,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4557,7 +4625,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>340</v>
       </c>
@@ -4568,7 +4636,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>343</v>
       </c>
@@ -4579,7 +4647,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -4590,7 +4658,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -4601,10 +4669,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="16" t="s">
         <v>352</v>
       </c>
@@ -4615,7 +4683,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="16" t="s">
         <v>355</v>
       </c>
@@ -4626,7 +4694,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="16" t="s">
         <v>358</v>
       </c>
@@ -4637,7 +4705,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="16" t="s">
         <v>361</v>
       </c>
@@ -4648,10 +4716,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="16" t="s">
         <v>364</v>
       </c>
@@ -4662,7 +4730,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="16" t="s">
         <v>367</v>
       </c>
@@ -4673,7 +4741,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="16" t="s">
         <v>370</v>
       </c>
@@ -4684,7 +4752,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="16" t="s">
         <v>373</v>
       </c>
@@ -4695,7 +4763,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="16" t="s">
         <v>376</v>
       </c>
@@ -4706,7 +4774,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="16" t="s">
         <v>379</v>
       </c>
@@ -4717,7 +4785,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="16" t="s">
         <v>382</v>
       </c>
@@ -4737,7 +4805,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="16" t="s">
         <v>388</v>
       </c>
@@ -4757,7 +4825,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>394</v>
       </c>
@@ -4777,7 +4845,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>400</v>
       </c>
@@ -4788,7 +4856,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>403</v>
       </c>
@@ -4799,7 +4867,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>406</v>
       </c>
@@ -4810,10 +4878,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="16" t="s">
         <v>409</v>
       </c>
@@ -4824,7 +4892,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="17" t="s">
         <v>6</v>
       </c>
@@ -4835,7 +4903,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="17" t="s">
         <v>414</v>
       </c>
@@ -4846,7 +4914,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="17" t="s">
         <v>417</v>
       </c>
@@ -4857,7 +4925,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="17" t="s">
         <v>420</v>
       </c>
@@ -4868,7 +4936,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="18" t="s">
         <v>423</v>
       </c>
@@ -4879,7 +4947,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="19" t="s">
         <v>426</v>
       </c>
@@ -4890,7 +4958,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
         <v>429</v>
       </c>
@@ -4901,7 +4969,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
         <v>432</v>
       </c>
@@ -4912,15 +4980,15 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="12"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="12"/>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>435</v>
       </c>
@@ -4931,7 +4999,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>438</v>
       </c>
@@ -4942,7 +5010,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -4953,7 +5021,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>444</v>
       </c>
@@ -4964,7 +5032,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>447</v>
       </c>
@@ -4975,7 +5043,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>450</v>
       </c>
@@ -4986,7 +5054,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
         <v>453</v>
       </c>
@@ -4997,11 +5065,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="20"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="16" t="s">
         <v>456</v>
       </c>
@@ -5012,7 +5080,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="16" t="s">
         <v>459</v>
       </c>
@@ -5023,7 +5091,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="16" t="s">
         <v>462</v>
       </c>
@@ -5034,7 +5102,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="16" t="s">
         <v>465</v>
       </c>
@@ -5045,7 +5113,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="16" t="s">
         <v>468</v>
       </c>
@@ -5056,7 +5124,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="s">
         <v>471</v>
       </c>
@@ -5067,7 +5135,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="16" t="s">
         <v>474</v>
       </c>
@@ -5078,7 +5146,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="16" t="s">
         <v>477</v>
       </c>
@@ -5089,7 +5157,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="s">
         <v>480</v>
       </c>
@@ -5100,7 +5168,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="16" t="s">
         <v>483</v>
       </c>
@@ -5111,7 +5179,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="16" t="s">
         <v>486</v>
       </c>
@@ -5122,7 +5190,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="16" t="s">
         <v>489</v>
       </c>
@@ -5133,7 +5201,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
         <v>843</v>
       </c>
@@ -5141,7 +5209,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="20" t="s">
         <v>845</v>
       </c>
@@ -5149,15 +5217,15 @@
         <v>846</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="20" t="s">
+        <v>849</v>
+      </c>
+      <c r="B162" t="s">
         <v>850</v>
       </c>
-      <c r="B162" t="s">
+      <c r="F162" t="s">
         <v>851</v>
-      </c>
-      <c r="F162" t="s">
-        <v>852</v>
       </c>
     </row>
   </sheetData>
@@ -5175,18 +5243,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" customWidth="1"/>
-    <col min="2" max="2" width="41.77734375" customWidth="1"/>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.77734375" customWidth="1"/>
-    <col min="6" max="6" width="56.21875" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="56.1796875" style="21" customWidth="1"/>
+    <col min="7" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5206,7 +5274,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -5226,7 +5294,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5246,7 +5314,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>533</v>
       </c>
@@ -5266,7 +5334,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>539</v>
       </c>
@@ -5286,7 +5354,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5306,7 +5374,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5326,7 +5394,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>557</v>
       </c>
@@ -5346,7 +5414,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>563</v>
       </c>
@@ -5366,7 +5434,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>569</v>
       </c>
@@ -5386,7 +5454,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>575</v>
       </c>
@@ -5406,7 +5474,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -5426,7 +5494,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>584</v>
       </c>
@@ -5446,7 +5514,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -5466,7 +5534,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>596</v>
       </c>
@@ -5486,7 +5554,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>602</v>
       </c>
@@ -5506,7 +5574,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>608</v>
       </c>
@@ -5526,7 +5594,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>614</v>
       </c>
@@ -5546,7 +5614,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>620</v>
       </c>
@@ -5566,7 +5634,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>626</v>
       </c>
@@ -5586,7 +5654,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>632</v>
       </c>
@@ -5606,7 +5674,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -5626,7 +5694,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>644</v>
       </c>
@@ -5646,7 +5714,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>650</v>
       </c>
@@ -5666,7 +5734,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>656</v>
       </c>
@@ -5686,7 +5754,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>661</v>
       </c>
@@ -5706,7 +5774,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>667</v>
       </c>
@@ -5726,7 +5794,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>673</v>
       </c>
@@ -5740,7 +5808,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>676</v>
       </c>
@@ -5754,7 +5822,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -5774,7 +5842,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>685</v>
       </c>
@@ -5794,12 +5862,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>691</v>
       </c>
@@ -5819,7 +5887,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>697</v>
       </c>
@@ -5839,7 +5907,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>703</v>
       </c>
@@ -5859,7 +5927,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="185.4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="176" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>709</v>
       </c>
@@ -5873,7 +5941,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>711</v>
       </c>
@@ -5893,7 +5961,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>717</v>
       </c>
@@ -5913,7 +5981,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -5933,7 +6001,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>729</v>
       </c>
@@ -5953,7 +6021,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>735</v>
       </c>
@@ -5973,7 +6041,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -5993,7 +6061,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -6013,7 +6081,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>751</v>
       </c>
@@ -6033,7 +6101,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>756</v>
       </c>
@@ -6053,7 +6121,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>762</v>
       </c>
@@ -6073,7 +6141,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>768</v>
       </c>
@@ -6093,7 +6161,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>774</v>
       </c>
@@ -6113,7 +6181,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>780</v>
       </c>
@@ -6133,7 +6201,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>785</v>
       </c>
@@ -6153,7 +6221,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>790</v>
       </c>
@@ -6173,7 +6241,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>795</v>
       </c>
@@ -6193,7 +6261,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>796</v>
       </c>
@@ -6213,7 +6281,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>802</v>
       </c>
@@ -6233,7 +6301,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>804</v>
       </c>
@@ -6248,7 +6316,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>806</v>
       </c>
@@ -6263,7 +6331,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>810</v>
       </c>
@@ -6278,7 +6346,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>814</v>
       </c>
@@ -6291,7 +6359,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>817</v>
       </c>
@@ -6304,7 +6372,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>820</v>
       </c>
@@ -6331,15 +6399,15 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="7" width="8.77734375" customWidth="1"/>
-    <col min="8" max="8" width="26.5546875" customWidth="1"/>
-    <col min="9" max="9" width="26.21875" customWidth="1"/>
-    <col min="10" max="12" width="21.77734375" customWidth="1"/>
-    <col min="13" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="7" width="8.81640625" customWidth="1"/>
+    <col min="8" max="8" width="26.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="10" max="12" width="21.81640625" customWidth="1"/>
+    <col min="13" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6436,7 +6504,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -6600,18 +6668,18 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="26.77734375" customWidth="1"/>
-    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -6652,10 +6720,32 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>852</v>
+      </c>
+      <c r="C4" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>853</v>
+      </c>
+      <c r="C5" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>856</v>
+      </c>
+      <c r="C6" t="s">
         <v>848</v>
-      </c>
-      <c r="C4" t="s">
-        <v>849</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Intermediate check-in for populating dept and PAM
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="867">
   <si>
     <t>comments</t>
   </si>
@@ -2643,6 +2643,21 @@
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('colombia_search')</t>
+  </si>
+  <si>
+    <t>choose_dept</t>
+  </si>
+  <si>
+    <t>Choose Department</t>
+  </si>
+  <si>
+    <t>choose_pam</t>
+  </si>
+  <si>
+    <t>continue</t>
+  </si>
+  <si>
+    <t>Choose PAM</t>
   </si>
 </sst>
 </file>
@@ -3109,14 +3124,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" customWidth="1"/>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3124,7 +3139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3143,19 +3158,19 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38.1796875" customWidth="1"/>
-    <col min="3" max="3" width="8.81640625" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="14.81640625" customWidth="1"/>
-    <col min="7" max="8" width="30.81640625" customWidth="1"/>
-    <col min="9" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="8" width="30.85546875" customWidth="1"/>
+    <col min="9" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3182,7 +3197,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -3191,7 +3206,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -3202,13 +3217,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -3219,23 +3234,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>841</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="23" t="s">
         <v>842</v>
@@ -3247,20 +3262,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="23" t="s">
         <v>25</v>
@@ -3272,20 +3287,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>852</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="23" t="s">
         <v>847</v>
@@ -3297,20 +3312,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>853</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="23" t="s">
         <v>854</v>
@@ -3322,20 +3337,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>856</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3"/>
       <c r="B21" s="23" t="s">
         <v>857</v>
@@ -3347,20 +3362,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>859</v>
       </c>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3"/>
       <c r="B24" s="23" t="s">
         <v>861</v>
@@ -3372,7 +3387,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -3387,23 +3402,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G166"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G160" sqref="G160"/>
+    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.1796875" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" customWidth="1"/>
-    <col min="3" max="3" width="62.1796875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.1796875" style="4" customWidth="1"/>
-    <col min="6" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
+    <col min="3" max="3" width="62.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
+    <col min="6" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -3423,7 +3438,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3443,7 +3458,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3463,7 +3478,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3475,7 +3490,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3496,7 +3511,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3507,7 +3522,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -3518,17 +3533,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3548,7 +3563,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3568,7 +3583,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3588,7 +3603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3608,7 +3623,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3619,7 +3634,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -3630,7 +3645,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3641,7 +3656,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -3652,7 +3667,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -3672,7 +3687,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -3683,7 +3698,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>86</v>
       </c>
@@ -3694,17 +3709,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3724,7 +3739,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -3744,7 +3759,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -3755,7 +3770,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -3766,7 +3781,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -3786,7 +3801,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -3806,15 +3821,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3834,7 +3849,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3854,7 +3869,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3874,7 +3889,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -3885,7 +3900,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3896,7 +3911,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3907,17 +3922,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3938,7 +3953,7 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3958,7 +3973,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3969,7 +3984,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -3980,7 +3995,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -4000,7 +4015,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -4020,7 +4035,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -4031,7 +4046,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -4042,7 +4057,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -4062,7 +4077,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -4073,7 +4088,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -4084,7 +4099,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -4095,7 +4110,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -4106,7 +4121,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -4117,7 +4132,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -4128,7 +4143,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -4139,7 +4154,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -4150,7 +4165,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -4161,7 +4176,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4172,7 +4187,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4183,7 +4198,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4194,16 +4209,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" s="3"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -4215,7 +4230,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>226</v>
       </c>
@@ -4226,15 +4241,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="12"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4245,7 +4260,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -4256,7 +4271,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -4267,15 +4282,15 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -4295,7 +4310,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>244</v>
       </c>
@@ -4306,7 +4321,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="35" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -4326,7 +4341,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>253</v>
       </c>
@@ -4337,7 +4352,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>256</v>
       </c>
@@ -4348,7 +4363,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>259</v>
       </c>
@@ -4359,7 +4374,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -4379,7 +4394,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>268</v>
       </c>
@@ -4399,10 +4414,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>274</v>
       </c>
@@ -4413,7 +4428,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>277</v>
       </c>
@@ -4424,7 +4439,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>280</v>
       </c>
@@ -4444,7 +4459,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>286</v>
       </c>
@@ -4464,13 +4479,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="12" t="s">
         <v>292</v>
       </c>
@@ -4481,7 +4496,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>295</v>
       </c>
@@ -4492,7 +4507,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>298</v>
       </c>
@@ -4503,7 +4518,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>301</v>
       </c>
@@ -4514,7 +4529,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
         <v>304</v>
       </c>
@@ -4525,13 +4540,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>307</v>
       </c>
@@ -4542,7 +4557,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>310</v>
       </c>
@@ -4553,7 +4568,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -4564,7 +4579,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
         <v>316</v>
       </c>
@@ -4575,7 +4590,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>319</v>
       </c>
@@ -4586,7 +4601,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
         <v>322</v>
       </c>
@@ -4597,7 +4612,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>325</v>
       </c>
@@ -4608,7 +4623,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
         <v>328</v>
       </c>
@@ -4619,7 +4634,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>331</v>
       </c>
@@ -4630,14 +4645,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4648,7 +4663,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4659,7 +4674,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>340</v>
       </c>
@@ -4670,7 +4685,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>343</v>
       </c>
@@ -4681,7 +4696,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -4692,7 +4707,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -4703,10 +4718,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="16" t="s">
         <v>352</v>
       </c>
@@ -4717,7 +4732,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="16" t="s">
         <v>355</v>
       </c>
@@ -4728,7 +4743,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="16" t="s">
         <v>358</v>
       </c>
@@ -4739,7 +4754,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="16" t="s">
         <v>361</v>
       </c>
@@ -4750,10 +4765,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
         <v>364</v>
       </c>
@@ -4764,7 +4779,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="16" t="s">
         <v>367</v>
       </c>
@@ -4775,7 +4790,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="16" t="s">
         <v>370</v>
       </c>
@@ -4786,7 +4801,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="16" t="s">
         <v>373</v>
       </c>
@@ -4797,7 +4812,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="16" t="s">
         <v>376</v>
       </c>
@@ -4808,7 +4823,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="16" t="s">
         <v>379</v>
       </c>
@@ -4819,7 +4834,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="16" t="s">
         <v>382</v>
       </c>
@@ -4839,7 +4854,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="16" t="s">
         <v>388</v>
       </c>
@@ -4859,7 +4874,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="16" t="s">
         <v>394</v>
       </c>
@@ -4879,7 +4894,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="16" t="s">
         <v>400</v>
       </c>
@@ -4890,7 +4905,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="16" t="s">
         <v>403</v>
       </c>
@@ -4901,7 +4916,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>406</v>
       </c>
@@ -4912,10 +4927,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="16" t="s">
         <v>409</v>
       </c>
@@ -4926,7 +4941,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
         <v>6</v>
       </c>
@@ -4937,7 +4952,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
         <v>414</v>
       </c>
@@ -4948,7 +4963,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="17" t="s">
         <v>417</v>
       </c>
@@ -4959,7 +4974,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="17" t="s">
         <v>420</v>
       </c>
@@ -4970,7 +4985,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="18" t="s">
         <v>423</v>
       </c>
@@ -4981,7 +4996,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="19" t="s">
         <v>426</v>
       </c>
@@ -4992,7 +5007,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="12" t="s">
         <v>429</v>
       </c>
@@ -5003,7 +5018,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>432</v>
       </c>
@@ -5014,15 +5029,15 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" s="12"/>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>435</v>
       </c>
@@ -5033,7 +5048,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>438</v>
       </c>
@@ -5044,7 +5059,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -5055,7 +5070,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>444</v>
       </c>
@@ -5066,7 +5081,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>447</v>
       </c>
@@ -5077,7 +5092,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>450</v>
       </c>
@@ -5088,7 +5103,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="20" t="s">
         <v>453</v>
       </c>
@@ -5099,11 +5114,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="20"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" s="16" t="s">
         <v>456</v>
       </c>
@@ -5114,7 +5129,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" s="16" t="s">
         <v>459</v>
       </c>
@@ -5125,7 +5140,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" s="16" t="s">
         <v>462</v>
       </c>
@@ -5136,7 +5151,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" s="16" t="s">
         <v>465</v>
       </c>
@@ -5147,7 +5162,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" s="16" t="s">
         <v>468</v>
       </c>
@@ -5158,7 +5173,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" s="16" t="s">
         <v>471</v>
       </c>
@@ -5169,7 +5184,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" s="16" t="s">
         <v>474</v>
       </c>
@@ -5180,7 +5195,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" s="16" t="s">
         <v>477</v>
       </c>
@@ -5191,7 +5206,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" s="16" t="s">
         <v>480</v>
       </c>
@@ -5202,7 +5217,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="16" t="s">
         <v>483</v>
       </c>
@@ -5213,7 +5228,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" s="16" t="s">
         <v>486</v>
       </c>
@@ -5224,7 +5239,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" s="16" t="s">
         <v>489</v>
       </c>
@@ -5235,7 +5250,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" s="20" t="s">
         <v>843</v>
       </c>
@@ -5243,7 +5258,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" s="20" t="s">
         <v>845</v>
       </c>
@@ -5251,7 +5266,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="s">
         <v>849</v>
       </c>
@@ -5260,6 +5275,30 @@
       </c>
       <c r="F162" t="s">
         <v>851</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" s="12" t="s">
+        <v>862</v>
+      </c>
+      <c r="B164" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A165" s="12" t="s">
+        <v>864</v>
+      </c>
+      <c r="B165" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A166" s="12" t="s">
+        <v>865</v>
+      </c>
+      <c r="B166" t="s">
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -5277,18 +5316,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.453125" customWidth="1"/>
-    <col min="2" max="2" width="41.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" customWidth="1"/>
-    <col min="6" max="6" width="56.1796875" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="56.140625" style="21" customWidth="1"/>
+    <col min="7" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5308,7 +5347,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -5328,7 +5367,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5348,7 +5387,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>533</v>
       </c>
@@ -5368,7 +5407,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>539</v>
       </c>
@@ -5388,7 +5427,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5408,7 +5447,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5428,7 +5467,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>557</v>
       </c>
@@ -5448,7 +5487,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>563</v>
       </c>
@@ -5468,7 +5507,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>569</v>
       </c>
@@ -5488,7 +5527,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>575</v>
       </c>
@@ -5508,7 +5547,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -5528,7 +5567,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>584</v>
       </c>
@@ -5548,7 +5587,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -5568,7 +5607,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>596</v>
       </c>
@@ -5588,7 +5627,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>602</v>
       </c>
@@ -5608,7 +5647,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>608</v>
       </c>
@@ -5628,7 +5667,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>614</v>
       </c>
@@ -5648,7 +5687,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>620</v>
       </c>
@@ -5668,7 +5707,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>626</v>
       </c>
@@ -5688,7 +5727,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>632</v>
       </c>
@@ -5708,7 +5747,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -5728,7 +5767,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>644</v>
       </c>
@@ -5748,7 +5787,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>650</v>
       </c>
@@ -5768,7 +5807,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>656</v>
       </c>
@@ -5788,7 +5827,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>661</v>
       </c>
@@ -5808,7 +5847,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>667</v>
       </c>
@@ -5828,7 +5867,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>673</v>
       </c>
@@ -5842,7 +5881,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>676</v>
       </c>
@@ -5856,7 +5895,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -5876,7 +5915,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>685</v>
       </c>
@@ -5896,12 +5935,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>691</v>
       </c>
@@ -5921,7 +5960,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>697</v>
       </c>
@@ -5941,7 +5980,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>703</v>
       </c>
@@ -5961,7 +6000,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="176" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" ht="179.25" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>709</v>
       </c>
@@ -5975,7 +6014,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>711</v>
       </c>
@@ -5995,7 +6034,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>717</v>
       </c>
@@ -6015,7 +6054,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -6035,7 +6074,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>729</v>
       </c>
@@ -6055,7 +6094,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>735</v>
       </c>
@@ -6075,7 +6114,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -6095,7 +6134,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -6115,7 +6154,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>751</v>
       </c>
@@ -6135,7 +6174,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>756</v>
       </c>
@@ -6155,7 +6194,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>762</v>
       </c>
@@ -6175,7 +6214,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>768</v>
       </c>
@@ -6195,7 +6234,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>774</v>
       </c>
@@ -6215,7 +6254,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>780</v>
       </c>
@@ -6235,7 +6274,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>785</v>
       </c>
@@ -6255,7 +6294,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>790</v>
       </c>
@@ -6275,7 +6314,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>795</v>
       </c>
@@ -6295,7 +6334,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>796</v>
       </c>
@@ -6315,7 +6354,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>802</v>
       </c>
@@ -6335,7 +6374,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>804</v>
       </c>
@@ -6350,7 +6389,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>806</v>
       </c>
@@ -6365,7 +6404,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>810</v>
       </c>
@@ -6380,7 +6419,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>814</v>
       </c>
@@ -6393,7 +6432,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>817</v>
       </c>
@@ -6406,7 +6445,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>820</v>
       </c>
@@ -6429,22 +6468,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.54296875" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="7" width="8.81640625" customWidth="1"/>
-    <col min="8" max="8" width="26.54296875" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
-    <col min="10" max="12" width="21.81640625" customWidth="1"/>
-    <col min="13" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="26.5703125" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" customWidth="1"/>
+    <col min="10" max="12" width="21.85546875" customWidth="1"/>
+    <col min="13" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6488,7 +6527,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>500</v>
       </c>
@@ -6506,7 +6545,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>502</v>
       </c>
@@ -6527,7 +6566,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>504</v>
       </c>
@@ -6538,7 +6577,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -6565,7 +6604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>829</v>
       </c>
@@ -6585,7 +6624,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>828</v>
       </c>
@@ -6611,7 +6650,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>830</v>
       </c>
@@ -6637,7 +6676,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>831</v>
       </c>
@@ -6663,7 +6702,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>832</v>
       </c>
@@ -6689,7 +6728,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>516</v>
       </c>
@@ -6708,15 +6747,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" customWidth="1"/>
-    <col min="3" max="3" width="26.81640625" customWidth="1"/>
-    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" customWidth="1"/>
+    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>517</v>
       </c>
@@ -6727,7 +6766,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -6738,7 +6777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -6749,7 +6788,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -6760,7 +6799,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -6771,7 +6810,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -6782,7 +6821,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add error dialogs with translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="867">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="871">
   <si>
     <t>comments</t>
   </si>
@@ -2658,6 +2658,18 @@
   </si>
   <si>
     <t>Choose PAM</t>
+  </si>
+  <si>
+    <t>beneficiary_not_entitled</t>
+  </si>
+  <si>
+    <t>no_id_found</t>
+  </si>
+  <si>
+    <t>No id found</t>
+  </si>
+  <si>
+    <t>Beneficiary is not entitled to any more of these items</t>
   </si>
 </sst>
 </file>
@@ -3402,10 +3414,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G166"/>
+  <dimension ref="A1:G168"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B165" sqref="B165"/>
+      <selection activeCell="A167" sqref="A167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5301,10 +5313,26 @@
         <v>570</v>
       </c>
     </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A167" s="12" t="s">
+        <v>867</v>
+      </c>
+      <c r="B167" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A168" s="12" t="s">
+        <v>868</v>
+      </c>
+      <c r="B168" t="s">
+        <v>869</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F103"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add in translations for errors
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8205" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8210" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="965" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="877">
   <si>
     <t>comments</t>
   </si>
@@ -2670,6 +2670,24 @@
   </si>
   <si>
     <t>Beneficiary is not entitled to any more of these items</t>
+  </si>
+  <si>
+    <t>Error while storing department and PAM</t>
+  </si>
+  <si>
+    <t>error_while_storing_department_and_PAM</t>
+  </si>
+  <si>
+    <t>error_while_initializing</t>
+  </si>
+  <si>
+    <t>Error while initializing</t>
+  </si>
+  <si>
+    <t>Error while retrieving department and PAM</t>
+  </si>
+  <si>
+    <t>error_while_retrieving_department_and_PAM</t>
   </si>
 </sst>
 </file>
@@ -3136,14 +3154,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3151,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -3170,19 +3188,19 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="7" max="8" width="30.85546875" customWidth="1"/>
-    <col min="9" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" customWidth="1"/>
+    <col min="3" max="3" width="8.81640625" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" customWidth="1"/>
+    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="8" width="30.81640625" customWidth="1"/>
+    <col min="9" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -3209,7 +3227,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -3218,7 +3236,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="17.850000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="17.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
         <v>12</v>
       </c>
@@ -3229,13 +3247,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>16</v>
       </c>
@@ -3246,23 +3264,23 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>841</v>
       </c>
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="23" t="s">
         <v>842</v>
@@ -3274,20 +3292,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="23" t="s">
         <v>25</v>
@@ -3299,20 +3317,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>852</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="23" t="s">
         <v>847</v>
@@ -3324,20 +3342,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>853</v>
       </c>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="23" t="s">
         <v>854</v>
@@ -3349,20 +3367,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>856</v>
       </c>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="23" t="s">
         <v>857</v>
@@ -3374,20 +3392,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>859</v>
       </c>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="23" t="s">
         <v>861</v>
@@ -3399,7 +3417,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" t="s">
@@ -3414,23 +3432,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G168"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A167" sqref="A167"/>
+      <selection activeCell="A172" sqref="A172:XFD172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" customWidth="1"/>
-    <col min="3" max="3" width="62.140625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" style="4" customWidth="1"/>
-    <col min="6" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.36328125" customWidth="1"/>
+    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="3" max="3" width="62.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" style="4" customWidth="1"/>
+    <col min="6" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -3450,7 +3468,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -3470,7 +3488,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -3490,7 +3508,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -3502,7 +3520,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -3523,7 +3541,7 @@
       </c>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>48</v>
       </c>
@@ -3534,7 +3552,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>51</v>
       </c>
@@ -3545,17 +3563,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="F8" s="13"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="F9" s="13"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -3575,7 +3593,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -3595,7 +3613,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>63</v>
       </c>
@@ -3615,7 +3633,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -3635,7 +3653,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>70</v>
       </c>
@@ -3646,7 +3664,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>72</v>
       </c>
@@ -3657,7 +3675,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>74</v>
       </c>
@@ -3668,7 +3686,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>76</v>
       </c>
@@ -3679,7 +3697,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -3699,7 +3717,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
         <v>83</v>
       </c>
@@ -3710,7 +3728,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
         <v>86</v>
       </c>
@@ -3721,17 +3739,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="F21" s="13"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="F22" s="13"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>89</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -3771,7 +3789,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -3782,7 +3800,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>104</v>
       </c>
@@ -3793,7 +3811,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>107</v>
       </c>
@@ -3813,7 +3831,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>113</v>
       </c>
@@ -3833,15 +3851,15 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="F30" s="13"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>119</v>
       </c>
@@ -3861,7 +3879,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>125</v>
       </c>
@@ -3881,7 +3899,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>131</v>
       </c>
@@ -3901,7 +3919,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>137</v>
       </c>
@@ -3912,7 +3930,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3923,7 +3941,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>143</v>
       </c>
@@ -3934,17 +3952,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="F37" s="7"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="F38" s="7"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3965,7 +3983,7 @@
       </c>
       <c r="G39" s="14"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3985,7 +4003,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -3996,7 +4014,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>161</v>
       </c>
@@ -4007,7 +4025,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>164</v>
       </c>
@@ -4027,7 +4045,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>170</v>
       </c>
@@ -4047,7 +4065,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>176</v>
       </c>
@@ -4058,7 +4076,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -4069,7 +4087,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -4089,7 +4107,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
         <v>187</v>
       </c>
@@ -4100,7 +4118,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="12" t="s">
         <v>190</v>
       </c>
@@ -4111,7 +4129,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>193</v>
       </c>
@@ -4122,7 +4140,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -4133,7 +4151,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>199</v>
       </c>
@@ -4144,7 +4162,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -4155,7 +4173,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>205</v>
       </c>
@@ -4166,7 +4184,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>208</v>
       </c>
@@ -4177,7 +4195,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>211</v>
       </c>
@@ -4188,7 +4206,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>214</v>
       </c>
@@ -4199,7 +4217,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>217</v>
       </c>
@@ -4210,7 +4228,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -4221,16 +4239,16 @@
         <v>222</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
       <c r="F60" s="7"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>223</v>
       </c>
@@ -4242,7 +4260,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
         <v>226</v>
       </c>
@@ -4253,15 +4271,15 @@
         <v>228</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="12"/>
       <c r="F64" s="7"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="12"/>
       <c r="F65" s="7"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>229</v>
       </c>
@@ -4272,7 +4290,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>232</v>
       </c>
@@ -4283,7 +4301,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>235</v>
       </c>
@@ -4294,15 +4312,15 @@
         <v>237</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F69" s="7"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="F70" s="7"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>238</v>
       </c>
@@ -4322,7 +4340,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>244</v>
       </c>
@@ -4333,7 +4351,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>247</v>
       </c>
@@ -4353,7 +4371,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="12" t="s">
         <v>253</v>
       </c>
@@ -4364,7 +4382,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="12" t="s">
         <v>256</v>
       </c>
@@ -4375,7 +4393,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="12" t="s">
         <v>259</v>
       </c>
@@ -4386,7 +4404,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>262</v>
       </c>
@@ -4406,7 +4424,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>268</v>
       </c>
@@ -4426,10 +4444,10 @@
         <v>273</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F79" s="7"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>274</v>
       </c>
@@ -4440,7 +4458,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>277</v>
       </c>
@@ -4451,7 +4469,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>280</v>
       </c>
@@ -4471,7 +4489,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>286</v>
       </c>
@@ -4491,13 +4509,13 @@
         <v>291</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F84" s="7"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F85" s="7"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="12" t="s">
         <v>292</v>
       </c>
@@ -4508,7 +4526,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="12" t="s">
         <v>295</v>
       </c>
@@ -4519,7 +4537,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="12" t="s">
         <v>298</v>
       </c>
@@ -4530,7 +4548,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="12" t="s">
         <v>301</v>
       </c>
@@ -4541,7 +4559,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="12" t="s">
         <v>304</v>
       </c>
@@ -4552,13 +4570,13 @@
         <v>306</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F91" s="7"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F92" s="7"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="12" t="s">
         <v>307</v>
       </c>
@@ -4569,7 +4587,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="12" t="s">
         <v>310</v>
       </c>
@@ -4580,7 +4598,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>313</v>
       </c>
@@ -4591,7 +4609,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="12" t="s">
         <v>316</v>
       </c>
@@ -4602,7 +4620,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="12" t="s">
         <v>319</v>
       </c>
@@ -4613,7 +4631,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="12" t="s">
         <v>322</v>
       </c>
@@ -4624,7 +4642,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="12" t="s">
         <v>325</v>
       </c>
@@ -4635,7 +4653,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="12" t="s">
         <v>328</v>
       </c>
@@ -4646,7 +4664,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="12" t="s">
         <v>331</v>
       </c>
@@ -4657,14 +4675,14 @@
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="12"/>
       <c r="F102" s="7"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F103" s="7"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>334</v>
       </c>
@@ -4675,7 +4693,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>337</v>
       </c>
@@ -4686,7 +4704,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>340</v>
       </c>
@@ -4697,7 +4715,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>343</v>
       </c>
@@ -4708,7 +4726,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -4719,7 +4737,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>349</v>
       </c>
@@ -4730,10 +4748,10 @@
         <v>351</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F110" s="7"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="16" t="s">
         <v>352</v>
       </c>
@@ -4744,7 +4762,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="16" t="s">
         <v>355</v>
       </c>
@@ -4755,7 +4773,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="16" t="s">
         <v>358</v>
       </c>
@@ -4766,7 +4784,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="16" t="s">
         <v>361</v>
       </c>
@@ -4777,10 +4795,10 @@
         <v>363</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F115" s="7"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="16" t="s">
         <v>364</v>
       </c>
@@ -4791,7 +4809,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="16" t="s">
         <v>367</v>
       </c>
@@ -4802,7 +4820,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="16" t="s">
         <v>370</v>
       </c>
@@ -4813,7 +4831,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="16" t="s">
         <v>373</v>
       </c>
@@ -4824,7 +4842,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="16" t="s">
         <v>376</v>
       </c>
@@ -4835,7 +4853,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="16" t="s">
         <v>379</v>
       </c>
@@ -4846,7 +4864,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="16" t="s">
         <v>382</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="16" t="s">
         <v>388</v>
       </c>
@@ -4886,7 +4904,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="16" t="s">
         <v>394</v>
       </c>
@@ -4906,7 +4924,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="16" t="s">
         <v>400</v>
       </c>
@@ -4917,7 +4935,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="16" t="s">
         <v>403</v>
       </c>
@@ -4928,7 +4946,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>406</v>
       </c>
@@ -4939,10 +4957,10 @@
         <v>408</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="F128" s="7"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="16" t="s">
         <v>409</v>
       </c>
@@ -4953,7 +4971,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="17" t="s">
         <v>6</v>
       </c>
@@ -4964,7 +4982,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="17" t="s">
         <v>414</v>
       </c>
@@ -4975,7 +4993,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="17" t="s">
         <v>417</v>
       </c>
@@ -4986,7 +5004,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="17" t="s">
         <v>420</v>
       </c>
@@ -4997,7 +5015,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="18" t="s">
         <v>423</v>
       </c>
@@ -5008,7 +5026,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="19" t="s">
         <v>426</v>
       </c>
@@ -5019,7 +5037,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="12" t="s">
         <v>429</v>
       </c>
@@ -5030,7 +5048,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="12" t="s">
         <v>432</v>
       </c>
@@ -5041,15 +5059,15 @@
         <v>434</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="12"/>
       <c r="F138" s="7"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="12"/>
       <c r="F139" s="7"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>435</v>
       </c>
@@ -5060,7 +5078,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>438</v>
       </c>
@@ -5071,7 +5089,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>441</v>
       </c>
@@ -5082,7 +5100,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>444</v>
       </c>
@@ -5093,7 +5111,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>447</v>
       </c>
@@ -5104,7 +5122,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>450</v>
       </c>
@@ -5115,7 +5133,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="20" t="s">
         <v>453</v>
       </c>
@@ -5126,11 +5144,11 @@
         <v>455</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="20"/>
       <c r="F147" s="7"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="16" t="s">
         <v>456</v>
       </c>
@@ -5141,7 +5159,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="16" t="s">
         <v>459</v>
       </c>
@@ -5152,7 +5170,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="16" t="s">
         <v>462</v>
       </c>
@@ -5163,7 +5181,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="16" t="s">
         <v>465</v>
       </c>
@@ -5174,7 +5192,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="16" t="s">
         <v>468</v>
       </c>
@@ -5185,7 +5203,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="16" t="s">
         <v>471</v>
       </c>
@@ -5196,7 +5214,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="16" t="s">
         <v>474</v>
       </c>
@@ -5207,7 +5225,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="16" t="s">
         <v>477</v>
       </c>
@@ -5218,7 +5236,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="16" t="s">
         <v>480</v>
       </c>
@@ -5229,7 +5247,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="16" t="s">
         <v>483</v>
       </c>
@@ -5240,7 +5258,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="16" t="s">
         <v>486</v>
       </c>
@@ -5251,7 +5269,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="16" t="s">
         <v>489</v>
       </c>
@@ -5262,7 +5280,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="20" t="s">
         <v>843</v>
       </c>
@@ -5270,7 +5288,7 @@
         <v>844</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="20" t="s">
         <v>845</v>
       </c>
@@ -5278,7 +5296,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="20" t="s">
         <v>849</v>
       </c>
@@ -5289,7 +5307,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="12" t="s">
         <v>862</v>
       </c>
@@ -5297,7 +5315,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="12" t="s">
         <v>864</v>
       </c>
@@ -5305,7 +5323,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="12" t="s">
         <v>865</v>
       </c>
@@ -5313,7 +5331,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="12" t="s">
         <v>867</v>
       </c>
@@ -5321,12 +5339,36 @@
         <v>870</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="12" t="s">
         <v>868</v>
       </c>
       <c r="B168" t="s">
         <v>869</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A169" s="12" t="s">
+        <v>872</v>
+      </c>
+      <c r="B169" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A170" s="12" t="s">
+        <v>873</v>
+      </c>
+      <c r="B170" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A171" s="12" t="s">
+        <v>876</v>
+      </c>
+      <c r="B171" t="s">
+        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -5344,18 +5386,18 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.42578125" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" customWidth="1"/>
-    <col min="6" max="6" width="56.140625" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="19.54296875" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" customWidth="1"/>
+    <col min="6" max="6" width="56.1796875" style="21" customWidth="1"/>
+    <col min="7" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -5375,7 +5417,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>521</v>
       </c>
@@ -5395,7 +5437,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>527</v>
       </c>
@@ -5415,7 +5457,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>533</v>
       </c>
@@ -5435,7 +5477,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>539</v>
       </c>
@@ -5455,7 +5497,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>545</v>
       </c>
@@ -5475,7 +5517,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>551</v>
       </c>
@@ -5495,7 +5537,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>557</v>
       </c>
@@ -5515,7 +5557,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>563</v>
       </c>
@@ -5535,7 +5577,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>569</v>
       </c>
@@ -5555,7 +5597,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>575</v>
       </c>
@@ -5575,7 +5617,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="14.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>581</v>
       </c>
@@ -5595,7 +5637,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>584</v>
       </c>
@@ -5615,7 +5657,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>590</v>
       </c>
@@ -5635,7 +5677,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>596</v>
       </c>
@@ -5655,7 +5697,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>602</v>
       </c>
@@ -5675,7 +5717,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>608</v>
       </c>
@@ -5695,7 +5737,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>614</v>
       </c>
@@ -5715,7 +5757,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>620</v>
       </c>
@@ -5735,7 +5777,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>626</v>
       </c>
@@ -5755,7 +5797,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>632</v>
       </c>
@@ -5775,7 +5817,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>638</v>
       </c>
@@ -5795,7 +5837,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>644</v>
       </c>
@@ -5815,7 +5857,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>650</v>
       </c>
@@ -5835,7 +5877,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>656</v>
       </c>
@@ -5855,7 +5897,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>661</v>
       </c>
@@ -5875,7 +5917,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>667</v>
       </c>
@@ -5895,7 +5937,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="28.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>673</v>
       </c>
@@ -5909,7 +5951,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>676</v>
       </c>
@@ -5923,7 +5965,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>679</v>
       </c>
@@ -5943,7 +5985,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>685</v>
       </c>
@@ -5963,12 +6005,12 @@
         <v>690</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>691</v>
       </c>
@@ -5988,7 +6030,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>697</v>
       </c>
@@ -6008,7 +6050,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>703</v>
       </c>
@@ -6028,7 +6070,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="179.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="176" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>709</v>
       </c>
@@ -6042,7 +6084,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>711</v>
       </c>
@@ -6062,7 +6104,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>717</v>
       </c>
@@ -6082,7 +6124,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>723</v>
       </c>
@@ -6102,7 +6144,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>729</v>
       </c>
@@ -6122,7 +6164,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>735</v>
       </c>
@@ -6142,7 +6184,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>741</v>
       </c>
@@ -6162,7 +6204,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>747</v>
       </c>
@@ -6182,7 +6224,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>751</v>
       </c>
@@ -6202,7 +6244,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>756</v>
       </c>
@@ -6222,7 +6264,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>762</v>
       </c>
@@ -6242,7 +6284,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>768</v>
       </c>
@@ -6262,7 +6304,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>774</v>
       </c>
@@ -6282,7 +6324,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>780</v>
       </c>
@@ -6302,7 +6344,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="13.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>785</v>
       </c>
@@ -6322,7 +6364,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>790</v>
       </c>
@@ -6342,7 +6384,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>795</v>
       </c>
@@ -6362,7 +6404,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>796</v>
       </c>
@@ -6382,7 +6424,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>802</v>
       </c>
@@ -6402,7 +6444,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>804</v>
       </c>
@@ -6417,7 +6459,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>806</v>
       </c>
@@ -6432,7 +6474,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>810</v>
       </c>
@@ -6447,7 +6489,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>814</v>
       </c>
@@ -6460,7 +6502,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>817</v>
       </c>
@@ -6473,7 +6515,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>820</v>
       </c>
@@ -6500,18 +6542,18 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="7" width="8.85546875" customWidth="1"/>
-    <col min="8" max="8" width="26.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" customWidth="1"/>
-    <col min="10" max="12" width="21.85546875" customWidth="1"/>
-    <col min="13" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.54296875" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="7" width="8.81640625" customWidth="1"/>
+    <col min="8" max="8" width="26.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="10" max="12" width="21.81640625" customWidth="1"/>
+    <col min="13" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>492</v>
       </c>
@@ -6555,7 +6597,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>500</v>
       </c>
@@ -6573,7 +6615,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>502</v>
       </c>
@@ -6594,7 +6636,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>504</v>
       </c>
@@ -6605,7 +6647,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>506</v>
       </c>
@@ -6632,7 +6674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>829</v>
       </c>
@@ -6652,7 +6694,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>828</v>
       </c>
@@ -6678,7 +6720,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>830</v>
       </c>
@@ -6704,7 +6746,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>831</v>
       </c>
@@ -6730,7 +6772,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>832</v>
       </c>
@@ -6756,7 +6798,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>516</v>
       </c>
@@ -6775,15 +6817,15 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.85546875" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" customWidth="1"/>
+    <col min="2" max="2" width="27.81640625" customWidth="1"/>
+    <col min="3" max="3" width="26.81640625" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>517</v>
       </c>
@@ -6794,7 +6836,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -6805,7 +6847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>13</v>
       </c>
@@ -6816,7 +6858,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -6827,7 +6869,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -6838,7 +6880,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -6849,7 +6891,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Add sentinel survey along with functionality to edit and view the survey
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\app-designer\app\config\assets\framework\forms\framework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clarice\cold-chain\cold-chain-app-designer\app\config\assets\framework\forms\framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
     <sheet name="framework_translations" sheetId="5" r:id="rId5"/>
     <sheet name="common_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913" calcMode="manual"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="637">
   <si>
     <t>comments</t>
   </si>
@@ -1995,12 +1995,30 @@
   <si>
     <t>Salida</t>
   </si>
+  <si>
+    <t>add_sentinel_survey</t>
+  </si>
+  <si>
+    <t>view_sentinel_survey</t>
+  </si>
+  <si>
+    <t>Add Sentinel Survey</t>
+  </si>
+  <si>
+    <t>View Sentinel Surveys</t>
+  </si>
+  <si>
+    <t>Añadir Encuesta Centinela</t>
+  </si>
+  <si>
+    <t>Ver encuestas de Centinela</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2043,6 +2061,17 @@
     <font>
       <sz val="10"/>
       <color rgb="FF212121"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2093,7 +2122,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2125,6 +2154,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2858,10 +2891,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4828,6 +4861,28 @@
       </c>
       <c r="C179" s="4" t="s">
         <v>541</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="13" t="s">
+        <v>631</v>
+      </c>
+      <c r="B180" s="12" t="s">
+        <v>633</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="13" t="s">
+        <v>632</v>
+      </c>
+      <c r="B181" s="12" t="s">
+        <v>634</v>
+      </c>
+      <c r="C181" s="14" t="s">
+        <v>636</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add indicators to framework for WHO testing
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16305" yWindow="5025" windowWidth="25605" windowHeight="16065" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="framework_translations" sheetId="5" r:id="rId5"/>
     <sheet name="common_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="652">
   <si>
     <t>comments</t>
   </si>
@@ -2012,6 +2012,51 @@
   </si>
   <si>
     <t>Ver encuestas de Centinela</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>opendatakit.getPlatformInfo().container == "Chrome"</t>
+  </si>
+  <si>
+    <t>user_branch</t>
+  </si>
+  <si>
+    <t>test_forms</t>
+  </si>
+  <si>
+    <t>Choose a test form (there are many)</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>This is the default form.</t>
+  </si>
+  <si>
+    <t>Set your url hash to #formPath=[relative path to form directory]/ to change forms.</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>exit section</t>
+  </si>
+  <si>
+    <t>external_link</t>
+  </si>
+  <si>
+    <t>Open form</t>
+  </si>
+  <si>
+    <t>indicators</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('indicators')</t>
+  </si>
+  <si>
+    <t>Indicators</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2167,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2158,6 +2203,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2529,14 +2584,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2544,7 +2599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2564,24 +2619,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="1025" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2608,94 +2663,149 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" t="s">
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="15" t="s">
+        <v>637</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>638</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="15" t="s">
+        <v>639</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>640</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>642</v>
+      </c>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:9" ht="41.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="G5" s="15" t="s">
+        <v>643</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>649</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18" t="s">
+        <v>650</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>647</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="15" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2715,15 +2825,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="6" width="24.7109375" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" customWidth="1"/>
-    <col min="8" max="1025" width="17.140625" customWidth="1"/>
+    <col min="1" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="6" width="24.7265625" customWidth="1"/>
+    <col min="7" max="7" width="41.1796875" customWidth="1"/>
+    <col min="8" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2749,7 +2859,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2761,7 +2871,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2776,7 +2886,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2787,7 +2897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2805,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2816,7 +2926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2827,7 +2937,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2837,9 +2947,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2853,21 +2963,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -2876,6 +2986,17 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>649</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>651</v>
       </c>
     </row>
   </sheetData>
@@ -2893,19 +3014,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A84" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.7109375" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="1025" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="49.7265625" customWidth="1"/>
+    <col min="2" max="2" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.26953125" customWidth="1"/>
+    <col min="4" max="1025" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -2916,7 +3037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -2927,7 +3048,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -2938,7 +3059,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -2949,7 +3070,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2960,7 +3081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -2971,7 +3092,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -2982,7 +3103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2993,7 +3114,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3004,7 +3125,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -3015,7 +3136,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3026,7 +3147,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3037,7 +3158,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -3048,7 +3169,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3059,7 +3180,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -3070,7 +3191,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -3081,7 +3202,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -3092,7 +3213,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3103,7 +3224,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -3114,7 +3235,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -3125,7 +3246,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -3136,7 +3257,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -3147,7 +3268,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3158,7 +3279,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -3169,7 +3290,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3180,7 +3301,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3191,7 +3312,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -3202,7 +3323,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3213,7 +3334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3224,7 +3345,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -3235,7 +3356,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3246,7 +3367,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -3257,7 +3378,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -3268,7 +3389,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3279,7 +3400,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="275" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3290,7 +3411,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -3301,7 +3422,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -3312,7 +3433,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -3323,7 +3444,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -3334,7 +3455,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3345,7 +3466,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>156</v>
       </c>
@@ -3356,7 +3477,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -3367,7 +3488,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -3378,7 +3499,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -3389,7 +3510,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3400,7 +3521,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -3411,7 +3532,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -3422,7 +3543,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -3433,7 +3554,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3444,7 +3565,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -3455,7 +3576,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -3466,7 +3587,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -3477,7 +3598,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>189</v>
       </c>
@@ -3488,7 +3609,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -3499,7 +3620,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -3510,7 +3631,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -3521,7 +3642,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>619</v>
       </c>
@@ -3532,7 +3653,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>621</v>
       </c>
@@ -3543,7 +3664,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>623</v>
       </c>
@@ -3554,7 +3675,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>616</v>
       </c>
@@ -3565,7 +3686,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>556</v>
       </c>
@@ -3576,7 +3697,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>558</v>
       </c>
@@ -3587,7 +3708,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -3598,7 +3719,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>201</v>
       </c>
@@ -3609,7 +3730,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>204</v>
       </c>
@@ -3620,7 +3741,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>207</v>
       </c>
@@ -3631,7 +3752,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>212</v>
       </c>
@@ -3642,7 +3763,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>213</v>
       </c>
@@ -3653,7 +3774,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>216</v>
       </c>
@@ -3664,7 +3785,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -3675,7 +3796,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -3686,7 +3807,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>224</v>
       </c>
@@ -3697,7 +3818,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>227</v>
       </c>
@@ -3708,7 +3829,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -3719,7 +3840,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -3730,7 +3851,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>236</v>
       </c>
@@ -3741,7 +3862,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -3752,7 +3873,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>242</v>
       </c>
@@ -3763,7 +3884,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>245</v>
       </c>
@@ -3774,7 +3895,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>248</v>
       </c>
@@ -3785,7 +3906,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -3796,7 +3917,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -3807,7 +3928,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>257</v>
       </c>
@@ -3818,7 +3939,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>260</v>
       </c>
@@ -3829,7 +3950,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>263</v>
       </c>
@@ -3840,7 +3961,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>265</v>
       </c>
@@ -3851,7 +3972,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -3862,7 +3983,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -3873,7 +3994,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -3884,7 +4005,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -3895,7 +4016,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -3906,7 +4027,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -3917,7 +4038,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -3928,7 +4049,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>289</v>
       </c>
@@ -3939,7 +4060,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>291</v>
       </c>
@@ -3950,7 +4071,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -3961,7 +4082,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -3972,7 +4093,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -3983,7 +4104,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -3994,7 +4115,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -4005,7 +4126,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>310</v>
       </c>
@@ -4016,7 +4137,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>313</v>
       </c>
@@ -4027,7 +4148,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -4038,7 +4159,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -4049,7 +4170,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>322</v>
       </c>
@@ -4060,7 +4181,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4071,7 +4192,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4082,7 +4203,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4093,7 +4214,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4104,7 +4225,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4115,7 +4236,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4126,7 +4247,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>343</v>
       </c>
@@ -4137,7 +4258,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>346</v>
       </c>
@@ -4148,7 +4269,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>349</v>
       </c>
@@ -4159,7 +4280,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>352</v>
       </c>
@@ -4170,7 +4291,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4181,7 +4302,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4192,7 +4313,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4203,7 +4324,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>364</v>
       </c>
@@ -4214,7 +4335,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>366</v>
       </c>
@@ -4225,7 +4346,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>370</v>
       </c>
@@ -4236,7 +4357,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4247,7 +4368,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -4258,7 +4379,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4269,7 +4390,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>382</v>
       </c>
@@ -4280,7 +4401,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>385</v>
       </c>
@@ -4291,7 +4412,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>388</v>
       </c>
@@ -4302,7 +4423,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -4313,7 +4434,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>394</v>
       </c>
@@ -4324,7 +4445,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>397</v>
       </c>
@@ -4335,7 +4456,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>400</v>
       </c>
@@ -4346,7 +4467,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>403</v>
       </c>
@@ -4357,7 +4478,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>406</v>
       </c>
@@ -4368,7 +4489,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>409</v>
       </c>
@@ -4379,7 +4500,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>412</v>
       </c>
@@ -4390,7 +4511,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>415</v>
       </c>
@@ -4401,7 +4522,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>418</v>
       </c>
@@ -4412,7 +4533,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>421</v>
       </c>
@@ -4423,7 +4544,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>424</v>
       </c>
@@ -4434,7 +4555,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>425</v>
       </c>
@@ -4445,7 +4566,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>428</v>
       </c>
@@ -4456,7 +4577,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>431</v>
       </c>
@@ -4467,7 +4588,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -4478,7 +4599,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -4489,7 +4610,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>440</v>
       </c>
@@ -4500,7 +4621,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>443</v>
       </c>
@@ -4511,7 +4632,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>446</v>
       </c>
@@ -4522,7 +4643,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>449</v>
       </c>
@@ -4533,7 +4654,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>452</v>
       </c>
@@ -4544,7 +4665,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>455</v>
       </c>
@@ -4555,7 +4676,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>458</v>
       </c>
@@ -4566,7 +4687,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>461</v>
       </c>
@@ -4577,7 +4698,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>464</v>
       </c>
@@ -4588,7 +4709,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>467</v>
       </c>
@@ -4599,7 +4720,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>470</v>
       </c>
@@ -4610,7 +4731,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>473</v>
       </c>
@@ -4621,7 +4742,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>476</v>
       </c>
@@ -4632,7 +4753,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>479</v>
       </c>
@@ -4643,7 +4764,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>482</v>
       </c>
@@ -4654,7 +4775,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>485</v>
       </c>
@@ -4665,7 +4786,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>488</v>
       </c>
@@ -4676,7 +4797,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>492</v>
       </c>
@@ -4687,7 +4808,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>494</v>
       </c>
@@ -4698,7 +4819,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>497</v>
       </c>
@@ -4709,7 +4830,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>500</v>
       </c>
@@ -4720,7 +4841,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>503</v>
       </c>
@@ -4731,7 +4852,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>506</v>
       </c>
@@ -4742,7 +4863,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>509</v>
       </c>
@@ -4753,7 +4874,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>512</v>
       </c>
@@ -4764,7 +4885,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>515</v>
       </c>
@@ -4775,7 +4896,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>518</v>
       </c>
@@ -4786,7 +4907,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>521</v>
       </c>
@@ -4797,7 +4918,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>524</v>
       </c>
@@ -4808,7 +4929,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>528</v>
       </c>
@@ -4819,7 +4940,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>531</v>
       </c>
@@ -4830,7 +4951,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>534</v>
       </c>
@@ -4841,7 +4962,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>537</v>
       </c>
@@ -4852,7 +4973,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>539</v>
       </c>
@@ -4863,7 +4984,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>631</v>
       </c>
@@ -4874,7 +4995,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>632</v>
       </c>
@@ -4904,14 +5025,14 @@
       <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.26953125" customWidth="1"/>
+    <col min="3" max="3" width="61.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -4922,7 +5043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -4933,7 +5054,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -4944,7 +5065,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -4955,7 +5076,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>603</v>
       </c>
@@ -4966,7 +5087,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -4977,7 +5098,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -4988,7 +5109,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>606</v>
       </c>
@@ -4999,7 +5120,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -5010,7 +5131,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -5021,7 +5142,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -5032,7 +5153,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -5043,7 +5164,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -5054,7 +5175,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -5065,7 +5186,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -5076,7 +5197,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -5087,7 +5208,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -5098,7 +5219,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -5109,7 +5230,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -5120,7 +5241,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>245</v>
       </c>
@@ -5131,7 +5252,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -5142,7 +5263,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -5153,7 +5274,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -5164,7 +5285,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -5175,7 +5296,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -5186,7 +5307,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -5197,7 +5318,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>265</v>
       </c>
@@ -5208,7 +5329,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5219,7 +5340,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5230,7 +5351,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5241,7 +5362,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5252,7 +5373,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5263,7 +5384,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5274,7 +5395,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>286</v>
       </c>
@@ -5285,7 +5406,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -5296,7 +5417,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>291</v>
       </c>
@@ -5307,7 +5428,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -5318,7 +5439,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -5329,7 +5450,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5340,7 +5461,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5351,7 +5472,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5362,7 +5483,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -5373,7 +5494,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>313</v>
       </c>
@@ -5384,7 +5505,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -5395,7 +5516,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5406,7 +5527,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>322</v>
       </c>
@@ -5417,7 +5538,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>325</v>
       </c>
@@ -5428,7 +5549,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>328</v>
       </c>
@@ -5439,7 +5560,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5450,7 +5571,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>334</v>
       </c>
@@ -5461,7 +5582,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5472,7 +5593,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5483,7 +5604,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>343</v>
       </c>
@@ -5494,7 +5615,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -5505,7 +5626,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>349</v>
       </c>
@@ -5516,7 +5637,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>352</v>
       </c>
@@ -5527,7 +5648,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5538,7 +5659,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -5549,7 +5670,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5560,7 +5681,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>364</v>
       </c>
@@ -5571,7 +5692,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -5582,7 +5703,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -5593,7 +5714,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5604,7 +5725,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>375</v>
       </c>
@@ -5615,7 +5736,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>379</v>
       </c>
@@ -5626,7 +5747,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>382</v>
       </c>
@@ -5637,7 +5758,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>555</v>
       </c>
@@ -5648,7 +5769,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>388</v>
       </c>
@@ -5659,7 +5780,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5670,7 +5791,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5681,7 +5802,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5692,7 +5813,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5703,7 +5824,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>403</v>
       </c>
@@ -5714,7 +5835,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5725,7 +5846,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -5736,7 +5857,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>412</v>
       </c>
@@ -5747,7 +5868,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>415</v>
       </c>
@@ -5758,7 +5879,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>418</v>
       </c>
@@ -5769,7 +5890,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>421</v>
       </c>
@@ -5780,7 +5901,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -5791,7 +5912,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>425</v>
       </c>
@@ -5802,7 +5923,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>428</v>
       </c>
@@ -5813,7 +5934,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>431</v>
       </c>
@@ -5824,7 +5945,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -5835,7 +5956,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>437</v>
       </c>
@@ -5846,7 +5967,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>440</v>
       </c>
@@ -5857,7 +5978,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>443</v>
       </c>
@@ -5868,7 +5989,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>446</v>
       </c>
@@ -5879,7 +6000,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>449</v>
       </c>
@@ -5890,7 +6011,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>452</v>
       </c>
@@ -5901,7 +6022,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>455</v>
       </c>
@@ -5912,7 +6033,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>458</v>
       </c>
@@ -5923,7 +6044,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>461</v>
       </c>
@@ -5934,7 +6055,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>464</v>
       </c>
@@ -5945,7 +6066,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>467</v>
       </c>
@@ -5956,7 +6077,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>470</v>
       </c>
@@ -5967,7 +6088,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>473</v>
       </c>
@@ -5978,7 +6099,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>476</v>
       </c>
@@ -5989,7 +6110,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>479</v>
       </c>
@@ -6000,7 +6121,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>482</v>
       </c>
@@ -6011,7 +6132,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>485</v>
       </c>
@@ -6022,7 +6143,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>488</v>
       </c>
@@ -6033,7 +6154,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>492</v>
       </c>
@@ -6044,7 +6165,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>494</v>
       </c>
@@ -6055,7 +6176,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>497</v>
       </c>
@@ -6066,7 +6187,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>500</v>
       </c>
@@ -6077,7 +6198,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>503</v>
       </c>
@@ -6088,7 +6209,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>506</v>
       </c>
@@ -6099,7 +6220,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>509</v>
       </c>
@@ -6110,7 +6231,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>512</v>
       </c>
@@ -6121,7 +6242,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>515</v>
       </c>
@@ -6132,7 +6253,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>518</v>
       </c>
@@ -6143,7 +6264,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>521</v>
       </c>
@@ -6154,7 +6275,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>524</v>
       </c>
@@ -6165,7 +6286,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>528</v>
       </c>
@@ -6176,7 +6297,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>531</v>
       </c>
@@ -6187,7 +6308,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>534</v>
       </c>
@@ -6198,7 +6319,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>537</v>
       </c>
@@ -6209,7 +6330,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>539</v>
       </c>
@@ -6220,7 +6341,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>550</v>
       </c>
@@ -6231,7 +6352,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>553</v>
       </c>
@@ -6242,7 +6363,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>556</v>
       </c>
@@ -6253,7 +6374,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>558</v>
       </c>
@@ -6264,7 +6385,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>560</v>
       </c>
@@ -6275,7 +6396,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>563</v>
       </c>
@@ -6286,7 +6407,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>566</v>
       </c>
@@ -6297,7 +6418,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>569</v>
       </c>
@@ -6308,7 +6429,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>571</v>
       </c>
@@ -6319,7 +6440,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>574</v>
       </c>
@@ -6330,7 +6451,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>577</v>
       </c>
@@ -6341,7 +6462,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>580</v>
       </c>
@@ -6352,7 +6473,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>585</v>
       </c>
@@ -6363,7 +6484,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>586</v>
       </c>
@@ -6374,7 +6495,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>589</v>
       </c>
@@ -6385,7 +6506,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>600</v>
       </c>
@@ -6396,7 +6517,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>609</v>
       </c>
@@ -6407,7 +6528,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>612</v>
       </c>
@@ -6418,7 +6539,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>616</v>
       </c>

</xml_diff>

<commit_message>
Change refrigerators to include WHO questions and choices
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -1402,15 +1402,6 @@
     <t>ID Del Refrigerador:</t>
   </si>
   <si>
-    <t>working_status</t>
-  </si>
-  <si>
-    <t>Working Status:</t>
-  </si>
-  <si>
-    <t>Estado De Trabajo:</t>
-  </si>
-  <si>
     <t>reason_not_working</t>
   </si>
   <si>
@@ -2057,6 +2048,15 @@
   </si>
   <si>
     <t>Indicators</t>
+  </si>
+  <si>
+    <t>functional_status</t>
+  </si>
+  <si>
+    <t>Functional Status:</t>
+  </si>
+  <si>
+    <t>Estado Funcional:</t>
   </si>
 </sst>
 </file>
@@ -2619,8 +2619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2665,27 +2665,27 @@
     </row>
     <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="15" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="I2" s="16"/>
     </row>
     <row r="3" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="15" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="I4" s="16"/>
     </row>
@@ -2694,45 +2694,45 @@
         <v>10</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="18" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="15" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2990,13 +2990,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -3014,8 +3014,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C181" sqref="C181"/>
+    <sheetView topLeftCell="A132" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3644,68 +3644,68 @@
     </row>
     <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C58" s="9" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C63" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
@@ -4612,398 +4612,398 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>440</v>
+        <v>649</v>
       </c>
       <c r="B146" t="s">
-        <v>441</v>
+        <v>650</v>
       </c>
       <c r="C146" s="4" t="s">
-        <v>442</v>
+        <v>651</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B147" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C147" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B148" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C148" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B149" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C149" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B150" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C150" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B151" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C151" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B152" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C152" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B153" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C153" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B154" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C154" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B155" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C155" s="4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B156" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C156" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B157" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C157" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B158" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C158" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B159" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C159" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B160" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C160" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B161" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C161" s="4" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B162" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C162" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B163" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C163" s="4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B164" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C164" s="4" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B165" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C165" s="4" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B166" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C166" s="4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B167" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C167" s="4" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B168" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C168" s="4" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B169" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C169" s="4" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B170" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C170" s="4" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B171" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C171" s="4" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B172" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C172" s="4" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B173" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C173" s="4" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B174" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
     </row>
     <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B175" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C175" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B176" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B177" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B178" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C178" s="4" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B179" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C179" s="4" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="B180" s="12" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="C180" s="12" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
   </sheetData>
@@ -5021,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A138" sqref="A138"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5078,13 +5078,13 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="B5" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C5" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -5111,13 +5111,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="B8" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C8" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -5172,7 +5172,7 @@
         <v>225</v>
       </c>
       <c r="C13" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -5216,7 +5216,7 @@
         <v>237</v>
       </c>
       <c r="C17" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
@@ -5370,7 +5370,7 @@
         <v>278</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
@@ -5513,7 +5513,7 @@
         <v>317</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
@@ -5612,7 +5612,7 @@
         <v>344</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -5752,21 +5752,21 @@
         <v>382</v>
       </c>
       <c r="B66" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B67" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -5865,7 +5865,7 @@
         <v>413</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -5876,7 +5876,7 @@
         <v>416</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -5909,7 +5909,7 @@
         <v>63</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -5969,585 +5969,585 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>440</v>
+        <v>649</v>
       </c>
       <c r="B86" t="s">
-        <v>441</v>
+        <v>650</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>442</v>
+        <v>651</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B87" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B88" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B89" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B90" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B91" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B92" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B93" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B94" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B95" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B96" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B97" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B98" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B99" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B100" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B101" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B102" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B103" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B104" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B105" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B106" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B107" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B108" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B109" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B110" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B111" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B112" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B113" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="B114" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="B115" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="B116" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B117" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B118" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="B119" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B120" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B121" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B122" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B123" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B124" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B125" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B126" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B127" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C127" s="4" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B128" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="C128" s="4" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B129" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C129" s="4" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B130" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C130" s="4" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="B131" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C131" s="4" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="B132" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C132" s="4" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="B133" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="C133" s="4" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="B134" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="B135" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="B136" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="B137" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B138" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add labels for filtering fridge inventory by age
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="654">
   <si>
     <t>comments</t>
   </si>
@@ -2057,6 +2057,12 @@
   </si>
   <si>
     <t>Estado Funcional:</t>
+  </si>
+  <si>
+    <t>Select Region</t>
+  </si>
+  <si>
+    <t>Seleccione Región</t>
   </si>
 </sst>
 </file>
@@ -5021,8 +5027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5059,10 +5065,10 @@
         <v>201</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>652</v>
       </c>
       <c r="C3" t="s">
-        <v>203</v>
+        <v>653</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Intermediate check-in for cold rooms
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="16308" yWindow="5028" windowWidth="25608" windowHeight="16068" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="675">
   <si>
     <t>comments</t>
   </si>
@@ -2063,6 +2063,69 @@
   </si>
   <si>
     <t>Seleccione Región</t>
+  </si>
+  <si>
+    <t>cold_rooms</t>
+  </si>
+  <si>
+    <t>Cold Rooms</t>
+  </si>
+  <si>
+    <t>Cuartos Fríos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cold_room </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cold Room </t>
+  </si>
+  <si>
+    <t>Cuarto Frío</t>
+  </si>
+  <si>
+    <t>basic_cold_room_information</t>
+  </si>
+  <si>
+    <t>Basic Cold Room Information</t>
+  </si>
+  <si>
+    <t>Información Básica Del Cuarto Frio</t>
+  </si>
+  <si>
+    <t>cold_room_id</t>
+  </si>
+  <si>
+    <t>Cold Room ID:</t>
+  </si>
+  <si>
+    <t>ID Del Cuarto Frio:</t>
+  </si>
+  <si>
+    <t>edit_cold_room_status</t>
+  </si>
+  <si>
+    <t>Edit Cold Room Status</t>
+  </si>
+  <si>
+    <t>edit_cold_room</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Cold Room  </t>
+  </si>
+  <si>
+    <t>delete_cold_room</t>
+  </si>
+  <si>
+    <t>Delete Cold Room</t>
+  </si>
+  <si>
+    <t>Editar El Estado Del Cuarto Frio</t>
+  </si>
+  <si>
+    <t>Editar Cuarto Frio</t>
+  </si>
+  <si>
+    <t>Borrar Cuarto Frio</t>
   </si>
 </sst>
 </file>
@@ -2590,11 +2653,11 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.77734375" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,20 +2692,20 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="101.1796875" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="101.21875" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" customWidth="1"/>
+    <col min="4" max="4" width="46.21875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
+    <col min="9" max="9" width="22.21875" customWidth="1"/>
+    <col min="10" max="1025" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2747,71 +2810,71 @@
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2831,12 +2894,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="6" width="24.7265625" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" customWidth="1"/>
-    <col min="8" max="1025" width="17.1796875" customWidth="1"/>
+    <col min="1" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="6" width="24.77734375" customWidth="1"/>
+    <col min="7" max="7" width="41.21875" customWidth="1"/>
+    <col min="8" max="1025" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2903,7 +2966,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2975,12 +3038,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,15 +3087,15 @@
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.7265625" customWidth="1"/>
-    <col min="2" max="2" width="52.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="1025" width="8.7265625" customWidth="1"/>
+    <col min="1" max="1" width="49.77734375" customWidth="1"/>
+    <col min="2" max="2" width="52.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3043,7 +3106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -3054,7 +3117,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3065,7 +3128,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -3076,7 +3139,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -3087,7 +3150,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3142,7 +3205,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3153,7 +3216,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3329,7 +3392,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3406,7 +3469,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="275" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="290.39999999999998" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3560,7 +3623,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3670,7 +3733,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>620</v>
       </c>
@@ -3714,7 +3777,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -3802,7 +3865,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -3835,7 +3898,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -3868,7 +3931,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -3923,7 +3986,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -3978,7 +4041,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -3989,7 +4052,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -4000,7 +4063,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -4011,7 +4074,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -4022,7 +4085,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -4033,7 +4096,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -4099,7 +4162,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4110,7 +4173,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -4121,7 +4184,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -4143,7 +4206,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>313</v>
       </c>
@@ -4154,7 +4217,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -4165,7 +4228,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -4176,7 +4239,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>322</v>
       </c>
@@ -4187,7 +4250,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4198,7 +4261,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4209,7 +4272,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4220,7 +4283,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4231,7 +4294,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4242,7 +4305,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4297,7 +4360,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4308,7 +4371,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4319,7 +4382,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4352,7 +4415,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>370</v>
       </c>
@@ -4363,7 +4426,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4374,7 +4437,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -4385,7 +4448,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4429,7 +4492,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -4440,7 +4503,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>394</v>
       </c>
@@ -4451,7 +4514,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>397</v>
       </c>
@@ -4462,7 +4525,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>400</v>
       </c>
@@ -4473,7 +4536,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>403</v>
       </c>
@@ -4484,7 +4547,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>406</v>
       </c>
@@ -4495,7 +4558,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>409</v>
       </c>
@@ -4594,7 +4657,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -4605,7 +4668,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -4627,7 +4690,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4649,7 +4712,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4660,7 +4723,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4671,7 +4734,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4704,7 +4767,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4715,7 +4778,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4726,7 +4789,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4737,7 +4800,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4748,7 +4811,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4759,7 +4822,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4781,7 +4844,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4792,7 +4855,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4803,7 +4866,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>489</v>
       </c>
@@ -4836,7 +4899,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4858,7 +4921,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4880,7 +4943,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4891,7 +4954,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -4902,7 +4965,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -4913,7 +4976,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -4924,7 +4987,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -4935,7 +4998,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>525</v>
       </c>
@@ -4946,7 +5009,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -4957,7 +5020,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>531</v>
       </c>
@@ -4979,7 +5042,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5025,17 +5088,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:C145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B132" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" customWidth="1"/>
-    <col min="2" max="2" width="33.26953125" customWidth="1"/>
-    <col min="3" max="3" width="61.7265625" customWidth="1"/>
+    <col min="1" max="1" width="37.77734375" customWidth="1"/>
+    <col min="2" max="2" width="33.21875" customWidth="1"/>
+    <col min="3" max="3" width="61.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5049,7 +5112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -5159,7 +5222,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -5192,7 +5255,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -5225,7 +5288,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -5280,7 +5343,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -5335,7 +5398,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5346,7 +5409,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5357,7 +5420,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5368,7 +5431,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5379,7 +5442,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5390,7 +5453,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5456,7 +5519,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5467,7 +5530,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5478,7 +5541,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5522,7 +5585,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5566,7 +5629,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5588,7 +5651,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5599,7 +5662,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5654,7 +5717,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5676,7 +5739,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5720,7 +5783,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5797,7 +5860,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5808,7 +5871,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5819,7 +5882,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5841,7 +5904,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5907,7 +5970,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -5951,7 +6014,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -6061,7 +6124,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>461</v>
       </c>
@@ -6072,7 +6135,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>464</v>
       </c>
@@ -6083,7 +6146,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>467</v>
       </c>
@@ -6138,7 +6201,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>482</v>
       </c>
@@ -6193,7 +6256,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>497</v>
       </c>
@@ -6215,7 +6278,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>503</v>
       </c>
@@ -6237,7 +6300,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>509</v>
       </c>
@@ -6248,7 +6311,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>512</v>
       </c>
@@ -6259,7 +6322,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>515</v>
       </c>
@@ -6270,7 +6333,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>518</v>
       </c>
@@ -6292,7 +6355,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>525</v>
       </c>
@@ -6303,7 +6366,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>528</v>
       </c>
@@ -6314,7 +6377,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>531</v>
       </c>
@@ -6391,7 +6454,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>557</v>
       </c>
@@ -6468,7 +6531,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>577</v>
       </c>
@@ -6479,7 +6542,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>582</v>
       </c>
@@ -6545,7 +6608,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>613</v>
       </c>
@@ -6556,9 +6619,86 @@
         <v>615</v>
       </c>
     </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>654</v>
+      </c>
+      <c r="B139" t="s">
+        <v>655</v>
+      </c>
+      <c r="C139" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>657</v>
+      </c>
+      <c r="B140" t="s">
+        <v>658</v>
+      </c>
+      <c r="C140" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>660</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>661</v>
+      </c>
+      <c r="C141" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="12" t="s">
+        <v>663</v>
+      </c>
+      <c r="B142" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="C142" s="11" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="12" t="s">
+        <v>666</v>
+      </c>
+      <c r="B143" s="12" t="s">
+        <v>667</v>
+      </c>
+      <c r="C143" s="11" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="12" t="s">
+        <v>668</v>
+      </c>
+      <c r="B144" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="12" t="s">
+        <v>670</v>
+      </c>
+      <c r="B145" s="12" t="s">
+        <v>671</v>
+      </c>
+      <c r="C145" s="11" t="s">
+        <v>674</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Add in more functionality for cold rooms and alphabetize region menu options
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16308" yWindow="5028" windowWidth="25608" windowHeight="16068" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="681">
   <si>
     <t>comments</t>
   </si>
@@ -2126,6 +2126,24 @@
   </si>
   <si>
     <t>Borrar Cuarto Frio</t>
+  </si>
+  <si>
+    <t>cold_room_inventory</t>
+  </si>
+  <si>
+    <t>add_cold_room</t>
+  </si>
+  <si>
+    <t>Add Cold Room</t>
+  </si>
+  <si>
+    <t>Añadir Cuarto Frio</t>
+  </si>
+  <si>
+    <t>Cold Room Inventory</t>
+  </si>
+  <si>
+    <t>Inventario De Cuarto Frio</t>
   </si>
 </sst>
 </file>
@@ -2653,11 +2671,11 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" customWidth="1"/>
-    <col min="3" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,20 +2710,20 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="101.21875" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" customWidth="1"/>
-    <col min="4" max="4" width="46.21875" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.77734375" customWidth="1"/>
-    <col min="8" max="8" width="31.44140625" customWidth="1"/>
-    <col min="9" max="9" width="22.21875" customWidth="1"/>
-    <col min="10" max="1025" width="17.21875" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2810,71 +2828,71 @@
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="17.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="58.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2894,12 +2912,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="6" width="24.77734375" customWidth="1"/>
-    <col min="7" max="7" width="41.21875" customWidth="1"/>
-    <col min="8" max="1025" width="17.21875" customWidth="1"/>
+    <col min="1" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="41.1796875" customWidth="1"/>
+    <col min="8" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2966,7 +2984,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3038,12 +3056,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -3087,15 +3105,15 @@
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.77734375" customWidth="1"/>
-    <col min="2" max="2" width="52.21875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="1025" width="8.77734375" customWidth="1"/>
+    <col min="1" max="1" width="49.81640625" customWidth="1"/>
+    <col min="2" max="2" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3106,7 +3124,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -3117,7 +3135,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3128,7 +3146,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -3139,7 +3157,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -3150,7 +3168,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3205,7 +3223,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3216,7 +3234,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3392,7 +3410,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3469,7 +3487,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="290.39999999999998" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="275" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3623,7 +3641,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3733,7 +3751,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="6" customFormat="1" ht="66" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>620</v>
       </c>
@@ -3777,7 +3795,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -3865,7 +3883,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -3898,7 +3916,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -3931,7 +3949,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -3986,7 +4004,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -4041,7 +4059,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -4052,7 +4070,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -4063,7 +4081,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -4074,7 +4092,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -4085,7 +4103,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -4096,7 +4114,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -4162,7 +4180,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4173,7 +4191,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -4206,7 +4224,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>313</v>
       </c>
@@ -4217,7 +4235,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -4228,7 +4246,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -4239,7 +4257,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>322</v>
       </c>
@@ -4250,7 +4268,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4261,7 +4279,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4272,7 +4290,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4283,7 +4301,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4294,7 +4312,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4305,7 +4323,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4360,7 +4378,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4371,7 +4389,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4382,7 +4400,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4415,7 +4433,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>370</v>
       </c>
@@ -4426,7 +4444,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4437,7 +4455,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -4448,7 +4466,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4492,7 +4510,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -4503,7 +4521,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>394</v>
       </c>
@@ -4514,7 +4532,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>397</v>
       </c>
@@ -4525,7 +4543,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>400</v>
       </c>
@@ -4536,7 +4554,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>403</v>
       </c>
@@ -4547,7 +4565,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>406</v>
       </c>
@@ -4558,7 +4576,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>409</v>
       </c>
@@ -4657,7 +4675,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -4668,7 +4686,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -4690,7 +4708,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4712,7 +4730,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4723,7 +4741,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4734,7 +4752,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4767,7 +4785,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4778,7 +4796,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4789,7 +4807,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4800,7 +4818,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4811,7 +4829,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4822,7 +4840,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4844,7 +4862,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4855,7 +4873,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>489</v>
       </c>
@@ -4899,7 +4917,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4921,7 +4939,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4943,7 +4961,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -4965,7 +4983,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -4976,7 +4994,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -4987,7 +5005,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -4998,7 +5016,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>525</v>
       </c>
@@ -5009,7 +5027,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -5020,7 +5038,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>531</v>
       </c>
@@ -5042,7 +5060,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5088,17 +5106,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C145"/>
+  <dimension ref="A1:C147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B132" workbookViewId="0">
-      <selection activeCell="C140" sqref="C140"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.77734375" customWidth="1"/>
-    <col min="2" max="2" width="33.21875" customWidth="1"/>
-    <col min="3" max="3" width="61.77734375" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
+    <col min="3" max="3" width="61.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -5112,7 +5130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -5222,7 +5240,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -5255,7 +5273,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -5288,7 +5306,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -5343,7 +5361,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -5398,7 +5416,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5409,7 +5427,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5420,7 +5438,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5431,7 +5449,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5442,7 +5460,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5453,7 +5471,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5519,7 +5537,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5530,7 +5548,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5541,7 +5559,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5585,7 +5603,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5629,7 +5647,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5651,7 +5669,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5662,7 +5680,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5717,7 +5735,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5739,7 +5757,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5783,7 +5801,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5860,7 +5878,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5871,7 +5889,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5882,7 +5900,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5904,7 +5922,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5970,7 +5988,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -6014,7 +6032,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -6124,7 +6142,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>461</v>
       </c>
@@ -6135,7 +6153,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>464</v>
       </c>
@@ -6146,7 +6164,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>467</v>
       </c>
@@ -6201,7 +6219,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>482</v>
       </c>
@@ -6256,7 +6274,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>497</v>
       </c>
@@ -6278,7 +6296,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>503</v>
       </c>
@@ -6300,7 +6318,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>509</v>
       </c>
@@ -6311,7 +6329,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>512</v>
       </c>
@@ -6322,7 +6340,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>515</v>
       </c>
@@ -6333,7 +6351,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>518</v>
       </c>
@@ -6355,7 +6373,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>525</v>
       </c>
@@ -6366,7 +6384,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>528</v>
       </c>
@@ -6377,7 +6395,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>531</v>
       </c>
@@ -6454,7 +6472,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>557</v>
       </c>
@@ -6531,7 +6549,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>577</v>
       </c>
@@ -6542,7 +6560,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>582</v>
       </c>
@@ -6608,7 +6626,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>613</v>
       </c>
@@ -6694,6 +6712,28 @@
       </c>
       <c r="C145" s="11" t="s">
         <v>674</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>675</v>
+      </c>
+      <c r="B146" t="s">
+        <v>679</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>676</v>
+      </c>
+      <c r="B147" t="s">
+        <v>677</v>
+      </c>
+      <c r="C147" t="s">
+        <v>678</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix foreign key relationship for refrigerators/cold_rooms to be _id -> <refrigerator/cold_room>_id
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="16305" yWindow="5025" windowWidth="25605" windowHeight="16065" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1040" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="687">
   <si>
     <t>comments</t>
   </si>
@@ -2144,6 +2144,24 @@
   </si>
   <si>
     <t>Inventario De Cuarto Frio</t>
+  </si>
+  <si>
+    <t>Reporting Period</t>
+  </si>
+  <si>
+    <t>Período de información</t>
+  </si>
+  <si>
+    <t>reporting_period_no_colon</t>
+  </si>
+  <si>
+    <t>Reporting Period:</t>
+  </si>
+  <si>
+    <t>Período de información:</t>
+  </si>
+  <si>
+    <t>reporting_period</t>
   </si>
 </sst>
 </file>
@@ -2671,14 +2689,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.81640625" customWidth="1"/>
-    <col min="2" max="2" width="20.81640625" customWidth="1"/>
-    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2686,7 +2704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2710,20 +2728,20 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" customWidth="1"/>
-    <col min="2" max="2" width="101.1796875" customWidth="1"/>
-    <col min="3" max="3" width="22.1796875" customWidth="1"/>
-    <col min="4" max="4" width="46.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="101.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.140625" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" customWidth="1"/>
-    <col min="8" max="8" width="31.453125" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" customWidth="1"/>
-    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="31.42578125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="1025" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2750,7 +2768,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="15" t="s">
         <v>634</v>
       </c>
@@ -2759,7 +2777,7 @@
       </c>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E3" s="15" t="s">
         <v>636</v>
       </c>
@@ -2770,13 +2788,13 @@
         <v>638</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="15" t="s">
         <v>639</v>
       </c>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E5" s="15" t="s">
         <v>10</v>
       </c>
@@ -2787,23 +2805,23 @@
         <v>641</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="15" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="15" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>646</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="17"/>
       <c r="B9" s="18" t="s">
         <v>647</v>
@@ -2815,84 +2833,84 @@
         <v>645</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="15" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2912,15 +2930,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="17.1796875" customWidth="1"/>
-    <col min="3" max="6" width="24.81640625" customWidth="1"/>
-    <col min="7" max="7" width="41.1796875" customWidth="1"/>
-    <col min="8" max="1025" width="17.1796875" customWidth="1"/>
+    <col min="1" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="41.140625" customWidth="1"/>
+    <col min="8" max="1025" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2946,7 +2964,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2958,7 +2976,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2973,7 +2991,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -2984,7 +3002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3002,7 +3020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -3013,7 +3031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3024,7 +3042,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -3034,9 +3052,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3056,15 +3074,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -3075,7 +3093,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>637</v>
       </c>
@@ -3105,15 +3123,15 @@
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="49.81640625" customWidth="1"/>
-    <col min="2" max="2" width="52.1796875" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" customWidth="1"/>
-    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
+    <col min="1" max="1" width="49.85546875" customWidth="1"/>
+    <col min="2" max="2" width="52.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3124,7 +3142,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -3135,7 +3153,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3146,7 +3164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -3157,7 +3175,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -3168,7 +3186,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3179,7 +3197,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3190,7 +3208,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3201,7 +3219,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3212,7 +3230,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -3223,7 +3241,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3234,7 +3252,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3245,7 +3263,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -3256,7 +3274,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3267,7 +3285,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -3278,7 +3296,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -3289,7 +3307,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -3300,7 +3318,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3311,7 +3329,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -3322,7 +3340,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -3333,7 +3351,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -3344,7 +3362,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -3355,7 +3373,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3366,7 +3384,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -3377,7 +3395,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3388,7 +3406,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3399,7 +3417,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -3410,7 +3428,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3421,7 +3439,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3432,7 +3450,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -3443,7 +3461,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3454,7 +3472,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -3465,7 +3483,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -3476,7 +3494,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3487,7 +3505,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="275" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="280.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3498,7 +3516,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -3509,7 +3527,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -3520,7 +3538,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -3531,7 +3549,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -3542,7 +3560,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3553,7 +3571,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>156</v>
       </c>
@@ -3564,7 +3582,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -3575,7 +3593,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -3586,7 +3604,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -3597,7 +3615,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3608,7 +3626,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -3619,7 +3637,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -3630,7 +3648,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -3641,7 +3659,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3652,7 +3670,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -3663,7 +3681,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -3674,7 +3692,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -3685,7 +3703,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>189</v>
       </c>
@@ -3696,7 +3714,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -3707,7 +3725,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -3718,7 +3736,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -3729,7 +3747,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>616</v>
       </c>
@@ -3740,7 +3758,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>618</v>
       </c>
@@ -3751,7 +3769,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>620</v>
       </c>
@@ -3762,7 +3780,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>613</v>
       </c>
@@ -3773,7 +3791,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>553</v>
       </c>
@@ -3784,7 +3802,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>555</v>
       </c>
@@ -3795,7 +3813,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -3806,7 +3824,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>201</v>
       </c>
@@ -3817,7 +3835,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>204</v>
       </c>
@@ -3828,7 +3846,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>207</v>
       </c>
@@ -3839,7 +3857,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>212</v>
       </c>
@@ -3850,7 +3868,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>213</v>
       </c>
@@ -3861,7 +3879,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>216</v>
       </c>
@@ -3872,7 +3890,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -3883,7 +3901,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -3894,7 +3912,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>224</v>
       </c>
@@ -3905,7 +3923,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>227</v>
       </c>
@@ -3916,7 +3934,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -3927,7 +3945,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -3938,7 +3956,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>236</v>
       </c>
@@ -3949,7 +3967,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -3960,7 +3978,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>242</v>
       </c>
@@ -3971,7 +3989,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>245</v>
       </c>
@@ -3982,7 +4000,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>248</v>
       </c>
@@ -3993,7 +4011,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -4004,7 +4022,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -4015,7 +4033,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>257</v>
       </c>
@@ -4026,7 +4044,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>260</v>
       </c>
@@ -4037,7 +4055,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>263</v>
       </c>
@@ -4048,7 +4066,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>265</v>
       </c>
@@ -4059,7 +4077,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -4070,7 +4088,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -4081,7 +4099,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -4092,7 +4110,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -4103,7 +4121,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -4114,7 +4132,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -4125,7 +4143,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -4136,7 +4154,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>289</v>
       </c>
@@ -4147,7 +4165,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>291</v>
       </c>
@@ -4158,7 +4176,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -4169,7 +4187,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -4180,7 +4198,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4191,7 +4209,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -4202,7 +4220,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -4213,7 +4231,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>310</v>
       </c>
@@ -4224,7 +4242,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>313</v>
       </c>
@@ -4235,7 +4253,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -4246,7 +4264,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -4257,7 +4275,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>322</v>
       </c>
@@ -4268,7 +4286,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4279,7 +4297,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4290,7 +4308,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4301,7 +4319,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4312,7 +4330,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4323,7 +4341,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4334,7 +4352,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>343</v>
       </c>
@@ -4345,7 +4363,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>346</v>
       </c>
@@ -4356,7 +4374,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>349</v>
       </c>
@@ -4367,7 +4385,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>352</v>
       </c>
@@ -4378,7 +4396,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4389,7 +4407,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4400,7 +4418,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4411,7 +4429,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>364</v>
       </c>
@@ -4422,7 +4440,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>366</v>
       </c>
@@ -4433,7 +4451,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>370</v>
       </c>
@@ -4444,7 +4462,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4455,7 +4473,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -4466,7 +4484,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4477,7 +4495,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>382</v>
       </c>
@@ -4488,7 +4506,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>385</v>
       </c>
@@ -4499,7 +4517,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>388</v>
       </c>
@@ -4510,7 +4528,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -4521,7 +4539,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>394</v>
       </c>
@@ -4532,7 +4550,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>397</v>
       </c>
@@ -4543,7 +4561,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>400</v>
       </c>
@@ -4554,7 +4572,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>403</v>
       </c>
@@ -4565,7 +4583,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>406</v>
       </c>
@@ -4576,7 +4594,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>409</v>
       </c>
@@ -4587,7 +4605,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>412</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>415</v>
       </c>
@@ -4609,7 +4627,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>418</v>
       </c>
@@ -4620,7 +4638,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>421</v>
       </c>
@@ -4631,7 +4649,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>424</v>
       </c>
@@ -4642,7 +4660,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>425</v>
       </c>
@@ -4653,7 +4671,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>428</v>
       </c>
@@ -4664,7 +4682,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>431</v>
       </c>
@@ -4675,7 +4693,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -4686,7 +4704,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -4697,7 +4715,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>649</v>
       </c>
@@ -4708,7 +4726,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4719,7 +4737,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>443</v>
       </c>
@@ -4730,7 +4748,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4741,7 +4759,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4752,7 +4770,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4763,7 +4781,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>455</v>
       </c>
@@ -4774,7 +4792,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>458</v>
       </c>
@@ -4785,7 +4803,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4796,7 +4814,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4807,7 +4825,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4818,7 +4836,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4829,7 +4847,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4840,7 +4858,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4851,7 +4869,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>479</v>
       </c>
@@ -4862,7 +4880,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4873,7 +4891,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4884,7 +4902,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>489</v>
       </c>
@@ -4895,7 +4913,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>491</v>
       </c>
@@ -4906,7 +4924,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>494</v>
       </c>
@@ -4917,7 +4935,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4928,7 +4946,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>500</v>
       </c>
@@ -4939,7 +4957,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4950,7 +4968,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -4961,7 +4979,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4972,7 +4990,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -4983,7 +5001,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -4994,7 +5012,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -5005,7 +5023,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -5016,7 +5034,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>525</v>
       </c>
@@ -5027,7 +5045,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -5038,7 +5056,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>531</v>
       </c>
@@ -5049,7 +5067,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>534</v>
       </c>
@@ -5060,7 +5078,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5071,7 +5089,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="13" t="s">
         <v>628</v>
       </c>
@@ -5082,7 +5100,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="13" t="s">
         <v>629</v>
       </c>
@@ -5106,20 +5124,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C147"/>
+  <dimension ref="A1:C149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="C141" sqref="C141"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="A150" sqref="A150"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.81640625" customWidth="1"/>
-    <col min="2" max="2" width="33.1796875" customWidth="1"/>
-    <col min="3" max="3" width="61.81640625" customWidth="1"/>
+    <col min="1" max="1" width="37.85546875" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -5130,7 +5148,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -5141,7 +5159,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -5152,7 +5170,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -5163,7 +5181,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>600</v>
       </c>
@@ -5174,7 +5192,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -5185,7 +5203,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -5196,7 +5214,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>603</v>
       </c>
@@ -5207,7 +5225,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -5218,7 +5236,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -5229,7 +5247,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -5240,7 +5258,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -5251,7 +5269,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -5262,7 +5280,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -5273,7 +5291,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -5284,7 +5302,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -5295,7 +5313,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -5306,7 +5324,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -5317,7 +5335,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -5328,7 +5346,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>245</v>
       </c>
@@ -5339,7 +5357,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -5350,7 +5368,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -5361,7 +5379,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -5372,7 +5390,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -5383,7 +5401,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -5394,7 +5412,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -5405,7 +5423,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>265</v>
       </c>
@@ -5416,7 +5434,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5427,7 +5445,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5438,7 +5456,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5449,7 +5467,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5460,7 +5478,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5471,7 +5489,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5482,7 +5500,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>286</v>
       </c>
@@ -5493,7 +5511,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -5504,7 +5522,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>291</v>
       </c>
@@ -5515,7 +5533,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -5526,7 +5544,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -5537,7 +5555,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5548,7 +5566,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5559,7 +5577,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5570,7 +5588,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -5581,7 +5599,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>313</v>
       </c>
@@ -5592,7 +5610,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -5603,7 +5621,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5614,7 +5632,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>322</v>
       </c>
@@ -5625,7 +5643,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>325</v>
       </c>
@@ -5636,7 +5654,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>328</v>
       </c>
@@ -5647,7 +5665,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5658,7 +5676,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>334</v>
       </c>
@@ -5669,7 +5687,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5680,7 +5698,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5691,7 +5709,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>343</v>
       </c>
@@ -5702,7 +5720,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -5713,7 +5731,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>349</v>
       </c>
@@ -5724,7 +5742,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>352</v>
       </c>
@@ -5735,7 +5753,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5746,7 +5764,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -5757,7 +5775,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5768,7 +5786,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>364</v>
       </c>
@@ -5779,7 +5797,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -5790,7 +5808,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -5801,7 +5819,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5812,7 +5830,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>375</v>
       </c>
@@ -5823,7 +5841,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>379</v>
       </c>
@@ -5834,7 +5852,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>382</v>
       </c>
@@ -5845,7 +5863,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>552</v>
       </c>
@@ -5856,7 +5874,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>388</v>
       </c>
@@ -5867,7 +5885,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5878,7 +5896,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5889,7 +5907,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5900,7 +5918,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5911,7 +5929,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>403</v>
       </c>
@@ -5922,7 +5940,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5933,7 +5951,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -5944,7 +5962,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>412</v>
       </c>
@@ -5955,7 +5973,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>415</v>
       </c>
@@ -5966,7 +5984,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>418</v>
       </c>
@@ -5977,7 +5995,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>421</v>
       </c>
@@ -5988,7 +6006,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -5999,7 +6017,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>425</v>
       </c>
@@ -6010,7 +6028,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>428</v>
       </c>
@@ -6021,7 +6039,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>431</v>
       </c>
@@ -6032,7 +6050,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -6043,7 +6061,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>437</v>
       </c>
@@ -6054,7 +6072,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>649</v>
       </c>
@@ -6065,7 +6083,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>440</v>
       </c>
@@ -6076,7 +6094,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>443</v>
       </c>
@@ -6087,7 +6105,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>446</v>
       </c>
@@ -6098,7 +6116,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>449</v>
       </c>
@@ -6109,7 +6127,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>452</v>
       </c>
@@ -6120,7 +6138,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>455</v>
       </c>
@@ -6131,7 +6149,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>458</v>
       </c>
@@ -6142,7 +6160,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>461</v>
       </c>
@@ -6153,7 +6171,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>464</v>
       </c>
@@ -6164,7 +6182,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>467</v>
       </c>
@@ -6175,7 +6193,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>470</v>
       </c>
@@ -6186,7 +6204,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>473</v>
       </c>
@@ -6197,7 +6215,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>476</v>
       </c>
@@ -6208,7 +6226,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>479</v>
       </c>
@@ -6219,7 +6237,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>482</v>
       </c>
@@ -6230,7 +6248,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>485</v>
       </c>
@@ -6241,7 +6259,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>489</v>
       </c>
@@ -6252,7 +6270,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>491</v>
       </c>
@@ -6263,7 +6281,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>494</v>
       </c>
@@ -6274,7 +6292,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>497</v>
       </c>
@@ -6285,7 +6303,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>500</v>
       </c>
@@ -6296,7 +6314,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>503</v>
       </c>
@@ -6307,7 +6325,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>506</v>
       </c>
@@ -6318,7 +6336,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>509</v>
       </c>
@@ -6329,7 +6347,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>512</v>
       </c>
@@ -6340,7 +6358,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>515</v>
       </c>
@@ -6351,7 +6369,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>518</v>
       </c>
@@ -6362,7 +6380,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>521</v>
       </c>
@@ -6373,7 +6391,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>525</v>
       </c>
@@ -6384,7 +6402,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>528</v>
       </c>
@@ -6395,7 +6413,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>531</v>
       </c>
@@ -6406,7 +6424,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>534</v>
       </c>
@@ -6417,7 +6435,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>536</v>
       </c>
@@ -6428,7 +6446,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>547</v>
       </c>
@@ -6439,7 +6457,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>550</v>
       </c>
@@ -6450,7 +6468,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>553</v>
       </c>
@@ -6461,7 +6479,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>555</v>
       </c>
@@ -6472,7 +6490,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>557</v>
       </c>
@@ -6483,7 +6501,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>560</v>
       </c>
@@ -6494,7 +6512,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>563</v>
       </c>
@@ -6505,7 +6523,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>566</v>
       </c>
@@ -6516,7 +6534,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>568</v>
       </c>
@@ -6527,7 +6545,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>571</v>
       </c>
@@ -6538,7 +6556,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>574</v>
       </c>
@@ -6549,7 +6567,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>577</v>
       </c>
@@ -6560,7 +6578,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>582</v>
       </c>
@@ -6571,7 +6589,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>583</v>
       </c>
@@ -6582,7 +6600,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>586</v>
       </c>
@@ -6593,7 +6611,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>597</v>
       </c>
@@ -6604,7 +6622,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>606</v>
       </c>
@@ -6615,7 +6633,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>609</v>
       </c>
@@ -6626,7 +6644,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>613</v>
       </c>
@@ -6637,7 +6655,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>654</v>
       </c>
@@ -6648,7 +6666,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>657</v>
       </c>
@@ -6659,7 +6677,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>660</v>
       </c>
@@ -6670,7 +6688,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="12" t="s">
         <v>663</v>
       </c>
@@ -6681,7 +6699,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="12" t="s">
         <v>666</v>
       </c>
@@ -6692,7 +6710,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="12" t="s">
         <v>668</v>
       </c>
@@ -6703,7 +6721,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="12" t="s">
         <v>670</v>
       </c>
@@ -6714,7 +6732,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>675</v>
       </c>
@@ -6725,7 +6743,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>676</v>
       </c>
@@ -6734,6 +6752,28 @@
       </c>
       <c r="C147" t="s">
         <v>678</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="12" t="s">
+        <v>683</v>
+      </c>
+      <c r="B148" s="12" t="s">
+        <v>681</v>
+      </c>
+      <c r="C148" s="11" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="12" t="s">
+        <v>686</v>
+      </c>
+      <c r="B149" s="12" t="s">
+        <v>684</v>
+      </c>
+      <c r="C149" s="11" t="s">
+        <v>685</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add serial_number to refrigerator detail view
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16305" yWindow="5025" windowWidth="25605" windowHeight="16065" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="690">
   <si>
     <t>comments</t>
   </si>
@@ -2162,6 +2162,15 @@
   </si>
   <si>
     <t>reporting_period</t>
+  </si>
+  <si>
+    <t>serial_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serial Number: </t>
+  </si>
+  <si>
+    <t>Número de serie:</t>
   </si>
 </sst>
 </file>
@@ -2689,14 +2698,14 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2704,7 +2713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -2728,20 +2737,20 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="1025" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2768,7 +2777,7 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="15" t="s">
         <v>634</v>
       </c>
@@ -2777,7 +2786,7 @@
       </c>
       <c r="I2" s="16"/>
     </row>
-    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" s="15" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="15" t="s">
         <v>636</v>
       </c>
@@ -2788,13 +2797,13 @@
         <v>638</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="15" t="s">
         <v>639</v>
       </c>
       <c r="I4" s="16"/>
     </row>
-    <row r="5" spans="1:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" s="15" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E5" s="15" t="s">
         <v>10</v>
       </c>
@@ -2805,23 +2814,23 @@
         <v>641</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="15" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>646</v>
       </c>
       <c r="B8" s="17"/>
     </row>
-    <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="17"/>
       <c r="B9" s="18" t="s">
         <v>647</v>
@@ -2833,84 +2842,84 @@
         <v>645</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
       <c r="B10" s="17"/>
       <c r="C10" s="15" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="17.45" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="62.1" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="57.95" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="66" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="62.15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="12" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="58" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -2930,15 +2939,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="6" width="24.85546875" customWidth="1"/>
-    <col min="7" max="7" width="41.140625" customWidth="1"/>
-    <col min="8" max="1025" width="17.140625" customWidth="1"/>
+    <col min="1" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="6" width="24.81640625" customWidth="1"/>
+    <col min="7" max="7" width="41.1796875" customWidth="1"/>
+    <col min="8" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2964,7 +2973,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -2976,7 +2985,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>20</v>
       </c>
@@ -2991,7 +3000,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -3002,7 +3011,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="28" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3020,7 +3029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -3031,7 +3040,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -3042,7 +3051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>34</v>
       </c>
@@ -3052,9 +3061,9 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -3074,15 +3083,15 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="22.1796875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -3093,7 +3102,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>637</v>
       </c>
@@ -3123,15 +3132,15 @@
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="49.81640625" customWidth="1"/>
+    <col min="2" max="2" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="17.1796875" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -3142,7 +3151,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -3153,7 +3162,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -3164,7 +3173,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -3175,7 +3184,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -3197,7 +3206,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3208,7 +3217,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -3219,7 +3228,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -3230,7 +3239,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3261,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="13.7" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="13.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -3263,7 +3272,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>73</v>
       </c>
@@ -3274,7 +3283,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>76</v>
       </c>
@@ -3285,7 +3294,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -3296,7 +3305,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>82</v>
       </c>
@@ -3307,7 +3316,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>85</v>
       </c>
@@ -3318,7 +3327,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3329,7 +3338,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>91</v>
       </c>
@@ -3340,7 +3349,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>94</v>
       </c>
@@ -3351,7 +3360,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -3362,7 +3371,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -3373,7 +3382,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>103</v>
       </c>
@@ -3384,7 +3393,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -3395,7 +3404,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>109</v>
       </c>
@@ -3406,7 +3415,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>111</v>
       </c>
@@ -3417,7 +3426,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>114</v>
       </c>
@@ -3428,7 +3437,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="28.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -3439,7 +3448,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>120</v>
       </c>
@@ -3450,7 +3459,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>123</v>
       </c>
@@ -3461,7 +3470,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>126</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>129</v>
       </c>
@@ -3483,7 +3492,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>135</v>
       </c>
@@ -3505,7 +3514,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" ht="275" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -3516,7 +3525,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -3527,7 +3536,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>144</v>
       </c>
@@ -3538,7 +3547,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>147</v>
       </c>
@@ -3549,7 +3558,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>150</v>
       </c>
@@ -3560,7 +3569,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3571,7 +3580,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>156</v>
       </c>
@@ -3582,7 +3591,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>159</v>
       </c>
@@ -3593,7 +3602,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>161</v>
       </c>
@@ -3604,7 +3613,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>164</v>
       </c>
@@ -3615,7 +3624,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>167</v>
       </c>
@@ -3626,7 +3635,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>170</v>
       </c>
@@ -3637,7 +3646,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>173</v>
       </c>
@@ -3648,7 +3657,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>176</v>
       </c>
@@ -3659,7 +3668,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -3670,7 +3679,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>182</v>
       </c>
@@ -3681,7 +3690,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>185</v>
       </c>
@@ -3692,7 +3701,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>186</v>
       </c>
@@ -3703,7 +3712,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>189</v>
       </c>
@@ -3714,7 +3723,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>190</v>
       </c>
@@ -3725,7 +3734,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>193</v>
       </c>
@@ -3736,7 +3745,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>196</v>
       </c>
@@ -3747,7 +3756,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>616</v>
       </c>
@@ -3758,7 +3767,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>618</v>
       </c>
@@ -3769,7 +3778,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="60" spans="1:3" s="6" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" s="6" customFormat="1" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>620</v>
       </c>
@@ -3780,7 +3789,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>613</v>
       </c>
@@ -3791,7 +3800,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>553</v>
       </c>
@@ -3802,7 +3811,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>555</v>
       </c>
@@ -3813,7 +3822,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -3824,7 +3833,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>201</v>
       </c>
@@ -3835,7 +3844,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>204</v>
       </c>
@@ -3846,7 +3855,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>207</v>
       </c>
@@ -3857,7 +3866,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>212</v>
       </c>
@@ -3868,7 +3877,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>213</v>
       </c>
@@ -3879,7 +3888,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>216</v>
       </c>
@@ -3890,7 +3899,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>219</v>
       </c>
@@ -3901,7 +3910,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -3912,7 +3921,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>224</v>
       </c>
@@ -3923,7 +3932,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>227</v>
       </c>
@@ -3934,7 +3943,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -3945,7 +3954,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>233</v>
       </c>
@@ -3956,7 +3965,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>236</v>
       </c>
@@ -3967,7 +3976,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -3978,7 +3987,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>242</v>
       </c>
@@ -3989,7 +3998,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>245</v>
       </c>
@@ -4000,7 +4009,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>248</v>
       </c>
@@ -4011,7 +4020,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>251</v>
       </c>
@@ -4022,7 +4031,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -4033,7 +4042,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>257</v>
       </c>
@@ -4044,7 +4053,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>260</v>
       </c>
@@ -4055,7 +4064,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>263</v>
       </c>
@@ -4066,7 +4075,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>265</v>
       </c>
@@ -4077,7 +4086,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -4088,7 +4097,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -4099,7 +4108,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -4110,7 +4119,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -4121,7 +4130,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -4132,7 +4141,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -4143,7 +4152,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>286</v>
       </c>
@@ -4154,7 +4163,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>289</v>
       </c>
@@ -4165,7 +4174,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>291</v>
       </c>
@@ -4176,7 +4185,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>294</v>
       </c>
@@ -4187,7 +4196,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>296</v>
       </c>
@@ -4198,7 +4207,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -4209,7 +4218,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -4220,7 +4229,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -4231,7 +4240,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>310</v>
       </c>
@@ -4242,7 +4251,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>313</v>
       </c>
@@ -4253,7 +4262,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -4264,7 +4273,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -4275,7 +4284,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>322</v>
       </c>
@@ -4286,7 +4295,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>325</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>328</v>
       </c>
@@ -4308,7 +4317,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -4319,7 +4328,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -4330,7 +4339,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -4341,7 +4350,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>343</v>
       </c>
@@ -4363,7 +4372,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>346</v>
       </c>
@@ -4374,7 +4383,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>349</v>
       </c>
@@ -4385,7 +4394,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>352</v>
       </c>
@@ -4396,7 +4405,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -4407,7 +4416,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>358</v>
       </c>
@@ -4418,7 +4427,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -4429,7 +4438,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>364</v>
       </c>
@@ -4440,7 +4449,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>366</v>
       </c>
@@ -4451,7 +4460,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>370</v>
       </c>
@@ -4462,7 +4471,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -4473,7 +4482,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -4484,7 +4493,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -4495,7 +4504,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>382</v>
       </c>
@@ -4506,7 +4515,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>385</v>
       </c>
@@ -4517,7 +4526,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>388</v>
       </c>
@@ -4528,7 +4537,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -4539,7 +4548,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>394</v>
       </c>
@@ -4550,7 +4559,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>397</v>
       </c>
@@ -4561,7 +4570,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>400</v>
       </c>
@@ -4572,7 +4581,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>403</v>
       </c>
@@ -4583,7 +4592,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>406</v>
       </c>
@@ -4594,7 +4603,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>409</v>
       </c>
@@ -4605,7 +4614,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>412</v>
       </c>
@@ -4616,7 +4625,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>415</v>
       </c>
@@ -4627,7 +4636,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>418</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>421</v>
       </c>
@@ -4649,7 +4658,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>424</v>
       </c>
@@ -4660,7 +4669,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>425</v>
       </c>
@@ -4671,7 +4680,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>428</v>
       </c>
@@ -4682,7 +4691,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>431</v>
       </c>
@@ -4693,7 +4702,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>434</v>
       </c>
@@ -4704,7 +4713,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>437</v>
       </c>
@@ -4715,7 +4724,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>649</v>
       </c>
@@ -4726,7 +4735,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>440</v>
       </c>
@@ -4737,7 +4746,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>443</v>
       </c>
@@ -4748,7 +4757,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>446</v>
       </c>
@@ -4759,7 +4768,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>449</v>
       </c>
@@ -4770,7 +4779,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>452</v>
       </c>
@@ -4781,7 +4790,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>455</v>
       </c>
@@ -4792,7 +4801,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>458</v>
       </c>
@@ -4803,7 +4812,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>461</v>
       </c>
@@ -4814,7 +4823,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>464</v>
       </c>
@@ -4825,7 +4834,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>467</v>
       </c>
@@ -4836,7 +4845,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>470</v>
       </c>
@@ -4847,7 +4856,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>473</v>
       </c>
@@ -4858,7 +4867,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>476</v>
       </c>
@@ -4869,7 +4878,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>479</v>
       </c>
@@ -4880,7 +4889,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>482</v>
       </c>
@@ -4891,7 +4900,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>485</v>
       </c>
@@ -4902,7 +4911,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>489</v>
       </c>
@@ -4913,7 +4922,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>491</v>
       </c>
@@ -4924,7 +4933,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>494</v>
       </c>
@@ -4935,7 +4944,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>497</v>
       </c>
@@ -4946,7 +4955,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>500</v>
       </c>
@@ -4957,7 +4966,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>503</v>
       </c>
@@ -4968,7 +4977,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>506</v>
       </c>
@@ -4979,7 +4988,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>509</v>
       </c>
@@ -4990,7 +4999,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>512</v>
       </c>
@@ -5001,7 +5010,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>515</v>
       </c>
@@ -5012,7 +5021,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>518</v>
       </c>
@@ -5023,7 +5032,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>521</v>
       </c>
@@ -5034,7 +5043,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>525</v>
       </c>
@@ -5045,7 +5054,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:3" ht="50" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>528</v>
       </c>
@@ -5056,7 +5065,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="177" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>531</v>
       </c>
@@ -5067,7 +5076,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>534</v>
       </c>
@@ -5078,7 +5087,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>536</v>
       </c>
@@ -5089,7 +5098,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
         <v>628</v>
       </c>
@@ -5100,7 +5109,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" s="13" t="s">
         <v>629</v>
       </c>
@@ -5124,20 +5133,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C149"/>
+  <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A150" sqref="A150"/>
+    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.85546875" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
-    <col min="3" max="3" width="61.85546875" customWidth="1"/>
+    <col min="1" max="1" width="37.81640625" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" customWidth="1"/>
+    <col min="3" max="3" width="61.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -5148,7 +5157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>199</v>
       </c>
@@ -5159,7 +5168,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>201</v>
       </c>
@@ -5170,7 +5179,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>204</v>
       </c>
@@ -5181,7 +5190,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>600</v>
       </c>
@@ -5192,7 +5201,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>207</v>
       </c>
@@ -5203,7 +5212,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>212</v>
       </c>
@@ -5214,7 +5223,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>603</v>
       </c>
@@ -5225,7 +5234,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>213</v>
       </c>
@@ -5236,7 +5245,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>216</v>
       </c>
@@ -5247,7 +5256,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>219</v>
       </c>
@@ -5258,7 +5267,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>223</v>
       </c>
@@ -5269,7 +5278,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>224</v>
       </c>
@@ -5280,7 +5289,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>227</v>
       </c>
@@ -5291,7 +5300,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>230</v>
       </c>
@@ -5302,7 +5311,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>233</v>
       </c>
@@ -5313,7 +5322,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>236</v>
       </c>
@@ -5324,7 +5333,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>239</v>
       </c>
@@ -5335,7 +5344,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -5346,7 +5355,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>245</v>
       </c>
@@ -5357,7 +5366,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>248</v>
       </c>
@@ -5368,7 +5377,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>251</v>
       </c>
@@ -5379,7 +5388,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>254</v>
       </c>
@@ -5390,7 +5399,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>257</v>
       </c>
@@ -5401,7 +5410,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>260</v>
       </c>
@@ -5412,7 +5421,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>263</v>
       </c>
@@ -5423,7 +5432,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>265</v>
       </c>
@@ -5434,7 +5443,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>267</v>
       </c>
@@ -5445,7 +5454,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>271</v>
       </c>
@@ -5456,7 +5465,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>274</v>
       </c>
@@ -5467,7 +5476,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>277</v>
       </c>
@@ -5478,7 +5487,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -5489,7 +5498,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>283</v>
       </c>
@@ -5500,7 +5509,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>286</v>
       </c>
@@ -5511,7 +5520,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>289</v>
       </c>
@@ -5522,7 +5531,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>291</v>
       </c>
@@ -5533,7 +5542,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>294</v>
       </c>
@@ -5544,7 +5553,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -5555,7 +5564,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>299</v>
       </c>
@@ -5566,7 +5575,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>304</v>
       </c>
@@ -5577,7 +5586,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>307</v>
       </c>
@@ -5588,7 +5597,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>310</v>
       </c>
@@ -5599,7 +5608,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>313</v>
       </c>
@@ -5610,7 +5619,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>316</v>
       </c>
@@ -5621,7 +5630,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>319</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>322</v>
       </c>
@@ -5643,7 +5652,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>325</v>
       </c>
@@ -5654,7 +5663,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>328</v>
       </c>
@@ -5665,7 +5674,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>331</v>
       </c>
@@ -5676,7 +5685,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>334</v>
       </c>
@@ -5687,7 +5696,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>337</v>
       </c>
@@ -5698,7 +5707,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>340</v>
       </c>
@@ -5709,7 +5718,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>343</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -5731,7 +5740,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>349</v>
       </c>
@@ -5742,7 +5751,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>352</v>
       </c>
@@ -5753,7 +5762,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>355</v>
       </c>
@@ -5764,7 +5773,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>358</v>
       </c>
@@ -5775,7 +5784,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>361</v>
       </c>
@@ -5786,7 +5795,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>364</v>
       </c>
@@ -5797,7 +5806,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -5808,7 +5817,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>370</v>
       </c>
@@ -5819,7 +5828,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>373</v>
       </c>
@@ -5830,7 +5839,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>375</v>
       </c>
@@ -5841,7 +5850,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>379</v>
       </c>
@@ -5852,7 +5861,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>382</v>
       </c>
@@ -5863,7 +5872,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>552</v>
       </c>
@@ -5874,7 +5883,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>388</v>
       </c>
@@ -5885,7 +5894,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>391</v>
       </c>
@@ -5896,7 +5905,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>394</v>
       </c>
@@ -5907,7 +5916,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>397</v>
       </c>
@@ -5918,7 +5927,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>400</v>
       </c>
@@ -5929,7 +5938,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>403</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>406</v>
       </c>
@@ -5951,7 +5960,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>409</v>
       </c>
@@ -5962,7 +5971,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>412</v>
       </c>
@@ -5973,7 +5982,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>415</v>
       </c>
@@ -5984,7 +5993,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>418</v>
       </c>
@@ -5995,7 +6004,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>421</v>
       </c>
@@ -6006,7 +6015,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>424</v>
       </c>
@@ -6017,7 +6026,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>425</v>
       </c>
@@ -6028,7 +6037,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>428</v>
       </c>
@@ -6039,7 +6048,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>431</v>
       </c>
@@ -6050,7 +6059,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>434</v>
       </c>
@@ -6061,7 +6070,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>437</v>
       </c>
@@ -6072,7 +6081,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>649</v>
       </c>
@@ -6083,7 +6092,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>440</v>
       </c>
@@ -6094,7 +6103,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>443</v>
       </c>
@@ -6105,7 +6114,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>446</v>
       </c>
@@ -6116,7 +6125,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>449</v>
       </c>
@@ -6127,7 +6136,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>452</v>
       </c>
@@ -6138,7 +6147,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>455</v>
       </c>
@@ -6149,7 +6158,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>458</v>
       </c>
@@ -6160,7 +6169,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>461</v>
       </c>
@@ -6171,7 +6180,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>464</v>
       </c>
@@ -6182,7 +6191,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>467</v>
       </c>
@@ -6193,7 +6202,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>470</v>
       </c>
@@ -6204,7 +6213,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>473</v>
       </c>
@@ -6215,7 +6224,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>476</v>
       </c>
@@ -6226,7 +6235,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>479</v>
       </c>
@@ -6237,7 +6246,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>482</v>
       </c>
@@ -6248,7 +6257,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>485</v>
       </c>
@@ -6259,7 +6268,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>489</v>
       </c>
@@ -6270,7 +6279,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>491</v>
       </c>
@@ -6281,7 +6290,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>494</v>
       </c>
@@ -6292,7 +6301,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>497</v>
       </c>
@@ -6303,7 +6312,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>500</v>
       </c>
@@ -6314,7 +6323,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>503</v>
       </c>
@@ -6325,7 +6334,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>506</v>
       </c>
@@ -6336,7 +6345,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>509</v>
       </c>
@@ -6347,7 +6356,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>512</v>
       </c>
@@ -6358,7 +6367,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>515</v>
       </c>
@@ -6369,7 +6378,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>518</v>
       </c>
@@ -6380,7 +6389,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>521</v>
       </c>
@@ -6391,7 +6400,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>525</v>
       </c>
@@ -6402,7 +6411,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="116" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>528</v>
       </c>
@@ -6413,7 +6422,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="117" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>531</v>
       </c>
@@ -6424,7 +6433,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>534</v>
       </c>
@@ -6435,7 +6444,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>536</v>
       </c>
@@ -6446,7 +6455,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>547</v>
       </c>
@@ -6457,7 +6466,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>550</v>
       </c>
@@ -6468,7 +6477,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>553</v>
       </c>
@@ -6479,7 +6488,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>555</v>
       </c>
@@ -6490,7 +6499,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="124" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>557</v>
       </c>
@@ -6501,7 +6510,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>560</v>
       </c>
@@ -6512,7 +6521,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>563</v>
       </c>
@@ -6523,7 +6532,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>566</v>
       </c>
@@ -6534,7 +6543,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>568</v>
       </c>
@@ -6545,7 +6554,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>571</v>
       </c>
@@ -6556,7 +6565,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>574</v>
       </c>
@@ -6567,7 +6576,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>577</v>
       </c>
@@ -6578,7 +6587,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>582</v>
       </c>
@@ -6589,7 +6598,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>583</v>
       </c>
@@ -6600,7 +6609,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>586</v>
       </c>
@@ -6611,7 +6620,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>597</v>
       </c>
@@ -6622,7 +6631,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>606</v>
       </c>
@@ -6633,7 +6642,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>609</v>
       </c>
@@ -6644,7 +6653,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:3" ht="25" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>613</v>
       </c>
@@ -6655,7 +6664,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>654</v>
       </c>
@@ -6666,7 +6675,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>657</v>
       </c>
@@ -6677,7 +6686,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>660</v>
       </c>
@@ -6688,7 +6697,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" s="12" t="s">
         <v>663</v>
       </c>
@@ -6699,7 +6708,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>666</v>
       </c>
@@ -6710,7 +6719,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>668</v>
       </c>
@@ -6721,7 +6730,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>670</v>
       </c>
@@ -6732,7 +6741,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>675</v>
       </c>
@@ -6743,7 +6752,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>676</v>
       </c>
@@ -6754,7 +6763,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="12" t="s">
         <v>683</v>
       </c>
@@ -6765,7 +6774,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>686</v>
       </c>
@@ -6774,6 +6783,17 @@
       </c>
       <c r="C149" s="11" t="s">
         <v>685</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="12" t="s">
+        <v>687</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>688</v>
+      </c>
+      <c r="C150" s="11" t="s">
+        <v>689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add spare parts categories to the app
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="692">
   <si>
     <t>comments</t>
   </si>
@@ -2171,6 +2171,12 @@
   </si>
   <si>
     <t>Número de serie:</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('maintenance_logs')</t>
+  </si>
+  <si>
+    <t>Maintenance Logs</t>
   </si>
 </sst>
 </file>
@@ -2734,7 +2740,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2849,9 +2855,31 @@
         <v>643</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>606</v>
+      </c>
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="17"/>
+      <c r="B12" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="15" t="s">
+        <v>643</v>
+      </c>
+    </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3077,10 +3105,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3111,6 +3139,17 @@
       </c>
       <c r="C2" s="4" t="s">
         <v>648</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>637</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>691</v>
       </c>
     </row>
   </sheetData>
@@ -5135,7 +5174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
+    <sheetView topLeftCell="A120" workbookViewId="0">
       <selection activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use birthdate for fields used to enter today's date
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="695">
   <si>
     <t>comments</t>
   </si>
@@ -2177,6 +2177,15 @@
   </si>
   <si>
     <t>Maintenance Logs</t>
+  </si>
+  <si>
+    <t>cold_room_maintenance_logs</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('cold_room_maintenance_logs')</t>
+  </si>
+  <si>
+    <t>Cold Room Maintenance Logs</t>
   </si>
 </sst>
 </file>
@@ -2700,7 +2709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2740,7 +2749,7 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2880,9 +2889,31 @@
         <v>643</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>692</v>
+      </c>
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:9" s="15" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17"/>
+      <c r="B15" s="18" t="s">
+        <v>693</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>644</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="15" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="15" t="s">
+        <v>643</v>
+      </c>
+    </row>
     <row r="17" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="59.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3105,16 +3136,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.453125" customWidth="1"/>
-    <col min="2" max="2" width="22.1796875" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
@@ -3150,6 +3181,17 @@
       </c>
       <c r="C3" s="4" t="s">
         <v>691</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>637</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>
@@ -3167,7 +3209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C181"/>
   <sheetViews>
-    <sheetView topLeftCell="A132" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A111" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix maintenance log detail views, add better layout, and translations
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500"/>
+    <workbookView xWindow="16310" yWindow="5030" windowWidth="25610" windowHeight="16070" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="framework_translations" sheetId="5" r:id="rId5"/>
     <sheet name="common_translations" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="713">
   <si>
     <t>comments</t>
   </si>
@@ -2186,6 +2186,60 @@
   </si>
   <si>
     <t>Cold Room Maintenance Logs</t>
+  </si>
+  <si>
+    <t>spare_parts_electrical</t>
+  </si>
+  <si>
+    <t>Spare Parts (Electrical):</t>
+  </si>
+  <si>
+    <t>spare_parts_hardware</t>
+  </si>
+  <si>
+    <t>Spare Parts (Hardware):</t>
+  </si>
+  <si>
+    <t>spare_parts_monitoring</t>
+  </si>
+  <si>
+    <t>Spare Parts (Monitoring):</t>
+  </si>
+  <si>
+    <t>spare_parts_power</t>
+  </si>
+  <si>
+    <t>Spare Parts (Power):</t>
+  </si>
+  <si>
+    <t>spare_parts_refrigeration</t>
+  </si>
+  <si>
+    <t>Spare Parts (Refrigeration):</t>
+  </si>
+  <si>
+    <t>spare_parts_solar</t>
+  </si>
+  <si>
+    <t>Spare Parts (Solar):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Eléctrico):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Hardware):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Vigilancia):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Energía):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Refrigeración):</t>
+  </si>
+  <si>
+    <t>Piezas De Repuesto (Solar):</t>
   </si>
 </sst>
 </file>
@@ -2709,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -5214,10 +5268,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C150"/>
+  <dimension ref="A1:C156"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="A151" sqref="A151"/>
+    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6877,6 +6931,72 @@
         <v>689</v>
       </c>
     </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>695</v>
+      </c>
+      <c r="B151" t="s">
+        <v>696</v>
+      </c>
+      <c r="C151" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>697</v>
+      </c>
+      <c r="B152" t="s">
+        <v>698</v>
+      </c>
+      <c r="C152" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>699</v>
+      </c>
+      <c r="B153" t="s">
+        <v>700</v>
+      </c>
+      <c r="C153" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>701</v>
+      </c>
+      <c r="B154" t="s">
+        <v>702</v>
+      </c>
+      <c r="C154" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>703</v>
+      </c>
+      <c r="B155" t="s">
+        <v>704</v>
+      </c>
+      <c r="C155" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>705</v>
+      </c>
+      <c r="B156" t="s">
+        <v>706</v>
+      </c>
+      <c r="C156" t="s">
+        <v>712</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Add units to health facility and refrigerator type detail view
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="721">
   <si>
     <t>comments</t>
   </si>
@@ -2240,6 +2240,30 @@
   </si>
   <si>
     <t>Piezas De Repuesto (Solar):</t>
+  </si>
+  <si>
+    <t>hours_per_day</t>
+  </si>
+  <si>
+    <t>hrs/day</t>
+  </si>
+  <si>
+    <t>hrs/día</t>
+  </si>
+  <si>
+    <t>weeks</t>
+  </si>
+  <si>
+    <t>semanas</t>
+  </si>
+  <si>
+    <t>km</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>liters_unit</t>
   </si>
 </sst>
 </file>
@@ -5268,10 +5292,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C156"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+      <selection activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -6997,6 +7021,50 @@
         <v>712</v>
       </c>
     </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>713</v>
+      </c>
+      <c r="B157" t="s">
+        <v>714</v>
+      </c>
+      <c r="C157" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>716</v>
+      </c>
+      <c r="B158" t="s">
+        <v>716</v>
+      </c>
+      <c r="C158" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>718</v>
+      </c>
+      <c r="B159" t="s">
+        <v>718</v>
+      </c>
+      <c r="C159" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>720</v>
+      </c>
+      <c r="B160" t="s">
+        <v>719</v>
+      </c>
+      <c r="C160" t="s">
+        <v>719</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed health facility to facility in refrigerator and cold room lists
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="721">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="724">
   <si>
     <t>comments</t>
   </si>
@@ -2264,6 +2264,15 @@
   </si>
   <si>
     <t>liters_unit</t>
+  </si>
+  <si>
+    <t>facility_no_colon</t>
+  </si>
+  <si>
+    <t>Facility</t>
+  </si>
+  <si>
+    <t>Institucion</t>
   </si>
 </sst>
 </file>
@@ -5292,10 +5301,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C160"/>
+  <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection activeCell="A160" sqref="A160"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -7065,6 +7074,17 @@
         <v>719</v>
       </c>
     </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>721</v>
+      </c>
+      <c r="B161" t="s">
+        <v>722</v>
+      </c>
+      <c r="C161" s="4" t="s">
+        <v>723</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Order the facility list views by facility_name
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1466" uniqueCount="965">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="971">
   <si>
     <t>comments</t>
   </si>
@@ -3000,6 +3000,24 @@
   </si>
   <si>
     <t>Hospital privado</t>
+  </si>
+  <si>
+    <t>view_map_of_all_health_facilities</t>
+  </si>
+  <si>
+    <t>View Map of All Health Facilities</t>
+  </si>
+  <si>
+    <t>view_list_of_all_health_facilities</t>
+  </si>
+  <si>
+    <t>View List of All Health Facilities</t>
+  </si>
+  <si>
+    <t>Ver mapa de todas las instalaciones de salud</t>
+  </si>
+  <si>
+    <t>Ver la lista de todas las instalaciones de salud</t>
   </si>
 </sst>
 </file>
@@ -6706,10 +6724,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C176" sqref="C176"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="C182" sqref="C182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -9059,6 +9077,28 @@
         <v>951</v>
       </c>
     </row>
+    <row r="176" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A176" t="s">
+        <v>965</v>
+      </c>
+      <c r="B176" t="s">
+        <v>966</v>
+      </c>
+      <c r="C176" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3">
+      <c r="A177" s="39" t="s">
+        <v>967</v>
+      </c>
+      <c r="B177" s="39" t="s">
+        <v>968</v>
+      </c>
+      <c r="C177" s="39" t="s">
+        <v>970</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Add temperature monitoring device to refrigerator detail view
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1472" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="974">
   <si>
     <t>comments</t>
   </si>
@@ -3018,6 +3018,16 @@
   </si>
   <si>
     <t>Ver la lista de todas las instalaciones de salud</t>
+  </si>
+  <si>
+    <t>temperature_monitoring_device</t>
+  </si>
+  <si>
+    <t>Temperature Monitoring Device?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+¿Dispositivo de monitoreo de temperatura?</t>
   </si>
 </sst>
 </file>
@@ -6724,10 +6734,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D177"/>
+  <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="C182" sqref="C182"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C178" sqref="C178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -9099,6 +9109,17 @@
         <v>970</v>
       </c>
     </row>
+    <row r="178" spans="1:3" ht="25">
+      <c r="A178" t="s">
+        <v>971</v>
+      </c>
+      <c r="B178" t="s">
+        <v>972</v>
+      </c>
+      <c r="C178" s="4" t="s">
+        <v>973</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Change notes to actions taken for the refrigerator and cold room maintenance logs
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1475" uniqueCount="974">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1478" uniqueCount="977">
   <si>
     <t>comments</t>
   </si>
@@ -3028,6 +3028,15 @@
   <si>
     <t xml:space="preserve">
 ¿Dispositivo de monitoreo de temperatura?</t>
+  </si>
+  <si>
+    <t>actions_taken</t>
+  </si>
+  <si>
+    <t>Actions Taken:</t>
+  </si>
+  <si>
+    <t>Acciones tomadas:</t>
   </si>
 </sst>
 </file>
@@ -6734,10 +6743,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D178"/>
+  <dimension ref="A1:D179"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="C178" sqref="C178"/>
+    <sheetView tabSelected="1" topLeftCell="A162" workbookViewId="0">
+      <selection activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5"/>
@@ -9120,6 +9129,17 @@
         <v>973</v>
       </c>
     </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
+        <v>974</v>
+      </c>
+      <c r="B179" t="s">
+        <v>975</v>
+      </c>
+      <c r="C179" t="s">
+        <v>976</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Add refrigerator temperature data in
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="1068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="1107">
   <si>
     <t>comments</t>
   </si>
@@ -3310,6 +3310,123 @@
   </si>
   <si>
     <t>El movimiento no se realizará: la nueva identificación de la instalación no es válida</t>
+  </si>
+  <si>
+    <t>refrigerator_temperature_data</t>
+  </si>
+  <si>
+    <t>average_temperature</t>
+  </si>
+  <si>
+    <t>lower_alarm_status</t>
+  </si>
+  <si>
+    <t>minimum_temperature</t>
+  </si>
+  <si>
+    <t>cumulative_duration_below_lower_limit</t>
+  </si>
+  <si>
+    <t>upper_alarm_status</t>
+  </si>
+  <si>
+    <t>maximum_temperature</t>
+  </si>
+  <si>
+    <t>cumulative_duration_above_upper_limit</t>
+  </si>
+  <si>
+    <t>edit_temperature_data</t>
+  </si>
+  <si>
+    <t>delete_temperature_data</t>
+  </si>
+  <si>
+    <t>Refrigerator Temperature Data</t>
+  </si>
+  <si>
+    <t>Edit Temperature Data</t>
+  </si>
+  <si>
+    <t>Delete Temperature Data</t>
+  </si>
+  <si>
+    <t>Average Temperature:</t>
+  </si>
+  <si>
+    <t>Minimum Temperature:</t>
+  </si>
+  <si>
+    <t>Maximum Temperature:</t>
+  </si>
+  <si>
+    <t>Lower Alarm Status:</t>
+  </si>
+  <si>
+    <t>Cumulative Duration Below Lower Limit:</t>
+  </si>
+  <si>
+    <t>Upper Alarm Status:</t>
+  </si>
+  <si>
+    <t>Cumulative Duration Above Upper Limit:</t>
+  </si>
+  <si>
+    <t>Datos de temperatura del refrigerador</t>
+  </si>
+  <si>
+    <t>Temperatura media:</t>
+  </si>
+  <si>
+    <t>Estado de alarma inferior:</t>
+  </si>
+  <si>
+    <t>Temperatura mínima:</t>
+  </si>
+  <si>
+    <t>Duración acumulativa por debajo del límite inferior:</t>
+  </si>
+  <si>
+    <t>Estado de alarma superior:</t>
+  </si>
+  <si>
+    <t>Temperatura máxima:</t>
+  </si>
+  <si>
+    <t>Duración acumulativa por encima del límite superior:</t>
+  </si>
+  <si>
+    <t>Editar datos de temperatura</t>
+  </si>
+  <si>
+    <t>Eliminar datos de temperatura</t>
+  </si>
+  <si>
+    <t>add_temperature_data</t>
+  </si>
+  <si>
+    <t>view_all_temperature_data</t>
+  </si>
+  <si>
+    <t>Add Temperature Data</t>
+  </si>
+  <si>
+    <t>View All Temperature Data</t>
+  </si>
+  <si>
+    <t>Agregar datos de temperatura</t>
+  </si>
+  <si>
+    <t>Ver todos los datos de temperatura</t>
+  </si>
+  <si>
+    <t>are_you_sure_you_want_to_delete_this_temperature_data</t>
+  </si>
+  <si>
+    <t>Are you sure you want to delete this temperature data?</t>
+  </si>
+  <si>
+    <t>¿Está seguro de que desea eliminar estos datos de temperatura?</t>
   </si>
 </sst>
 </file>
@@ -7002,15 +7119,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D212"/>
+  <dimension ref="A1:D225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="C215" sqref="C215"/>
+    <sheetView tabSelected="1" topLeftCell="A204" workbookViewId="0">
+      <selection activeCell="C229" sqref="C229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="49" customWidth="1"/>
+    <col min="1" max="1" width="52.85546875" customWidth="1"/>
     <col min="2" max="2" width="50.140625" customWidth="1"/>
     <col min="3" max="3" width="61.85546875" customWidth="1"/>
     <col min="4" max="4" width="37.28515625" customWidth="1"/>
@@ -9768,6 +9885,149 @@
         <v>1067</v>
       </c>
     </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B213" s="39" t="s">
+        <v>1078</v>
+      </c>
+      <c r="C213" s="39" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3">
+      <c r="A214" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B214" s="39" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C214" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3">
+      <c r="A215" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B215" s="39" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C215" t="s">
+        <v>1090</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3">
+      <c r="A216" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B216" s="39" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C216" t="s">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B217" s="39" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C217" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" s="39" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B218" s="39" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C218" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" s="39" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B219" s="39" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C219" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B220" s="39" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C220" t="s">
+        <v>1095</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" s="39" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B221" s="39" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C221" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3">
+      <c r="A222" s="39" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B222" s="39" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C222" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" s="39" t="s">
+        <v>1098</v>
+      </c>
+      <c r="B223" s="39" t="s">
+        <v>1100</v>
+      </c>
+      <c r="C223" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3">
+      <c r="A224" s="39" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B224" s="39" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C224" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
+      <c r="A225" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B225" s="39" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C225" s="39" t="s">
+        <v>1106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>

<commit_message>
Add confirmation dialog to refrigerator_move functionality and edit some fields
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7635" windowHeight="135" tabRatio="500" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7640" windowHeight="140" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1610" uniqueCount="1107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1613" uniqueCount="1110">
   <si>
     <t>comments</t>
   </si>
@@ -3427,6 +3427,15 @@
   </si>
   <si>
     <t>¿Está seguro de que desea eliminar estos datos de temperatura?</t>
+  </si>
+  <si>
+    <t>move_performed_successfully</t>
+  </si>
+  <si>
+    <t>Move performed successfully</t>
+  </si>
+  <si>
+    <t>Movimiento realizado con éxito</t>
   </si>
 </sst>
 </file>
@@ -4027,11 +4036,11 @@
       <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.81640625" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" customWidth="1"/>
+    <col min="3" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4066,20 +4075,20 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="101.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.1796875" customWidth="1"/>
+    <col min="2" max="2" width="101.1796875" customWidth="1"/>
+    <col min="3" max="3" width="22.1796875" customWidth="1"/>
+    <col min="4" max="4" width="46.1796875" customWidth="1"/>
     <col min="5" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="8" max="8" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="1025" width="17.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.81640625" customWidth="1"/>
+    <col min="8" max="8" width="31.453125" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
+    <col min="10" max="1025" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17.45" customHeight="1">
+    <row r="1" spans="1:9" ht="17.5" customHeight="1">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -4115,7 +4124,7 @@
       </c>
       <c r="I2" s="15"/>
     </row>
-    <row r="3" spans="1:9" s="14" customFormat="1" ht="17.45" customHeight="1">
+    <row r="3" spans="1:9" s="14" customFormat="1" ht="17.5" customHeight="1">
       <c r="E3" s="14" t="s">
         <v>633</v>
       </c>
@@ -4228,71 +4237,71 @@
         <v>640</v>
       </c>
     </row>
-    <row r="17" ht="17.45" customHeight="1"/>
+    <row r="17" ht="17.5" customHeight="1"/>
     <row r="18" ht="59.25" customHeight="1"/>
     <row r="19" ht="17.25" customHeight="1"/>
-    <row r="20" ht="17.45" customHeight="1"/>
+    <row r="20" ht="17.5" customHeight="1"/>
     <row r="21" ht="66" customHeight="1"/>
     <row r="22" ht="17.25" customHeight="1"/>
-    <row r="23" ht="17.45" customHeight="1"/>
+    <row r="23" ht="17.5" customHeight="1"/>
     <row r="24" ht="66" customHeight="1"/>
     <row r="25" ht="17.25" customHeight="1"/>
-    <row r="26" ht="17.45" customHeight="1"/>
+    <row r="26" ht="17.5" customHeight="1"/>
     <row r="27" ht="66" customHeight="1"/>
     <row r="28" ht="17.25" customHeight="1"/>
-    <row r="29" ht="17.45" customHeight="1"/>
+    <row r="29" ht="17.5" customHeight="1"/>
     <row r="30" ht="66" customHeight="1"/>
     <row r="31" ht="17.25" customHeight="1"/>
-    <row r="32" ht="17.45" customHeight="1"/>
+    <row r="32" ht="17.5" customHeight="1"/>
     <row r="33" ht="66" customHeight="1"/>
     <row r="34" ht="17.25" customHeight="1"/>
-    <row r="35" ht="17.45" customHeight="1"/>
+    <row r="35" ht="17.5" customHeight="1"/>
     <row r="36" ht="66" customHeight="1"/>
     <row r="37" ht="17.25" customHeight="1"/>
-    <row r="38" ht="17.45" customHeight="1"/>
+    <row r="38" ht="17.5" customHeight="1"/>
     <row r="39" ht="66" customHeight="1"/>
     <row r="40" ht="17.25" customHeight="1"/>
-    <row r="41" ht="17.45" customHeight="1"/>
+    <row r="41" ht="17.5" customHeight="1"/>
     <row r="42" ht="66" customHeight="1"/>
     <row r="43" ht="17.25" customHeight="1"/>
-    <row r="44" ht="17.45" customHeight="1"/>
+    <row r="44" ht="17.5" customHeight="1"/>
     <row r="45" ht="66" customHeight="1"/>
     <row r="46" ht="17.25" customHeight="1"/>
-    <row r="47" ht="17.45" customHeight="1"/>
+    <row r="47" ht="17.5" customHeight="1"/>
     <row r="48" ht="66" customHeight="1"/>
     <row r="49" ht="17.25" customHeight="1"/>
-    <row r="50" ht="17.45" customHeight="1"/>
+    <row r="50" ht="17.5" customHeight="1"/>
     <row r="51" ht="66" customHeight="1"/>
     <row r="52" ht="17.25" customHeight="1"/>
-    <row r="53" ht="17.45" customHeight="1"/>
+    <row r="53" ht="17.5" customHeight="1"/>
     <row r="54" ht="66" customHeight="1"/>
     <row r="55" ht="17.25" customHeight="1"/>
-    <row r="56" ht="17.45" customHeight="1"/>
+    <row r="56" ht="17.5" customHeight="1"/>
     <row r="57" ht="66" customHeight="1"/>
     <row r="58" ht="17.25" customHeight="1"/>
-    <row r="59" ht="17.45" customHeight="1"/>
+    <row r="59" ht="17.5" customHeight="1"/>
     <row r="60" ht="66" customHeight="1"/>
     <row r="61" ht="17.25" customHeight="1"/>
-    <row r="62" ht="17.45" customHeight="1"/>
+    <row r="62" ht="17.5" customHeight="1"/>
     <row r="63" ht="66" customHeight="1"/>
     <row r="64" ht="17.25" customHeight="1"/>
-    <row r="65" ht="17.45" customHeight="1"/>
+    <row r="65" ht="17.5" customHeight="1"/>
     <row r="66" ht="66" customHeight="1"/>
     <row r="67" ht="17.25" customHeight="1"/>
-    <row r="68" ht="17.45" customHeight="1"/>
+    <row r="68" ht="17.5" customHeight="1"/>
     <row r="69" ht="66" customHeight="1"/>
     <row r="70" ht="17.25" customHeight="1"/>
-    <row r="71" ht="17.45" customHeight="1"/>
+    <row r="71" ht="17.5" customHeight="1"/>
     <row r="72" ht="66" customHeight="1"/>
-    <row r="73" ht="17.100000000000001" customHeight="1"/>
-    <row r="75" ht="62.1" customHeight="1"/>
-    <row r="78" ht="62.1" customHeight="1"/>
+    <row r="73" ht="17.149999999999999" customHeight="1"/>
+    <row r="75" ht="62.15" customHeight="1"/>
+    <row r="78" ht="62.15" customHeight="1"/>
     <row r="80" ht="12" customHeight="1"/>
-    <row r="81" ht="57.95" customHeight="1"/>
+    <row r="81" ht="58" customHeight="1"/>
     <row r="83" ht="12" customHeight="1"/>
-    <row r="84" ht="57.95" customHeight="1"/>
+    <row r="84" ht="58" customHeight="1"/>
     <row r="86" ht="12" customHeight="1"/>
-    <row r="87" ht="57.95" customHeight="1"/>
+    <row r="87" ht="58" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4312,15 +4321,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="4" width="24.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="24" customWidth="1"/>
-    <col min="6" max="7" width="24.85546875" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" style="24" customWidth="1"/>
-    <col min="9" max="9" width="41.140625" customWidth="1"/>
-    <col min="10" max="1027" width="17.140625" customWidth="1"/>
+    <col min="1" max="2" width="17.1796875" customWidth="1"/>
+    <col min="3" max="4" width="24.81640625" customWidth="1"/>
+    <col min="5" max="5" width="24.81640625" style="24" customWidth="1"/>
+    <col min="6" max="7" width="24.81640625" customWidth="1"/>
+    <col min="8" max="8" width="24.81640625" style="24" customWidth="1"/>
+    <col min="9" max="9" width="41.1796875" customWidth="1"/>
+    <col min="10" max="1027" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1">
@@ -4397,7 +4406,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="27.95" customHeight="1">
+    <row r="5" spans="1:10" ht="28" customHeight="1">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -4490,12 +4499,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="31.54296875" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
-    <col min="4" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="4" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -4531,7 +4540,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.45" customHeight="1">
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
       <c r="A4" t="s">
         <v>634</v>
       </c>
@@ -4561,16 +4570,16 @@
       <selection activeCell="A174" sqref="A174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" customWidth="1"/>
-    <col min="2" max="2" width="52.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="1025" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="49.81640625" customWidth="1"/>
+    <col min="2" max="2" width="52.1796875" customWidth="1"/>
+    <col min="3" max="3" width="33.1796875" customWidth="1"/>
+    <col min="4" max="4" width="23.54296875" customWidth="1"/>
+    <col min="5" max="1025" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12.95" customHeight="1">
+    <row r="1" spans="1:4" ht="13" customHeight="1">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -4584,7 +4593,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="12.95" customHeight="1">
+    <row r="2" spans="1:4" ht="13" customHeight="1">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -4598,7 +4607,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="12.95" customHeight="1">
+    <row r="3" spans="1:4" ht="13" customHeight="1">
       <c r="A3" t="s">
         <v>44</v>
       </c>
@@ -4612,7 +4621,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="12.95" customHeight="1">
+    <row r="4" spans="1:4" ht="13" customHeight="1">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -4626,7 +4635,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12.95" customHeight="1">
+    <row r="5" spans="1:4" ht="13" customHeight="1">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -4640,7 +4649,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12.95" customHeight="1">
+    <row r="6" spans="1:4" ht="13" customHeight="1">
       <c r="A6" t="s">
         <v>53</v>
       </c>
@@ -4710,7 +4719,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="13.7" customHeight="1">
+    <row r="11" spans="1:4" ht="13.75" customHeight="1">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -4724,7 +4733,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="13.7" customHeight="1">
+    <row r="12" spans="1:4" ht="13.75" customHeight="1">
       <c r="A12" t="s">
         <v>71</v>
       </c>
@@ -4948,7 +4957,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="28.35" customHeight="1">
+    <row r="28" spans="1:4" ht="28.4" customHeight="1">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -5044,7 +5053,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="242.25">
+    <row r="36" spans="1:4" ht="237.5">
       <c r="A36" t="s">
         <v>138</v>
       </c>
@@ -5240,7 +5249,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="12.95" customHeight="1">
+    <row r="50" spans="1:4" ht="13" customHeight="1">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -5380,7 +5389,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" ht="38.25">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="37.5">
       <c r="A60" s="7" t="s">
         <v>620</v>
       </c>
@@ -5394,7 +5403,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="6" customFormat="1" ht="25.5">
+    <row r="61" spans="1:4" s="6" customFormat="1" ht="25">
       <c r="A61" s="7" t="s">
         <v>613</v>
       </c>
@@ -5436,7 +5445,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="25.5">
+    <row r="64" spans="1:4" ht="25">
       <c r="A64" t="s">
         <v>199</v>
       </c>
@@ -5548,7 +5557,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="25.5">
+    <row r="72" spans="1:4" ht="25">
       <c r="A72" t="s">
         <v>223</v>
       </c>
@@ -5562,7 +5571,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="25.5">
+    <row r="73" spans="1:4" ht="25">
       <c r="A73" t="s">
         <v>224</v>
       </c>
@@ -5590,7 +5599,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="25.5">
+    <row r="75" spans="1:4" ht="25">
       <c r="A75" t="s">
         <v>230</v>
       </c>
@@ -5618,7 +5627,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="25.5">
+    <row r="77" spans="1:4" ht="25">
       <c r="A77" t="s">
         <v>236</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="25.5">
+    <row r="78" spans="1:4" ht="25">
       <c r="A78" t="s">
         <v>239</v>
       </c>
@@ -5702,7 +5711,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="25.5">
+    <row r="83" spans="1:4" ht="25">
       <c r="A83" t="s">
         <v>254</v>
       </c>
@@ -5758,7 +5767,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="25.5">
+    <row r="87" spans="1:4">
       <c r="A87" t="s">
         <v>265</v>
       </c>
@@ -5772,7 +5781,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="25.5">
+    <row r="88" spans="1:4" ht="25">
       <c r="A88" t="s">
         <v>267</v>
       </c>
@@ -5786,7 +5795,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="25.5">
+    <row r="89" spans="1:4" ht="25">
       <c r="A89" t="s">
         <v>271</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="25.5">
+    <row r="90" spans="1:4" ht="25">
       <c r="A90" t="s">
         <v>274</v>
       </c>
@@ -5814,7 +5823,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="38.25">
+    <row r="91" spans="1:4" ht="37.5">
       <c r="A91" t="s">
         <v>277</v>
       </c>
@@ -5828,7 +5837,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="25.5">
+    <row r="92" spans="1:4" ht="25">
       <c r="A92" t="s">
         <v>280</v>
       </c>
@@ -5842,7 +5851,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="25.5">
+    <row r="93" spans="1:4" ht="25">
       <c r="A93" t="s">
         <v>283</v>
       </c>
@@ -5926,7 +5935,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="25.5">
+    <row r="99" spans="1:4" ht="25">
       <c r="A99" t="s">
         <v>299</v>
       </c>
@@ -5940,7 +5949,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="25.5">
+    <row r="100" spans="1:4" ht="25">
       <c r="A100" t="s">
         <v>304</v>
       </c>
@@ -5954,7 +5963,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="25.5">
+    <row r="101" spans="1:4" ht="25">
       <c r="A101" t="s">
         <v>307</v>
       </c>
@@ -5996,7 +6005,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="25.5">
+    <row r="104" spans="1:4" ht="25">
       <c r="A104" t="s">
         <v>316</v>
       </c>
@@ -6010,7 +6019,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="25.5">
+    <row r="105" spans="1:4" ht="25">
       <c r="A105" t="s">
         <v>319</v>
       </c>
@@ -6066,7 +6075,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="25.5">
+    <row r="109" spans="1:4" ht="25">
       <c r="A109" t="s">
         <v>331</v>
       </c>
@@ -6080,7 +6089,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="51">
+    <row r="110" spans="1:4" ht="37.5">
       <c r="A110" t="s">
         <v>334</v>
       </c>
@@ -6094,7 +6103,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="25.5">
+    <row r="111" spans="1:4" ht="25">
       <c r="A111" t="s">
         <v>337</v>
       </c>
@@ -6108,7 +6117,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="25.5">
+    <row r="112" spans="1:4" ht="25">
       <c r="A112" t="s">
         <v>340</v>
       </c>
@@ -6178,7 +6187,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="117" spans="1:4" ht="25.5">
+    <row r="117" spans="1:4" ht="25">
       <c r="A117" t="s">
         <v>355</v>
       </c>
@@ -6206,7 +6215,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="25.5">
+    <row r="119" spans="1:4" ht="25">
       <c r="A119" t="s">
         <v>361</v>
       </c>
@@ -6262,7 +6271,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="25.5">
+    <row r="123" spans="1:4" ht="25">
       <c r="A123" t="s">
         <v>373</v>
       </c>
@@ -6276,7 +6285,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="25.5">
+    <row r="124" spans="1:4" ht="25">
       <c r="A124" t="s">
         <v>375</v>
       </c>
@@ -6290,7 +6299,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="25.5">
+    <row r="125" spans="1:4" ht="25">
       <c r="A125" t="s">
         <v>379</v>
       </c>
@@ -6346,7 +6355,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="129" spans="1:4" ht="25.5">
+    <row r="129" spans="1:4">
       <c r="A129" t="s">
         <v>391</v>
       </c>
@@ -6360,7 +6369,7 @@
         <v>789</v>
   